<commit_message>
TFS 9544 - New Subcoaching Reason for Supervisor Module
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C39255
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="132" windowWidth="22992" windowHeight="12840" firstSheet="2" activeTab="8"/>
+    <workbookView xWindow="480" yWindow="132" windowWidth="22992" windowHeight="12840"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_History" sheetId="14" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3378" uniqueCount="900">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3383" uniqueCount="902">
   <si>
     <t>SourceID</t>
   </si>
@@ -2746,6 +2746,12 @@
   </si>
   <si>
     <t>Set Arlington to Inactive in DIM Site table and WISO13 to 0 for all modules in Employee selection table</t>
+  </si>
+  <si>
+    <t>Add ‘Supervisor Callback’ under ‘CCO Processes and Procedures’ in Supervisor module</t>
+  </si>
+  <si>
+    <t>Supervisor Callback</t>
   </si>
 </sst>
 </file>
@@ -3117,10 +3123,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E64"/>
+  <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="E66" sqref="E66"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4197,6 +4203,23 @@
       </c>
       <c r="E64" t="s">
         <v>899</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>57</v>
+      </c>
+      <c r="B65" s="1">
+        <v>43098</v>
+      </c>
+      <c r="C65" t="s">
+        <v>432</v>
+      </c>
+      <c r="D65">
+        <v>9544</v>
+      </c>
+      <c r="E65" t="s">
+        <v>900</v>
       </c>
     </row>
   </sheetData>
@@ -5622,10 +5645,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P307"/>
+  <dimension ref="A1:P308"/>
   <sheetViews>
-    <sheetView topLeftCell="A282" workbookViewId="0">
-      <selection activeCell="A307" sqref="A307:P307"/>
+    <sheetView topLeftCell="A290" workbookViewId="0">
+      <selection activeCell="A308" sqref="A308:P308"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20934,52 +20957,102 @@
       </c>
     </row>
     <row r="307" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A307" s="5">
+      <c r="A307">
         <v>3</v>
       </c>
-      <c r="B307" s="5" t="s">
+      <c r="B307" t="s">
         <v>86</v>
       </c>
-      <c r="C307" s="5">
+      <c r="C307">
         <v>243</v>
       </c>
-      <c r="D307" s="5" t="s">
+      <c r="D307" t="s">
         <v>897</v>
       </c>
-      <c r="E307" s="5">
-        <v>1</v>
-      </c>
-      <c r="F307" s="5">
-        <v>1</v>
-      </c>
-      <c r="G307" s="5">
-        <v>1</v>
-      </c>
-      <c r="H307" s="5">
-        <v>1</v>
-      </c>
-      <c r="I307" s="5">
-        <v>1</v>
-      </c>
-      <c r="J307" s="5">
-        <v>1</v>
-      </c>
-      <c r="K307" s="5">
-        <v>0</v>
-      </c>
-      <c r="L307" s="5">
-        <v>1</v>
-      </c>
-      <c r="M307" s="5">
-        <v>0</v>
-      </c>
-      <c r="N307" s="5">
-        <v>0</v>
-      </c>
-      <c r="O307" s="5">
-        <v>0</v>
-      </c>
-      <c r="P307" s="5">
+      <c r="E307">
+        <v>1</v>
+      </c>
+      <c r="F307">
+        <v>1</v>
+      </c>
+      <c r="G307">
+        <v>1</v>
+      </c>
+      <c r="H307">
+        <v>1</v>
+      </c>
+      <c r="I307">
+        <v>1</v>
+      </c>
+      <c r="J307">
+        <v>1</v>
+      </c>
+      <c r="K307">
+        <v>0</v>
+      </c>
+      <c r="L307">
+        <v>1</v>
+      </c>
+      <c r="M307">
+        <v>0</v>
+      </c>
+      <c r="N307">
+        <v>0</v>
+      </c>
+      <c r="O307">
+        <v>0</v>
+      </c>
+      <c r="P307">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="308" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A308" s="5">
+        <v>4</v>
+      </c>
+      <c r="B308" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="C308" s="5">
+        <v>244</v>
+      </c>
+      <c r="D308" s="5" t="s">
+        <v>901</v>
+      </c>
+      <c r="E308" s="5">
+        <v>1</v>
+      </c>
+      <c r="F308" s="5">
+        <v>1</v>
+      </c>
+      <c r="G308" s="5">
+        <v>1</v>
+      </c>
+      <c r="H308" s="5">
+        <v>1</v>
+      </c>
+      <c r="I308" s="5">
+        <v>1</v>
+      </c>
+      <c r="J308" s="5">
+        <v>0</v>
+      </c>
+      <c r="K308" s="5">
+        <v>0</v>
+      </c>
+      <c r="L308" s="5">
+        <v>1</v>
+      </c>
+      <c r="M308" s="5">
+        <v>0</v>
+      </c>
+      <c r="N308" s="5">
+        <v>0</v>
+      </c>
+      <c r="O308" s="5">
+        <v>0</v>
+      </c>
+      <c r="P308" s="5">
         <v>0</v>
       </c>
     </row>
@@ -32242,10 +32315,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B245"/>
+  <dimension ref="A1:B246"/>
   <sheetViews>
     <sheetView topLeftCell="A230" workbookViewId="0">
-      <selection activeCell="B245" sqref="A245:B245"/>
+      <selection activeCell="A246" sqref="A246"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -34207,11 +34280,19 @@
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A245" s="5">
+      <c r="A245">
         <v>243</v>
       </c>
-      <c r="B245" s="5" t="s">
+      <c r="B245" t="s">
         <v>897</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A246" s="5">
+        <v>244</v>
+      </c>
+      <c r="B246" s="5" t="s">
+        <v>901</v>
       </c>
     </row>
   </sheetData>
@@ -35004,7 +35085,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>

</xml_diff>

<commit_message>
TFS 9511 - New pilot question in CSR Survey
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C39467
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
@@ -32,8 +32,9 @@
     <sheet name="Survey_DIM_Question" sheetId="18" r:id="rId18"/>
     <sheet name="Survey_DIM_Response" sheetId="19" r:id="rId19"/>
     <sheet name="Survey_DIM_QAnswer" sheetId="20" r:id="rId20"/>
-    <sheet name="HR_Access" sheetId="21" r:id="rId21"/>
-    <sheet name="NPN Description" sheetId="23" r:id="rId22"/>
+    <sheet name="Survey_Sites" sheetId="24" r:id="rId21"/>
+    <sheet name="HR_Access" sheetId="21" r:id="rId22"/>
+    <sheet name="NPN Description" sheetId="23" r:id="rId23"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">Coaching_Reason_Selection!$A$1:$P$292</definedName>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3383" uniqueCount="902">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3434" uniqueCount="912">
   <si>
     <t>SourceID</t>
   </si>
@@ -2752,6 +2753,36 @@
   </si>
   <si>
     <t>Supervisor Callback</t>
+  </si>
+  <si>
+    <t>isPilot</t>
+  </si>
+  <si>
+    <t>How prepared was your supervisor during your coaching session?| Please explain below.</t>
+  </si>
+  <si>
+    <t>Hot Topic question</t>
+  </si>
+  <si>
+    <t>1 - Very Unprepared</t>
+  </si>
+  <si>
+    <t>2 - Unprepared</t>
+  </si>
+  <si>
+    <t>3 - Neither Prepared or Unprepared</t>
+  </si>
+  <si>
+    <t>4 - Prepared</t>
+  </si>
+  <si>
+    <t>5 - Very Prepared</t>
+  </si>
+  <si>
+    <t>ResponseOrder</t>
+  </si>
+  <si>
+    <t>Pilot Project to have 6th survey question in eCoaching. Added records to Survey Question DIM, Response DIM and Survey Qanswer. Added new tab Survey_Sites</t>
   </si>
 </sst>
 </file>
@@ -2810,7 +2841,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2819,6 +2850,7 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3123,11 +3155,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E65"/>
+  <dimension ref="A1:E66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -4220,6 +4250,23 @@
       </c>
       <c r="E65" t="s">
         <v>900</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>58</v>
+      </c>
+      <c r="B66" s="1">
+        <v>43129</v>
+      </c>
+      <c r="C66" t="s">
+        <v>432</v>
+      </c>
+      <c r="D66">
+        <v>9511</v>
+      </c>
+      <c r="E66" t="s">
+        <v>911</v>
       </c>
     </row>
   </sheetData>
@@ -27922,10 +27969,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+      <selection activeCell="I1" sqref="I1:I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -27938,7 +27985,7 @@
     <col min="8" max="8" width="22" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>711</v>
       </c>
@@ -27963,8 +28010,11 @@
       <c r="H1" s="4" t="s">
         <v>709</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" s="5" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>-1</v>
       </c>
@@ -27989,8 +28039,11 @@
       <c r="H2" s="4">
         <v>42248</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -28015,8 +28068,11 @@
       <c r="H3" s="4">
         <v>42248</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I3" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -28041,8 +28097,11 @@
       <c r="H4" s="4">
         <v>42248</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I4" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -28067,8 +28126,11 @@
       <c r="H5" s="4">
         <v>42248</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I5" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -28093,8 +28155,11 @@
       <c r="H6" s="4">
         <v>42248</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I6" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -28118,6 +28183,67 @@
       </c>
       <c r="H7" s="4">
         <v>42248</v>
+      </c>
+      <c r="I7" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>904</v>
+      </c>
+      <c r="C8">
+        <v>6</v>
+      </c>
+      <c r="D8">
+        <v>20150901</v>
+      </c>
+      <c r="E8">
+        <v>20150930</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8" s="4">
+        <v>42248</v>
+      </c>
+      <c r="I8" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="5">
+        <v>7</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>903</v>
+      </c>
+      <c r="C9" s="5">
+        <v>7</v>
+      </c>
+      <c r="D9" s="5">
+        <v>20180201</v>
+      </c>
+      <c r="E9" s="5">
+        <v>99991231</v>
+      </c>
+      <c r="F9" s="5">
+        <v>0</v>
+      </c>
+      <c r="G9" s="5">
+        <v>1</v>
+      </c>
+      <c r="H9" s="6">
+        <v>43132</v>
+      </c>
+      <c r="I9" s="5">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -28128,9 +28254,11 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:D19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -28336,6 +28464,76 @@
         <v>42248</v>
       </c>
     </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="5">
+        <v>13</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>905</v>
+      </c>
+      <c r="C15" s="5">
+        <v>1</v>
+      </c>
+      <c r="D15" s="6">
+        <v>43132</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="5">
+        <v>14</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>906</v>
+      </c>
+      <c r="C16" s="5">
+        <v>1</v>
+      </c>
+      <c r="D16" s="6">
+        <v>43132</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="5">
+        <v>15</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>907</v>
+      </c>
+      <c r="C17" s="5">
+        <v>1</v>
+      </c>
+      <c r="D17" s="6">
+        <v>43132</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="5">
+        <v>16</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>908</v>
+      </c>
+      <c r="C18" s="5">
+        <v>1</v>
+      </c>
+      <c r="D18" s="6">
+        <v>43132</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="5">
+        <v>17</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>909</v>
+      </c>
+      <c r="C19" s="5">
+        <v>1</v>
+      </c>
+      <c r="D19" s="6">
+        <v>43132</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -28346,7 +28544,7 @@
   <dimension ref="A1:I69"/>
   <sheetViews>
     <sheetView topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69:I69"/>
+      <selection activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -30329,31 +30527,31 @@
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A69" s="5">
+      <c r="A69">
         <v>233</v>
       </c>
-      <c r="B69" s="5" t="s">
+      <c r="B69" t="s">
         <v>3</v>
       </c>
-      <c r="C69" s="5" t="s">
+      <c r="C69" t="s">
         <v>828</v>
       </c>
-      <c r="D69" s="5">
-        <v>1</v>
-      </c>
-      <c r="E69" s="5">
-        <v>0</v>
-      </c>
-      <c r="F69" s="5">
-        <v>0</v>
-      </c>
-      <c r="G69" s="5">
-        <v>0</v>
-      </c>
-      <c r="H69" s="5">
-        <v>0</v>
-      </c>
-      <c r="I69" s="5">
+      <c r="D69">
+        <v>1</v>
+      </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
+      <c r="F69">
+        <v>0</v>
+      </c>
+      <c r="G69">
+        <v>0</v>
+      </c>
+      <c r="H69">
+        <v>0</v>
+      </c>
+      <c r="I69">
         <v>0</v>
       </c>
     </row>
@@ -30364,16 +30562,18 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:M25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="11" max="11" width="24" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>705</v>
       </c>
@@ -30407,8 +30607,14 @@
       <c r="K1" s="4" t="s">
         <v>709</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L1" t="s">
+        <v>902</v>
+      </c>
+      <c r="M1" t="s">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -30442,8 +30648,14 @@
       <c r="K2" s="4">
         <v>42248</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -30477,8 +30689,14 @@
       <c r="K3" s="4">
         <v>42248</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -30512,8 +30730,14 @@
       <c r="K4" s="4">
         <v>42248</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -30547,8 +30771,14 @@
       <c r="K5" s="4">
         <v>42248</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -30582,8 +30812,14 @@
       <c r="K6" s="4">
         <v>42248</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -30617,8 +30853,14 @@
       <c r="K7" s="4">
         <v>42248</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -30652,8 +30894,14 @@
       <c r="K8" s="4">
         <v>42248</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
@@ -30687,8 +30935,14 @@
       <c r="K9" s="4">
         <v>42248</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
@@ -30722,8 +30976,14 @@
       <c r="K10" s="4">
         <v>42248</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
@@ -30757,8 +31017,14 @@
       <c r="K11" s="4">
         <v>42248</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1</v>
       </c>
@@ -30792,8 +31058,14 @@
       <c r="K12" s="4">
         <v>42248</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1</v>
       </c>
@@ -30827,8 +31099,14 @@
       <c r="K13" s="4">
         <v>42248</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>1</v>
       </c>
@@ -30862,8 +31140,14 @@
       <c r="K14" s="4">
         <v>42248</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1</v>
       </c>
@@ -30897,8 +31181,14 @@
       <c r="K15" s="4">
         <v>42248</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1</v>
       </c>
@@ -30932,8 +31222,14 @@
       <c r="K16" s="4">
         <v>42248</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1</v>
       </c>
@@ -30967,8 +31263,14 @@
       <c r="K17" s="4">
         <v>42248</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1</v>
       </c>
@@ -31001,6 +31303,299 @@
       </c>
       <c r="K18" s="4">
         <v>42248</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19">
+        <v>6</v>
+      </c>
+      <c r="C19">
+        <v>6</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>714</v>
+      </c>
+      <c r="F19" t="s">
+        <v>730</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>20150901</v>
+      </c>
+      <c r="I19">
+        <v>20150930</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19" s="4">
+        <v>42248</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <v>6</v>
+      </c>
+      <c r="C20">
+        <v>6</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+      <c r="E20" t="s">
+        <v>715</v>
+      </c>
+      <c r="F20" t="s">
+        <v>730</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>20150901</v>
+      </c>
+      <c r="I20">
+        <v>20150930</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20" s="4">
+        <v>42248</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" s="5">
+        <v>1</v>
+      </c>
+      <c r="B21" s="5">
+        <v>7</v>
+      </c>
+      <c r="C21" s="5">
+        <v>7</v>
+      </c>
+      <c r="D21" s="5">
+        <v>13</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>905</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>730</v>
+      </c>
+      <c r="G21" s="5">
+        <v>0</v>
+      </c>
+      <c r="H21" s="5">
+        <v>20180201</v>
+      </c>
+      <c r="I21" s="5">
+        <v>99991231</v>
+      </c>
+      <c r="J21" s="5">
+        <v>1</v>
+      </c>
+      <c r="K21" s="6">
+        <v>43132</v>
+      </c>
+      <c r="L21" s="5">
+        <v>1</v>
+      </c>
+      <c r="M21" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" s="5">
+        <v>1</v>
+      </c>
+      <c r="B22" s="5">
+        <v>7</v>
+      </c>
+      <c r="C22" s="5">
+        <v>7</v>
+      </c>
+      <c r="D22" s="5">
+        <v>14</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>906</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>730</v>
+      </c>
+      <c r="G22" s="5">
+        <v>0</v>
+      </c>
+      <c r="H22" s="5">
+        <v>20180201</v>
+      </c>
+      <c r="I22" s="5">
+        <v>99991231</v>
+      </c>
+      <c r="J22" s="5">
+        <v>1</v>
+      </c>
+      <c r="K22" s="6">
+        <v>43132</v>
+      </c>
+      <c r="L22" s="5">
+        <v>1</v>
+      </c>
+      <c r="M22" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" s="5">
+        <v>1</v>
+      </c>
+      <c r="B23" s="5">
+        <v>7</v>
+      </c>
+      <c r="C23" s="5">
+        <v>7</v>
+      </c>
+      <c r="D23" s="5">
+        <v>15</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>907</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>730</v>
+      </c>
+      <c r="G23" s="5">
+        <v>0</v>
+      </c>
+      <c r="H23" s="5">
+        <v>20180201</v>
+      </c>
+      <c r="I23" s="5">
+        <v>99991231</v>
+      </c>
+      <c r="J23" s="5">
+        <v>1</v>
+      </c>
+      <c r="K23" s="6">
+        <v>43132</v>
+      </c>
+      <c r="L23" s="5">
+        <v>1</v>
+      </c>
+      <c r="M23" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" s="5">
+        <v>1</v>
+      </c>
+      <c r="B24" s="5">
+        <v>7</v>
+      </c>
+      <c r="C24" s="5">
+        <v>7</v>
+      </c>
+      <c r="D24" s="5">
+        <v>16</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>908</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>730</v>
+      </c>
+      <c r="G24" s="5">
+        <v>0</v>
+      </c>
+      <c r="H24" s="5">
+        <v>20180201</v>
+      </c>
+      <c r="I24" s="5">
+        <v>99991231</v>
+      </c>
+      <c r="J24" s="5">
+        <v>1</v>
+      </c>
+      <c r="K24" s="6">
+        <v>43132</v>
+      </c>
+      <c r="L24" s="5">
+        <v>1</v>
+      </c>
+      <c r="M24" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" s="5">
+        <v>1</v>
+      </c>
+      <c r="B25" s="5">
+        <v>7</v>
+      </c>
+      <c r="C25" s="5">
+        <v>7</v>
+      </c>
+      <c r="D25" s="5">
+        <v>17</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>909</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>730</v>
+      </c>
+      <c r="G25" s="5">
+        <v>0</v>
+      </c>
+      <c r="H25" s="5">
+        <v>20180201</v>
+      </c>
+      <c r="I25" s="5">
+        <v>99991231</v>
+      </c>
+      <c r="J25" s="5">
+        <v>1</v>
+      </c>
+      <c r="K25" s="6">
+        <v>43132</v>
+      </c>
+      <c r="L25" s="5">
+        <v>1</v>
+      </c>
+      <c r="M25" s="5">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -31010,6 +31605,378 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D1" t="s">
+        <v>902</v>
+      </c>
+      <c r="E1" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>-1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>76</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>78</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>80</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
@@ -31284,7 +32251,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -31355,7 +32322,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>

<commit_message>
TFS 10890 - Disable Pilot Survey and enable Regular Survey for Lawrence
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C39981
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="132" windowWidth="22992" windowHeight="12840"/>
+    <workbookView xWindow="480" yWindow="132" windowWidth="22992" windowHeight="12840" firstSheet="17" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_History" sheetId="14" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3436" uniqueCount="912">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3438" uniqueCount="913">
   <si>
     <t>SourceID</t>
   </si>
@@ -2783,6 +2783,9 @@
   </si>
   <si>
     <t>Move Submissions to new architecture. CallID_selection tab-Updated NGD ID to NGDID. Updated body for Supervisor Module, Walk-By direct Employee review in Email_notifications tab to add end &lt;/strong&gt; tag.</t>
+  </si>
+  <si>
+    <t>Disable Pilot survey in lawrence.set isPilot to 0 in Survey_sites table for Lawrence.</t>
   </si>
 </sst>
 </file>
@@ -3156,10 +3159,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E67"/>
+  <dimension ref="A1:E68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67"/>
+    <sheetView topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="E68" sqref="E68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4287,6 +4290,23 @@
       </c>
       <c r="E67" t="s">
         <v>911</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>60</v>
+      </c>
+      <c r="B68" s="1">
+        <v>43224</v>
+      </c>
+      <c r="C68" t="s">
+        <v>430</v>
+      </c>
+      <c r="D68">
+        <v>10890</v>
+      </c>
+      <c r="E68" t="s">
+        <v>912</v>
       </c>
     </row>
   </sheetData>
@@ -31630,9 +31650,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E21"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -31833,8 +31851,8 @@
       <c r="C12">
         <v>1</v>
       </c>
-      <c r="D12">
-        <v>1</v>
+      <c r="D12" s="5">
+        <v>0</v>
       </c>
       <c r="E12">
         <v>0</v>

</xml_diff>

<commit_message>
TFS 7137 and TFS 7138 - Historical and My Dashboards move to new architecture
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C40320
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="132" windowWidth="22992" windowHeight="12840" firstSheet="17" activeTab="20"/>
+    <workbookView xWindow="480" yWindow="132" windowWidth="22992" windowHeight="12840" firstSheet="19" activeTab="23"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_History" sheetId="14" r:id="rId1"/>
@@ -35,6 +35,10 @@
     <sheet name="Survey_Sites" sheetId="24" r:id="rId21"/>
     <sheet name="HR_Access" sheetId="21" r:id="rId22"/>
     <sheet name="NPN Description" sheetId="23" r:id="rId23"/>
+    <sheet name="UI_User_Role" sheetId="25" r:id="rId24"/>
+    <sheet name="UI_Role_Page_Access" sheetId="26" r:id="rId25"/>
+    <sheet name="UI_Dashboard_Summary_Display" sheetId="27" r:id="rId26"/>
+    <sheet name="Reasons_By_ReportCode" sheetId="28" r:id="rId27"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">Coaching_Reason_Selection!$A$1:$P$292</definedName>
@@ -46,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3438" uniqueCount="913">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3528" uniqueCount="956">
   <si>
     <t>SourceID</t>
   </si>
@@ -2786,6 +2790,135 @@
   </si>
   <si>
     <t>Disable Pilot survey in lawrence.set isPilot to 0 in Survey_sites table for Lawrence.</t>
+  </si>
+  <si>
+    <t>Move My dashboard to new architecture. Add tabs for 4 new tables UI_User_Role, UI_Role_Page_Access, UI_Dashboard_Summary_Display, Reasons_By_ReportCode</t>
+  </si>
+  <si>
+    <t>RoleId</t>
+  </si>
+  <si>
+    <t>RoleName</t>
+  </si>
+  <si>
+    <t>RoleDescription</t>
+  </si>
+  <si>
+    <t>SrManager</t>
+  </si>
+  <si>
+    <t>Director</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>Restricted</t>
+  </si>
+  <si>
+    <t>RoleID</t>
+  </si>
+  <si>
+    <t>NewSubmission</t>
+  </si>
+  <si>
+    <t>HistoricalDashboard</t>
+  </si>
+  <si>
+    <t>MyPending</t>
+  </si>
+  <si>
+    <t>MyCompleted</t>
+  </si>
+  <si>
+    <t>MyTeamPending</t>
+  </si>
+  <si>
+    <t>MyTeamcompleted</t>
+  </si>
+  <si>
+    <t>MyTeamWarning</t>
+  </si>
+  <si>
+    <t>MySubmission</t>
+  </si>
+  <si>
+    <t>Reason</t>
+  </si>
+  <si>
+    <t>OMR/BRL</t>
+  </si>
+  <si>
+    <t>Approved accommodation on file</t>
+  </si>
+  <si>
+    <t>OMR/BRN</t>
+  </si>
+  <si>
+    <t>OMR/IAE</t>
+  </si>
+  <si>
+    <t>Agent no longer employed or on LOA</t>
+  </si>
+  <si>
+    <t>Escalation was appropriate</t>
+  </si>
+  <si>
+    <t>ISG or Supervisor told agent to escalate</t>
+  </si>
+  <si>
+    <t>Not enough information to coach</t>
+  </si>
+  <si>
+    <t>OTH/DTT</t>
+  </si>
+  <si>
+    <t>ATT Updated - with Approved Absence</t>
+  </si>
+  <si>
+    <t>ATT Updated - with Unapproved Absence</t>
+  </si>
+  <si>
+    <t>ATT Not Updated - SWP notified that Empower is inaccurate</t>
+  </si>
+  <si>
+    <t>ATT Not Updated and Empower will not be updated</t>
+  </si>
+  <si>
+    <t>ATT Not Updated - CSR Termed</t>
+  </si>
+  <si>
+    <t>CSR on a Leave of Absence</t>
+  </si>
+  <si>
+    <t>Absence is pending HR approval (LOA or WPA)</t>
+  </si>
+  <si>
+    <t>WACS0% and No ARC Role in ACL</t>
+  </si>
+  <si>
+    <t>WACS0% and ARC Role in ACL</t>
+  </si>
+  <si>
+    <t>%40 or WTTI%</t>
+  </si>
+  <si>
+    <t>%50 or WEEX% or WISO% or WISY% or WPWL% or WSTE%</t>
+  </si>
+  <si>
+    <t>SRM in ACL</t>
+  </si>
+  <si>
+    <t>DIR in ACL</t>
+  </si>
+  <si>
+    <t>Not meeting any of the Other Roles</t>
+  </si>
+  <si>
+    <t>WH%</t>
+  </si>
+  <si>
+    <t>WABA%, WACS04, WBCO12,  WCWF04, WIHD0%, WIIS15, WISA03, WISA12, WISE14, WMPL%, WTID%, WTTC14, WTTI02, WTTR1%</t>
   </si>
 </sst>
 </file>
@@ -2853,8 +2986,8 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3159,11 +3292,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E68"/>
+  <dimension ref="A1:E69"/>
   <sheetViews>
-    <sheetView topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="E68" sqref="E68"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -4307,6 +4438,23 @@
       </c>
       <c r="E68" t="s">
         <v>912</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>61</v>
+      </c>
+      <c r="B69" s="1">
+        <v>43264</v>
+      </c>
+      <c r="C69" t="s">
+        <v>430</v>
+      </c>
+      <c r="D69">
+        <v>7137</v>
+      </c>
+      <c r="E69" t="s">
+        <v>913</v>
       </c>
     </row>
   </sheetData>
@@ -27181,213 +27329,213 @@
         <v>175</v>
       </c>
     </row>
-    <row r="169" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A169" s="7" t="s">
+    <row r="169" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A169" s="6" t="s">
         <v>890</v>
       </c>
-      <c r="B169" s="7" t="s">
+      <c r="B169" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="C169" s="7" t="s">
+      <c r="C169" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D169" s="7" t="s">
+      <c r="D169" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E169" s="7">
-        <v>0</v>
-      </c>
-      <c r="F169" s="7" t="s">
+      <c r="E169" s="6">
+        <v>0</v>
+      </c>
+      <c r="F169" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G169" s="7" t="s">
+      <c r="G169" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="H169" s="7" t="s">
+      <c r="H169" s="6" t="s">
         <v>383</v>
       </c>
-      <c r="I169" s="7" t="s">
+      <c r="I169" s="6" t="s">
         <v>696</v>
       </c>
-      <c r="J169" s="7">
-        <v>0</v>
-      </c>
-      <c r="K169" s="7" t="s">
+      <c r="J169" s="6">
+        <v>0</v>
+      </c>
+      <c r="K169" s="6" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="170" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A170" s="7" t="s">
+    <row r="170" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A170" s="6" t="s">
         <v>891</v>
       </c>
-      <c r="B170" s="7" t="s">
+      <c r="B170" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="C170" s="7" t="s">
+      <c r="C170" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D170" s="7" t="s">
+      <c r="D170" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E170" s="7">
-        <v>0</v>
-      </c>
-      <c r="F170" s="7" t="s">
+      <c r="E170" s="6">
+        <v>0</v>
+      </c>
+      <c r="F170" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G170" s="7" t="s">
+      <c r="G170" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="H170" s="7" t="s">
+      <c r="H170" s="6" t="s">
         <v>383</v>
       </c>
-      <c r="I170" s="7" t="s">
+      <c r="I170" s="6" t="s">
         <v>696</v>
       </c>
-      <c r="J170" s="7">
-        <v>0</v>
-      </c>
-      <c r="K170" s="7" t="s">
+      <c r="J170" s="6">
+        <v>0</v>
+      </c>
+      <c r="K170" s="6" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="171" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A171" s="7" t="s">
+    <row r="171" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A171" s="6" t="s">
         <v>892</v>
       </c>
-      <c r="B171" s="7" t="s">
+      <c r="B171" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="C171" s="7" t="s">
+      <c r="C171" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D171" s="7" t="s">
+      <c r="D171" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E171" s="7">
-        <v>0</v>
-      </c>
-      <c r="F171" s="7" t="s">
+      <c r="E171" s="6">
+        <v>0</v>
+      </c>
+      <c r="F171" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G171" s="7" t="s">
+      <c r="G171" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="H171" s="7" t="s">
+      <c r="H171" s="6" t="s">
         <v>383</v>
       </c>
-      <c r="I171" s="7" t="s">
+      <c r="I171" s="6" t="s">
         <v>696</v>
       </c>
-      <c r="J171" s="7">
-        <v>0</v>
-      </c>
-      <c r="K171" s="7" t="s">
+      <c r="J171" s="6">
+        <v>0</v>
+      </c>
+      <c r="K171" s="6" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="172" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A172" s="7" t="s">
+    <row r="172" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A172" s="6" t="s">
         <v>893</v>
       </c>
-      <c r="B172" s="7" t="s">
+      <c r="B172" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="C172" s="7" t="s">
+      <c r="C172" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D172" s="7" t="s">
+      <c r="D172" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E172" s="7">
-        <v>0</v>
-      </c>
-      <c r="F172" s="7" t="s">
+      <c r="E172" s="6">
+        <v>0</v>
+      </c>
+      <c r="F172" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G172" s="7" t="s">
+      <c r="G172" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="H172" s="7" t="s">
+      <c r="H172" s="6" t="s">
         <v>383</v>
       </c>
-      <c r="I172" s="7" t="s">
+      <c r="I172" s="6" t="s">
         <v>696</v>
       </c>
-      <c r="J172" s="7">
-        <v>0</v>
-      </c>
-      <c r="K172" s="7" t="s">
+      <c r="J172" s="6">
+        <v>0</v>
+      </c>
+      <c r="K172" s="6" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="173" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A173" s="7" t="s">
+    <row r="173" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A173" s="6" t="s">
         <v>477</v>
       </c>
-      <c r="B173" s="7" t="s">
+      <c r="B173" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="C173" s="7" t="s">
+      <c r="C173" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D173" s="7" t="s">
+      <c r="D173" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E173" s="7">
-        <v>0</v>
-      </c>
-      <c r="F173" s="7" t="s">
+      <c r="E173" s="6">
+        <v>0</v>
+      </c>
+      <c r="F173" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G173" s="7" t="s">
+      <c r="G173" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="H173" s="7" t="s">
+      <c r="H173" s="6" t="s">
         <v>383</v>
       </c>
-      <c r="I173" s="7" t="s">
+      <c r="I173" s="6" t="s">
         <v>696</v>
       </c>
-      <c r="J173" s="7">
-        <v>0</v>
-      </c>
-      <c r="K173" s="7" t="s">
+      <c r="J173" s="6">
+        <v>0</v>
+      </c>
+      <c r="K173" s="6" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="174" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A174" s="7" t="s">
+    <row r="174" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A174" s="6" t="s">
         <v>546</v>
       </c>
-      <c r="B174" s="7" t="s">
+      <c r="B174" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="C174" s="7" t="s">
+      <c r="C174" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D174" s="7" t="s">
+      <c r="D174" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E174" s="7">
-        <v>0</v>
-      </c>
-      <c r="F174" s="7" t="s">
+      <c r="E174" s="6">
+        <v>0</v>
+      </c>
+      <c r="F174" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G174" s="7" t="s">
+      <c r="G174" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="H174" s="7" t="s">
+      <c r="H174" s="6" t="s">
         <v>383</v>
       </c>
-      <c r="I174" s="7" t="s">
+      <c r="I174" s="6" t="s">
         <v>696</v>
       </c>
-      <c r="J174" s="7">
-        <v>0</v>
-      </c>
-      <c r="K174" s="7" t="s">
+      <c r="J174" s="6">
+        <v>0</v>
+      </c>
+      <c r="K174" s="6" t="s">
         <v>378</v>
       </c>
     </row>
@@ -27402,7 +27550,7 @@
   <dimension ref="A1:C71"/>
   <sheetViews>
     <sheetView topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58:C71"/>
+      <selection activeCell="A58" sqref="A58:XFD71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -27777,99 +27925,63 @@
         <v>876</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A58" s="5" t="s">
+    <row r="58" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="6" t="s">
         <v>877</v>
       </c>
-      <c r="B58" s="5" t="s">
+      <c r="B58" s="6" t="s">
         <v>827</v>
       </c>
-      <c r="C58" s="5" t="s">
+      <c r="C58" s="6" t="s">
         <v>878</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A59" s="5"/>
-      <c r="B59" s="5"/>
-      <c r="C59" s="5"/>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A60" s="5" t="s">
+    <row r="59" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="60" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="6" t="s">
         <v>879</v>
       </c>
-      <c r="B60" s="5"/>
-      <c r="C60" s="5"/>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A61" s="5"/>
-      <c r="B61" s="5"/>
-      <c r="C61" s="5"/>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A62" s="5" t="s">
+    </row>
+    <row r="61" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="62" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="6" t="s">
         <v>880</v>
       </c>
-      <c r="B62" s="5"/>
-      <c r="C62" s="5"/>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A63" s="5"/>
-      <c r="B63" s="5"/>
-      <c r="C63" s="5"/>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A64" s="5" t="s">
+    </row>
+    <row r="63" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="64" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="6" t="s">
         <v>881</v>
       </c>
-      <c r="B64" s="5"/>
-      <c r="C64" s="5"/>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A65" s="5" t="s">
+    </row>
+    <row r="65" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="6" t="s">
         <v>882</v>
       </c>
-      <c r="B65" s="5" t="s">
+      <c r="B65" s="6" t="s">
         <v>883</v>
       </c>
-      <c r="C65" s="5" t="s">
+      <c r="C65" s="6" t="s">
         <v>884</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A66" s="5"/>
-      <c r="B66" s="5"/>
-      <c r="C66" s="5"/>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A67" s="5" t="s">
+    <row r="66" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="67" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="6" t="s">
         <v>885</v>
       </c>
-      <c r="B67" s="5"/>
-      <c r="C67" s="5"/>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A68" s="5"/>
-      <c r="B68" s="5"/>
-      <c r="C68" s="5"/>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A69" s="5" t="s">
+    </row>
+    <row r="68" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="69" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="6" t="s">
         <v>886</v>
       </c>
-      <c r="B69" s="5"/>
-      <c r="C69" s="5"/>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A70" s="5"/>
-      <c r="B70" s="5"/>
-      <c r="C70" s="5"/>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A71" s="5" t="s">
+    </row>
+    <row r="70" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="71" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="6" t="s">
         <v>887</v>
       </c>
-      <c r="B71" s="5"/>
-      <c r="C71" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -28013,8 +28125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I9"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -28052,7 +28164,7 @@
       <c r="H1" s="4" t="s">
         <v>707</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="6" t="s">
         <v>900</v>
       </c>
     </row>
@@ -28081,7 +28193,7 @@
       <c r="H2" s="4">
         <v>42248</v>
       </c>
-      <c r="I2" s="5">
+      <c r="I2" s="6">
         <v>0</v>
       </c>
     </row>
@@ -28110,7 +28222,7 @@
       <c r="H3" s="4">
         <v>42248</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3" s="6">
         <v>0</v>
       </c>
     </row>
@@ -28139,7 +28251,7 @@
       <c r="H4" s="4">
         <v>42248</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="6">
         <v>0</v>
       </c>
     </row>
@@ -28168,7 +28280,7 @@
       <c r="H5" s="4">
         <v>42248</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="6">
         <v>0</v>
       </c>
     </row>
@@ -28197,7 +28309,7 @@
       <c r="H6" s="4">
         <v>42248</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="6">
         <v>0</v>
       </c>
     </row>
@@ -28226,7 +28338,7 @@
       <c r="H7" s="4">
         <v>42248</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I7" s="6">
         <v>0</v>
       </c>
     </row>
@@ -28255,36 +28367,36 @@
       <c r="H8" s="4">
         <v>42248</v>
       </c>
-      <c r="I8" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="5">
+      <c r="I8" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="6">
         <v>7</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="6" t="s">
         <v>901</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="6">
         <v>7</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="6">
         <v>20180201</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="6">
         <v>99991231</v>
       </c>
-      <c r="F9" s="5">
-        <v>0</v>
-      </c>
-      <c r="G9" s="5">
-        <v>1</v>
-      </c>
-      <c r="H9" s="6">
+      <c r="F9" s="6">
+        <v>0</v>
+      </c>
+      <c r="G9" s="6">
+        <v>1</v>
+      </c>
+      <c r="H9" s="7">
         <v>43132</v>
       </c>
-      <c r="I9" s="5">
+      <c r="I9" s="6">
         <v>1</v>
       </c>
     </row>
@@ -28507,72 +28619,72 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="5">
+      <c r="A15" s="6">
         <v>13</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="6" t="s">
         <v>903</v>
       </c>
-      <c r="C15" s="5">
-        <v>1</v>
-      </c>
-      <c r="D15" s="6">
+      <c r="C15" s="6">
+        <v>1</v>
+      </c>
+      <c r="D15" s="7">
         <v>43132</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="5">
+      <c r="A16" s="6">
         <v>14</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="6" t="s">
         <v>904</v>
       </c>
-      <c r="C16" s="5">
-        <v>1</v>
-      </c>
-      <c r="D16" s="6">
+      <c r="C16" s="6">
+        <v>1</v>
+      </c>
+      <c r="D16" s="7">
         <v>43132</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="5">
+      <c r="A17" s="6">
         <v>15</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="6" t="s">
         <v>905</v>
       </c>
-      <c r="C17" s="5">
-        <v>1</v>
-      </c>
-      <c r="D17" s="6">
+      <c r="C17" s="6">
+        <v>1</v>
+      </c>
+      <c r="D17" s="7">
         <v>43132</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="5">
+      <c r="A18" s="6">
         <v>16</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="6" t="s">
         <v>906</v>
       </c>
-      <c r="C18" s="5">
-        <v>1</v>
-      </c>
-      <c r="D18" s="6">
+      <c r="C18" s="6">
+        <v>1</v>
+      </c>
+      <c r="D18" s="7">
         <v>43132</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="5">
+      <c r="A19" s="6">
         <v>17</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="6" t="s">
         <v>907</v>
       </c>
-      <c r="C19" s="5">
-        <v>1</v>
-      </c>
-      <c r="D19" s="6">
+      <c r="C19" s="6">
+        <v>1</v>
+      </c>
+      <c r="D19" s="7">
         <v>43132</v>
       </c>
     </row>
@@ -31436,207 +31548,207 @@
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21" s="5">
-        <v>1</v>
-      </c>
-      <c r="B21" s="5">
+      <c r="A21" s="6">
+        <v>1</v>
+      </c>
+      <c r="B21" s="6">
         <v>7</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C21" s="6">
         <v>7</v>
       </c>
-      <c r="D21" s="5">
+      <c r="D21" s="6">
         <v>13</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="E21" s="6" t="s">
         <v>903</v>
       </c>
-      <c r="F21" s="5" t="s">
+      <c r="F21" s="6" t="s">
         <v>728</v>
       </c>
-      <c r="G21" s="5">
-        <v>0</v>
-      </c>
-      <c r="H21" s="5">
+      <c r="G21" s="6">
+        <v>0</v>
+      </c>
+      <c r="H21" s="6">
         <v>20180201</v>
       </c>
-      <c r="I21" s="5">
+      <c r="I21" s="6">
         <v>99991231</v>
       </c>
-      <c r="J21" s="5">
-        <v>1</v>
-      </c>
-      <c r="K21" s="6">
+      <c r="J21" s="6">
+        <v>1</v>
+      </c>
+      <c r="K21" s="7">
         <v>43132</v>
       </c>
-      <c r="L21" s="5">
-        <v>1</v>
-      </c>
-      <c r="M21" s="5">
+      <c r="L21" s="6">
+        <v>1</v>
+      </c>
+      <c r="M21" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22" s="5">
-        <v>1</v>
-      </c>
-      <c r="B22" s="5">
+      <c r="A22" s="6">
+        <v>1</v>
+      </c>
+      <c r="B22" s="6">
         <v>7</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="6">
         <v>7</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D22" s="6">
         <v>14</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="E22" s="6" t="s">
         <v>904</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="F22" s="6" t="s">
         <v>728</v>
       </c>
-      <c r="G22" s="5">
-        <v>0</v>
-      </c>
-      <c r="H22" s="5">
+      <c r="G22" s="6">
+        <v>0</v>
+      </c>
+      <c r="H22" s="6">
         <v>20180201</v>
       </c>
-      <c r="I22" s="5">
+      <c r="I22" s="6">
         <v>99991231</v>
       </c>
-      <c r="J22" s="5">
-        <v>1</v>
-      </c>
-      <c r="K22" s="6">
+      <c r="J22" s="6">
+        <v>1</v>
+      </c>
+      <c r="K22" s="7">
         <v>43132</v>
       </c>
-      <c r="L22" s="5">
-        <v>1</v>
-      </c>
-      <c r="M22" s="5">
+      <c r="L22" s="6">
+        <v>1</v>
+      </c>
+      <c r="M22" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A23" s="5">
-        <v>1</v>
-      </c>
-      <c r="B23" s="5">
+      <c r="A23" s="6">
+        <v>1</v>
+      </c>
+      <c r="B23" s="6">
         <v>7</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C23" s="6">
         <v>7</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D23" s="6">
         <v>15</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="E23" s="6" t="s">
         <v>905</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="F23" s="6" t="s">
         <v>728</v>
       </c>
-      <c r="G23" s="5">
-        <v>0</v>
-      </c>
-      <c r="H23" s="5">
+      <c r="G23" s="6">
+        <v>0</v>
+      </c>
+      <c r="H23" s="6">
         <v>20180201</v>
       </c>
-      <c r="I23" s="5">
+      <c r="I23" s="6">
         <v>99991231</v>
       </c>
-      <c r="J23" s="5">
-        <v>1</v>
-      </c>
-      <c r="K23" s="6">
+      <c r="J23" s="6">
+        <v>1</v>
+      </c>
+      <c r="K23" s="7">
         <v>43132</v>
       </c>
-      <c r="L23" s="5">
-        <v>1</v>
-      </c>
-      <c r="M23" s="5">
+      <c r="L23" s="6">
+        <v>1</v>
+      </c>
+      <c r="M23" s="6">
         <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A24" s="5">
-        <v>1</v>
-      </c>
-      <c r="B24" s="5">
+      <c r="A24" s="6">
+        <v>1</v>
+      </c>
+      <c r="B24" s="6">
         <v>7</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C24" s="6">
         <v>7</v>
       </c>
-      <c r="D24" s="5">
+      <c r="D24" s="6">
         <v>16</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="E24" s="6" t="s">
         <v>906</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="F24" s="6" t="s">
         <v>728</v>
       </c>
-      <c r="G24" s="5">
-        <v>0</v>
-      </c>
-      <c r="H24" s="5">
+      <c r="G24" s="6">
+        <v>0</v>
+      </c>
+      <c r="H24" s="6">
         <v>20180201</v>
       </c>
-      <c r="I24" s="5">
+      <c r="I24" s="6">
         <v>99991231</v>
       </c>
-      <c r="J24" s="5">
-        <v>1</v>
-      </c>
-      <c r="K24" s="6">
+      <c r="J24" s="6">
+        <v>1</v>
+      </c>
+      <c r="K24" s="7">
         <v>43132</v>
       </c>
-      <c r="L24" s="5">
-        <v>1</v>
-      </c>
-      <c r="M24" s="5">
+      <c r="L24" s="6">
+        <v>1</v>
+      </c>
+      <c r="M24" s="6">
         <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A25" s="5">
-        <v>1</v>
-      </c>
-      <c r="B25" s="5">
+      <c r="A25" s="6">
+        <v>1</v>
+      </c>
+      <c r="B25" s="6">
         <v>7</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C25" s="6">
         <v>7</v>
       </c>
-      <c r="D25" s="5">
+      <c r="D25" s="6">
         <v>17</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="E25" s="6" t="s">
         <v>907</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="F25" s="6" t="s">
         <v>728</v>
       </c>
-      <c r="G25" s="5">
-        <v>0</v>
-      </c>
-      <c r="H25" s="5">
+      <c r="G25" s="6">
+        <v>0</v>
+      </c>
+      <c r="H25" s="6">
         <v>20180201</v>
       </c>
-      <c r="I25" s="5">
+      <c r="I25" s="6">
         <v>99991231</v>
       </c>
-      <c r="J25" s="5">
-        <v>1</v>
-      </c>
-      <c r="K25" s="6">
+      <c r="J25" s="6">
+        <v>1</v>
+      </c>
+      <c r="K25" s="7">
         <v>43132</v>
       </c>
-      <c r="L25" s="5">
-        <v>1</v>
-      </c>
-      <c r="M25" s="5">
+      <c r="L25" s="6">
+        <v>1</v>
+      </c>
+      <c r="M25" s="6">
         <v>5</v>
       </c>
     </row>
@@ -31650,7 +31762,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -31851,7 +31965,7 @@
       <c r="C12">
         <v>1</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="6">
         <v>0</v>
       </c>
       <c r="E12">
@@ -32358,6 +32472,750 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="109.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>914</v>
+      </c>
+      <c r="B1" t="s">
+        <v>915</v>
+      </c>
+      <c r="C1" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>101</v>
+      </c>
+      <c r="B2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C2" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>102</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>103</v>
+      </c>
+      <c r="B4" t="s">
+        <v>175</v>
+      </c>
+      <c r="C4" t="s">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>104</v>
+      </c>
+      <c r="B5" t="s">
+        <v>379</v>
+      </c>
+      <c r="C5" t="s">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>105</v>
+      </c>
+      <c r="B6" t="s">
+        <v>917</v>
+      </c>
+      <c r="C6" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>106</v>
+      </c>
+      <c r="B7" t="s">
+        <v>918</v>
+      </c>
+      <c r="C7" t="s">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>107</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>108</v>
+      </c>
+      <c r="B9" t="s">
+        <v>919</v>
+      </c>
+      <c r="C9" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>109</v>
+      </c>
+      <c r="B10" t="s">
+        <v>920</v>
+      </c>
+      <c r="C10" t="s">
+        <v>955</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>921</v>
+      </c>
+      <c r="B1" t="s">
+        <v>915</v>
+      </c>
+      <c r="C1" t="s">
+        <v>922</v>
+      </c>
+      <c r="D1" t="s">
+        <v>758</v>
+      </c>
+      <c r="E1" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>101</v>
+      </c>
+      <c r="B2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>102</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>103</v>
+      </c>
+      <c r="B4" t="s">
+        <v>175</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>104</v>
+      </c>
+      <c r="B5" t="s">
+        <v>379</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>105</v>
+      </c>
+      <c r="B6" t="s">
+        <v>917</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>106</v>
+      </c>
+      <c r="B7" t="s">
+        <v>918</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>107</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>108</v>
+      </c>
+      <c r="B9" t="s">
+        <v>919</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>109</v>
+      </c>
+      <c r="B10" t="s">
+        <v>920</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>914</v>
+      </c>
+      <c r="B1" t="s">
+        <v>915</v>
+      </c>
+      <c r="C1" t="s">
+        <v>924</v>
+      </c>
+      <c r="D1" t="s">
+        <v>925</v>
+      </c>
+      <c r="E1" t="s">
+        <v>926</v>
+      </c>
+      <c r="F1" t="s">
+        <v>927</v>
+      </c>
+      <c r="G1" t="s">
+        <v>928</v>
+      </c>
+      <c r="H1" t="s">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>101</v>
+      </c>
+      <c r="B2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>102</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>103</v>
+      </c>
+      <c r="B4" t="s">
+        <v>175</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>104</v>
+      </c>
+      <c r="B5" t="s">
+        <v>379</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>105</v>
+      </c>
+      <c r="B6" t="s">
+        <v>917</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>106</v>
+      </c>
+      <c r="B7" t="s">
+        <v>918</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>107</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>108</v>
+      </c>
+      <c r="B9" t="s">
+        <v>919</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>109</v>
+      </c>
+      <c r="B10" t="s">
+        <v>920</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>501</v>
+      </c>
+      <c r="B1" t="s">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>931</v>
+      </c>
+      <c r="B2" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>931</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>933</v>
+      </c>
+      <c r="B4" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>933</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>934</v>
+      </c>
+      <c r="B6" t="s">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>934</v>
+      </c>
+      <c r="B7" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>934</v>
+      </c>
+      <c r="B8" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>934</v>
+      </c>
+      <c r="B9" t="s">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>934</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>939</v>
+      </c>
+      <c r="B12" t="s">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>939</v>
+      </c>
+      <c r="B13" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>939</v>
+      </c>
+      <c r="B14" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>939</v>
+      </c>
+      <c r="B15" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>939</v>
+      </c>
+      <c r="B16" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>939</v>
+      </c>
+      <c r="B17" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>939</v>
+      </c>
+      <c r="B18" t="s">
+        <v>946</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>

</xml_diff>

<commit_message>
TFS 7136/7137/7138 Move dashboards to new architecture
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C40438
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="132" windowWidth="22992" windowHeight="12840" firstSheet="19" activeTab="23"/>
+    <workbookView xWindow="480" yWindow="132" windowWidth="22992" windowHeight="12840"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_History" sheetId="14" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3528" uniqueCount="956">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3531" uniqueCount="957">
   <si>
     <t>SourceID</t>
   </si>
@@ -2900,12 +2900,6 @@
     <t>WACS0% and ARC Role in ACL</t>
   </si>
   <si>
-    <t>%40 or WTTI%</t>
-  </si>
-  <si>
-    <t>%50 or WEEX% or WISO% or WISY% or WPWL% or WSTE%</t>
-  </si>
-  <si>
     <t>SRM in ACL</t>
   </si>
   <si>
@@ -2918,7 +2912,16 @@
     <t>WH%</t>
   </si>
   <si>
-    <t>WABA%, WACS04, WBCO12,  WCWF04, WIHD0%, WIIS15, WISA03, WISA12, WISE14, WMPL%, WTID%, WTTC14, WTTI02, WTTR1%</t>
+    <t>%40 or WTTI% or WACQ13</t>
+  </si>
+  <si>
+    <t>%50 or %60 or %70 or WEEX% or WISO% or WISY% or WPWL% or WSTE%</t>
+  </si>
+  <si>
+    <t>WACQ0% or WACQ12 or WIHD0% or WTTR1% or WTID%</t>
+  </si>
+  <si>
+    <t>Added DisplayOrder col in Reasons_By_ReportCode table and updated UI_ Tables with revised records</t>
   </si>
 </sst>
 </file>
@@ -3292,9 +3295,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E69"/>
+  <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -4455,6 +4458,23 @@
       </c>
       <c r="E69" t="s">
         <v>913</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>61.1</v>
+      </c>
+      <c r="B70" s="1">
+        <v>43284</v>
+      </c>
+      <c r="C70" t="s">
+        <v>430</v>
+      </c>
+      <c r="D70">
+        <v>7137</v>
+      </c>
+      <c r="E70" t="s">
+        <v>956</v>
       </c>
     </row>
   </sheetData>
@@ -32476,13 +32496,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="109.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -32526,7 +32548,7 @@
         <v>175</v>
       </c>
       <c r="C4" t="s">
-        <v>949</v>
+        <v>953</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -32537,7 +32559,7 @@
         <v>379</v>
       </c>
       <c r="C5" t="s">
-        <v>950</v>
+        <v>954</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -32548,7 +32570,7 @@
         <v>917</v>
       </c>
       <c r="C6" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -32559,7 +32581,7 @@
         <v>918</v>
       </c>
       <c r="C7" t="s">
-        <v>952</v>
+        <v>950</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -32567,10 +32589,10 @@
         <v>107</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>423</v>
       </c>
       <c r="C8" t="s">
-        <v>953</v>
+        <v>955</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -32581,7 +32603,7 @@
         <v>919</v>
       </c>
       <c r="C9" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -32592,7 +32614,7 @@
         <v>920</v>
       </c>
       <c r="C10" t="s">
-        <v>955</v>
+        <v>951</v>
       </c>
     </row>
   </sheetData>
@@ -32604,9 +32626,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -32732,7 +32763,7 @@
         <v>107</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>423</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -32741,7 +32772,7 @@
         <v>1</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -32769,10 +32800,10 @@
         <v>920</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -32787,9 +32818,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -32978,7 +33021,7 @@
         <v>107</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>423</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -32987,13 +33030,13 @@
         <v>1</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H8">
         <v>1</v>
@@ -33048,7 +33091,7 @@
         <v>0</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -33058,157 +33101,215 @@
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>501</v>
       </c>
       <c r="B1" t="s">
         <v>930</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" s="5" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>931</v>
       </c>
       <c r="B2" t="s">
         <v>932</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2" s="5">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>931</v>
       </c>
       <c r="B3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3" s="5">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>933</v>
       </c>
       <c r="B4" t="s">
         <v>932</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C4" s="5">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>933</v>
       </c>
       <c r="B5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C5" s="5">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>934</v>
       </c>
       <c r="B6" t="s">
         <v>935</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C6" s="5">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>934</v>
       </c>
       <c r="B7" t="s">
         <v>936</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C7" s="5">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>934</v>
       </c>
       <c r="B8" t="s">
         <v>937</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C8" s="5">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>934</v>
       </c>
       <c r="B9" t="s">
         <v>938</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C9" s="5">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>934</v>
       </c>
       <c r="B10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C10" s="5">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>17</v>
       </c>
       <c r="B11" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C11" s="5">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>939</v>
       </c>
       <c r="B12" t="s">
         <v>940</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C12" s="5">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>939</v>
       </c>
       <c r="B13" t="s">
         <v>941</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C13" s="5">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>939</v>
       </c>
       <c r="B14" t="s">
         <v>942</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C14" s="5">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>939</v>
       </c>
       <c r="B15" t="s">
         <v>943</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C15" s="5">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>939</v>
       </c>
       <c r="B16" t="s">
         <v>944</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C16" s="5">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>939</v>
       </c>
       <c r="B17" t="s">
         <v>945</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C17" s="5">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>939</v>
       </c>
       <c r="B18" t="s">
         <v>946</v>
+      </c>
+      <c r="C18" s="5">
+        <v>407</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TFS 11500 - New Subcoachingreason to OMR
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C40479
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="132" windowWidth="22992" windowHeight="12840"/>
+    <workbookView xWindow="480" yWindow="132" windowWidth="22992" windowHeight="12840" firstSheet="7" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_History" sheetId="14" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3531" uniqueCount="957">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3536" uniqueCount="959">
   <si>
     <t>SourceID</t>
   </si>
@@ -2922,6 +2922,12 @@
   </si>
   <si>
     <t>Added DisplayOrder col in Reasons_By_ReportCode table and updated UI_ Tables with revised records</t>
+  </si>
+  <si>
+    <t>New sub-coaching reason Potential hardship to OMR/Exceptions for CSR Module.. Updated Dim SubCoaching Reason and Coaching Reason Selection tabs.</t>
+  </si>
+  <si>
+    <t>OMR: Potential Hardship</t>
   </si>
 </sst>
 </file>
@@ -3295,9 +3301,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E70"/>
+  <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="E71" sqref="E71"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -4475,6 +4483,23 @@
       </c>
       <c r="E70" t="s">
         <v>956</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>62</v>
+      </c>
+      <c r="B71" s="1">
+        <v>43292</v>
+      </c>
+      <c r="C71" t="s">
+        <v>430</v>
+      </c>
+      <c r="D71">
+        <v>11500</v>
+      </c>
+      <c r="E71" t="s">
+        <v>957</v>
       </c>
     </row>
   </sheetData>
@@ -5900,10 +5925,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P308"/>
+  <dimension ref="A1:P309"/>
   <sheetViews>
-    <sheetView topLeftCell="A290" workbookViewId="0">
-      <selection activeCell="A308" sqref="A308:P308"/>
+    <sheetView tabSelected="1" topLeftCell="A290" workbookViewId="0">
+      <selection activeCell="A309" sqref="A309"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -21262,52 +21287,102 @@
       </c>
     </row>
     <row r="308" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A308" s="5">
+      <c r="A308">
         <v>4</v>
       </c>
-      <c r="B308" s="5" t="s">
+      <c r="B308" t="s">
         <v>181</v>
       </c>
-      <c r="C308" s="5">
+      <c r="C308">
         <v>244</v>
       </c>
-      <c r="D308" s="5" t="s">
+      <c r="D308" t="s">
         <v>899</v>
       </c>
-      <c r="E308" s="5">
-        <v>1</v>
-      </c>
-      <c r="F308" s="5">
-        <v>1</v>
-      </c>
-      <c r="G308" s="5">
-        <v>1</v>
-      </c>
-      <c r="H308" s="5">
-        <v>1</v>
-      </c>
-      <c r="I308" s="5">
-        <v>1</v>
-      </c>
-      <c r="J308" s="5">
-        <v>0</v>
-      </c>
-      <c r="K308" s="5">
-        <v>0</v>
-      </c>
-      <c r="L308" s="5">
-        <v>1</v>
-      </c>
-      <c r="M308" s="5">
-        <v>0</v>
-      </c>
-      <c r="N308" s="5">
-        <v>0</v>
-      </c>
-      <c r="O308" s="5">
-        <v>0</v>
-      </c>
-      <c r="P308" s="5">
+      <c r="E308">
+        <v>1</v>
+      </c>
+      <c r="F308">
+        <v>1</v>
+      </c>
+      <c r="G308">
+        <v>1</v>
+      </c>
+      <c r="H308">
+        <v>1</v>
+      </c>
+      <c r="I308">
+        <v>1</v>
+      </c>
+      <c r="J308">
+        <v>0</v>
+      </c>
+      <c r="K308">
+        <v>0</v>
+      </c>
+      <c r="L308">
+        <v>1</v>
+      </c>
+      <c r="M308">
+        <v>0</v>
+      </c>
+      <c r="N308">
+        <v>0</v>
+      </c>
+      <c r="O308">
+        <v>0</v>
+      </c>
+      <c r="P308">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="309" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A309" s="5">
+        <v>9</v>
+      </c>
+      <c r="B309" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C309" s="5">
+        <v>245</v>
+      </c>
+      <c r="D309" s="5" t="s">
+        <v>958</v>
+      </c>
+      <c r="E309" s="5">
+        <v>1</v>
+      </c>
+      <c r="F309" s="5">
+        <v>1</v>
+      </c>
+      <c r="G309" s="5">
+        <v>1</v>
+      </c>
+      <c r="H309" s="5">
+        <v>1</v>
+      </c>
+      <c r="I309" s="5">
+        <v>1</v>
+      </c>
+      <c r="J309" s="5">
+        <v>1</v>
+      </c>
+      <c r="K309" s="5">
+        <v>0</v>
+      </c>
+      <c r="L309" s="5">
+        <v>0</v>
+      </c>
+      <c r="M309" s="5">
+        <v>0</v>
+      </c>
+      <c r="N309" s="5">
+        <v>0</v>
+      </c>
+      <c r="O309" s="5">
+        <v>0</v>
+      </c>
+      <c r="P309" s="5">
         <v>0</v>
       </c>
     </row>
@@ -34283,10 +34358,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B246"/>
+  <dimension ref="A1:B247"/>
   <sheetViews>
-    <sheetView topLeftCell="A230" workbookViewId="0">
-      <selection activeCell="A246" sqref="A246"/>
+    <sheetView topLeftCell="A232" workbookViewId="0">
+      <selection activeCell="A247" sqref="A247:B247"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -36256,11 +36331,19 @@
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A246" s="5">
+      <c r="A246">
         <v>244</v>
       </c>
-      <c r="B246" s="5" t="s">
+      <c r="B246" t="s">
         <v>899</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A247" s="5">
+        <v>245</v>
+      </c>
+      <c r="B247" s="5" t="s">
+        <v>958</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TFS 11451 - New feed file for CSRs who took inappropriate action.
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C40575
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3536" uniqueCount="959">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3538" uniqueCount="960">
   <si>
     <t>SourceID</t>
   </si>
@@ -2928,6 +2928,9 @@
   </si>
   <si>
     <t>OMR: Potential Hardship</t>
+  </si>
+  <si>
+    <t>Set Active to 0 for sub-coaching reason Potential hardship to OMR/Exceptions in Coaching Reason Selection tab.</t>
   </si>
 </sst>
 </file>
@@ -3301,10 +3304,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E71"/>
+  <dimension ref="A1:E72"/>
   <sheetViews>
     <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="E71" sqref="E71"/>
+      <selection activeCell="E72" sqref="E72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4500,6 +4503,23 @@
       </c>
       <c r="E71" t="s">
         <v>957</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>63</v>
+      </c>
+      <c r="B72" s="1">
+        <v>43311</v>
+      </c>
+      <c r="C72" t="s">
+        <v>430</v>
+      </c>
+      <c r="D72">
+        <v>11451</v>
+      </c>
+      <c r="E72" t="s">
+        <v>959</v>
       </c>
     </row>
   </sheetData>
@@ -5927,8 +5947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P309"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A290" workbookViewId="0">
-      <selection activeCell="A309" sqref="A309"/>
+    <sheetView tabSelected="1" topLeftCell="A289" workbookViewId="0">
+      <selection activeCell="A308" sqref="A308:P308"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -21350,7 +21370,7 @@
         <v>958</v>
       </c>
       <c r="E309" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F309" s="5">
         <v>1</v>

</xml_diff>

<commit_message>
TFS 12308 - New sub coaching reason for warnings
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C41015
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3538" uniqueCount="960">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3561" uniqueCount="964">
   <si>
     <t>SourceID</t>
   </si>
@@ -2931,6 +2931,18 @@
   </si>
   <si>
     <t>Set Active to 0 for sub-coaching reason Potential hardship to OMR/Exceptions in Coaching Reason Selection tab.</t>
+  </si>
+  <si>
+    <t>New sub coaching reason for warnings. Added records to SubCoaching Reason and Coaching Reason Selection table tabs</t>
+  </si>
+  <si>
+    <t>Adherence</t>
+  </si>
+  <si>
+    <t>Quality/Performance – Failed Calls</t>
+  </si>
+  <si>
+    <t>Quality/Performance – Critical Fails</t>
   </si>
 </sst>
 </file>
@@ -3304,10 +3316,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E72"/>
+  <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="E72" sqref="E72"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4520,6 +4532,23 @@
       </c>
       <c r="E72" t="s">
         <v>959</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>64</v>
+      </c>
+      <c r="B73" s="1">
+        <v>43383</v>
+      </c>
+      <c r="C73" t="s">
+        <v>430</v>
+      </c>
+      <c r="D73">
+        <v>12308</v>
+      </c>
+      <c r="E73" t="s">
+        <v>960</v>
       </c>
     </row>
   </sheetData>
@@ -5945,10 +5974,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P309"/>
+  <dimension ref="A1:P318"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A289" workbookViewId="0">
-      <selection activeCell="A308" sqref="A308:P308"/>
+    <sheetView tabSelected="1" topLeftCell="A298" workbookViewId="0">
+      <selection activeCell="A319" sqref="A319"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -21357,53 +21386,503 @@
       </c>
     </row>
     <row r="309" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A309" s="5">
+      <c r="A309">
         <v>9</v>
       </c>
-      <c r="B309" s="5" t="s">
+      <c r="B309" t="s">
         <v>91</v>
       </c>
-      <c r="C309" s="5">
+      <c r="C309">
         <v>245</v>
       </c>
-      <c r="D309" s="5" t="s">
+      <c r="D309" t="s">
         <v>958</v>
       </c>
-      <c r="E309" s="5">
-        <v>0</v>
-      </c>
-      <c r="F309" s="5">
-        <v>1</v>
-      </c>
-      <c r="G309" s="5">
-        <v>1</v>
-      </c>
-      <c r="H309" s="5">
-        <v>1</v>
-      </c>
-      <c r="I309" s="5">
-        <v>1</v>
-      </c>
-      <c r="J309" s="5">
-        <v>1</v>
-      </c>
-      <c r="K309" s="5">
-        <v>0</v>
-      </c>
-      <c r="L309" s="5">
-        <v>0</v>
-      </c>
-      <c r="M309" s="5">
-        <v>0</v>
-      </c>
-      <c r="N309" s="5">
-        <v>0</v>
-      </c>
-      <c r="O309" s="5">
-        <v>0</v>
-      </c>
-      <c r="P309" s="5">
-        <v>0</v>
+      <c r="E309">
+        <v>0</v>
+      </c>
+      <c r="F309">
+        <v>1</v>
+      </c>
+      <c r="G309">
+        <v>1</v>
+      </c>
+      <c r="H309">
+        <v>1</v>
+      </c>
+      <c r="I309">
+        <v>1</v>
+      </c>
+      <c r="J309">
+        <v>1</v>
+      </c>
+      <c r="K309">
+        <v>0</v>
+      </c>
+      <c r="L309">
+        <v>0</v>
+      </c>
+      <c r="M309">
+        <v>0</v>
+      </c>
+      <c r="N309">
+        <v>0</v>
+      </c>
+      <c r="O309">
+        <v>0</v>
+      </c>
+      <c r="P309">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="310" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A310" s="5">
+        <v>28</v>
+      </c>
+      <c r="B310" s="5" t="s">
+        <v>438</v>
+      </c>
+      <c r="C310" s="5">
+        <v>246</v>
+      </c>
+      <c r="D310" s="5" t="s">
+        <v>961</v>
+      </c>
+      <c r="E310" s="5">
+        <v>1</v>
+      </c>
+      <c r="F310" s="5">
+        <v>1</v>
+      </c>
+      <c r="G310" s="5">
+        <v>0</v>
+      </c>
+      <c r="H310" s="5">
+        <v>1</v>
+      </c>
+      <c r="I310" s="5">
+        <v>0</v>
+      </c>
+      <c r="J310" s="5">
+        <v>1</v>
+      </c>
+      <c r="K310" s="5">
+        <v>1</v>
+      </c>
+      <c r="L310" s="5">
+        <v>1</v>
+      </c>
+      <c r="M310" s="5">
+        <v>1</v>
+      </c>
+      <c r="N310" s="5">
+        <v>1</v>
+      </c>
+      <c r="O310" s="5">
+        <v>1</v>
+      </c>
+      <c r="P310" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="311" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A311" s="5">
+        <v>28</v>
+      </c>
+      <c r="B311" s="5" t="s">
+        <v>438</v>
+      </c>
+      <c r="C311" s="5">
+        <v>247</v>
+      </c>
+      <c r="D311" s="5" t="s">
+        <v>962</v>
+      </c>
+      <c r="E311" s="5">
+        <v>1</v>
+      </c>
+      <c r="F311" s="5">
+        <v>1</v>
+      </c>
+      <c r="G311" s="5">
+        <v>0</v>
+      </c>
+      <c r="H311" s="5">
+        <v>1</v>
+      </c>
+      <c r="I311" s="5">
+        <v>0</v>
+      </c>
+      <c r="J311" s="5">
+        <v>1</v>
+      </c>
+      <c r="K311" s="5">
+        <v>1</v>
+      </c>
+      <c r="L311" s="5">
+        <v>1</v>
+      </c>
+      <c r="M311" s="5">
+        <v>1</v>
+      </c>
+      <c r="N311" s="5">
+        <v>1</v>
+      </c>
+      <c r="O311" s="5">
+        <v>1</v>
+      </c>
+      <c r="P311" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="312" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A312" s="5">
+        <v>28</v>
+      </c>
+      <c r="B312" s="5" t="s">
+        <v>438</v>
+      </c>
+      <c r="C312" s="5">
+        <v>248</v>
+      </c>
+      <c r="D312" s="5" t="s">
+        <v>963</v>
+      </c>
+      <c r="E312" s="5">
+        <v>1</v>
+      </c>
+      <c r="F312" s="5">
+        <v>1</v>
+      </c>
+      <c r="G312" s="5">
+        <v>0</v>
+      </c>
+      <c r="H312" s="5">
+        <v>1</v>
+      </c>
+      <c r="I312" s="5">
+        <v>0</v>
+      </c>
+      <c r="J312" s="5">
+        <v>1</v>
+      </c>
+      <c r="K312" s="5">
+        <v>1</v>
+      </c>
+      <c r="L312" s="5">
+        <v>1</v>
+      </c>
+      <c r="M312" s="5">
+        <v>1</v>
+      </c>
+      <c r="N312" s="5">
+        <v>1</v>
+      </c>
+      <c r="O312" s="5">
+        <v>1</v>
+      </c>
+      <c r="P312" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="313" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A313" s="5">
+        <v>29</v>
+      </c>
+      <c r="B313" s="5" t="s">
+        <v>439</v>
+      </c>
+      <c r="C313" s="5">
+        <v>246</v>
+      </c>
+      <c r="D313" s="5" t="s">
+        <v>961</v>
+      </c>
+      <c r="E313" s="5">
+        <v>1</v>
+      </c>
+      <c r="F313" s="5">
+        <v>1</v>
+      </c>
+      <c r="G313" s="5">
+        <v>0</v>
+      </c>
+      <c r="H313" s="5">
+        <v>1</v>
+      </c>
+      <c r="I313" s="5">
+        <v>0</v>
+      </c>
+      <c r="J313" s="5">
+        <v>1</v>
+      </c>
+      <c r="K313" s="5">
+        <v>1</v>
+      </c>
+      <c r="L313" s="5">
+        <v>1</v>
+      </c>
+      <c r="M313" s="5">
+        <v>1</v>
+      </c>
+      <c r="N313" s="5">
+        <v>1</v>
+      </c>
+      <c r="O313" s="5">
+        <v>1</v>
+      </c>
+      <c r="P313" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="314" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A314" s="5">
+        <v>29</v>
+      </c>
+      <c r="B314" s="5" t="s">
+        <v>439</v>
+      </c>
+      <c r="C314" s="5">
+        <v>247</v>
+      </c>
+      <c r="D314" s="5" t="s">
+        <v>962</v>
+      </c>
+      <c r="E314" s="5">
+        <v>1</v>
+      </c>
+      <c r="F314" s="5">
+        <v>1</v>
+      </c>
+      <c r="G314" s="5">
+        <v>0</v>
+      </c>
+      <c r="H314" s="5">
+        <v>1</v>
+      </c>
+      <c r="I314" s="5">
+        <v>0</v>
+      </c>
+      <c r="J314" s="5">
+        <v>1</v>
+      </c>
+      <c r="K314" s="5">
+        <v>1</v>
+      </c>
+      <c r="L314" s="5">
+        <v>1</v>
+      </c>
+      <c r="M314" s="5">
+        <v>1</v>
+      </c>
+      <c r="N314" s="5">
+        <v>1</v>
+      </c>
+      <c r="O314" s="5">
+        <v>1</v>
+      </c>
+      <c r="P314" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="315" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A315" s="5">
+        <v>29</v>
+      </c>
+      <c r="B315" s="5" t="s">
+        <v>439</v>
+      </c>
+      <c r="C315" s="5">
+        <v>248</v>
+      </c>
+      <c r="D315" s="5" t="s">
+        <v>963</v>
+      </c>
+      <c r="E315" s="5">
+        <v>1</v>
+      </c>
+      <c r="F315" s="5">
+        <v>1</v>
+      </c>
+      <c r="G315" s="5">
+        <v>0</v>
+      </c>
+      <c r="H315" s="5">
+        <v>1</v>
+      </c>
+      <c r="I315" s="5">
+        <v>0</v>
+      </c>
+      <c r="J315" s="5">
+        <v>1</v>
+      </c>
+      <c r="K315" s="5">
+        <v>1</v>
+      </c>
+      <c r="L315" s="5">
+        <v>1</v>
+      </c>
+      <c r="M315" s="5">
+        <v>1</v>
+      </c>
+      <c r="N315" s="5">
+        <v>1</v>
+      </c>
+      <c r="O315" s="5">
+        <v>1</v>
+      </c>
+      <c r="P315" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="316" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A316" s="5">
+        <v>30</v>
+      </c>
+      <c r="B316" s="5" t="s">
+        <v>440</v>
+      </c>
+      <c r="C316" s="5">
+        <v>246</v>
+      </c>
+      <c r="D316" s="5" t="s">
+        <v>961</v>
+      </c>
+      <c r="E316" s="5">
+        <v>1</v>
+      </c>
+      <c r="F316" s="5">
+        <v>1</v>
+      </c>
+      <c r="G316" s="5">
+        <v>0</v>
+      </c>
+      <c r="H316" s="5">
+        <v>1</v>
+      </c>
+      <c r="I316" s="5">
+        <v>0</v>
+      </c>
+      <c r="J316" s="5">
+        <v>1</v>
+      </c>
+      <c r="K316" s="5">
+        <v>1</v>
+      </c>
+      <c r="L316" s="5">
+        <v>1</v>
+      </c>
+      <c r="M316" s="5">
+        <v>1</v>
+      </c>
+      <c r="N316" s="5">
+        <v>1</v>
+      </c>
+      <c r="O316" s="5">
+        <v>1</v>
+      </c>
+      <c r="P316" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="317" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A317" s="5">
+        <v>30</v>
+      </c>
+      <c r="B317" s="5" t="s">
+        <v>440</v>
+      </c>
+      <c r="C317" s="5">
+        <v>247</v>
+      </c>
+      <c r="D317" s="5" t="s">
+        <v>962</v>
+      </c>
+      <c r="E317" s="5">
+        <v>1</v>
+      </c>
+      <c r="F317" s="5">
+        <v>1</v>
+      </c>
+      <c r="G317" s="5">
+        <v>0</v>
+      </c>
+      <c r="H317" s="5">
+        <v>1</v>
+      </c>
+      <c r="I317" s="5">
+        <v>0</v>
+      </c>
+      <c r="J317" s="5">
+        <v>1</v>
+      </c>
+      <c r="K317" s="5">
+        <v>1</v>
+      </c>
+      <c r="L317" s="5">
+        <v>1</v>
+      </c>
+      <c r="M317" s="5">
+        <v>1</v>
+      </c>
+      <c r="N317" s="5">
+        <v>1</v>
+      </c>
+      <c r="O317" s="5">
+        <v>1</v>
+      </c>
+      <c r="P317" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="318" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A318" s="5">
+        <v>30</v>
+      </c>
+      <c r="B318" s="5" t="s">
+        <v>440</v>
+      </c>
+      <c r="C318" s="5">
+        <v>248</v>
+      </c>
+      <c r="D318" s="5" t="s">
+        <v>963</v>
+      </c>
+      <c r="E318" s="5">
+        <v>1</v>
+      </c>
+      <c r="F318" s="5">
+        <v>1</v>
+      </c>
+      <c r="G318" s="5">
+        <v>0</v>
+      </c>
+      <c r="H318" s="5">
+        <v>1</v>
+      </c>
+      <c r="I318" s="5">
+        <v>0</v>
+      </c>
+      <c r="J318" s="5">
+        <v>1</v>
+      </c>
+      <c r="K318" s="5">
+        <v>1</v>
+      </c>
+      <c r="L318" s="5">
+        <v>1</v>
+      </c>
+      <c r="M318" s="5">
+        <v>1</v>
+      </c>
+      <c r="N318" s="5">
+        <v>1</v>
+      </c>
+      <c r="O318" s="5">
+        <v>1</v>
+      </c>
+      <c r="P318" s="5">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -34378,10 +34857,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B247"/>
+  <dimension ref="A1:B250"/>
   <sheetViews>
-    <sheetView topLeftCell="A232" workbookViewId="0">
-      <selection activeCell="A247" sqref="A247:B247"/>
+    <sheetView topLeftCell="A230" workbookViewId="0">
+      <selection activeCell="B253" sqref="B253"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -36359,11 +36838,35 @@
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A247" s="5">
+      <c r="A247">
         <v>245</v>
       </c>
-      <c r="B247" s="5" t="s">
+      <c r="B247" t="s">
         <v>958</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A248" s="5">
+        <v>246</v>
+      </c>
+      <c r="B248" s="5" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A249" s="5">
+        <v>247</v>
+      </c>
+      <c r="B249" s="5" t="s">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A250" s="5">
+        <v>248</v>
+      </c>
+      <c r="B250" s="5" t="s">
+        <v>963</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TFS 12320 - Coach the Coach as new sub-coaching reason to supervisor module
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C41018
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3561" uniqueCount="964">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3566" uniqueCount="966">
   <si>
     <t>SourceID</t>
   </si>
@@ -2933,9 +2933,6 @@
     <t>Set Active to 0 for sub-coaching reason Potential hardship to OMR/Exceptions in Coaching Reason Selection tab.</t>
   </si>
   <si>
-    <t>New sub coaching reason for warnings. Added records to SubCoaching Reason and Coaching Reason Selection table tabs</t>
-  </si>
-  <si>
     <t>Adherence</t>
   </si>
   <si>
@@ -2943,6 +2940,15 @@
   </si>
   <si>
     <t>Quality/Performance – Critical Fails</t>
+  </si>
+  <si>
+    <t>New sub coaching reason for warnings. Added records to SubCoaching Reasons (246/247/248) and Coaching Reason Selection table tabs</t>
+  </si>
+  <si>
+    <t>New sub coaching reason for Supervisors. Added records to SubCoaching Reason (249) and Coaching Reason Selection table tabs</t>
+  </si>
+  <si>
+    <t>Coach the Coach</t>
   </si>
 </sst>
 </file>
@@ -3001,7 +3007,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -3012,6 +3018,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3316,10 +3323,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E73"/>
+  <dimension ref="A1:E74"/>
   <sheetViews>
     <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="E73" sqref="E73"/>
+      <selection activeCell="E74" sqref="E74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4535,20 +4542,37 @@
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A73">
+      <c r="A73" s="5">
         <v>64</v>
       </c>
-      <c r="B73" s="1">
+      <c r="B73" s="8">
         <v>43383</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C73" s="5" t="s">
         <v>430</v>
       </c>
-      <c r="D73">
+      <c r="D73" s="5">
         <v>12308</v>
       </c>
-      <c r="E73" t="s">
-        <v>960</v>
+      <c r="E73" s="5" t="s">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A74" s="5">
+        <v>65</v>
+      </c>
+      <c r="B74" s="8">
+        <v>43383</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>430</v>
+      </c>
+      <c r="D74" s="5">
+        <v>12308</v>
+      </c>
+      <c r="E74" s="5" t="s">
+        <v>964</v>
       </c>
     </row>
   </sheetData>
@@ -5974,10 +5998,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P318"/>
+  <dimension ref="A1:P319"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A298" workbookViewId="0">
-      <selection activeCell="A319" sqref="A319"/>
+      <selection activeCell="A319" sqref="A319:P319"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -21446,7 +21470,7 @@
         <v>246</v>
       </c>
       <c r="D310" s="5" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="E310" s="5">
         <v>1</v>
@@ -21496,7 +21520,7 @@
         <v>247</v>
       </c>
       <c r="D311" s="5" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="E311" s="5">
         <v>1</v>
@@ -21546,7 +21570,7 @@
         <v>248</v>
       </c>
       <c r="D312" s="5" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="E312" s="5">
         <v>1</v>
@@ -21596,7 +21620,7 @@
         <v>246</v>
       </c>
       <c r="D313" s="5" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="E313" s="5">
         <v>1</v>
@@ -21646,7 +21670,7 @@
         <v>247</v>
       </c>
       <c r="D314" s="5" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="E314" s="5">
         <v>1</v>
@@ -21696,7 +21720,7 @@
         <v>248</v>
       </c>
       <c r="D315" s="5" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="E315" s="5">
         <v>1</v>
@@ -21746,7 +21770,7 @@
         <v>246</v>
       </c>
       <c r="D316" s="5" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="E316" s="5">
         <v>1</v>
@@ -21796,7 +21820,7 @@
         <v>247</v>
       </c>
       <c r="D317" s="5" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="E317" s="5">
         <v>1</v>
@@ -21846,7 +21870,7 @@
         <v>248</v>
       </c>
       <c r="D318" s="5" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="E318" s="5">
         <v>1</v>
@@ -21883,6 +21907,56 @@
       </c>
       <c r="P318" s="5">
         <v>1</v>
+      </c>
+    </row>
+    <row r="319" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A319" s="5">
+        <v>25</v>
+      </c>
+      <c r="B319" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C319" s="5">
+        <v>249</v>
+      </c>
+      <c r="D319" s="5" t="s">
+        <v>965</v>
+      </c>
+      <c r="E319" s="5">
+        <v>1</v>
+      </c>
+      <c r="F319" s="5">
+        <v>1</v>
+      </c>
+      <c r="G319" s="5">
+        <v>1</v>
+      </c>
+      <c r="H319" s="5">
+        <v>1</v>
+      </c>
+      <c r="I319" s="5">
+        <v>1</v>
+      </c>
+      <c r="J319" s="5">
+        <v>0</v>
+      </c>
+      <c r="K319" s="5">
+        <v>0</v>
+      </c>
+      <c r="L319" s="5">
+        <v>1</v>
+      </c>
+      <c r="M319" s="5">
+        <v>0</v>
+      </c>
+      <c r="N319" s="5">
+        <v>0</v>
+      </c>
+      <c r="O319" s="5">
+        <v>0</v>
+      </c>
+      <c r="P319" s="5">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -34857,10 +34931,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B250"/>
+  <dimension ref="A1:B251"/>
   <sheetViews>
     <sheetView topLeftCell="A230" workbookViewId="0">
-      <selection activeCell="B253" sqref="B253"/>
+      <selection activeCell="B251" sqref="B251"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -36850,7 +36924,7 @@
         <v>246</v>
       </c>
       <c r="B248" s="5" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.3">
@@ -36858,7 +36932,7 @@
         <v>247</v>
       </c>
       <c r="B249" s="5" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.3">
@@ -36866,7 +36940,15 @@
         <v>248</v>
       </c>
       <c r="B250" s="5" t="s">
-        <v>963</v>
+        <v>962</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A251" s="5">
+        <v>249</v>
+      </c>
+      <c r="B251" s="5" t="s">
+        <v>965</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TFS 12316 - Historical dashboard access for select analysts
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C41022
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="132" windowWidth="22992" windowHeight="12840" firstSheet="7" activeTab="11"/>
+    <workbookView xWindow="480" yWindow="132" windowWidth="22992" windowHeight="12840" firstSheet="22" activeTab="25"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_History" sheetId="14" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3566" uniqueCount="966">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3572" uniqueCount="969">
   <si>
     <t>SourceID</t>
   </si>
@@ -2949,6 +2949,15 @@
   </si>
   <si>
     <t>Coach the Coach</t>
+  </si>
+  <si>
+    <t>Added new Analyst Role in UI_User_Role, UI_Role_Page_Access, UI_Dashboard_Summary_Display tabs</t>
+  </si>
+  <si>
+    <t>Analyst</t>
+  </si>
+  <si>
+    <t>WPPM% and ECL Role in ACL</t>
   </si>
 </sst>
 </file>
@@ -2975,7 +2984,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2994,6 +3003,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -3007,7 +3022,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -3019,6 +3034,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3323,10 +3340,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E74"/>
+  <dimension ref="A1:E76"/>
   <sheetViews>
     <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="E74" sqref="E74"/>
+      <selection activeCell="A75" sqref="A75:E76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4542,38 +4559,62 @@
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A73" s="5">
+      <c r="A73" s="9">
         <v>64</v>
       </c>
-      <c r="B73" s="8">
+      <c r="B73" s="10">
         <v>43383</v>
       </c>
-      <c r="C73" s="5" t="s">
+      <c r="C73" s="9" t="s">
         <v>430</v>
       </c>
-      <c r="D73" s="5">
+      <c r="D73" s="9">
         <v>12308</v>
       </c>
-      <c r="E73" s="5" t="s">
+      <c r="E73" s="9" t="s">
         <v>963</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A74" s="5">
+      <c r="A74" s="9">
         <v>65</v>
       </c>
-      <c r="B74" s="8">
+      <c r="B74" s="10">
         <v>43383</v>
       </c>
-      <c r="C74" s="5" t="s">
+      <c r="C74" s="9" t="s">
         <v>430</v>
       </c>
-      <c r="D74" s="5">
+      <c r="D74" s="9">
         <v>12308</v>
       </c>
-      <c r="E74" s="5" t="s">
+      <c r="E74" s="9" t="s">
         <v>964</v>
       </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A75" s="5">
+        <v>66</v>
+      </c>
+      <c r="B75" s="8">
+        <v>43385</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>430</v>
+      </c>
+      <c r="D75" s="5">
+        <v>12316</v>
+      </c>
+      <c r="E75" s="5" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A76" s="5"/>
+      <c r="B76" s="5"/>
+      <c r="C76" s="5"/>
+      <c r="D76" s="5"/>
+      <c r="E76" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6000,7 +6041,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P319"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A298" workbookViewId="0">
+    <sheetView topLeftCell="A298" workbookViewId="0">
       <selection activeCell="A319" sqref="A319:P319"/>
     </sheetView>
   </sheetViews>
@@ -33142,10 +33183,10 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A11" sqref="A11:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -33265,6 +33306,17 @@
         <v>951</v>
       </c>
     </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="5">
+        <v>110</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>967</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>968</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -33272,10 +33324,10 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A11" sqref="A11:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -33457,6 +33509,23 @@
         <v>0</v>
       </c>
     </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="5">
+        <v>110</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>967</v>
+      </c>
+      <c r="C11" s="5">
+        <v>1</v>
+      </c>
+      <c r="D11" s="5">
+        <v>0</v>
+      </c>
+      <c r="E11" s="5">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -33464,10 +33533,10 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -33739,6 +33808,32 @@
         <v>0</v>
       </c>
       <c r="H10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="5">
+        <v>110</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>967</v>
+      </c>
+      <c r="C11" s="5">
+        <v>0</v>
+      </c>
+      <c r="D11" s="5">
+        <v>0</v>
+      </c>
+      <c r="E11" s="5">
+        <v>0</v>
+      </c>
+      <c r="F11" s="5">
+        <v>0</v>
+      </c>
+      <c r="G11" s="5">
+        <v>0</v>
+      </c>
+      <c r="H11" s="5">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
TFS 12455– Requesting access for WEEXDV to all modules
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C41087
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="132" windowWidth="22992" windowHeight="12840" firstSheet="22" activeTab="25"/>
+    <workbookView xWindow="480" yWindow="132" windowWidth="22992" windowHeight="12840" firstSheet="4" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_History" sheetId="14" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3572" uniqueCount="969">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3576" uniqueCount="972">
   <si>
     <t>SourceID</t>
   </si>
@@ -2958,6 +2958,15 @@
   </si>
   <si>
     <t>WPPM% and ECL Role in ACL</t>
+  </si>
+  <si>
+    <t>Requesting access for Brian Dye to all modules. Updated Module_Submission tab</t>
+  </si>
+  <si>
+    <t>WEEXDV</t>
+  </si>
+  <si>
+    <t>Division Vice President</t>
   </si>
 </sst>
 </file>
@@ -3022,7 +3031,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -3036,6 +3045,7 @@
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3342,8 +3352,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E76"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="A75" sqref="A75:E76"/>
+    <sheetView topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="E82" sqref="E82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4592,29 +4602,39 @@
         <v>964</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A75" s="5">
+    <row r="75" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="6">
         <v>66</v>
       </c>
-      <c r="B75" s="8">
+      <c r="B75" s="11">
         <v>43385</v>
       </c>
-      <c r="C75" s="5" t="s">
+      <c r="C75" s="6" t="s">
         <v>430</v>
       </c>
-      <c r="D75" s="5">
+      <c r="D75" s="6">
         <v>12316</v>
       </c>
-      <c r="E75" s="5" t="s">
+      <c r="E75" s="6" t="s">
         <v>966</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A76" s="5"/>
-      <c r="B76" s="5"/>
-      <c r="C76" s="5"/>
-      <c r="D76" s="5"/>
-      <c r="E76" s="5"/>
+    <row r="76" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="5">
+        <v>67</v>
+      </c>
+      <c r="B76" s="8">
+        <v>43396</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>430</v>
+      </c>
+      <c r="D76" s="5">
+        <v>12455</v>
+      </c>
+      <c r="E76" s="5" t="s">
+        <v>969</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4624,9 +4644,11 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G58"/>
+  <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59:G59"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -5962,6 +5984,29 @@
       </c>
       <c r="G58">
         <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A59" s="5" t="s">
+        <v>970</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>971</v>
+      </c>
+      <c r="C59" s="5">
+        <v>1</v>
+      </c>
+      <c r="D59" s="5">
+        <v>1</v>
+      </c>
+      <c r="E59" s="5">
+        <v>1</v>
+      </c>
+      <c r="F59" s="5">
+        <v>1</v>
+      </c>
+      <c r="G59" s="5">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -33535,7 +33580,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11:H11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
TFS 12467 - Assign Manager Role to WPPM job codes
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C41111
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="132" windowWidth="22992" windowHeight="12840" firstSheet="4" activeTab="9"/>
+    <workbookView xWindow="480" yWindow="132" windowWidth="22992" windowHeight="12840" firstSheet="19" activeTab="23"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_History" sheetId="14" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3576" uniqueCount="972">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3578" uniqueCount="973">
   <si>
     <t>SourceID</t>
   </si>
@@ -2915,9 +2915,6 @@
     <t>%40 or WTTI% or WACQ13</t>
   </si>
   <si>
-    <t>%50 or %60 or %70 or WEEX% or WISO% or WISY% or WPWL% or WSTE%</t>
-  </si>
-  <si>
     <t>WACQ0% or WACQ12 or WIHD0% or WTTR1% or WTID%</t>
   </si>
   <si>
@@ -2957,9 +2954,6 @@
     <t>Analyst</t>
   </si>
   <si>
-    <t>WPPM% and ECL Role in ACL</t>
-  </si>
-  <si>
     <t>Requesting access for Brian Dye to all modules. Updated Module_Submission tab</t>
   </si>
   <si>
@@ -2967,6 +2961,15 @@
   </si>
   <si>
     <t>Division Vice President</t>
+  </si>
+  <si>
+    <t>Assign Manager Role to WPPM job codes . Updated RoleDescription in UI_User_Role tab for Analyst and Manager roles.</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>%50 or %60 or %70 or WEEX% or WISO% or WISY% or WPWL% or WSTE% or WPPM%</t>
   </si>
 </sst>
 </file>
@@ -3031,7 +3034,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -3046,6 +3049,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3350,10 +3356,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E76"/>
+  <dimension ref="A1:L77"/>
   <sheetViews>
     <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="E82" sqref="E82"/>
+      <selection activeCell="E77" sqref="E77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4432,7 +4438,7 @@
         <v>897</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>57</v>
       </c>
@@ -4449,7 +4455,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>58</v>
       </c>
@@ -4466,7 +4472,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>59</v>
       </c>
@@ -4483,7 +4489,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>60</v>
       </c>
@@ -4500,7 +4506,7 @@
         <v>912</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>61</v>
       </c>
@@ -4517,7 +4523,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>61.1</v>
       </c>
@@ -4531,10 +4537,10 @@
         <v>7137</v>
       </c>
       <c r="E70" t="s">
-        <v>956</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>62</v>
       </c>
@@ -4548,10 +4554,10 @@
         <v>11500</v>
       </c>
       <c r="E71" t="s">
-        <v>957</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>63</v>
       </c>
@@ -4565,10 +4571,10 @@
         <v>11451</v>
       </c>
       <c r="E72" t="s">
-        <v>959</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73" s="9">
         <v>64</v>
       </c>
@@ -4582,10 +4588,10 @@
         <v>12308</v>
       </c>
       <c r="E73" s="9" t="s">
-        <v>963</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74" s="9">
         <v>65</v>
       </c>
@@ -4599,10 +4605,10 @@
         <v>12308</v>
       </c>
       <c r="E74" s="9" t="s">
-        <v>964</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A75" s="6">
         <v>66</v>
       </c>
@@ -4616,24 +4622,48 @@
         <v>12316</v>
       </c>
       <c r="E75" s="6" t="s">
-        <v>966</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="5">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="6">
         <v>67</v>
       </c>
-      <c r="B76" s="8">
+      <c r="B76" s="6">
         <v>43396</v>
       </c>
-      <c r="C76" s="5" t="s">
+      <c r="C76" s="6" t="s">
         <v>430</v>
       </c>
-      <c r="D76" s="5">
+      <c r="D76" s="11">
         <v>12455</v>
       </c>
-      <c r="E76" s="5" t="s">
-        <v>969</v>
+      <c r="E76" s="6" t="s">
+        <v>967</v>
+      </c>
+      <c r="F76" s="6"/>
+      <c r="G76" s="11"/>
+      <c r="H76" s="6"/>
+      <c r="I76" s="6"/>
+      <c r="J76" s="11"/>
+      <c r="K76" s="6"/>
+      <c r="L76" s="6"/>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A77" s="5">
+        <v>68</v>
+      </c>
+      <c r="B77" s="8">
+        <v>43402</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>430</v>
+      </c>
+      <c r="D77" s="5">
+        <v>12467</v>
+      </c>
+      <c r="E77" s="5" t="s">
+        <v>970</v>
       </c>
     </row>
   </sheetData>
@@ -4646,7 +4676,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+    <sheetView topLeftCell="A46" workbookViewId="0">
       <selection activeCell="A59" sqref="A59:G59"/>
     </sheetView>
   </sheetViews>
@@ -5988,10 +6018,10 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
       <c r="C59" s="5">
         <v>1</v>
@@ -21506,7 +21536,7 @@
         <v>245</v>
       </c>
       <c r="D309" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="E309">
         <v>0</v>
@@ -21556,7 +21586,7 @@
         <v>246</v>
       </c>
       <c r="D310" s="5" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="E310" s="5">
         <v>1</v>
@@ -21606,7 +21636,7 @@
         <v>247</v>
       </c>
       <c r="D311" s="5" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="E311" s="5">
         <v>1</v>
@@ -21656,7 +21686,7 @@
         <v>248</v>
       </c>
       <c r="D312" s="5" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="E312" s="5">
         <v>1</v>
@@ -21706,7 +21736,7 @@
         <v>246</v>
       </c>
       <c r="D313" s="5" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="E313" s="5">
         <v>1</v>
@@ -21756,7 +21786,7 @@
         <v>247</v>
       </c>
       <c r="D314" s="5" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="E314" s="5">
         <v>1</v>
@@ -21806,7 +21836,7 @@
         <v>248</v>
       </c>
       <c r="D315" s="5" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="E315" s="5">
         <v>1</v>
@@ -21856,7 +21886,7 @@
         <v>246</v>
       </c>
       <c r="D316" s="5" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="E316" s="5">
         <v>1</v>
@@ -21906,7 +21936,7 @@
         <v>247</v>
       </c>
       <c r="D317" s="5" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="E317" s="5">
         <v>1</v>
@@ -21956,7 +21986,7 @@
         <v>248</v>
       </c>
       <c r="D318" s="5" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="E318" s="5">
         <v>1</v>
@@ -22006,7 +22036,7 @@
         <v>249</v>
       </c>
       <c r="D319" s="5" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="E319" s="5">
         <v>1</v>
@@ -33230,9 +33260,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:C11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -33285,15 +33313,15 @@
         <v>953</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5">
+    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="5">
         <v>104</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="5" t="s">
         <v>379</v>
       </c>
-      <c r="C5" t="s">
-        <v>954</v>
+      <c r="C5" s="12" t="s">
+        <v>972</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -33326,7 +33354,7 @@
         <v>423</v>
       </c>
       <c r="C8" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -33356,14 +33384,15 @@
         <v>110</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>968</v>
+        <v>971</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -33559,7 +33588,7 @@
         <v>110</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="C11" s="5">
         <v>1</v>
@@ -33861,7 +33890,7 @@
         <v>110</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="C11" s="5">
         <v>0</v>
@@ -37056,7 +37085,7 @@
         <v>245</v>
       </c>
       <c r="B247" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.3">
@@ -37064,7 +37093,7 @@
         <v>246</v>
       </c>
       <c r="B248" s="5" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.3">
@@ -37072,7 +37101,7 @@
         <v>247</v>
       </c>
       <c r="B249" s="5" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.3">
@@ -37080,7 +37109,7 @@
         <v>248</v>
       </c>
       <c r="B250" s="5" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.3">
@@ -37088,7 +37117,7 @@
         <v>249</v>
       </c>
       <c r="B251" s="5" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TFS 12591 - Overturned quality appeal coaching logs
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C41321
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="132" windowWidth="22992" windowHeight="12840" firstSheet="19" activeTab="23"/>
+    <workbookView xWindow="480" yWindow="132" windowWidth="22992" windowHeight="12840"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_History" sheetId="14" r:id="rId1"/>
@@ -42,7 +42,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">Coaching_Reason_Selection!$A$1:$P$292</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">DIM_Source!$A$1:$H$57</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">DIM_Source!$A$1:$H$58</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">Email_Notifications!$A$1:$K$163</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3578" uniqueCount="973">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3593" uniqueCount="975">
   <si>
     <t>SourceID</t>
   </si>
@@ -2970,6 +2970,12 @@
   </si>
   <si>
     <t>%50 or %60 or %70 or WEEX% or WISO% or WISY% or WPWL% or WSTE% or WPPM%</t>
+  </si>
+  <si>
+    <t>Added new source 'Quality Alignment' in DIM_Source tab and new record in Email Notification tab for Quality Module and Quality Alignment source</t>
+  </si>
+  <si>
+    <t>Quality Alignment</t>
   </si>
 </sst>
 </file>
@@ -3356,10 +3362,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L77"/>
+  <dimension ref="A1:L78"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="E77" sqref="E77"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="A78" sqref="A78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4649,21 +4655,38 @@
       <c r="K76" s="6"/>
       <c r="L76" s="6"/>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A77" s="5">
+    <row r="77" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="6">
         <v>68</v>
       </c>
-      <c r="B77" s="8">
+      <c r="B77" s="11">
         <v>43402</v>
       </c>
-      <c r="C77" s="5" t="s">
+      <c r="C77" s="6" t="s">
         <v>430</v>
       </c>
-      <c r="D77" s="5">
+      <c r="D77" s="6">
         <v>12467</v>
       </c>
-      <c r="E77" s="5" t="s">
+      <c r="E77" s="6" t="s">
         <v>970</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A78" s="5">
+        <v>69</v>
+      </c>
+      <c r="B78" s="8">
+        <v>43433</v>
+      </c>
+      <c r="C78" s="5" t="s">
+        <v>430</v>
+      </c>
+      <c r="D78" s="5">
+        <v>12591</v>
+      </c>
+      <c r="E78" s="5" t="s">
+        <v>973</v>
       </c>
     </row>
   </sheetData>
@@ -6017,25 +6040,25 @@
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A59" s="5" t="s">
+      <c r="A59" s="6" t="s">
         <v>968</v>
       </c>
-      <c r="B59" s="5" t="s">
+      <c r="B59" s="6" t="s">
         <v>969</v>
       </c>
-      <c r="C59" s="5">
-        <v>1</v>
-      </c>
-      <c r="D59" s="5">
-        <v>1</v>
-      </c>
-      <c r="E59" s="5">
-        <v>1</v>
-      </c>
-      <c r="F59" s="5">
-        <v>1</v>
-      </c>
-      <c r="G59" s="5">
+      <c r="C59" s="6">
+        <v>1</v>
+      </c>
+      <c r="D59" s="6">
+        <v>1</v>
+      </c>
+      <c r="E59" s="6">
+        <v>1</v>
+      </c>
+      <c r="F59" s="6">
+        <v>1</v>
+      </c>
+      <c r="G59" s="6">
         <v>1</v>
       </c>
     </row>
@@ -6117,7 +6140,7 @@
   <dimension ref="A1:P319"/>
   <sheetViews>
     <sheetView topLeftCell="A298" workbookViewId="0">
-      <selection activeCell="A319" sqref="A319:P319"/>
+      <selection activeCell="A310" sqref="A310:P319"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -21576,502 +21599,502 @@
       </c>
     </row>
     <row r="310" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A310" s="5">
+      <c r="A310">
         <v>28</v>
       </c>
-      <c r="B310" s="5" t="s">
+      <c r="B310" t="s">
         <v>438</v>
       </c>
-      <c r="C310" s="5">
+      <c r="C310">
         <v>246</v>
       </c>
-      <c r="D310" s="5" t="s">
+      <c r="D310" t="s">
         <v>959</v>
       </c>
-      <c r="E310" s="5">
-        <v>1</v>
-      </c>
-      <c r="F310" s="5">
-        <v>1</v>
-      </c>
-      <c r="G310" s="5">
-        <v>0</v>
-      </c>
-      <c r="H310" s="5">
-        <v>1</v>
-      </c>
-      <c r="I310" s="5">
-        <v>0</v>
-      </c>
-      <c r="J310" s="5">
-        <v>1</v>
-      </c>
-      <c r="K310" s="5">
-        <v>1</v>
-      </c>
-      <c r="L310" s="5">
-        <v>1</v>
-      </c>
-      <c r="M310" s="5">
-        <v>1</v>
-      </c>
-      <c r="N310" s="5">
-        <v>1</v>
-      </c>
-      <c r="O310" s="5">
-        <v>1</v>
-      </c>
-      <c r="P310" s="5">
+      <c r="E310">
+        <v>1</v>
+      </c>
+      <c r="F310">
+        <v>1</v>
+      </c>
+      <c r="G310">
+        <v>0</v>
+      </c>
+      <c r="H310">
+        <v>1</v>
+      </c>
+      <c r="I310">
+        <v>0</v>
+      </c>
+      <c r="J310">
+        <v>1</v>
+      </c>
+      <c r="K310">
+        <v>1</v>
+      </c>
+      <c r="L310">
+        <v>1</v>
+      </c>
+      <c r="M310">
+        <v>1</v>
+      </c>
+      <c r="N310">
+        <v>1</v>
+      </c>
+      <c r="O310">
+        <v>1</v>
+      </c>
+      <c r="P310">
         <v>1</v>
       </c>
     </row>
     <row r="311" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A311" s="5">
+      <c r="A311">
         <v>28</v>
       </c>
-      <c r="B311" s="5" t="s">
+      <c r="B311" t="s">
         <v>438</v>
       </c>
-      <c r="C311" s="5">
+      <c r="C311">
         <v>247</v>
       </c>
-      <c r="D311" s="5" t="s">
+      <c r="D311" t="s">
         <v>960</v>
       </c>
-      <c r="E311" s="5">
-        <v>1</v>
-      </c>
-      <c r="F311" s="5">
-        <v>1</v>
-      </c>
-      <c r="G311" s="5">
-        <v>0</v>
-      </c>
-      <c r="H311" s="5">
-        <v>1</v>
-      </c>
-      <c r="I311" s="5">
-        <v>0</v>
-      </c>
-      <c r="J311" s="5">
-        <v>1</v>
-      </c>
-      <c r="K311" s="5">
-        <v>1</v>
-      </c>
-      <c r="L311" s="5">
-        <v>1</v>
-      </c>
-      <c r="M311" s="5">
-        <v>1</v>
-      </c>
-      <c r="N311" s="5">
-        <v>1</v>
-      </c>
-      <c r="O311" s="5">
-        <v>1</v>
-      </c>
-      <c r="P311" s="5">
+      <c r="E311">
+        <v>1</v>
+      </c>
+      <c r="F311">
+        <v>1</v>
+      </c>
+      <c r="G311">
+        <v>0</v>
+      </c>
+      <c r="H311">
+        <v>1</v>
+      </c>
+      <c r="I311">
+        <v>0</v>
+      </c>
+      <c r="J311">
+        <v>1</v>
+      </c>
+      <c r="K311">
+        <v>1</v>
+      </c>
+      <c r="L311">
+        <v>1</v>
+      </c>
+      <c r="M311">
+        <v>1</v>
+      </c>
+      <c r="N311">
+        <v>1</v>
+      </c>
+      <c r="O311">
+        <v>1</v>
+      </c>
+      <c r="P311">
         <v>1</v>
       </c>
     </row>
     <row r="312" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A312" s="5">
+      <c r="A312">
         <v>28</v>
       </c>
-      <c r="B312" s="5" t="s">
+      <c r="B312" t="s">
         <v>438</v>
       </c>
-      <c r="C312" s="5">
+      <c r="C312">
         <v>248</v>
       </c>
-      <c r="D312" s="5" t="s">
+      <c r="D312" t="s">
         <v>961</v>
       </c>
-      <c r="E312" s="5">
-        <v>1</v>
-      </c>
-      <c r="F312" s="5">
-        <v>1</v>
-      </c>
-      <c r="G312" s="5">
-        <v>0</v>
-      </c>
-      <c r="H312" s="5">
-        <v>1</v>
-      </c>
-      <c r="I312" s="5">
-        <v>0</v>
-      </c>
-      <c r="J312" s="5">
-        <v>1</v>
-      </c>
-      <c r="K312" s="5">
-        <v>1</v>
-      </c>
-      <c r="L312" s="5">
-        <v>1</v>
-      </c>
-      <c r="M312" s="5">
-        <v>1</v>
-      </c>
-      <c r="N312" s="5">
-        <v>1</v>
-      </c>
-      <c r="O312" s="5">
-        <v>1</v>
-      </c>
-      <c r="P312" s="5">
+      <c r="E312">
+        <v>1</v>
+      </c>
+      <c r="F312">
+        <v>1</v>
+      </c>
+      <c r="G312">
+        <v>0</v>
+      </c>
+      <c r="H312">
+        <v>1</v>
+      </c>
+      <c r="I312">
+        <v>0</v>
+      </c>
+      <c r="J312">
+        <v>1</v>
+      </c>
+      <c r="K312">
+        <v>1</v>
+      </c>
+      <c r="L312">
+        <v>1</v>
+      </c>
+      <c r="M312">
+        <v>1</v>
+      </c>
+      <c r="N312">
+        <v>1</v>
+      </c>
+      <c r="O312">
+        <v>1</v>
+      </c>
+      <c r="P312">
         <v>1</v>
       </c>
     </row>
     <row r="313" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A313" s="5">
+      <c r="A313">
         <v>29</v>
       </c>
-      <c r="B313" s="5" t="s">
+      <c r="B313" t="s">
         <v>439</v>
       </c>
-      <c r="C313" s="5">
+      <c r="C313">
         <v>246</v>
       </c>
-      <c r="D313" s="5" t="s">
+      <c r="D313" t="s">
         <v>959</v>
       </c>
-      <c r="E313" s="5">
-        <v>1</v>
-      </c>
-      <c r="F313" s="5">
-        <v>1</v>
-      </c>
-      <c r="G313" s="5">
-        <v>0</v>
-      </c>
-      <c r="H313" s="5">
-        <v>1</v>
-      </c>
-      <c r="I313" s="5">
-        <v>0</v>
-      </c>
-      <c r="J313" s="5">
-        <v>1</v>
-      </c>
-      <c r="K313" s="5">
-        <v>1</v>
-      </c>
-      <c r="L313" s="5">
-        <v>1</v>
-      </c>
-      <c r="M313" s="5">
-        <v>1</v>
-      </c>
-      <c r="N313" s="5">
-        <v>1</v>
-      </c>
-      <c r="O313" s="5">
-        <v>1</v>
-      </c>
-      <c r="P313" s="5">
+      <c r="E313">
+        <v>1</v>
+      </c>
+      <c r="F313">
+        <v>1</v>
+      </c>
+      <c r="G313">
+        <v>0</v>
+      </c>
+      <c r="H313">
+        <v>1</v>
+      </c>
+      <c r="I313">
+        <v>0</v>
+      </c>
+      <c r="J313">
+        <v>1</v>
+      </c>
+      <c r="K313">
+        <v>1</v>
+      </c>
+      <c r="L313">
+        <v>1</v>
+      </c>
+      <c r="M313">
+        <v>1</v>
+      </c>
+      <c r="N313">
+        <v>1</v>
+      </c>
+      <c r="O313">
+        <v>1</v>
+      </c>
+      <c r="P313">
         <v>1</v>
       </c>
     </row>
     <row r="314" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A314" s="5">
+      <c r="A314">
         <v>29</v>
       </c>
-      <c r="B314" s="5" t="s">
+      <c r="B314" t="s">
         <v>439</v>
       </c>
-      <c r="C314" s="5">
+      <c r="C314">
         <v>247</v>
       </c>
-      <c r="D314" s="5" t="s">
+      <c r="D314" t="s">
         <v>960</v>
       </c>
-      <c r="E314" s="5">
-        <v>1</v>
-      </c>
-      <c r="F314" s="5">
-        <v>1</v>
-      </c>
-      <c r="G314" s="5">
-        <v>0</v>
-      </c>
-      <c r="H314" s="5">
-        <v>1</v>
-      </c>
-      <c r="I314" s="5">
-        <v>0</v>
-      </c>
-      <c r="J314" s="5">
-        <v>1</v>
-      </c>
-      <c r="K314" s="5">
-        <v>1</v>
-      </c>
-      <c r="L314" s="5">
-        <v>1</v>
-      </c>
-      <c r="M314" s="5">
-        <v>1</v>
-      </c>
-      <c r="N314" s="5">
-        <v>1</v>
-      </c>
-      <c r="O314" s="5">
-        <v>1</v>
-      </c>
-      <c r="P314" s="5">
+      <c r="E314">
+        <v>1</v>
+      </c>
+      <c r="F314">
+        <v>1</v>
+      </c>
+      <c r="G314">
+        <v>0</v>
+      </c>
+      <c r="H314">
+        <v>1</v>
+      </c>
+      <c r="I314">
+        <v>0</v>
+      </c>
+      <c r="J314">
+        <v>1</v>
+      </c>
+      <c r="K314">
+        <v>1</v>
+      </c>
+      <c r="L314">
+        <v>1</v>
+      </c>
+      <c r="M314">
+        <v>1</v>
+      </c>
+      <c r="N314">
+        <v>1</v>
+      </c>
+      <c r="O314">
+        <v>1</v>
+      </c>
+      <c r="P314">
         <v>1</v>
       </c>
     </row>
     <row r="315" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A315" s="5">
+      <c r="A315">
         <v>29</v>
       </c>
-      <c r="B315" s="5" t="s">
+      <c r="B315" t="s">
         <v>439</v>
       </c>
-      <c r="C315" s="5">
+      <c r="C315">
         <v>248</v>
       </c>
-      <c r="D315" s="5" t="s">
+      <c r="D315" t="s">
         <v>961</v>
       </c>
-      <c r="E315" s="5">
-        <v>1</v>
-      </c>
-      <c r="F315" s="5">
-        <v>1</v>
-      </c>
-      <c r="G315" s="5">
-        <v>0</v>
-      </c>
-      <c r="H315" s="5">
-        <v>1</v>
-      </c>
-      <c r="I315" s="5">
-        <v>0</v>
-      </c>
-      <c r="J315" s="5">
-        <v>1</v>
-      </c>
-      <c r="K315" s="5">
-        <v>1</v>
-      </c>
-      <c r="L315" s="5">
-        <v>1</v>
-      </c>
-      <c r="M315" s="5">
-        <v>1</v>
-      </c>
-      <c r="N315" s="5">
-        <v>1</v>
-      </c>
-      <c r="O315" s="5">
-        <v>1</v>
-      </c>
-      <c r="P315" s="5">
+      <c r="E315">
+        <v>1</v>
+      </c>
+      <c r="F315">
+        <v>1</v>
+      </c>
+      <c r="G315">
+        <v>0</v>
+      </c>
+      <c r="H315">
+        <v>1</v>
+      </c>
+      <c r="I315">
+        <v>0</v>
+      </c>
+      <c r="J315">
+        <v>1</v>
+      </c>
+      <c r="K315">
+        <v>1</v>
+      </c>
+      <c r="L315">
+        <v>1</v>
+      </c>
+      <c r="M315">
+        <v>1</v>
+      </c>
+      <c r="N315">
+        <v>1</v>
+      </c>
+      <c r="O315">
+        <v>1</v>
+      </c>
+      <c r="P315">
         <v>1</v>
       </c>
     </row>
     <row r="316" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A316" s="5">
+      <c r="A316">
         <v>30</v>
       </c>
-      <c r="B316" s="5" t="s">
+      <c r="B316" t="s">
         <v>440</v>
       </c>
-      <c r="C316" s="5">
+      <c r="C316">
         <v>246</v>
       </c>
-      <c r="D316" s="5" t="s">
+      <c r="D316" t="s">
         <v>959</v>
       </c>
-      <c r="E316" s="5">
-        <v>1</v>
-      </c>
-      <c r="F316" s="5">
-        <v>1</v>
-      </c>
-      <c r="G316" s="5">
-        <v>0</v>
-      </c>
-      <c r="H316" s="5">
-        <v>1</v>
-      </c>
-      <c r="I316" s="5">
-        <v>0</v>
-      </c>
-      <c r="J316" s="5">
-        <v>1</v>
-      </c>
-      <c r="K316" s="5">
-        <v>1</v>
-      </c>
-      <c r="L316" s="5">
-        <v>1</v>
-      </c>
-      <c r="M316" s="5">
-        <v>1</v>
-      </c>
-      <c r="N316" s="5">
-        <v>1</v>
-      </c>
-      <c r="O316" s="5">
-        <v>1</v>
-      </c>
-      <c r="P316" s="5">
+      <c r="E316">
+        <v>1</v>
+      </c>
+      <c r="F316">
+        <v>1</v>
+      </c>
+      <c r="G316">
+        <v>0</v>
+      </c>
+      <c r="H316">
+        <v>1</v>
+      </c>
+      <c r="I316">
+        <v>0</v>
+      </c>
+      <c r="J316">
+        <v>1</v>
+      </c>
+      <c r="K316">
+        <v>1</v>
+      </c>
+      <c r="L316">
+        <v>1</v>
+      </c>
+      <c r="M316">
+        <v>1</v>
+      </c>
+      <c r="N316">
+        <v>1</v>
+      </c>
+      <c r="O316">
+        <v>1</v>
+      </c>
+      <c r="P316">
         <v>1</v>
       </c>
     </row>
     <row r="317" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A317" s="5">
+      <c r="A317">
         <v>30</v>
       </c>
-      <c r="B317" s="5" t="s">
+      <c r="B317" t="s">
         <v>440</v>
       </c>
-      <c r="C317" s="5">
+      <c r="C317">
         <v>247</v>
       </c>
-      <c r="D317" s="5" t="s">
+      <c r="D317" t="s">
         <v>960</v>
       </c>
-      <c r="E317" s="5">
-        <v>1</v>
-      </c>
-      <c r="F317" s="5">
-        <v>1</v>
-      </c>
-      <c r="G317" s="5">
-        <v>0</v>
-      </c>
-      <c r="H317" s="5">
-        <v>1</v>
-      </c>
-      <c r="I317" s="5">
-        <v>0</v>
-      </c>
-      <c r="J317" s="5">
-        <v>1</v>
-      </c>
-      <c r="K317" s="5">
-        <v>1</v>
-      </c>
-      <c r="L317" s="5">
-        <v>1</v>
-      </c>
-      <c r="M317" s="5">
-        <v>1</v>
-      </c>
-      <c r="N317" s="5">
-        <v>1</v>
-      </c>
-      <c r="O317" s="5">
-        <v>1</v>
-      </c>
-      <c r="P317" s="5">
+      <c r="E317">
+        <v>1</v>
+      </c>
+      <c r="F317">
+        <v>1</v>
+      </c>
+      <c r="G317">
+        <v>0</v>
+      </c>
+      <c r="H317">
+        <v>1</v>
+      </c>
+      <c r="I317">
+        <v>0</v>
+      </c>
+      <c r="J317">
+        <v>1</v>
+      </c>
+      <c r="K317">
+        <v>1</v>
+      </c>
+      <c r="L317">
+        <v>1</v>
+      </c>
+      <c r="M317">
+        <v>1</v>
+      </c>
+      <c r="N317">
+        <v>1</v>
+      </c>
+      <c r="O317">
+        <v>1</v>
+      </c>
+      <c r="P317">
         <v>1</v>
       </c>
     </row>
     <row r="318" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A318" s="5">
+      <c r="A318">
         <v>30</v>
       </c>
-      <c r="B318" s="5" t="s">
+      <c r="B318" t="s">
         <v>440</v>
       </c>
-      <c r="C318" s="5">
+      <c r="C318">
         <v>248</v>
       </c>
-      <c r="D318" s="5" t="s">
+      <c r="D318" t="s">
         <v>961</v>
       </c>
-      <c r="E318" s="5">
-        <v>1</v>
-      </c>
-      <c r="F318" s="5">
-        <v>1</v>
-      </c>
-      <c r="G318" s="5">
-        <v>0</v>
-      </c>
-      <c r="H318" s="5">
-        <v>1</v>
-      </c>
-      <c r="I318" s="5">
-        <v>0</v>
-      </c>
-      <c r="J318" s="5">
-        <v>1</v>
-      </c>
-      <c r="K318" s="5">
-        <v>1</v>
-      </c>
-      <c r="L318" s="5">
-        <v>1</v>
-      </c>
-      <c r="M318" s="5">
-        <v>1</v>
-      </c>
-      <c r="N318" s="5">
-        <v>1</v>
-      </c>
-      <c r="O318" s="5">
-        <v>1</v>
-      </c>
-      <c r="P318" s="5">
+      <c r="E318">
+        <v>1</v>
+      </c>
+      <c r="F318">
+        <v>1</v>
+      </c>
+      <c r="G318">
+        <v>0</v>
+      </c>
+      <c r="H318">
+        <v>1</v>
+      </c>
+      <c r="I318">
+        <v>0</v>
+      </c>
+      <c r="J318">
+        <v>1</v>
+      </c>
+      <c r="K318">
+        <v>1</v>
+      </c>
+      <c r="L318">
+        <v>1</v>
+      </c>
+      <c r="M318">
+        <v>1</v>
+      </c>
+      <c r="N318">
+        <v>1</v>
+      </c>
+      <c r="O318">
+        <v>1</v>
+      </c>
+      <c r="P318">
         <v>1</v>
       </c>
     </row>
     <row r="319" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A319" s="5">
+      <c r="A319">
         <v>25</v>
       </c>
-      <c r="B319" s="5" t="s">
+      <c r="B319" t="s">
         <v>191</v>
       </c>
-      <c r="C319" s="5">
+      <c r="C319">
         <v>249</v>
       </c>
-      <c r="D319" s="5" t="s">
+      <c r="D319" t="s">
         <v>964</v>
       </c>
-      <c r="E319" s="5">
-        <v>1</v>
-      </c>
-      <c r="F319" s="5">
-        <v>1</v>
-      </c>
-      <c r="G319" s="5">
-        <v>1</v>
-      </c>
-      <c r="H319" s="5">
-        <v>1</v>
-      </c>
-      <c r="I319" s="5">
-        <v>1</v>
-      </c>
-      <c r="J319" s="5">
-        <v>0</v>
-      </c>
-      <c r="K319" s="5">
-        <v>0</v>
-      </c>
-      <c r="L319" s="5">
-        <v>1</v>
-      </c>
-      <c r="M319" s="5">
-        <v>0</v>
-      </c>
-      <c r="N319" s="5">
-        <v>0</v>
-      </c>
-      <c r="O319" s="5">
-        <v>0</v>
-      </c>
-      <c r="P319" s="5">
+      <c r="E319">
+        <v>1</v>
+      </c>
+      <c r="F319">
+        <v>1</v>
+      </c>
+      <c r="G319">
+        <v>1</v>
+      </c>
+      <c r="H319">
+        <v>1</v>
+      </c>
+      <c r="I319">
+        <v>1</v>
+      </c>
+      <c r="J319">
+        <v>0</v>
+      </c>
+      <c r="K319">
+        <v>0</v>
+      </c>
+      <c r="L319">
+        <v>1</v>
+      </c>
+      <c r="M319">
+        <v>0</v>
+      </c>
+      <c r="N319">
+        <v>0</v>
+      </c>
+      <c r="O319">
+        <v>0</v>
+      </c>
+      <c r="P319">
         <v>0</v>
       </c>
     </row>
@@ -22137,7 +22160,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" t="s">
         <v>910</v>
       </c>
       <c r="B3" t="s">
@@ -22212,10 +22235,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K174"/>
+  <dimension ref="A1:K175"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+    <sheetView topLeftCell="A159" workbookViewId="0">
+      <selection activeCell="A175" sqref="A175:K175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23388,38 +23411,38 @@
         <v>378</v>
       </c>
     </row>
-    <row r="34" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="5" t="s">
+    <row r="34" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="6" t="s">
         <v>377</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C34" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="D34" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E34" s="5">
-        <v>0</v>
-      </c>
-      <c r="F34" s="5" t="s">
+      <c r="E34" s="6">
+        <v>0</v>
+      </c>
+      <c r="F34" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="G34" s="5" t="s">
+      <c r="G34" s="6" t="s">
         <v>423</v>
       </c>
-      <c r="H34" s="5" t="s">
+      <c r="H34" s="6" t="s">
         <v>382</v>
       </c>
-      <c r="I34" s="5" t="s">
+      <c r="I34" s="6" t="s">
         <v>413</v>
       </c>
-      <c r="J34" s="5">
-        <v>0</v>
-      </c>
-      <c r="K34" s="5" t="s">
+      <c r="J34" s="6">
+        <v>0</v>
+      </c>
+      <c r="K34" s="6" t="s">
         <v>378</v>
       </c>
     </row>
@@ -28320,6 +28343,41 @@
         <v>0</v>
       </c>
       <c r="K174" s="6" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="175" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A175" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B175" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C175" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D175" s="5" t="s">
+        <v>974</v>
+      </c>
+      <c r="E175" s="5">
+        <v>0</v>
+      </c>
+      <c r="F175" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="G175" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="H175" s="5" t="s">
+        <v>389</v>
+      </c>
+      <c r="I175" s="5" t="s">
+        <v>420</v>
+      </c>
+      <c r="J175" s="5">
+        <v>0</v>
+      </c>
+      <c r="K175" s="5" t="s">
         <v>378</v>
       </c>
     </row>
@@ -29479,10 +29537,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I69"/>
+  <dimension ref="A1:I71"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A71" sqref="A71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -30537,43 +30595,43 @@
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37">
-        <v>201</v>
-      </c>
-      <c r="B37" t="s">
-        <v>3</v>
-      </c>
-      <c r="C37" t="s">
-        <v>6</v>
-      </c>
-      <c r="D37">
-        <v>1</v>
-      </c>
-      <c r="E37">
-        <v>1</v>
-      </c>
-      <c r="F37">
-        <v>0</v>
-      </c>
-      <c r="G37">
-        <v>0</v>
-      </c>
-      <c r="H37">
-        <v>0</v>
-      </c>
-      <c r="I37">
+      <c r="A37" s="5">
+        <v>134</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>974</v>
+      </c>
+      <c r="D37" s="5">
+        <v>0</v>
+      </c>
+      <c r="E37" s="5">
+        <v>0</v>
+      </c>
+      <c r="F37" s="5">
+        <v>0</v>
+      </c>
+      <c r="G37" s="5">
+        <v>0</v>
+      </c>
+      <c r="H37" s="5">
+        <v>0</v>
+      </c>
+      <c r="I37" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B38" t="s">
         <v>3</v>
       </c>
       <c r="C38" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D38">
         <v>1</v>
@@ -30585,24 +30643,24 @@
         <v>0</v>
       </c>
       <c r="G38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H38">
         <v>0</v>
       </c>
       <c r="I38">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B39" t="s">
         <v>3</v>
       </c>
       <c r="C39" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D39">
         <v>1</v>
@@ -30617,7 +30675,7 @@
         <v>1</v>
       </c>
       <c r="H39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I39">
         <v>1</v>
@@ -30625,13 +30683,13 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B40" t="s">
         <v>3</v>
       </c>
       <c r="C40" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D40">
         <v>1</v>
@@ -30646,21 +30704,21 @@
         <v>1</v>
       </c>
       <c r="H40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I40">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B41" t="s">
         <v>3</v>
       </c>
       <c r="C41" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D41">
         <v>1</v>
@@ -30678,18 +30736,18 @@
         <v>0</v>
       </c>
       <c r="I41">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B42" t="s">
         <v>3</v>
       </c>
       <c r="C42" t="s">
-        <v>170</v>
+        <v>10</v>
       </c>
       <c r="D42">
         <v>1</v>
@@ -30704,7 +30762,7 @@
         <v>1</v>
       </c>
       <c r="H42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I42">
         <v>1</v>
@@ -30712,13 +30770,13 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B43" t="s">
         <v>3</v>
       </c>
       <c r="C43" t="s">
-        <v>11</v>
+        <v>170</v>
       </c>
       <c r="D43">
         <v>1</v>
@@ -30733,7 +30791,7 @@
         <v>1</v>
       </c>
       <c r="H43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I43">
         <v>1</v>
@@ -30741,13 +30799,13 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B44" t="s">
         <v>3</v>
       </c>
       <c r="C44" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D44">
         <v>1</v>
@@ -30756,27 +30814,27 @@
         <v>1</v>
       </c>
       <c r="F44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G44">
         <v>1</v>
       </c>
       <c r="H44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I44">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B45" t="s">
         <v>3</v>
       </c>
       <c r="C45" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D45">
         <v>1</v>
@@ -30791,21 +30849,21 @@
         <v>1</v>
       </c>
       <c r="H45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I45">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B46" t="s">
         <v>3</v>
       </c>
       <c r="C46" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D46">
         <v>1</v>
@@ -30823,30 +30881,30 @@
         <v>0</v>
       </c>
       <c r="I46">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B47" t="s">
         <v>3</v>
       </c>
       <c r="C47" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D47">
         <v>1</v>
       </c>
       <c r="E47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H47">
         <v>0</v>
@@ -30857,13 +30915,13 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B48" t="s">
         <v>3</v>
       </c>
       <c r="C48" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D48">
         <v>1</v>
@@ -30886,13 +30944,13 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B49" t="s">
         <v>3</v>
       </c>
       <c r="C49" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D49">
         <v>1</v>
@@ -30915,13 +30973,13 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B50" t="s">
         <v>3</v>
       </c>
       <c r="C50" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D50">
         <v>1</v>
@@ -30944,13 +31002,13 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B51" t="s">
         <v>3</v>
       </c>
       <c r="C51" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D51">
         <v>1</v>
@@ -30973,13 +31031,13 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B52" t="s">
         <v>3</v>
       </c>
       <c r="C52" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D52">
         <v>1</v>
@@ -31002,13 +31060,13 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B53" t="s">
         <v>3</v>
       </c>
       <c r="C53" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D53">
         <v>1</v>
@@ -31031,71 +31089,71 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B54" t="s">
         <v>3</v>
       </c>
       <c r="C54" t="s">
-        <v>171</v>
+        <v>21</v>
       </c>
       <c r="D54">
         <v>1</v>
       </c>
       <c r="E54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H54">
         <v>0</v>
       </c>
       <c r="I54">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B55" t="s">
         <v>3</v>
       </c>
       <c r="C55" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D55">
         <v>1</v>
       </c>
       <c r="E55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F55">
         <v>1</v>
       </c>
       <c r="G55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H55">
         <v>0</v>
       </c>
       <c r="I55">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B56" t="s">
         <v>3</v>
       </c>
       <c r="C56" t="s">
-        <v>437</v>
+        <v>176</v>
       </c>
       <c r="D56">
         <v>1</v>
@@ -31104,7 +31162,7 @@
         <v>0</v>
       </c>
       <c r="F56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G56">
         <v>0</v>
@@ -31118,13 +31176,13 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B57" t="s">
         <v>3</v>
       </c>
       <c r="C57" t="s">
-        <v>172</v>
+        <v>437</v>
       </c>
       <c r="D57">
         <v>1</v>
@@ -31147,13 +31205,13 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B58" t="s">
         <v>3</v>
       </c>
       <c r="C58" t="s">
-        <v>470</v>
+        <v>172</v>
       </c>
       <c r="D58">
         <v>1</v>
@@ -31176,13 +31234,13 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B59" t="s">
         <v>3</v>
       </c>
       <c r="C59" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="D59">
         <v>1</v>
@@ -31205,13 +31263,13 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B60" t="s">
         <v>3</v>
       </c>
       <c r="C60" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D60">
         <v>1</v>
@@ -31234,13 +31292,13 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B61" t="s">
         <v>3</v>
       </c>
       <c r="C61" t="s">
-        <v>487</v>
+        <v>469</v>
       </c>
       <c r="D61">
         <v>1</v>
@@ -31255,7 +31313,7 @@
         <v>0</v>
       </c>
       <c r="H61">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I61">
         <v>0</v>
@@ -31263,16 +31321,16 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B62" t="s">
         <v>3</v>
       </c>
       <c r="C62" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E62">
         <v>0</v>
@@ -31284,7 +31342,7 @@
         <v>0</v>
       </c>
       <c r="H62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I62">
         <v>0</v>
@@ -31292,16 +31350,16 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B63" t="s">
         <v>3</v>
       </c>
       <c r="C63" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="D63">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E63">
         <v>0</v>
@@ -31313,7 +31371,7 @@
         <v>0</v>
       </c>
       <c r="H63">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I63">
         <v>0</v>
@@ -31321,13 +31379,13 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B64" t="s">
         <v>3</v>
       </c>
       <c r="C64" t="s">
-        <v>548</v>
+        <v>489</v>
       </c>
       <c r="D64">
         <v>1</v>
@@ -31342,21 +31400,21 @@
         <v>0</v>
       </c>
       <c r="H64">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I64">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B65" t="s">
         <v>3</v>
       </c>
       <c r="C65" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="D65">
         <v>1</v>
@@ -31379,13 +31437,13 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B66" t="s">
         <v>3</v>
       </c>
       <c r="C66" t="s">
-        <v>692</v>
+        <v>549</v>
       </c>
       <c r="D66">
         <v>1</v>
@@ -31403,21 +31461,21 @@
         <v>0</v>
       </c>
       <c r="I66">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B67" t="s">
         <v>3</v>
       </c>
       <c r="C67" t="s">
-        <v>740</v>
+        <v>692</v>
       </c>
       <c r="D67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E67">
         <v>0</v>
@@ -31437,16 +31495,16 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B68" t="s">
         <v>3</v>
       </c>
       <c r="C68" t="s">
-        <v>823</v>
+        <v>740</v>
       </c>
       <c r="D68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E68">
         <v>0</v>
@@ -31466,30 +31524,88 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B69" t="s">
         <v>3</v>
       </c>
       <c r="C69" t="s">
+        <v>823</v>
+      </c>
+      <c r="D69">
+        <v>1</v>
+      </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
+      <c r="F69">
+        <v>0</v>
+      </c>
+      <c r="G69">
+        <v>0</v>
+      </c>
+      <c r="H69">
+        <v>0</v>
+      </c>
+      <c r="I69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>233</v>
+      </c>
+      <c r="B70" t="s">
+        <v>3</v>
+      </c>
+      <c r="C70" t="s">
         <v>826</v>
       </c>
-      <c r="D69">
-        <v>1</v>
-      </c>
-      <c r="E69">
-        <v>0</v>
-      </c>
-      <c r="F69">
-        <v>0</v>
-      </c>
-      <c r="G69">
-        <v>0</v>
-      </c>
-      <c r="H69">
-        <v>0</v>
-      </c>
-      <c r="I69">
+      <c r="D70">
+        <v>1</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
+      </c>
+      <c r="F70">
+        <v>0</v>
+      </c>
+      <c r="G70">
+        <v>0</v>
+      </c>
+      <c r="H70">
+        <v>0</v>
+      </c>
+      <c r="I70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A71" s="5">
+        <v>234</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>974</v>
+      </c>
+      <c r="D71" s="5">
+        <v>1</v>
+      </c>
+      <c r="E71" s="5">
+        <v>0</v>
+      </c>
+      <c r="F71" s="5">
+        <v>0</v>
+      </c>
+      <c r="G71" s="5">
+        <v>0</v>
+      </c>
+      <c r="H71" s="5">
+        <v>0</v>
+      </c>
+      <c r="I71" s="5">
         <v>0</v>
       </c>
     </row>
@@ -33260,7 +33376,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -35103,7 +35219,7 @@
   <dimension ref="A1:B251"/>
   <sheetViews>
     <sheetView topLeftCell="A230" workbookViewId="0">
-      <selection activeCell="B251" sqref="B251"/>
+      <selection activeCell="B254" sqref="B254"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -37089,34 +37205,34 @@
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A248" s="5">
+      <c r="A248">
         <v>246</v>
       </c>
-      <c r="B248" s="5" t="s">
+      <c r="B248" t="s">
         <v>959</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A249" s="5">
+      <c r="A249">
         <v>247</v>
       </c>
-      <c r="B249" s="5" t="s">
+      <c r="B249" t="s">
         <v>960</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A250" s="5">
+      <c r="A250">
         <v>248</v>
       </c>
-      <c r="B250" s="5" t="s">
+      <c r="B250" t="s">
         <v>961</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A251" s="5">
+      <c r="A251">
         <v>249</v>
       </c>
-      <c r="B251" s="5" t="s">
+      <c r="B251" t="s">
         <v>964</v>
       </c>
     </row>
@@ -37822,82 +37938,82 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="5">
+      <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" t="s">
         <v>890</v>
       </c>
-      <c r="C8" s="5">
-        <v>0</v>
-      </c>
-      <c r="D8" s="5">
-        <v>0</v>
-      </c>
-      <c r="E8" s="5">
-        <v>0</v>
-      </c>
-      <c r="F8" s="5">
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="5">
+      <c r="A9">
         <v>7</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" t="s">
         <v>891</v>
       </c>
-      <c r="C9" s="5">
-        <v>0</v>
-      </c>
-      <c r="D9" s="5">
-        <v>0</v>
-      </c>
-      <c r="E9" s="5">
-        <v>0</v>
-      </c>
-      <c r="F9" s="5">
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="5">
+      <c r="A10">
         <v>8</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" t="s">
         <v>892</v>
       </c>
-      <c r="C10" s="5">
-        <v>0</v>
-      </c>
-      <c r="D10" s="5">
-        <v>0</v>
-      </c>
-      <c r="E10" s="5">
-        <v>0</v>
-      </c>
-      <c r="F10" s="5">
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="5">
+      <c r="A11">
         <v>9</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" t="s">
         <v>893</v>
       </c>
-      <c r="C11" s="5">
-        <v>0</v>
-      </c>
-      <c r="D11" s="5">
-        <v>0</v>
-      </c>
-      <c r="E11" s="5">
-        <v>0</v>
-      </c>
-      <c r="F11" s="5">
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
TFS 13334 -Changes to survey process to support Quality Now initiative
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C41811
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="132" windowWidth="22992" windowHeight="12840" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="132" windowWidth="22992" windowHeight="12840"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_History" sheetId="14" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3595" uniqueCount="976">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3605" uniqueCount="979">
   <si>
     <t>SourceID</t>
   </si>
@@ -2979,6 +2979,15 @@
   </si>
   <si>
     <t>Set Active = 1 for Direct quality Alignment in DIM_Source</t>
+  </si>
+  <si>
+    <t>Verint-CCO</t>
+  </si>
+  <si>
+    <t>Verint-CCO Supervisor</t>
+  </si>
+  <si>
+    <t>Pilot Increase Quality surveys for London. Added new QualityNow Sources in DIM_Sources and set London as Pilot site in Survey_Sites tab.</t>
   </si>
 </sst>
 </file>
@@ -3043,7 +3052,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -3054,7 +3063,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -3365,10 +3373,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L79"/>
+  <dimension ref="A1:L80"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="A80" sqref="A80"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="E80" sqref="E80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4584,36 +4592,36 @@
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A73" s="9">
+      <c r="A73" s="8">
         <v>64</v>
       </c>
-      <c r="B73" s="10">
+      <c r="B73" s="9">
         <v>43383</v>
       </c>
-      <c r="C73" s="9" t="s">
+      <c r="C73" s="8" t="s">
         <v>430</v>
       </c>
-      <c r="D73" s="9">
+      <c r="D73" s="8">
         <v>12308</v>
       </c>
-      <c r="E73" s="9" t="s">
+      <c r="E73" s="8" t="s">
         <v>962</v>
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A74" s="9">
+      <c r="A74" s="8">
         <v>65</v>
       </c>
-      <c r="B74" s="10">
+      <c r="B74" s="9">
         <v>43383</v>
       </c>
-      <c r="C74" s="9" t="s">
+      <c r="C74" s="8" t="s">
         <v>430</v>
       </c>
-      <c r="D74" s="9">
+      <c r="D74" s="8">
         <v>12308</v>
       </c>
-      <c r="E74" s="9" t="s">
+      <c r="E74" s="8" t="s">
         <v>963</v>
       </c>
     </row>
@@ -4621,7 +4629,7 @@
       <c r="A75" s="6">
         <v>66</v>
       </c>
-      <c r="B75" s="11">
+      <c r="B75" s="10">
         <v>43385</v>
       </c>
       <c r="C75" s="6" t="s">
@@ -4644,17 +4652,17 @@
       <c r="C76" s="6" t="s">
         <v>430</v>
       </c>
-      <c r="D76" s="11">
+      <c r="D76" s="10">
         <v>12455</v>
       </c>
       <c r="E76" s="6" t="s">
         <v>967</v>
       </c>
       <c r="F76" s="6"/>
-      <c r="G76" s="11"/>
+      <c r="G76" s="10"/>
       <c r="H76" s="6"/>
       <c r="I76" s="6"/>
-      <c r="J76" s="11"/>
+      <c r="J76" s="10"/>
       <c r="K76" s="6"/>
       <c r="L76" s="6"/>
     </row>
@@ -4662,7 +4670,7 @@
       <c r="A77" s="6">
         <v>68</v>
       </c>
-      <c r="B77" s="11">
+      <c r="B77" s="10">
         <v>43402</v>
       </c>
       <c r="C77" s="6" t="s">
@@ -4675,38 +4683,55 @@
         <v>970</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A78" s="5">
+    <row r="78" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="8">
         <v>69</v>
       </c>
-      <c r="B78" s="8">
+      <c r="B78" s="9">
         <v>43433</v>
       </c>
-      <c r="C78" s="5" t="s">
+      <c r="C78" s="8" t="s">
         <v>430</v>
       </c>
-      <c r="D78" s="5">
+      <c r="D78" s="8">
         <v>12591</v>
       </c>
-      <c r="E78" s="5" t="s">
+      <c r="E78" s="8" t="s">
         <v>973</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A79" s="5">
+    <row r="79" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="8">
         <v>69.099999999999994</v>
       </c>
-      <c r="B79" s="8">
+      <c r="B79" s="9">
         <v>43439</v>
       </c>
-      <c r="C79" s="5" t="s">
+      <c r="C79" s="8" t="s">
         <v>430</v>
       </c>
-      <c r="D79" s="5">
+      <c r="D79" s="8">
         <v>12591</v>
       </c>
-      <c r="E79" s="5" t="s">
+      <c r="E79" s="8" t="s">
         <v>975</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A80" s="6">
+        <v>70</v>
+      </c>
+      <c r="B80" s="1">
+        <v>43522</v>
+      </c>
+      <c r="C80" s="6" t="s">
+        <v>430</v>
+      </c>
+      <c r="D80">
+        <v>13334</v>
+      </c>
+      <c r="E80" s="6" t="s">
+        <v>978</v>
       </c>
     </row>
   </sheetData>
@@ -29557,10 +29582,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I71"/>
+  <dimension ref="A1:I75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="A74" sqref="A74:I75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -30615,101 +30640,101 @@
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="5">
+      <c r="A37">
         <v>134</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B37" t="s">
         <v>5</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C37" t="s">
         <v>974</v>
       </c>
-      <c r="D37" s="5">
-        <v>1</v>
-      </c>
-      <c r="E37" s="5">
-        <v>0</v>
-      </c>
-      <c r="F37" s="5">
-        <v>0</v>
-      </c>
-      <c r="G37" s="5">
-        <v>0</v>
-      </c>
-      <c r="H37" s="5">
-        <v>0</v>
-      </c>
-      <c r="I37" s="5">
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37">
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38">
-        <v>201</v>
-      </c>
-      <c r="B38" t="s">
-        <v>3</v>
-      </c>
-      <c r="C38" t="s">
-        <v>6</v>
-      </c>
-      <c r="D38">
-        <v>1</v>
-      </c>
-      <c r="E38">
-        <v>1</v>
-      </c>
-      <c r="F38">
-        <v>0</v>
-      </c>
-      <c r="G38">
-        <v>0</v>
-      </c>
-      <c r="H38">
-        <v>0</v>
-      </c>
-      <c r="I38">
+      <c r="A38" s="5">
+        <v>135</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>976</v>
+      </c>
+      <c r="D38" s="5">
+        <v>1</v>
+      </c>
+      <c r="E38" s="5">
+        <v>0</v>
+      </c>
+      <c r="F38" s="5">
+        <v>0</v>
+      </c>
+      <c r="G38" s="5">
+        <v>0</v>
+      </c>
+      <c r="H38" s="5">
+        <v>0</v>
+      </c>
+      <c r="I38" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39">
-        <v>202</v>
-      </c>
-      <c r="B39" t="s">
-        <v>3</v>
-      </c>
-      <c r="C39" t="s">
-        <v>7</v>
-      </c>
-      <c r="D39">
-        <v>1</v>
-      </c>
-      <c r="E39">
-        <v>1</v>
-      </c>
-      <c r="F39">
-        <v>0</v>
-      </c>
-      <c r="G39">
-        <v>1</v>
-      </c>
-      <c r="H39">
-        <v>0</v>
-      </c>
-      <c r="I39">
-        <v>1</v>
+      <c r="A39" s="5">
+        <v>136</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>977</v>
+      </c>
+      <c r="D39" s="5">
+        <v>1</v>
+      </c>
+      <c r="E39" s="5">
+        <v>0</v>
+      </c>
+      <c r="F39" s="5">
+        <v>0</v>
+      </c>
+      <c r="G39" s="5">
+        <v>0</v>
+      </c>
+      <c r="H39" s="5">
+        <v>0</v>
+      </c>
+      <c r="I39" s="5">
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B40" t="s">
         <v>3</v>
       </c>
       <c r="C40" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D40">
         <v>1</v>
@@ -30721,24 +30746,24 @@
         <v>0</v>
       </c>
       <c r="G40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I40">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B41" t="s">
         <v>3</v>
       </c>
       <c r="C41" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D41">
         <v>1</v>
@@ -30756,18 +30781,18 @@
         <v>0</v>
       </c>
       <c r="I41">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B42" t="s">
         <v>3</v>
       </c>
       <c r="C42" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D42">
         <v>1</v>
@@ -30782,7 +30807,7 @@
         <v>1</v>
       </c>
       <c r="H42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I42">
         <v>1</v>
@@ -30790,13 +30815,13 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B43" t="s">
         <v>3</v>
       </c>
       <c r="C43" t="s">
-        <v>170</v>
+        <v>9</v>
       </c>
       <c r="D43">
         <v>1</v>
@@ -30811,21 +30836,21 @@
         <v>1</v>
       </c>
       <c r="H43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I43">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B44" t="s">
         <v>3</v>
       </c>
       <c r="C44" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D44">
         <v>1</v>
@@ -30848,13 +30873,13 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B45" t="s">
         <v>3</v>
       </c>
       <c r="C45" t="s">
-        <v>12</v>
+        <v>170</v>
       </c>
       <c r="D45">
         <v>1</v>
@@ -30863,7 +30888,7 @@
         <v>1</v>
       </c>
       <c r="F45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G45">
         <v>1</v>
@@ -30872,18 +30897,18 @@
         <v>1</v>
       </c>
       <c r="I45">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B46" t="s">
         <v>3</v>
       </c>
       <c r="C46" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D46">
         <v>1</v>
@@ -30892,7 +30917,7 @@
         <v>1</v>
       </c>
       <c r="F46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G46">
         <v>1</v>
@@ -30906,13 +30931,13 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B47" t="s">
         <v>3</v>
       </c>
       <c r="C47" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D47">
         <v>1</v>
@@ -30927,7 +30952,7 @@
         <v>1</v>
       </c>
       <c r="H47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I47">
         <v>0</v>
@@ -30935,54 +30960,54 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B48" t="s">
         <v>3</v>
       </c>
       <c r="C48" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D48">
         <v>1</v>
       </c>
       <c r="E48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H48">
         <v>0</v>
       </c>
       <c r="I48">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B49" t="s">
         <v>3</v>
       </c>
       <c r="C49" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D49">
         <v>1</v>
       </c>
       <c r="E49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H49">
         <v>0</v>
@@ -30993,13 +31018,13 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B50" t="s">
         <v>3</v>
       </c>
       <c r="C50" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D50">
         <v>1</v>
@@ -31022,13 +31047,13 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B51" t="s">
         <v>3</v>
       </c>
       <c r="C51" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D51">
         <v>1</v>
@@ -31051,13 +31076,13 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B52" t="s">
         <v>3</v>
       </c>
       <c r="C52" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D52">
         <v>1</v>
@@ -31080,13 +31105,13 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B53" t="s">
         <v>3</v>
       </c>
       <c r="C53" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D53">
         <v>1</v>
@@ -31109,13 +31134,13 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B54" t="s">
         <v>3</v>
       </c>
       <c r="C54" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D54">
         <v>1</v>
@@ -31138,42 +31163,42 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B55" t="s">
         <v>3</v>
       </c>
       <c r="C55" t="s">
-        <v>171</v>
+        <v>20</v>
       </c>
       <c r="D55">
         <v>1</v>
       </c>
       <c r="E55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H55">
         <v>0</v>
       </c>
       <c r="I55">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B56" t="s">
         <v>3</v>
       </c>
       <c r="C56" t="s">
-        <v>176</v>
+        <v>21</v>
       </c>
       <c r="D56">
         <v>1</v>
@@ -31182,7 +31207,7 @@
         <v>0</v>
       </c>
       <c r="F56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G56">
         <v>0</v>
@@ -31196,42 +31221,42 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B57" t="s">
         <v>3</v>
       </c>
       <c r="C57" t="s">
-        <v>437</v>
+        <v>171</v>
       </c>
       <c r="D57">
         <v>1</v>
       </c>
       <c r="E57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H57">
         <v>0</v>
       </c>
       <c r="I57">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B58" t="s">
         <v>3</v>
       </c>
       <c r="C58" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D58">
         <v>1</v>
@@ -31240,7 +31265,7 @@
         <v>0</v>
       </c>
       <c r="F58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G58">
         <v>0</v>
@@ -31254,13 +31279,13 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B59" t="s">
         <v>3</v>
       </c>
       <c r="C59" t="s">
-        <v>470</v>
+        <v>437</v>
       </c>
       <c r="D59">
         <v>1</v>
@@ -31283,13 +31308,13 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B60" t="s">
         <v>3</v>
       </c>
       <c r="C60" t="s">
-        <v>468</v>
+        <v>172</v>
       </c>
       <c r="D60">
         <v>1</v>
@@ -31312,13 +31337,13 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B61" t="s">
         <v>3</v>
       </c>
       <c r="C61" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="D61">
         <v>1</v>
@@ -31341,13 +31366,13 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B62" t="s">
         <v>3</v>
       </c>
       <c r="C62" t="s">
-        <v>487</v>
+        <v>468</v>
       </c>
       <c r="D62">
         <v>1</v>
@@ -31362,7 +31387,7 @@
         <v>0</v>
       </c>
       <c r="H62">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I62">
         <v>0</v>
@@ -31370,16 +31395,16 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B63" t="s">
         <v>3</v>
       </c>
       <c r="C63" t="s">
-        <v>488</v>
+        <v>469</v>
       </c>
       <c r="D63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E63">
         <v>0</v>
@@ -31399,13 +31424,13 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B64" t="s">
         <v>3</v>
       </c>
       <c r="C64" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="D64">
         <v>1</v>
@@ -31428,16 +31453,16 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B65" t="s">
         <v>3</v>
       </c>
       <c r="C65" t="s">
-        <v>548</v>
+        <v>488</v>
       </c>
       <c r="D65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E65">
         <v>0</v>
@@ -31452,18 +31477,18 @@
         <v>0</v>
       </c>
       <c r="I65">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B66" t="s">
         <v>3</v>
       </c>
       <c r="C66" t="s">
-        <v>549</v>
+        <v>489</v>
       </c>
       <c r="D66">
         <v>1</v>
@@ -31478,21 +31503,21 @@
         <v>0</v>
       </c>
       <c r="H66">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I66">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B67" t="s">
         <v>3</v>
       </c>
       <c r="C67" t="s">
-        <v>692</v>
+        <v>548</v>
       </c>
       <c r="D67">
         <v>1</v>
@@ -31510,21 +31535,21 @@
         <v>0</v>
       </c>
       <c r="I67">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B68" t="s">
         <v>3</v>
       </c>
       <c r="C68" t="s">
-        <v>740</v>
+        <v>549</v>
       </c>
       <c r="D68">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E68">
         <v>0</v>
@@ -31539,18 +31564,18 @@
         <v>0</v>
       </c>
       <c r="I68">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B69" t="s">
         <v>3</v>
       </c>
       <c r="C69" t="s">
-        <v>823</v>
+        <v>692</v>
       </c>
       <c r="D69">
         <v>1</v>
@@ -31573,59 +31598,175 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B70" t="s">
         <v>3</v>
       </c>
       <c r="C70" t="s">
+        <v>740</v>
+      </c>
+      <c r="D70">
+        <v>0</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
+      </c>
+      <c r="F70">
+        <v>0</v>
+      </c>
+      <c r="G70">
+        <v>0</v>
+      </c>
+      <c r="H70">
+        <v>0</v>
+      </c>
+      <c r="I70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="8">
+        <v>232</v>
+      </c>
+      <c r="B71" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C71" s="8" t="s">
+        <v>823</v>
+      </c>
+      <c r="D71" s="8">
+        <v>1</v>
+      </c>
+      <c r="E71" s="8">
+        <v>0</v>
+      </c>
+      <c r="F71" s="8">
+        <v>0</v>
+      </c>
+      <c r="G71" s="8">
+        <v>0</v>
+      </c>
+      <c r="H71" s="8">
+        <v>0</v>
+      </c>
+      <c r="I71" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>233</v>
+      </c>
+      <c r="B72" t="s">
+        <v>3</v>
+      </c>
+      <c r="C72" t="s">
         <v>826</v>
       </c>
-      <c r="D70">
-        <v>1</v>
-      </c>
-      <c r="E70">
-        <v>0</v>
-      </c>
-      <c r="F70">
-        <v>0</v>
-      </c>
-      <c r="G70">
-        <v>0</v>
-      </c>
-      <c r="H70">
-        <v>0</v>
-      </c>
-      <c r="I70">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A71" s="5">
+      <c r="D72">
+        <v>1</v>
+      </c>
+      <c r="E72">
+        <v>0</v>
+      </c>
+      <c r="F72">
+        <v>0</v>
+      </c>
+      <c r="G72">
+        <v>0</v>
+      </c>
+      <c r="H72">
+        <v>0</v>
+      </c>
+      <c r="I72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A73">
         <v>234</v>
       </c>
-      <c r="B71" s="5" t="s">
+      <c r="B73" t="s">
         <v>3</v>
       </c>
-      <c r="C71" s="5" t="s">
+      <c r="C73" t="s">
         <v>974</v>
       </c>
-      <c r="D71" s="5">
-        <v>1</v>
-      </c>
-      <c r="E71" s="5">
-        <v>0</v>
-      </c>
-      <c r="F71" s="5">
-        <v>0</v>
-      </c>
-      <c r="G71" s="5">
-        <v>0</v>
-      </c>
-      <c r="H71" s="5">
-        <v>0</v>
-      </c>
-      <c r="I71" s="5">
+      <c r="D73">
+        <v>1</v>
+      </c>
+      <c r="E73">
+        <v>0</v>
+      </c>
+      <c r="F73">
+        <v>0</v>
+      </c>
+      <c r="G73">
+        <v>0</v>
+      </c>
+      <c r="H73">
+        <v>0</v>
+      </c>
+      <c r="I73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A74" s="5">
+        <v>235</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>976</v>
+      </c>
+      <c r="D74" s="5">
+        <v>1</v>
+      </c>
+      <c r="E74" s="5">
+        <v>0</v>
+      </c>
+      <c r="F74" s="5">
+        <v>0</v>
+      </c>
+      <c r="G74" s="5">
+        <v>0</v>
+      </c>
+      <c r="H74" s="5">
+        <v>0</v>
+      </c>
+      <c r="I74" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A75" s="5">
+        <v>236</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>977</v>
+      </c>
+      <c r="D75" s="5">
+        <v>1</v>
+      </c>
+      <c r="E75" s="5">
+        <v>0</v>
+      </c>
+      <c r="F75" s="5">
+        <v>0</v>
+      </c>
+      <c r="G75" s="5">
+        <v>0</v>
+      </c>
+      <c r="H75" s="5">
+        <v>0</v>
+      </c>
+      <c r="I75" s="5">
         <v>0</v>
       </c>
     </row>
@@ -32683,7 +32824,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -32868,8 +33009,8 @@
       <c r="C11">
         <v>1</v>
       </c>
-      <c r="D11">
-        <v>0</v>
+      <c r="D11" s="5">
+        <v>1</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -33456,7 +33597,7 @@
       <c r="B5" s="5" t="s">
         <v>379</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>972</v>
       </c>
     </row>

</xml_diff>

<commit_message>
TFS 13643 - Add Dual as a Program
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C41860
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3605" uniqueCount="979">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3609" uniqueCount="982">
   <si>
     <t>SourceID</t>
   </si>
@@ -2988,6 +2988,15 @@
   </si>
   <si>
     <t>Pilot Increase Quality surveys for London. Added new QualityNow Sources in DIM_Sources and set London as Pilot site in Survey_Sites tab.</t>
+  </si>
+  <si>
+    <t>Add Dual as a record in DIM_Program and added column for Sort Order</t>
+  </si>
+  <si>
+    <t>SortOrder</t>
+  </si>
+  <si>
+    <t>Dual</t>
   </si>
 </sst>
 </file>
@@ -3373,10 +3382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L80"/>
+  <dimension ref="A1:L81"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="E80" sqref="E80"/>
+      <selection activeCell="A81" sqref="A81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4732,6 +4741,23 @@
       </c>
       <c r="E80" s="6" t="s">
         <v>978</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A81" s="6">
+        <v>71</v>
+      </c>
+      <c r="B81" s="1">
+        <v>43531</v>
+      </c>
+      <c r="C81" s="6" t="s">
+        <v>430</v>
+      </c>
+      <c r="D81">
+        <v>13643</v>
+      </c>
+      <c r="E81" s="6" t="s">
+        <v>979</v>
       </c>
     </row>
   </sheetData>
@@ -6114,13 +6140,18 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>335</v>
       </c>
@@ -6130,8 +6161,11 @@
       <c r="C1" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" s="5" t="s">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>-1</v>
       </c>
@@ -6141,38 +6175,64 @@
       <c r="C2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="D2" s="5">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="5">
+        <v>4</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>981</v>
+      </c>
+      <c r="C3" s="5">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
         <v>337</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
         <v>338</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
         <v>378</v>
       </c>
-      <c r="C5">
-        <v>1</v>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" s="5">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -29585,7 +29645,7 @@
   <dimension ref="A1:I75"/>
   <sheetViews>
     <sheetView topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="A74" sqref="A74:I75"/>
+      <selection activeCell="A74" sqref="A74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -31713,60 +31773,60 @@
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A74" s="5">
+      <c r="A74">
         <v>235</v>
       </c>
-      <c r="B74" s="5" t="s">
+      <c r="B74" t="s">
         <v>3</v>
       </c>
-      <c r="C74" s="5" t="s">
+      <c r="C74" t="s">
         <v>976</v>
       </c>
-      <c r="D74" s="5">
-        <v>1</v>
-      </c>
-      <c r="E74" s="5">
-        <v>0</v>
-      </c>
-      <c r="F74" s="5">
-        <v>0</v>
-      </c>
-      <c r="G74" s="5">
-        <v>0</v>
-      </c>
-      <c r="H74" s="5">
-        <v>0</v>
-      </c>
-      <c r="I74" s="5">
+      <c r="D74">
+        <v>1</v>
+      </c>
+      <c r="E74">
+        <v>0</v>
+      </c>
+      <c r="F74">
+        <v>0</v>
+      </c>
+      <c r="G74">
+        <v>0</v>
+      </c>
+      <c r="H74">
+        <v>0</v>
+      </c>
+      <c r="I74">
         <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A75" s="5">
+      <c r="A75">
         <v>236</v>
       </c>
-      <c r="B75" s="5" t="s">
+      <c r="B75" t="s">
         <v>3</v>
       </c>
-      <c r="C75" s="5" t="s">
+      <c r="C75" t="s">
         <v>977</v>
       </c>
-      <c r="D75" s="5">
-        <v>1</v>
-      </c>
-      <c r="E75" s="5">
-        <v>0</v>
-      </c>
-      <c r="F75" s="5">
-        <v>0</v>
-      </c>
-      <c r="G75" s="5">
-        <v>0</v>
-      </c>
-      <c r="H75" s="5">
-        <v>0</v>
-      </c>
-      <c r="I75" s="5">
+      <c r="D75">
+        <v>1</v>
+      </c>
+      <c r="E75">
+        <v>0</v>
+      </c>
+      <c r="F75">
+        <v>0</v>
+      </c>
+      <c r="G75">
+        <v>0</v>
+      </c>
+      <c r="H75">
+        <v>0</v>
+      </c>
+      <c r="I75">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
TFS 13332 - Quality Now Initiative
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C41968
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3609" uniqueCount="982">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3613" uniqueCount="985">
   <si>
     <t>SourceID</t>
   </si>
@@ -2997,6 +2997,15 @@
   </si>
   <si>
     <t>Dual</t>
+  </si>
+  <si>
+    <t>Quality Now</t>
+  </si>
+  <si>
+    <t>ATA Alignment Now</t>
+  </si>
+  <si>
+    <t>Added 2 new Coaching Reasons in DIM_Coaching_Reason table (ids 57 and 58) to support Quality Now</t>
   </si>
 </sst>
 </file>
@@ -3075,9 +3084,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3382,10 +3389,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L81"/>
+  <dimension ref="A1:L82"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="A81" sqref="A81"/>
+      <selection activeCell="E82" sqref="E82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4760,6 +4767,23 @@
         <v>979</v>
       </c>
     </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A82" s="5">
+        <v>72</v>
+      </c>
+      <c r="B82" s="11">
+        <v>43546</v>
+      </c>
+      <c r="C82" s="5" t="s">
+        <v>430</v>
+      </c>
+      <c r="D82" s="5">
+        <v>13332</v>
+      </c>
+      <c r="E82" s="5" t="s">
+        <v>984</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4771,7 +4795,7 @@
   <dimension ref="A1:G59"/>
   <sheetViews>
     <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59:G59"/>
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6142,9 +6166,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -6161,7 +6183,7 @@
       <c r="C1" t="s">
         <v>173</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" t="s">
         <v>980</v>
       </c>
     </row>
@@ -6175,21 +6197,21 @@
       <c r="C2">
         <v>0</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2">
         <v>-1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="5">
+      <c r="A3">
         <v>4</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" t="s">
         <v>981</v>
       </c>
-      <c r="C3" s="5">
-        <v>1</v>
-      </c>
-      <c r="D3" s="5">
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
         <v>1</v>
       </c>
     </row>
@@ -6203,7 +6225,7 @@
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4">
         <v>2</v>
       </c>
     </row>
@@ -6217,7 +6239,7 @@
       <c r="C5">
         <v>1</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5">
         <v>3</v>
       </c>
     </row>
@@ -6231,7 +6253,7 @@
       <c r="C6">
         <v>1</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6">
         <v>4</v>
       </c>
     </row>
@@ -6244,9 +6266,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P319"/>
   <sheetViews>
-    <sheetView topLeftCell="A298" workbookViewId="0">
-      <selection activeCell="A310" sqref="A310:P319"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -22212,9 +22232,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -22343,7 +22361,7 @@
   <dimension ref="A1:K175"/>
   <sheetViews>
     <sheetView topLeftCell="A159" workbookViewId="0">
-      <selection activeCell="A175" sqref="A175:K175"/>
+      <selection activeCell="A159" sqref="A159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -28451,38 +28469,38 @@
         <v>378</v>
       </c>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A175" s="5" t="s">
+    <row r="175" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A175" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="B175" s="5" t="s">
+      <c r="B175" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="C175" s="5" t="s">
+      <c r="C175" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D175" s="5" t="s">
+      <c r="D175" s="6" t="s">
         <v>974</v>
       </c>
-      <c r="E175" s="5">
-        <v>0</v>
-      </c>
-      <c r="F175" s="5" t="s">
+      <c r="E175" s="6">
+        <v>0</v>
+      </c>
+      <c r="F175" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="G175" s="5" t="s">
+      <c r="G175" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="H175" s="5" t="s">
+      <c r="H175" s="6" t="s">
         <v>389</v>
       </c>
-      <c r="I175" s="5" t="s">
+      <c r="I175" s="6" t="s">
         <v>420</v>
       </c>
-      <c r="J175" s="5">
-        <v>0</v>
-      </c>
-      <c r="K175" s="5" t="s">
+      <c r="J175" s="6">
+        <v>0</v>
+      </c>
+      <c r="K175" s="6" t="s">
         <v>378</v>
       </c>
     </row>
@@ -28497,7 +28515,7 @@
   <dimension ref="A1:C71"/>
   <sheetViews>
     <sheetView topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58:XFD71"/>
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -28984,9 +29002,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -29072,8 +29088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C9" sqref="A9:XFD9"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -29357,9 +29373,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:D19"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -29644,9 +29658,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I75"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="A74" sqref="A74"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -30728,61 +30740,61 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="5">
+    <row r="38" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="6">
         <v>135</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C38" s="6" t="s">
         <v>976</v>
       </c>
-      <c r="D38" s="5">
-        <v>1</v>
-      </c>
-      <c r="E38" s="5">
-        <v>0</v>
-      </c>
-      <c r="F38" s="5">
-        <v>0</v>
-      </c>
-      <c r="G38" s="5">
-        <v>0</v>
-      </c>
-      <c r="H38" s="5">
-        <v>0</v>
-      </c>
-      <c r="I38" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="5">
+      <c r="D38" s="6">
+        <v>1</v>
+      </c>
+      <c r="E38" s="6">
+        <v>0</v>
+      </c>
+      <c r="F38" s="6">
+        <v>0</v>
+      </c>
+      <c r="G38" s="6">
+        <v>0</v>
+      </c>
+      <c r="H38" s="6">
+        <v>0</v>
+      </c>
+      <c r="I38" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="6">
         <v>136</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B39" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C39" s="5" t="s">
+      <c r="C39" s="6" t="s">
         <v>977</v>
       </c>
-      <c r="D39" s="5">
-        <v>1</v>
-      </c>
-      <c r="E39" s="5">
-        <v>0</v>
-      </c>
-      <c r="F39" s="5">
-        <v>0</v>
-      </c>
-      <c r="G39" s="5">
-        <v>0</v>
-      </c>
-      <c r="H39" s="5">
-        <v>0</v>
-      </c>
-      <c r="I39" s="5">
+      <c r="D39" s="6">
+        <v>1</v>
+      </c>
+      <c r="E39" s="6">
+        <v>0</v>
+      </c>
+      <c r="F39" s="6">
+        <v>0</v>
+      </c>
+      <c r="G39" s="6">
+        <v>0</v>
+      </c>
+      <c r="H39" s="6">
+        <v>0</v>
+      </c>
+      <c r="I39" s="6">
         <v>0</v>
       </c>
     </row>
@@ -31839,9 +31851,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:M25"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -32883,9 +32893,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -33069,7 +33077,7 @@
       <c r="C11">
         <v>1</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11">
         <v>1</v>
       </c>
       <c r="E11">
@@ -33530,9 +33538,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -33650,14 +33656,14 @@
         <v>953</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="5">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
         <v>104</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" t="s">
         <v>379</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" t="s">
         <v>972</v>
       </c>
     </row>
@@ -33717,13 +33723,13 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="5">
+      <c r="A11">
         <v>110</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" t="s">
         <v>966</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" t="s">
         <v>971</v>
       </c>
     </row>
@@ -33737,9 +33743,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:E11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -33921,19 +33925,19 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="5">
+      <c r="A11">
         <v>110</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" t="s">
         <v>966</v>
       </c>
-      <c r="C11" s="5">
-        <v>1</v>
-      </c>
-      <c r="D11" s="5">
-        <v>0</v>
-      </c>
-      <c r="E11" s="5">
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
         <v>1</v>
       </c>
     </row>
@@ -33946,9 +33950,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:H11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -34223,28 +34225,28 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="5">
+      <c r="A11">
         <v>110</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" t="s">
         <v>966</v>
       </c>
-      <c r="C11" s="5">
-        <v>0</v>
-      </c>
-      <c r="D11" s="5">
-        <v>0</v>
-      </c>
-      <c r="E11" s="5">
-        <v>0</v>
-      </c>
-      <c r="F11" s="5">
-        <v>0</v>
-      </c>
-      <c r="G11" s="5">
-        <v>0</v>
-      </c>
-      <c r="H11" s="5">
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
         <v>1</v>
       </c>
     </row>
@@ -34257,9 +34259,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C18"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -34275,7 +34275,7 @@
       <c r="B1" t="s">
         <v>930</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>732</v>
       </c>
     </row>
@@ -34286,7 +34286,7 @@
       <c r="B2" t="s">
         <v>932</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="6">
         <v>101</v>
       </c>
     </row>
@@ -34297,7 +34297,7 @@
       <c r="B3" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="6">
         <v>999</v>
       </c>
     </row>
@@ -34308,7 +34308,7 @@
       <c r="B4" t="s">
         <v>932</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="6">
         <v>201</v>
       </c>
     </row>
@@ -34319,7 +34319,7 @@
       <c r="B5" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="6">
         <v>999</v>
       </c>
     </row>
@@ -34330,7 +34330,7 @@
       <c r="B6" t="s">
         <v>935</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="6">
         <v>301</v>
       </c>
     </row>
@@ -34341,7 +34341,7 @@
       <c r="B7" t="s">
         <v>936</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="6">
         <v>302</v>
       </c>
     </row>
@@ -34352,7 +34352,7 @@
       <c r="B8" t="s">
         <v>937</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="6">
         <v>303</v>
       </c>
     </row>
@@ -34363,7 +34363,7 @@
       <c r="B9" t="s">
         <v>938</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="6">
         <v>304</v>
       </c>
     </row>
@@ -34374,7 +34374,7 @@
       <c r="B10" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="6">
         <v>999</v>
       </c>
     </row>
@@ -34385,7 +34385,7 @@
       <c r="B11" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="6">
         <v>999</v>
       </c>
     </row>
@@ -34396,7 +34396,7 @@
       <c r="B12" t="s">
         <v>940</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="6">
         <v>401</v>
       </c>
     </row>
@@ -34407,7 +34407,7 @@
       <c r="B13" t="s">
         <v>941</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="6">
         <v>402</v>
       </c>
     </row>
@@ -34418,7 +34418,7 @@
       <c r="B14" t="s">
         <v>942</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="6">
         <v>403</v>
       </c>
     </row>
@@ -34429,7 +34429,7 @@
       <c r="B15" t="s">
         <v>943</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="6">
         <v>404</v>
       </c>
     </row>
@@ -34440,7 +34440,7 @@
       <c r="B16" t="s">
         <v>944</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="6">
         <v>405</v>
       </c>
     </row>
@@ -34451,7 +34451,7 @@
       <c r="B17" t="s">
         <v>945</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="6">
         <v>406</v>
       </c>
     </row>
@@ -34462,7 +34462,7 @@
       <c r="B18" t="s">
         <v>946</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="6">
         <v>407</v>
       </c>
     </row>
@@ -34475,9 +34475,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -34956,9 +34954,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B58"/>
+  <dimension ref="A1:B60"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59:B60"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -35430,6 +35430,22 @@
         <v>815</v>
       </c>
     </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" s="5">
+        <v>57</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" s="5">
+        <v>58</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>983</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -35439,9 +35455,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B251"/>
   <sheetViews>
-    <sheetView topLeftCell="A230" workbookViewId="0">
-      <selection activeCell="B254" sqref="B254"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -38012,9 +38026,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:F11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>

</xml_diff>

<commit_message>
TFS 14178 - Add Hot topic Question for London surveys
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C42192
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cms\eCoaching_V2\Design\DD\DB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OmniCloud\eCoaching_V2\Design\DD\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3613" uniqueCount="985">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3636" uniqueCount="993">
   <si>
     <t>SourceID</t>
   </si>
@@ -2759,9 +2759,6 @@
     <t>How prepared was your supervisor during your coaching session?| Please explain below.</t>
   </si>
   <si>
-    <t>Hot Topic question</t>
-  </si>
-  <si>
     <t>1 - Very Unprepared</t>
   </si>
   <si>
@@ -3006,6 +3003,33 @@
   </si>
   <si>
     <t>Added 2 new Coaching Reasons in DIM_Coaching_Reason table (ids 57 and 58) to support Quality Now</t>
+  </si>
+  <si>
+    <t>Updated attributes for Question 6 in Survey_DIM_Question and added new values to Survey_DIM_Response and Survey_DIM_QAnswer</t>
+  </si>
+  <si>
+    <t>Quality Now has improved my experience working on the CCO. | Please explain below.</t>
+  </si>
+  <si>
+    <t>1 - Strongly Disagree</t>
+  </si>
+  <si>
+    <t>2 - Disagree</t>
+  </si>
+  <si>
+    <t>3 - Somewhat Disagree</t>
+  </si>
+  <si>
+    <t>4 - Neutral</t>
+  </si>
+  <si>
+    <t>5 - Somewhat Agree</t>
+  </si>
+  <si>
+    <t>6 - Agree</t>
+  </si>
+  <si>
+    <t>7 - Strongly Agree</t>
   </si>
 </sst>
 </file>
@@ -3070,7 +3094,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -3085,6 +3109,7 @@
     <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3389,10 +3414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L82"/>
+  <dimension ref="A1:L83"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="E82" sqref="E82"/>
+      <selection activeCell="A83" sqref="A83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4502,7 +4527,7 @@
         <v>9511</v>
       </c>
       <c r="E66" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.3">
@@ -4519,7 +4544,7 @@
         <v>7136</v>
       </c>
       <c r="E67" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.3">
@@ -4536,7 +4561,7 @@
         <v>10890</v>
       </c>
       <c r="E68" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.3">
@@ -4553,7 +4578,7 @@
         <v>7137</v>
       </c>
       <c r="E69" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.3">
@@ -4570,7 +4595,7 @@
         <v>7137</v>
       </c>
       <c r="E70" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.3">
@@ -4587,7 +4612,7 @@
         <v>11500</v>
       </c>
       <c r="E71" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.3">
@@ -4604,7 +4629,7 @@
         <v>11451</v>
       </c>
       <c r="E72" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.3">
@@ -4621,7 +4646,7 @@
         <v>12308</v>
       </c>
       <c r="E73" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.3">
@@ -4638,7 +4663,7 @@
         <v>12308</v>
       </c>
       <c r="E74" s="8" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="75" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -4655,7 +4680,7 @@
         <v>12316</v>
       </c>
       <c r="E75" s="6" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="76" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -4672,7 +4697,7 @@
         <v>12455</v>
       </c>
       <c r="E76" s="6" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="F76" s="6"/>
       <c r="G76" s="10"/>
@@ -4696,7 +4721,7 @@
         <v>12467</v>
       </c>
       <c r="E77" s="6" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
     </row>
     <row r="78" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -4713,7 +4738,7 @@
         <v>12591</v>
       </c>
       <c r="E78" s="8" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="79" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -4730,7 +4755,7 @@
         <v>12591</v>
       </c>
       <c r="E79" s="8" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.3">
@@ -4747,7 +4772,7 @@
         <v>13334</v>
       </c>
       <c r="E80" s="6" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
@@ -4764,23 +4789,40 @@
         <v>13643</v>
       </c>
       <c r="E81" s="6" t="s">
-        <v>979</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A82" s="5">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="8">
         <v>72</v>
       </c>
-      <c r="B82" s="11">
+      <c r="B82" s="9">
         <v>43546</v>
       </c>
-      <c r="C82" s="5" t="s">
+      <c r="C82" s="8" t="s">
         <v>430</v>
       </c>
-      <c r="D82" s="5">
+      <c r="D82" s="8">
         <v>13332</v>
       </c>
-      <c r="E82" s="5" t="s">
+      <c r="E82" s="8" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A83" s="5">
+        <v>73</v>
+      </c>
+      <c r="B83" s="11">
+        <v>43577</v>
+      </c>
+      <c r="C83" s="5" t="s">
+        <v>430</v>
+      </c>
+      <c r="D83" s="5">
+        <v>14178</v>
+      </c>
+      <c r="E83" s="5" t="s">
         <v>984</v>
       </c>
     </row>
@@ -6136,10 +6178,10 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="6" t="s">
+        <v>967</v>
+      </c>
+      <c r="B59" s="6" t="s">
         <v>968</v>
-      </c>
-      <c r="B59" s="6" t="s">
-        <v>969</v>
       </c>
       <c r="C59" s="6">
         <v>1</v>
@@ -6184,7 +6226,7 @@
         <v>173</v>
       </c>
       <c r="D1" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -6206,7 +6248,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -6266,7 +6308,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P319"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A294" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -21684,7 +21726,7 @@
         <v>245</v>
       </c>
       <c r="D309" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="E309">
         <v>0</v>
@@ -21734,7 +21776,7 @@
         <v>246</v>
       </c>
       <c r="D310" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="E310">
         <v>1</v>
@@ -21784,7 +21826,7 @@
         <v>247</v>
       </c>
       <c r="D311" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="E311">
         <v>1</v>
@@ -21834,7 +21876,7 @@
         <v>248</v>
       </c>
       <c r="D312" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="E312">
         <v>1</v>
@@ -21884,7 +21926,7 @@
         <v>246</v>
       </c>
       <c r="D313" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="E313">
         <v>1</v>
@@ -21934,7 +21976,7 @@
         <v>247</v>
       </c>
       <c r="D314" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="E314">
         <v>1</v>
@@ -21984,7 +22026,7 @@
         <v>248</v>
       </c>
       <c r="D315" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="E315">
         <v>1</v>
@@ -22034,7 +22076,7 @@
         <v>246</v>
       </c>
       <c r="D316" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="E316">
         <v>1</v>
@@ -22084,7 +22126,7 @@
         <v>247</v>
       </c>
       <c r="D317" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="E317">
         <v>1</v>
@@ -22134,7 +22176,7 @@
         <v>248</v>
       </c>
       <c r="D318" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="E318">
         <v>1</v>
@@ -22184,7 +22226,7 @@
         <v>249</v>
       </c>
       <c r="D319" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="E319">
         <v>1</v>
@@ -22284,7 +22326,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="B3" t="s">
         <v>363</v>
@@ -22360,7 +22402,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K175"/>
   <sheetViews>
-    <sheetView topLeftCell="A159" workbookViewId="0">
+    <sheetView topLeftCell="A153" workbookViewId="0">
       <selection activeCell="A159" sqref="A159"/>
     </sheetView>
   </sheetViews>
@@ -28480,7 +28522,7 @@
         <v>3</v>
       </c>
       <c r="D175" s="6" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="E175" s="6">
         <v>0</v>
@@ -29088,8 +29130,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -29099,7 +29141,7 @@
     <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="9" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.21875" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -29306,61 +29348,61 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="A8" s="5">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
-        <v>902</v>
-      </c>
-      <c r="C8">
-        <v>6</v>
-      </c>
-      <c r="D8">
-        <v>20150901</v>
-      </c>
-      <c r="E8">
-        <v>20150930</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8" s="4">
-        <v>42248</v>
-      </c>
-      <c r="I8" s="6">
-        <v>0</v>
+      <c r="B8" s="5" t="s">
+        <v>985</v>
+      </c>
+      <c r="C8" s="5">
+        <v>98</v>
+      </c>
+      <c r="D8" s="5">
+        <v>20190501</v>
+      </c>
+      <c r="E8" s="5">
+        <v>20190731</v>
+      </c>
+      <c r="F8" s="5">
+        <v>1</v>
+      </c>
+      <c r="G8" s="5">
+        <v>1</v>
+      </c>
+      <c r="H8" s="12">
+        <v>43577.559065011577</v>
+      </c>
+      <c r="I8" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="6">
+      <c r="A9" s="5">
         <v>7</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>901</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <v>7</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="5">
         <v>20180201</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="5">
         <v>99991231</v>
       </c>
-      <c r="F9" s="6">
-        <v>0</v>
-      </c>
-      <c r="G9" s="6">
-        <v>1</v>
-      </c>
-      <c r="H9" s="7">
-        <v>43132</v>
-      </c>
-      <c r="I9" s="6">
-        <v>1</v>
+      <c r="F9" s="5">
+        <v>0</v>
+      </c>
+      <c r="G9" s="5">
+        <v>0</v>
+      </c>
+      <c r="H9" s="12">
+        <v>43577.559065011577</v>
+      </c>
+      <c r="I9" s="5">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -29371,9 +29413,11 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:D26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -29584,7 +29628,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="C15" s="6">
         <v>1</v>
@@ -29598,7 +29642,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="C16" s="6">
         <v>1</v>
@@ -29612,7 +29656,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="C17" s="6">
         <v>1</v>
@@ -29626,7 +29670,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="C18" s="6">
         <v>1</v>
@@ -29640,13 +29684,111 @@
         <v>17</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="C19" s="6">
         <v>1</v>
       </c>
       <c r="D19" s="7">
         <v>43132</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="5">
+        <v>18</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>986</v>
+      </c>
+      <c r="C20" s="5">
+        <v>1</v>
+      </c>
+      <c r="D20" s="12">
+        <v>43586</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="5">
+        <v>19</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>987</v>
+      </c>
+      <c r="C21" s="5">
+        <v>1</v>
+      </c>
+      <c r="D21" s="12">
+        <v>43586</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="5">
+        <v>20</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>988</v>
+      </c>
+      <c r="C22" s="5">
+        <v>1</v>
+      </c>
+      <c r="D22" s="12">
+        <v>43586</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="5">
+        <v>21</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>989</v>
+      </c>
+      <c r="C23" s="5">
+        <v>1</v>
+      </c>
+      <c r="D23" s="12">
+        <v>43586</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="5">
+        <v>22</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>990</v>
+      </c>
+      <c r="C24" s="5">
+        <v>1</v>
+      </c>
+      <c r="D24" s="12">
+        <v>43586</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="5">
+        <v>23</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>991</v>
+      </c>
+      <c r="C25" s="5">
+        <v>1</v>
+      </c>
+      <c r="D25" s="12">
+        <v>43586</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="5">
+        <v>24</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>992</v>
+      </c>
+      <c r="C26" s="5">
+        <v>1</v>
+      </c>
+      <c r="D26" s="12">
+        <v>43586</v>
       </c>
     </row>
   </sheetData>
@@ -29658,7 +29800,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I75"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A58" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -30719,7 +30861,7 @@
         <v>5</v>
       </c>
       <c r="C37" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -30748,7 +30890,7 @@
         <v>5</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="D38" s="6">
         <v>1</v>
@@ -30777,7 +30919,7 @@
         <v>5</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="D39" s="6">
         <v>1</v>
@@ -31763,7 +31905,7 @@
         <v>3</v>
       </c>
       <c r="C73" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="D73">
         <v>1</v>
@@ -31792,7 +31934,7 @@
         <v>3</v>
       </c>
       <c r="C74" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="D74">
         <v>1</v>
@@ -31821,7 +31963,7 @@
         <v>3</v>
       </c>
       <c r="C75" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="D75">
         <v>1</v>
@@ -31849,9 +31991,11 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M25"/>
+  <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:M32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -31896,7 +32040,7 @@
         <v>900</v>
       </c>
       <c r="M1" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -32692,7 +32836,7 @@
         <v>13</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="F21" s="6" t="s">
         <v>728</v>
@@ -32733,7 +32877,7 @@
         <v>14</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>728</v>
@@ -32774,7 +32918,7 @@
         <v>15</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="F23" s="6" t="s">
         <v>728</v>
@@ -32815,7 +32959,7 @@
         <v>16</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="F24" s="6" t="s">
         <v>728</v>
@@ -32856,7 +33000,7 @@
         <v>17</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="F25" s="6" t="s">
         <v>728</v>
@@ -32881,6 +33025,293 @@
       </c>
       <c r="M25" s="6">
         <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26" s="5">
+        <v>1</v>
+      </c>
+      <c r="B26" s="5">
+        <v>6</v>
+      </c>
+      <c r="C26" s="5">
+        <v>6</v>
+      </c>
+      <c r="D26" s="5">
+        <v>18</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>986</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>728</v>
+      </c>
+      <c r="G26" s="5">
+        <v>1</v>
+      </c>
+      <c r="H26" s="5">
+        <v>20190501</v>
+      </c>
+      <c r="I26" s="5">
+        <v>20190731</v>
+      </c>
+      <c r="J26" s="5">
+        <v>1</v>
+      </c>
+      <c r="K26" s="12">
+        <v>43586</v>
+      </c>
+      <c r="L26" s="5">
+        <v>1</v>
+      </c>
+      <c r="M26" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" s="5">
+        <v>1</v>
+      </c>
+      <c r="B27" s="5">
+        <v>6</v>
+      </c>
+      <c r="C27" s="5">
+        <v>6</v>
+      </c>
+      <c r="D27" s="5">
+        <v>19</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>987</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>728</v>
+      </c>
+      <c r="G27" s="5">
+        <v>1</v>
+      </c>
+      <c r="H27" s="5">
+        <v>20190501</v>
+      </c>
+      <c r="I27" s="5">
+        <v>20190731</v>
+      </c>
+      <c r="J27" s="5">
+        <v>1</v>
+      </c>
+      <c r="K27" s="12">
+        <v>43586</v>
+      </c>
+      <c r="L27" s="5">
+        <v>1</v>
+      </c>
+      <c r="M27" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28" s="5">
+        <v>1</v>
+      </c>
+      <c r="B28" s="5">
+        <v>6</v>
+      </c>
+      <c r="C28" s="5">
+        <v>6</v>
+      </c>
+      <c r="D28" s="5">
+        <v>20</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>988</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>728</v>
+      </c>
+      <c r="G28" s="5">
+        <v>1</v>
+      </c>
+      <c r="H28" s="5">
+        <v>20190501</v>
+      </c>
+      <c r="I28" s="5">
+        <v>20190731</v>
+      </c>
+      <c r="J28" s="5">
+        <v>1</v>
+      </c>
+      <c r="K28" s="12">
+        <v>43586</v>
+      </c>
+      <c r="L28" s="5">
+        <v>1</v>
+      </c>
+      <c r="M28" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29" s="5">
+        <v>1</v>
+      </c>
+      <c r="B29" s="5">
+        <v>6</v>
+      </c>
+      <c r="C29" s="5">
+        <v>6</v>
+      </c>
+      <c r="D29" s="5">
+        <v>21</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>989</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>728</v>
+      </c>
+      <c r="G29" s="5">
+        <v>1</v>
+      </c>
+      <c r="H29" s="5">
+        <v>20190501</v>
+      </c>
+      <c r="I29" s="5">
+        <v>20190731</v>
+      </c>
+      <c r="J29" s="5">
+        <v>1</v>
+      </c>
+      <c r="K29" s="12">
+        <v>43586</v>
+      </c>
+      <c r="L29" s="5">
+        <v>1</v>
+      </c>
+      <c r="M29" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A30" s="5">
+        <v>1</v>
+      </c>
+      <c r="B30" s="5">
+        <v>6</v>
+      </c>
+      <c r="C30" s="5">
+        <v>6</v>
+      </c>
+      <c r="D30" s="5">
+        <v>22</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>990</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>728</v>
+      </c>
+      <c r="G30" s="5">
+        <v>1</v>
+      </c>
+      <c r="H30" s="5">
+        <v>20190501</v>
+      </c>
+      <c r="I30" s="5">
+        <v>20190731</v>
+      </c>
+      <c r="J30" s="5">
+        <v>1</v>
+      </c>
+      <c r="K30" s="12">
+        <v>43586</v>
+      </c>
+      <c r="L30" s="5">
+        <v>1</v>
+      </c>
+      <c r="M30" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A31" s="5">
+        <v>1</v>
+      </c>
+      <c r="B31" s="5">
+        <v>6</v>
+      </c>
+      <c r="C31" s="5">
+        <v>6</v>
+      </c>
+      <c r="D31" s="5">
+        <v>23</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>991</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>728</v>
+      </c>
+      <c r="G31" s="5">
+        <v>1</v>
+      </c>
+      <c r="H31" s="5">
+        <v>20190501</v>
+      </c>
+      <c r="I31" s="5">
+        <v>20190731</v>
+      </c>
+      <c r="J31" s="5">
+        <v>1</v>
+      </c>
+      <c r="K31" s="12">
+        <v>43586</v>
+      </c>
+      <c r="L31" s="5">
+        <v>1</v>
+      </c>
+      <c r="M31" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A32" s="5">
+        <v>1</v>
+      </c>
+      <c r="B32" s="5">
+        <v>6</v>
+      </c>
+      <c r="C32" s="5">
+        <v>6</v>
+      </c>
+      <c r="D32" s="5">
+        <v>24</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>992</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>728</v>
+      </c>
+      <c r="G32" s="5">
+        <v>1</v>
+      </c>
+      <c r="H32" s="5">
+        <v>20190501</v>
+      </c>
+      <c r="I32" s="5">
+        <v>20190731</v>
+      </c>
+      <c r="J32" s="5">
+        <v>1</v>
+      </c>
+      <c r="K32" s="12">
+        <v>43586</v>
+      </c>
+      <c r="L32" s="5">
+        <v>1</v>
+      </c>
+      <c r="M32" s="5">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -33614,13 +34045,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>913</v>
+      </c>
+      <c r="B1" t="s">
         <v>914</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>915</v>
-      </c>
-      <c r="C1" t="s">
-        <v>916</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -33631,7 +34062,7 @@
         <v>174</v>
       </c>
       <c r="C2" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -33642,7 +34073,7 @@
         <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -33653,7 +34084,7 @@
         <v>175</v>
       </c>
       <c r="C4" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -33664,7 +34095,7 @@
         <v>379</v>
       </c>
       <c r="C5" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -33672,10 +34103,10 @@
         <v>105</v>
       </c>
       <c r="B6" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="C6" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -33683,10 +34114,10 @@
         <v>106</v>
       </c>
       <c r="B7" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="C7" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -33697,7 +34128,7 @@
         <v>423</v>
       </c>
       <c r="C8" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -33705,10 +34136,10 @@
         <v>108</v>
       </c>
       <c r="B9" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="C9" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -33716,10 +34147,10 @@
         <v>109</v>
       </c>
       <c r="B10" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="C10" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -33727,10 +34158,10 @@
         <v>110</v>
       </c>
       <c r="B11" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="C11" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
     </row>
   </sheetData>
@@ -33756,19 +34187,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>920</v>
+      </c>
+      <c r="B1" t="s">
+        <v>914</v>
+      </c>
+      <c r="C1" t="s">
         <v>921</v>
-      </c>
-      <c r="B1" t="s">
-        <v>915</v>
-      </c>
-      <c r="C1" t="s">
-        <v>922</v>
       </c>
       <c r="D1" t="s">
         <v>758</v>
       </c>
       <c r="E1" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -33844,7 +34275,7 @@
         <v>105</v>
       </c>
       <c r="B6" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -33861,7 +34292,7 @@
         <v>106</v>
       </c>
       <c r="B7" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -33895,7 +34326,7 @@
         <v>108</v>
       </c>
       <c r="B9" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -33912,7 +34343,7 @@
         <v>109</v>
       </c>
       <c r="B10" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -33929,7 +34360,7 @@
         <v>110</v>
       </c>
       <c r="B11" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -33966,28 +34397,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>913</v>
+      </c>
+      <c r="B1" t="s">
         <v>914</v>
       </c>
-      <c r="B1" t="s">
-        <v>915</v>
-      </c>
       <c r="C1" t="s">
+        <v>923</v>
+      </c>
+      <c r="D1" t="s">
         <v>924</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>925</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>926</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>927</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>928</v>
-      </c>
-      <c r="H1" t="s">
-        <v>929</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -34099,7 +34530,7 @@
         <v>105</v>
       </c>
       <c r="B6" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -34125,7 +34556,7 @@
         <v>106</v>
       </c>
       <c r="B7" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -34177,7 +34608,7 @@
         <v>108</v>
       </c>
       <c r="B9" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -34203,7 +34634,7 @@
         <v>109</v>
       </c>
       <c r="B10" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -34229,7 +34660,7 @@
         <v>110</v>
       </c>
       <c r="B11" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -34273,7 +34704,7 @@
         <v>501</v>
       </c>
       <c r="B1" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>732</v>
@@ -34281,10 +34712,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>930</v>
+      </c>
+      <c r="B2" t="s">
         <v>931</v>
-      </c>
-      <c r="B2" t="s">
-        <v>932</v>
       </c>
       <c r="C2" s="6">
         <v>101</v>
@@ -34292,7 +34723,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="B3" t="s">
         <v>17</v>
@@ -34303,10 +34734,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="B4" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="C4" s="6">
         <v>201</v>
@@ -34314,7 +34745,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="B5" t="s">
         <v>17</v>
@@ -34325,10 +34756,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>933</v>
+      </c>
+      <c r="B6" t="s">
         <v>934</v>
-      </c>
-      <c r="B6" t="s">
-        <v>935</v>
       </c>
       <c r="C6" s="6">
         <v>301</v>
@@ -34336,10 +34767,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="B7" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="C7" s="6">
         <v>302</v>
@@ -34347,10 +34778,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="B8" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="C8" s="6">
         <v>303</v>
@@ -34358,10 +34789,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="B9" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="C9" s="6">
         <v>304</v>
@@ -34369,7 +34800,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="B10" t="s">
         <v>17</v>
@@ -34391,10 +34822,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>938</v>
+      </c>
+      <c r="B12" t="s">
         <v>939</v>
-      </c>
-      <c r="B12" t="s">
-        <v>940</v>
       </c>
       <c r="C12" s="6">
         <v>401</v>
@@ -34402,10 +34833,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="B13" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="C13" s="6">
         <v>402</v>
@@ -34413,10 +34844,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="B14" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="C14" s="6">
         <v>403</v>
@@ -34424,10 +34855,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="B15" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="C15" s="6">
         <v>404</v>
@@ -34435,10 +34866,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="B16" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="C16" s="6">
         <v>405</v>
@@ -34446,10 +34877,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="B17" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="C17" s="6">
         <v>406</v>
@@ -34457,10 +34888,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="B18" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="C18" s="6">
         <v>407</v>
@@ -35431,19 +35862,19 @@
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A59" s="5">
+      <c r="A59" s="8">
         <v>57</v>
       </c>
-      <c r="B59" s="5" t="s">
+      <c r="B59" s="8" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" s="8">
+        <v>58</v>
+      </c>
+      <c r="B60" s="8" t="s">
         <v>982</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A60" s="5">
-        <v>58</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>983</v>
       </c>
     </row>
   </sheetData>
@@ -35455,7 +35886,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B251"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A227" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -37436,7 +37867,7 @@
         <v>245</v>
       </c>
       <c r="B247" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.3">
@@ -37444,7 +37875,7 @@
         <v>246</v>
       </c>
       <c r="B248" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.3">
@@ -37452,7 +37883,7 @@
         <v>247</v>
       </c>
       <c r="B249" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.3">
@@ -37460,7 +37891,7 @@
         <v>248</v>
       </c>
       <c r="B250" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.3">
@@ -37468,7 +37899,7 @@
         <v>249</v>
       </c>
       <c r="B251" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TFS 14108 - Updates to OMR short calls handling
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C42775
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
@@ -39,6 +39,9 @@
     <sheet name="UI_Role_Page_Access" sheetId="26" r:id="rId25"/>
     <sheet name="UI_Dashboard_Summary_Display" sheetId="27" r:id="rId26"/>
     <sheet name="Reasons_By_ReportCode" sheetId="28" r:id="rId27"/>
+    <sheet name="ShortCalls_Behavior" sheetId="29" r:id="rId28"/>
+    <sheet name="ShortCalls_Actions" sheetId="30" r:id="rId29"/>
+    <sheet name="ShortCalls_BAL" sheetId="31" r:id="rId30"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">Coaching_Reason_Selection!$A$1:$P$292</definedName>
@@ -50,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3636" uniqueCount="993">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3667" uniqueCount="1017">
   <si>
     <t>SourceID</t>
   </si>
@@ -3030,6 +3033,78 @@
   </si>
   <si>
     <t>7 - Strongly Agree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added new tables to support OMR Short Calls </t>
+  </si>
+  <si>
+    <t>Valid</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>Calling Kudos Line</t>
+  </si>
+  <si>
+    <t>Good Call</t>
+  </si>
+  <si>
+    <t>Incorrect blind transfer</t>
+  </si>
+  <si>
+    <t>Incorrect phone status (calls still coming in)</t>
+  </si>
+  <si>
+    <t>Intentionally disconnecting calls</t>
+  </si>
+  <si>
+    <t>Not following call flow (not opening a call)</t>
+  </si>
+  <si>
+    <t>Not following procedure for disconnect by caller (ghost calls, greeting 3x's, template)</t>
+  </si>
+  <si>
+    <t>Spanish Transfer</t>
+  </si>
+  <si>
+    <t>SSA Transfer</t>
+  </si>
+  <si>
+    <t>Technical Issue (CSR Error &amp; Technical Error)</t>
+  </si>
+  <si>
+    <t>Valid Password Reset</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Coach the CSR to Immediately notify Supervisor/LSA of Technical Issues</t>
+  </si>
+  <si>
+    <t>Coach to the behavior (Progressive disciplinary course details in coaching comments)</t>
+  </si>
+  <si>
+    <t>Inform IT or Telecom - Ticket Submitted</t>
+  </si>
+  <si>
+    <t>Inform LSA - Ticket Submitted</t>
+  </si>
+  <si>
+    <t>Issue verbal warning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Issue written warning  </t>
+  </si>
+  <si>
+    <t>Start termination process</t>
+  </si>
+  <si>
+    <t>BehaviorId</t>
+  </si>
+  <si>
+    <t>ActionId</t>
   </si>
 </sst>
 </file>
@@ -3414,10 +3489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L83"/>
+  <dimension ref="A1:L84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="A83" sqref="A83"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="A84" sqref="A84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4809,21 +4884,38 @@
         <v>983</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A83" s="5">
+    <row r="83" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="8">
         <v>73</v>
       </c>
-      <c r="B83" s="11">
+      <c r="B83" s="9">
         <v>43577</v>
       </c>
-      <c r="C83" s="5" t="s">
+      <c r="C83" s="8" t="s">
         <v>430</v>
       </c>
-      <c r="D83" s="5">
+      <c r="D83" s="8">
         <v>14178</v>
       </c>
-      <c r="E83" s="5" t="s">
+      <c r="E83" s="8" t="s">
         <v>984</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A84" s="5">
+        <v>74</v>
+      </c>
+      <c r="B84" s="11">
+        <v>43654</v>
+      </c>
+      <c r="C84" s="5" t="s">
+        <v>430</v>
+      </c>
+      <c r="D84" s="5">
+        <v>14108</v>
+      </c>
+      <c r="E84" s="5" t="s">
+        <v>993</v>
       </c>
     </row>
   </sheetData>
@@ -34902,6 +34994,292 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" t="s">
+        <v>503</v>
+      </c>
+      <c r="C1" t="s">
+        <v>994</v>
+      </c>
+      <c r="D1" t="s">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>101</v>
+      </c>
+      <c r="B2" t="s">
+        <v>996</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>102</v>
+      </c>
+      <c r="B3" t="s">
+        <v>997</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>103</v>
+      </c>
+      <c r="B4" t="s">
+        <v>998</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>104</v>
+      </c>
+      <c r="B5" t="s">
+        <v>999</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>105</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1000</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>106</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1001</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>107</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1002</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>108</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1003</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>109</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1004</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>110</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1005</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>111</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1006</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1007</v>
+      </c>
+      <c r="C1" t="s">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1008</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1009</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1010</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1011</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1012</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1013</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1014</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
@@ -35000,6 +35378,357 @@
       </c>
       <c r="B11" t="s">
         <v>180</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1016</v>
+      </c>
+      <c r="C1" t="s">
+        <v>732</v>
+      </c>
+      <c r="D1" t="s">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>101</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>101</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>101</v>
+      </c>
+      <c r="B4">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>101</v>
+      </c>
+      <c r="B5">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>103</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>103</v>
+      </c>
+      <c r="B7">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>104</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>104</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>104</v>
+      </c>
+      <c r="B10">
+        <v>6</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>104</v>
+      </c>
+      <c r="B11">
+        <v>7</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>105</v>
+      </c>
+      <c r="B12">
+        <v>6</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>105</v>
+      </c>
+      <c r="B13">
+        <v>7</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>106</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>106</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>106</v>
+      </c>
+      <c r="B16">
+        <v>6</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>106</v>
+      </c>
+      <c r="B17">
+        <v>7</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>107</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>107</v>
+      </c>
+      <c r="B19">
+        <v>5</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>107</v>
+      </c>
+      <c r="B20">
+        <v>6</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>107</v>
+      </c>
+      <c r="B21">
+        <v>7</v>
+      </c>
+      <c r="C21">
+        <v>4</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>110</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>110</v>
+      </c>
+      <c r="B23">
+        <v>3</v>
+      </c>
+      <c r="C23">
+        <v>3</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>110</v>
+      </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TFS 15063 - Quality Now Rewards and Recognition (Bingo)
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C43062
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="132" windowWidth="22992" windowHeight="12840"/>
+    <workbookView xWindow="480" yWindow="132" windowWidth="22992" windowHeight="12840" firstSheet="26" activeTab="30"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_History" sheetId="14" r:id="rId1"/>
@@ -42,6 +42,7 @@
     <sheet name="ShortCalls_Behavior" sheetId="29" r:id="rId28"/>
     <sheet name="ShortCalls_Actions" sheetId="30" r:id="rId29"/>
     <sheet name="ShortCalls_BAL" sheetId="31" r:id="rId30"/>
+    <sheet name="Quality_Now_Bingo_Images" sheetId="32" r:id="rId31"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">Coaching_Reason_Selection!$A$1:$P$292</definedName>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3667" uniqueCount="1017">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3687" uniqueCount="1035">
   <si>
     <t>SourceID</t>
   </si>
@@ -3105,6 +3106,60 @@
   </si>
   <si>
     <t>ActionId</t>
+  </si>
+  <si>
+    <t>Added a new record toSubCoaching Reason table(250) to support QN Bingo and a new tab for table Quality_Now_Bingo_Images</t>
+  </si>
+  <si>
+    <t>ImageID</t>
+  </si>
+  <si>
+    <t>ImageDesc</t>
+  </si>
+  <si>
+    <t>Competency</t>
+  </si>
+  <si>
+    <t>&lt;img border="20" src="cid:aa.png"&gt;</t>
+  </si>
+  <si>
+    <t>Accurate Arrow</t>
+  </si>
+  <si>
+    <t>&lt;img border="20" src="cid:al.png"&gt;</t>
+  </si>
+  <si>
+    <t>Active Listener</t>
+  </si>
+  <si>
+    <t>&lt;img border="20" src="cid:cc.png"&gt;</t>
+  </si>
+  <si>
+    <t>Compassionate Communicator</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;img border="20" src="cid:nn.png"&gt;</t>
+  </si>
+  <si>
+    <t>Nimble Navigator</t>
+  </si>
+  <si>
+    <t>&lt;img border="20" src="cid:pp.png"&gt;</t>
+  </si>
+  <si>
+    <t>Privacy Protector</t>
+  </si>
+  <si>
+    <t>&lt;img border="20" src="cid:pr.png"&gt;</t>
+  </si>
+  <si>
+    <t>Process Pro</t>
+  </si>
+  <si>
+    <t>&lt;img border="20" src="cid:so.png"&gt;</t>
+  </si>
+  <si>
+    <t>Smooth Operator</t>
   </si>
 </sst>
 </file>
@@ -3489,10 +3544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L84"/>
+  <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="A84" sqref="A84"/>
+    <sheetView topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="E85" sqref="E85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4901,21 +4956,38 @@
         <v>984</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A84" s="5">
+    <row r="84" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="6">
         <v>74</v>
       </c>
-      <c r="B84" s="11">
+      <c r="B84" s="10">
         <v>43654</v>
       </c>
-      <c r="C84" s="5" t="s">
+      <c r="C84" s="6" t="s">
         <v>430</v>
       </c>
-      <c r="D84" s="5">
+      <c r="D84" s="6">
         <v>14108</v>
       </c>
-      <c r="E84" s="5" t="s">
+      <c r="E84" s="6" t="s">
         <v>993</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A85" s="5">
+        <v>75</v>
+      </c>
+      <c r="B85" s="11">
+        <v>43693</v>
+      </c>
+      <c r="C85" s="5" t="s">
+        <v>430</v>
+      </c>
+      <c r="D85" s="5">
+        <v>15063</v>
+      </c>
+      <c r="E85" s="5" t="s">
+        <v>1017</v>
       </c>
     </row>
   </sheetData>
@@ -35736,6 +35808,114 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1019</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1021</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1023</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1025</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1026</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1027</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1030</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1031</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1032</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1033</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1034</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
@@ -36613,9 +36793,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B251"/>
+  <dimension ref="A1:B252"/>
   <sheetViews>
-    <sheetView topLeftCell="A227" workbookViewId="0"/>
+    <sheetView topLeftCell="A227" workbookViewId="0">
+      <selection activeCell="A252" sqref="A252:B252"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -38629,6 +38811,14 @@
       </c>
       <c r="B251" t="s">
         <v>963</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A252" s="5">
+        <v>250</v>
+      </c>
+      <c r="B252" s="5" t="s">
+        <v>981</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TFS 15095 – Feed to eCL for Attendance Policy Earnback
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C43177
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="132" windowWidth="22992" windowHeight="12840" firstSheet="7" activeTab="11"/>
+    <workbookView xWindow="480" yWindow="132" windowWidth="22992" windowHeight="12840" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_History" sheetId="14" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3681" uniqueCount="1037">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3684" uniqueCount="1039">
   <si>
     <t>SourceID</t>
   </si>
@@ -3162,10 +3162,16 @@
     <t>Smooth Operator</t>
   </si>
   <si>
-    <t>Add Deltek as Coaching and Sub Coaching reason. Updates to DIM_Coaching_Reason, DIM_Sub_Coaching_Reason and Coaching_Reason_Selection tables</t>
-  </si>
-  <si>
     <t>Deltek</t>
+  </si>
+  <si>
+    <t>Add Deltek (59) as Coaching and Sub Coaching reason(251). Updates to DIM_Coaching_Reason, DIM_Sub_Coaching_Reason and Coaching_Reason_Selection tables</t>
+  </si>
+  <si>
+    <t>feed to eCL for Attendance Policy Earnback. Added new subcoachingreason(252)</t>
+  </si>
+  <si>
+    <t>Attendance Hours Earned Back</t>
   </si>
 </sst>
 </file>
@@ -3549,10 +3555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L86"/>
+  <dimension ref="A1:L87"/>
   <sheetViews>
     <sheetView topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="E86" sqref="E86"/>
+      <selection activeCell="E87" sqref="E87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4822,13 +4828,13 @@
       <c r="A76" s="6">
         <v>67</v>
       </c>
-      <c r="B76" s="6">
+      <c r="B76" s="10">
         <v>43396</v>
       </c>
       <c r="C76" s="6" t="s">
         <v>430</v>
       </c>
-      <c r="D76" s="10">
+      <c r="D76" s="6">
         <v>12455</v>
       </c>
       <c r="E76" s="6" t="s">
@@ -5009,7 +5015,24 @@
         <v>15144</v>
       </c>
       <c r="E86" t="s">
-        <v>1035</v>
+        <v>1036</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A87" s="6">
+        <v>77</v>
+      </c>
+      <c r="B87" s="1">
+        <v>43704</v>
+      </c>
+      <c r="C87" s="6" t="s">
+        <v>430</v>
+      </c>
+      <c r="D87">
+        <v>15095</v>
+      </c>
+      <c r="E87" t="s">
+        <v>1037</v>
       </c>
     </row>
   </sheetData>
@@ -6494,8 +6517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P314"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A289" workbookViewId="0">
-      <selection activeCell="A314" sqref="A314"/>
+    <sheetView topLeftCell="A289" workbookViewId="0">
+      <selection activeCell="A314" sqref="A314:P314"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6564,7 +6587,7 @@
         <v>251</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="E2" s="5">
         <v>1</v>
@@ -6864,7 +6887,7 @@
         <v>251</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="E8" s="5">
         <v>1</v>
@@ -7164,7 +7187,7 @@
         <v>251</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="E14" s="5">
         <v>1</v>
@@ -22154,52 +22177,52 @@
       </c>
     </row>
     <row r="314" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A314" s="5">
+      <c r="A314" s="6">
         <v>59</v>
       </c>
-      <c r="B314" s="5" t="s">
-        <v>1036</v>
-      </c>
-      <c r="C314" s="5">
+      <c r="B314" s="6" t="s">
+        <v>1035</v>
+      </c>
+      <c r="C314" s="6">
         <v>42</v>
       </c>
-      <c r="D314" s="5" t="s">
+      <c r="D314" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="E314" s="5">
-        <v>1</v>
-      </c>
-      <c r="F314" s="5">
-        <v>1</v>
-      </c>
-      <c r="G314" s="5">
-        <v>1</v>
-      </c>
-      <c r="H314" s="5">
-        <v>1</v>
-      </c>
-      <c r="I314" s="5">
-        <v>1</v>
-      </c>
-      <c r="J314" s="5">
-        <v>1</v>
-      </c>
-      <c r="K314" s="5">
-        <v>1</v>
-      </c>
-      <c r="L314" s="5">
-        <v>1</v>
-      </c>
-      <c r="M314" s="5">
-        <v>0</v>
-      </c>
-      <c r="N314" s="5">
-        <v>0</v>
-      </c>
-      <c r="O314" s="5">
-        <v>1</v>
-      </c>
-      <c r="P314" s="5">
+      <c r="E314" s="6">
+        <v>1</v>
+      </c>
+      <c r="F314" s="6">
+        <v>1</v>
+      </c>
+      <c r="G314" s="6">
+        <v>1</v>
+      </c>
+      <c r="H314" s="6">
+        <v>1</v>
+      </c>
+      <c r="I314" s="6">
+        <v>1</v>
+      </c>
+      <c r="J314" s="6">
+        <v>1</v>
+      </c>
+      <c r="K314" s="6">
+        <v>1</v>
+      </c>
+      <c r="L314" s="6">
+        <v>1</v>
+      </c>
+      <c r="M314" s="6">
+        <v>0</v>
+      </c>
+      <c r="N314" s="6">
+        <v>0</v>
+      </c>
+      <c r="O314" s="6">
+        <v>1</v>
+      </c>
+      <c r="P314" s="6">
         <v>1</v>
       </c>
     </row>
@@ -36072,7 +36095,7 @@
   <dimension ref="A1:B61"/>
   <sheetViews>
     <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61:B61"/>
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -36562,11 +36585,11 @@
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A61" s="5">
+      <c r="A61">
         <v>59</v>
       </c>
-      <c r="B61" s="5" t="s">
-        <v>1036</v>
+      <c r="B61" t="s">
+        <v>1035</v>
       </c>
     </row>
   </sheetData>
@@ -36576,10 +36599,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B253"/>
+  <dimension ref="A1:B254"/>
   <sheetViews>
-    <sheetView topLeftCell="A227" workbookViewId="0">
-      <selection activeCell="A253" sqref="A253:B253"/>
+    <sheetView tabSelected="1" topLeftCell="A227" workbookViewId="0">
+      <selection activeCell="A254" sqref="A254:B254"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -38597,19 +38620,27 @@
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A252">
+      <c r="A252" s="6">
         <v>250</v>
       </c>
-      <c r="B252" t="s">
+      <c r="B252" s="6" t="s">
         <v>981</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A253" s="5">
+      <c r="A253" s="6">
         <v>251</v>
       </c>
-      <c r="B253" s="5" t="s">
-        <v>1036</v>
+      <c r="B253" s="6" t="s">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A254" s="5">
+        <v>252</v>
+      </c>
+      <c r="B254" s="5" t="s">
+        <v>1038</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TFS 15621 - Display MyFollowup for CSRs
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C43433
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3687" uniqueCount="1041">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3690" uniqueCount="1043">
   <si>
     <t>SourceID</t>
   </si>
@@ -3178,6 +3178,12 @@
   </si>
   <si>
     <t>Incorporate a follow-up process for eCoaching submissions. Added new status in DIM_Status tab</t>
+  </si>
+  <si>
+    <t>MyFollowup</t>
+  </si>
+  <si>
+    <t>Display lMyFollowup for CSRs. Added new col MyFollowup in UI_Dashboard_Summary_Display tab</t>
   </si>
 </sst>
 </file>
@@ -3562,10 +3568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L88"/>
+  <dimension ref="A1:L89"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="A88" sqref="A88"/>
+      <selection activeCell="A89" sqref="A89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5042,21 +5048,38 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A88" s="5">
+    <row r="88" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="6">
         <v>78</v>
       </c>
-      <c r="B88" s="12">
+      <c r="B88" s="10">
         <v>43714</v>
       </c>
-      <c r="C88" s="5" t="s">
+      <c r="C88" s="6" t="s">
         <v>430</v>
       </c>
-      <c r="D88" s="5">
+      <c r="D88" s="6">
         <v>13644</v>
       </c>
-      <c r="E88" s="5" t="s">
+      <c r="E88" s="6" t="s">
         <v>1040</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A89" s="5">
+        <v>79</v>
+      </c>
+      <c r="B89" s="12">
+        <v>43725</v>
+      </c>
+      <c r="C89" s="5" t="s">
+        <v>430</v>
+      </c>
+      <c r="D89" s="5">
+        <v>15621</v>
+      </c>
+      <c r="E89" s="5" t="s">
+        <v>1042</v>
       </c>
     </row>
   </sheetData>
@@ -34365,9 +34388,11 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -34381,7 +34406,7 @@
     <col min="8" max="8" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>913</v>
       </c>
@@ -34406,8 +34431,11 @@
       <c r="H1" t="s">
         <v>928</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" s="5" t="s">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>101</v>
       </c>
@@ -34432,8 +34460,11 @@
       <c r="H2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>102</v>
       </c>
@@ -34458,8 +34489,11 @@
       <c r="H3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I3" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>103</v>
       </c>
@@ -34484,8 +34518,11 @@
       <c r="H4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I4" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>104</v>
       </c>
@@ -34510,8 +34547,11 @@
       <c r="H5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I5" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>105</v>
       </c>
@@ -34536,8 +34576,11 @@
       <c r="H6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I6" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>106</v>
       </c>
@@ -34562,8 +34605,11 @@
       <c r="H7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I7" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>107</v>
       </c>
@@ -34588,8 +34634,11 @@
       <c r="H8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I8" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>108</v>
       </c>
@@ -34614,8 +34663,11 @@
       <c r="H9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I9" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>109</v>
       </c>
@@ -34640,8 +34692,11 @@
       <c r="H10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I10" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>110</v>
       </c>
@@ -34665,6 +34720,9 @@
       </c>
       <c r="H11">
         <v>1</v>
+      </c>
+      <c r="I11" s="5">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TFS 15465 - eCoaching - London Alternate Channel Bingo logs
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C43566
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="132" windowWidth="22992" windowHeight="12840"/>
+    <workbookView xWindow="480" yWindow="132" windowWidth="22992" windowHeight="12840" firstSheet="26" activeTab="30"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_History" sheetId="14" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3692" uniqueCount="1045">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3723" uniqueCount="1058">
   <si>
     <t>SourceID</t>
   </si>
@@ -3135,9 +3135,6 @@
     <t>Compassionate Communicator</t>
   </si>
   <si>
-    <t xml:space="preserve"> &lt;img border="20" src="cid:nn.png"&gt;</t>
-  </si>
-  <si>
     <t>Nimble Navigator</t>
   </si>
   <si>
@@ -3190,6 +3187,48 @@
   </si>
   <si>
     <t>FL - Tampa</t>
+  </si>
+  <si>
+    <t>New column and records to Quality_Now_Bingo_Images tab</t>
+  </si>
+  <si>
+    <t>BingoType</t>
+  </si>
+  <si>
+    <t>QN</t>
+  </si>
+  <si>
+    <t>&lt;img border="20" src="cid:nn.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img border="20" src="cid:aa_qm.png"&gt;</t>
+  </si>
+  <si>
+    <t>QM</t>
+  </si>
+  <si>
+    <t>&lt;img border="20" src="cid:cc_qm.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img border="20" src="cid:mm_qm.png"&gt;</t>
+  </si>
+  <si>
+    <t>Message Master</t>
+  </si>
+  <si>
+    <t>&lt;img border="20" src="cid:pp_qm.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img border="20" src="cid:pr_qm.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img border="20" src="cid:rr_qm.png"&gt;</t>
+  </si>
+  <si>
+    <t>Resolution Rock Star</t>
+  </si>
+  <si>
+    <t>&lt;img border="20" src="cid:so_qm.png"&gt;</t>
   </si>
 </sst>
 </file>
@@ -3254,7 +3293,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -3268,9 +3307,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3577,10 +3615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L90"/>
+  <dimension ref="A1:L91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="A90" sqref="A90"/>
+    <sheetView topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="A91" sqref="A91:E91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5037,7 +5075,7 @@
         <v>15144</v>
       </c>
       <c r="E86" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
@@ -5054,7 +5092,7 @@
         <v>15095</v>
       </c>
       <c r="E87" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="88" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -5071,7 +5109,7 @@
         <v>13644</v>
       </c>
       <c r="E88" s="6" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
@@ -5088,24 +5126,41 @@
         <v>15621</v>
       </c>
       <c r="E89" s="8" t="s">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A90" s="8">
+        <v>80</v>
+      </c>
+      <c r="B90" s="9">
+        <v>43731</v>
+      </c>
+      <c r="C90" s="8" t="s">
+        <v>429</v>
+      </c>
+      <c r="D90" s="8">
+        <v>15450</v>
+      </c>
+      <c r="E90" s="12" t="s">
         <v>1041</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A90" s="5">
-        <v>80</v>
-      </c>
-      <c r="B90" s="12">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A91" s="5">
+        <v>81</v>
+      </c>
+      <c r="B91" s="11">
         <v>43731</v>
       </c>
-      <c r="C90" s="5" t="s">
+      <c r="C91" s="5" t="s">
         <v>429</v>
       </c>
-      <c r="D90" s="5">
-        <v>15450</v>
-      </c>
-      <c r="E90" s="13" t="s">
-        <v>1042</v>
+      <c r="D91" s="5">
+        <v>15465</v>
+      </c>
+      <c r="E91" s="5" t="s">
+        <v>1044</v>
       </c>
     </row>
   </sheetData>
@@ -6660,7 +6715,7 @@
         <v>251</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="E2" s="5">
         <v>1</v>
@@ -6960,7 +7015,7 @@
         <v>251</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="E8" s="5">
         <v>1</v>
@@ -7260,7 +7315,7 @@
         <v>251</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="E14" s="5">
         <v>1</v>
@@ -22254,7 +22309,7 @@
         <v>59</v>
       </c>
       <c r="B314" s="6" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="C314" s="6">
         <v>42</v>
@@ -29166,7 +29221,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A9" sqref="A9:I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -29383,60 +29438,60 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="5">
+      <c r="A8" s="6">
         <v>6</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="6" t="s">
         <v>984</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="6">
         <v>98</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="6">
         <v>20190501</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="6">
         <v>20190731</v>
       </c>
-      <c r="F8" s="5">
-        <v>1</v>
-      </c>
-      <c r="G8" s="5">
-        <v>1</v>
-      </c>
-      <c r="H8" s="11">
+      <c r="F8" s="6">
+        <v>1</v>
+      </c>
+      <c r="G8" s="6">
+        <v>1</v>
+      </c>
+      <c r="H8" s="7">
         <v>43577.559065011577</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="5">
+      <c r="A9" s="6">
         <v>7</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="6" t="s">
         <v>900</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="6">
         <v>7</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="6">
         <v>20180201</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="6">
         <v>99991231</v>
       </c>
-      <c r="F9" s="5">
-        <v>0</v>
-      </c>
-      <c r="G9" s="5">
-        <v>0</v>
-      </c>
-      <c r="H9" s="11">
+      <c r="F9" s="6">
+        <v>0</v>
+      </c>
+      <c r="G9" s="6">
+        <v>0</v>
+      </c>
+      <c r="H9" s="7">
         <v>43577.559065011577</v>
       </c>
-      <c r="I9" s="5">
+      <c r="I9" s="6">
         <v>0</v>
       </c>
     </row>
@@ -29729,100 +29784,100 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="5">
+      <c r="A20" s="6">
         <v>18</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="6" t="s">
         <v>985</v>
       </c>
-      <c r="C20" s="5">
-        <v>1</v>
-      </c>
-      <c r="D20" s="11">
+      <c r="C20" s="6">
+        <v>1</v>
+      </c>
+      <c r="D20" s="7">
         <v>43586</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="5">
+      <c r="A21" s="6">
         <v>19</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="6" t="s">
         <v>986</v>
       </c>
-      <c r="C21" s="5">
-        <v>1</v>
-      </c>
-      <c r="D21" s="11">
+      <c r="C21" s="6">
+        <v>1</v>
+      </c>
+      <c r="D21" s="7">
         <v>43586</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="5">
+      <c r="A22" s="6">
         <v>20</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="6" t="s">
         <v>987</v>
       </c>
-      <c r="C22" s="5">
-        <v>1</v>
-      </c>
-      <c r="D22" s="11">
+      <c r="C22" s="6">
+        <v>1</v>
+      </c>
+      <c r="D22" s="7">
         <v>43586</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="5">
+      <c r="A23" s="6">
         <v>21</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="6" t="s">
         <v>988</v>
       </c>
-      <c r="C23" s="5">
-        <v>1</v>
-      </c>
-      <c r="D23" s="11">
+      <c r="C23" s="6">
+        <v>1</v>
+      </c>
+      <c r="D23" s="7">
         <v>43586</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="5">
+      <c r="A24" s="6">
         <v>22</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="6" t="s">
         <v>989</v>
       </c>
-      <c r="C24" s="5">
-        <v>1</v>
-      </c>
-      <c r="D24" s="11">
+      <c r="C24" s="6">
+        <v>1</v>
+      </c>
+      <c r="D24" s="7">
         <v>43586</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="5">
+      <c r="A25" s="6">
         <v>23</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="6" t="s">
         <v>990</v>
       </c>
-      <c r="C25" s="5">
-        <v>1</v>
-      </c>
-      <c r="D25" s="11">
+      <c r="C25" s="6">
+        <v>1</v>
+      </c>
+      <c r="D25" s="7">
         <v>43586</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="5">
+      <c r="A26" s="6">
         <v>24</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="6" t="s">
         <v>991</v>
       </c>
-      <c r="C26" s="5">
-        <v>1</v>
-      </c>
-      <c r="D26" s="11">
+      <c r="C26" s="6">
+        <v>1</v>
+      </c>
+      <c r="D26" s="7">
         <v>43586</v>
       </c>
     </row>
@@ -32028,7 +32083,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="A26" sqref="A26:M32"/>
     </sheetView>
   </sheetViews>
@@ -33063,289 +33118,289 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A26" s="5">
-        <v>1</v>
-      </c>
-      <c r="B26" s="5">
+      <c r="A26" s="6">
+        <v>1</v>
+      </c>
+      <c r="B26" s="6">
         <v>6</v>
       </c>
-      <c r="C26" s="5">
+      <c r="C26" s="6">
         <v>6</v>
       </c>
-      <c r="D26" s="5">
+      <c r="D26" s="6">
         <v>18</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="E26" s="6" t="s">
         <v>985</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="F26" s="6" t="s">
         <v>727</v>
       </c>
-      <c r="G26" s="5">
-        <v>1</v>
-      </c>
-      <c r="H26" s="5">
+      <c r="G26" s="6">
+        <v>1</v>
+      </c>
+      <c r="H26" s="6">
         <v>20190501</v>
       </c>
-      <c r="I26" s="5">
+      <c r="I26" s="6">
         <v>20190731</v>
       </c>
-      <c r="J26" s="5">
-        <v>1</v>
-      </c>
-      <c r="K26" s="11">
+      <c r="J26" s="6">
+        <v>1</v>
+      </c>
+      <c r="K26" s="7">
         <v>43586</v>
       </c>
-      <c r="L26" s="5">
-        <v>1</v>
-      </c>
-      <c r="M26" s="5">
+      <c r="L26" s="6">
+        <v>1</v>
+      </c>
+      <c r="M26" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27" s="5">
-        <v>1</v>
-      </c>
-      <c r="B27" s="5">
+      <c r="A27" s="6">
+        <v>1</v>
+      </c>
+      <c r="B27" s="6">
         <v>6</v>
       </c>
-      <c r="C27" s="5">
+      <c r="C27" s="6">
         <v>6</v>
       </c>
-      <c r="D27" s="5">
+      <c r="D27" s="6">
         <v>19</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="E27" s="6" t="s">
         <v>986</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="F27" s="6" t="s">
         <v>727</v>
       </c>
-      <c r="G27" s="5">
-        <v>1</v>
-      </c>
-      <c r="H27" s="5">
+      <c r="G27" s="6">
+        <v>1</v>
+      </c>
+      <c r="H27" s="6">
         <v>20190501</v>
       </c>
-      <c r="I27" s="5">
+      <c r="I27" s="6">
         <v>20190731</v>
       </c>
-      <c r="J27" s="5">
-        <v>1</v>
-      </c>
-      <c r="K27" s="11">
+      <c r="J27" s="6">
+        <v>1</v>
+      </c>
+      <c r="K27" s="7">
         <v>43586</v>
       </c>
-      <c r="L27" s="5">
-        <v>1</v>
-      </c>
-      <c r="M27" s="5">
+      <c r="L27" s="6">
+        <v>1</v>
+      </c>
+      <c r="M27" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A28" s="5">
-        <v>1</v>
-      </c>
-      <c r="B28" s="5">
+      <c r="A28" s="6">
+        <v>1</v>
+      </c>
+      <c r="B28" s="6">
         <v>6</v>
       </c>
-      <c r="C28" s="5">
+      <c r="C28" s="6">
         <v>6</v>
       </c>
-      <c r="D28" s="5">
+      <c r="D28" s="6">
         <v>20</v>
       </c>
-      <c r="E28" s="5" t="s">
+      <c r="E28" s="6" t="s">
         <v>987</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="F28" s="6" t="s">
         <v>727</v>
       </c>
-      <c r="G28" s="5">
-        <v>1</v>
-      </c>
-      <c r="H28" s="5">
+      <c r="G28" s="6">
+        <v>1</v>
+      </c>
+      <c r="H28" s="6">
         <v>20190501</v>
       </c>
-      <c r="I28" s="5">
+      <c r="I28" s="6">
         <v>20190731</v>
       </c>
-      <c r="J28" s="5">
-        <v>1</v>
-      </c>
-      <c r="K28" s="11">
+      <c r="J28" s="6">
+        <v>1</v>
+      </c>
+      <c r="K28" s="7">
         <v>43586</v>
       </c>
-      <c r="L28" s="5">
-        <v>1</v>
-      </c>
-      <c r="M28" s="5">
+      <c r="L28" s="6">
+        <v>1</v>
+      </c>
+      <c r="M28" s="6">
         <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A29" s="5">
-        <v>1</v>
-      </c>
-      <c r="B29" s="5">
+      <c r="A29" s="6">
+        <v>1</v>
+      </c>
+      <c r="B29" s="6">
         <v>6</v>
       </c>
-      <c r="C29" s="5">
+      <c r="C29" s="6">
         <v>6</v>
       </c>
-      <c r="D29" s="5">
+      <c r="D29" s="6">
         <v>21</v>
       </c>
-      <c r="E29" s="5" t="s">
+      <c r="E29" s="6" t="s">
         <v>988</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="F29" s="6" t="s">
         <v>727</v>
       </c>
-      <c r="G29" s="5">
-        <v>1</v>
-      </c>
-      <c r="H29" s="5">
+      <c r="G29" s="6">
+        <v>1</v>
+      </c>
+      <c r="H29" s="6">
         <v>20190501</v>
       </c>
-      <c r="I29" s="5">
+      <c r="I29" s="6">
         <v>20190731</v>
       </c>
-      <c r="J29" s="5">
-        <v>1</v>
-      </c>
-      <c r="K29" s="11">
+      <c r="J29" s="6">
+        <v>1</v>
+      </c>
+      <c r="K29" s="7">
         <v>43586</v>
       </c>
-      <c r="L29" s="5">
-        <v>1</v>
-      </c>
-      <c r="M29" s="5">
+      <c r="L29" s="6">
+        <v>1</v>
+      </c>
+      <c r="M29" s="6">
         <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A30" s="5">
-        <v>1</v>
-      </c>
-      <c r="B30" s="5">
+      <c r="A30" s="6">
+        <v>1</v>
+      </c>
+      <c r="B30" s="6">
         <v>6</v>
       </c>
-      <c r="C30" s="5">
+      <c r="C30" s="6">
         <v>6</v>
       </c>
-      <c r="D30" s="5">
+      <c r="D30" s="6">
         <v>22</v>
       </c>
-      <c r="E30" s="5" t="s">
+      <c r="E30" s="6" t="s">
         <v>989</v>
       </c>
-      <c r="F30" s="5" t="s">
+      <c r="F30" s="6" t="s">
         <v>727</v>
       </c>
-      <c r="G30" s="5">
-        <v>1</v>
-      </c>
-      <c r="H30" s="5">
+      <c r="G30" s="6">
+        <v>1</v>
+      </c>
+      <c r="H30" s="6">
         <v>20190501</v>
       </c>
-      <c r="I30" s="5">
+      <c r="I30" s="6">
         <v>20190731</v>
       </c>
-      <c r="J30" s="5">
-        <v>1</v>
-      </c>
-      <c r="K30" s="11">
+      <c r="J30" s="6">
+        <v>1</v>
+      </c>
+      <c r="K30" s="7">
         <v>43586</v>
       </c>
-      <c r="L30" s="5">
-        <v>1</v>
-      </c>
-      <c r="M30" s="5">
+      <c r="L30" s="6">
+        <v>1</v>
+      </c>
+      <c r="M30" s="6">
         <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A31" s="5">
-        <v>1</v>
-      </c>
-      <c r="B31" s="5">
+      <c r="A31" s="6">
+        <v>1</v>
+      </c>
+      <c r="B31" s="6">
         <v>6</v>
       </c>
-      <c r="C31" s="5">
+      <c r="C31" s="6">
         <v>6</v>
       </c>
-      <c r="D31" s="5">
+      <c r="D31" s="6">
         <v>23</v>
       </c>
-      <c r="E31" s="5" t="s">
+      <c r="E31" s="6" t="s">
         <v>990</v>
       </c>
-      <c r="F31" s="5" t="s">
+      <c r="F31" s="6" t="s">
         <v>727</v>
       </c>
-      <c r="G31" s="5">
-        <v>1</v>
-      </c>
-      <c r="H31" s="5">
+      <c r="G31" s="6">
+        <v>1</v>
+      </c>
+      <c r="H31" s="6">
         <v>20190501</v>
       </c>
-      <c r="I31" s="5">
+      <c r="I31" s="6">
         <v>20190731</v>
       </c>
-      <c r="J31" s="5">
-        <v>1</v>
-      </c>
-      <c r="K31" s="11">
+      <c r="J31" s="6">
+        <v>1</v>
+      </c>
+      <c r="K31" s="7">
         <v>43586</v>
       </c>
-      <c r="L31" s="5">
-        <v>1</v>
-      </c>
-      <c r="M31" s="5">
+      <c r="L31" s="6">
+        <v>1</v>
+      </c>
+      <c r="M31" s="6">
         <v>6</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A32" s="5">
-        <v>1</v>
-      </c>
-      <c r="B32" s="5">
+      <c r="A32" s="6">
+        <v>1</v>
+      </c>
+      <c r="B32" s="6">
         <v>6</v>
       </c>
-      <c r="C32" s="5">
+      <c r="C32" s="6">
         <v>6</v>
       </c>
-      <c r="D32" s="5">
+      <c r="D32" s="6">
         <v>24</v>
       </c>
-      <c r="E32" s="5" t="s">
+      <c r="E32" s="6" t="s">
         <v>991</v>
       </c>
-      <c r="F32" s="5" t="s">
+      <c r="F32" s="6" t="s">
         <v>727</v>
       </c>
-      <c r="G32" s="5">
-        <v>1</v>
-      </c>
-      <c r="H32" s="5">
+      <c r="G32" s="6">
+        <v>1</v>
+      </c>
+      <c r="H32" s="6">
         <v>20190501</v>
       </c>
-      <c r="I32" s="5">
+      <c r="I32" s="6">
         <v>20190731</v>
       </c>
-      <c r="J32" s="5">
-        <v>1</v>
-      </c>
-      <c r="K32" s="11">
+      <c r="J32" s="6">
+        <v>1</v>
+      </c>
+      <c r="K32" s="7">
         <v>43586</v>
       </c>
-      <c r="L32" s="5">
-        <v>1</v>
-      </c>
-      <c r="M32" s="5">
+      <c r="L32" s="6">
+        <v>1</v>
+      </c>
+      <c r="M32" s="6">
         <v>7</v>
       </c>
     </row>
@@ -34457,8 +34512,8 @@
       <c r="H1" t="s">
         <v>927</v>
       </c>
-      <c r="I1" s="5" t="s">
-        <v>1040</v>
+      <c r="I1" s="6" t="s">
+        <v>1039</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -34486,7 +34541,7 @@
       <c r="H2">
         <v>0</v>
       </c>
-      <c r="I2" s="5">
+      <c r="I2" s="6">
         <v>1</v>
       </c>
     </row>
@@ -34515,7 +34570,7 @@
       <c r="H3">
         <v>1</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3" s="6">
         <v>1</v>
       </c>
     </row>
@@ -34544,7 +34599,7 @@
       <c r="H4">
         <v>1</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="6">
         <v>0</v>
       </c>
     </row>
@@ -34573,7 +34628,7 @@
       <c r="H5">
         <v>1</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="6">
         <v>0</v>
       </c>
     </row>
@@ -34602,7 +34657,7 @@
       <c r="H6">
         <v>1</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="6">
         <v>0</v>
       </c>
     </row>
@@ -34631,7 +34686,7 @@
       <c r="H7">
         <v>0</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I7" s="6">
         <v>0</v>
       </c>
     </row>
@@ -34660,7 +34715,7 @@
       <c r="H8">
         <v>1</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="6">
         <v>0</v>
       </c>
     </row>
@@ -34689,7 +34744,7 @@
       <c r="H9">
         <v>0</v>
       </c>
-      <c r="I9" s="5">
+      <c r="I9" s="6">
         <v>0</v>
       </c>
     </row>
@@ -34718,7 +34773,7 @@
       <c r="H10">
         <v>1</v>
       </c>
-      <c r="I10" s="5">
+      <c r="I10" s="6">
         <v>0</v>
       </c>
     </row>
@@ -34747,7 +34802,7 @@
       <c r="H11">
         <v>1</v>
       </c>
-      <c r="I11" s="5">
+      <c r="I11" s="6">
         <v>0</v>
       </c>
     </row>
@@ -35361,11 +35416,11 @@
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="5">
+      <c r="A12" s="6">
         <v>10</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>1038</v>
+      <c r="B12" s="6" t="s">
+        <v>1037</v>
       </c>
     </row>
   </sheetData>
@@ -35726,31 +35781,34 @@
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.109375" customWidth="1"/>
     <col min="3" max="3" width="26.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>1017</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>1018</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>1019</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" s="5" t="s">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -35760,8 +35818,11 @@
       <c r="C2" t="s">
         <v>1021</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" s="5" t="s">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -35771,8 +35832,11 @@
       <c r="C3" t="s">
         <v>1023</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" s="5" t="s">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -35782,49 +35846,162 @@
       <c r="C4" t="s">
         <v>1025</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" s="5" t="s">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>1047</v>
+      </c>
+      <c r="C5" t="s">
         <v>1026</v>
       </c>
-      <c r="C5" t="s">
-        <v>1027</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5" s="5" t="s">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>1027</v>
+      </c>
+      <c r="C6" t="s">
         <v>1028</v>
       </c>
-      <c r="C6" t="s">
-        <v>1029</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" s="5" t="s">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C7" t="s">
         <v>1030</v>
       </c>
-      <c r="C7" t="s">
-        <v>1031</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7" s="5" t="s">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>1031</v>
+      </c>
+      <c r="C8" t="s">
         <v>1032</v>
       </c>
-      <c r="C8" t="s">
-        <v>1033</v>
+      <c r="D8" s="5" t="s">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="5">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>1048</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>1021</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="5">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>1050</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>1025</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="5">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>1051</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>1052</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="5">
+        <v>11</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>1053</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>1028</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="5">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>1054</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>1030</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="5">
+        <v>13</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>1055</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>1056</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="5">
+        <v>14</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>1057</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>1032</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>1049</v>
       </c>
     </row>
   </sheetData>
@@ -35837,7 +36014,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="B17" sqref="B17:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -35929,7 +36106,7 @@
       <c r="D5" t="s">
         <v>41</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="6">
         <v>1</v>
       </c>
     </row>
@@ -35946,7 +36123,7 @@
       <c r="D6" t="s">
         <v>44</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="6">
         <v>1</v>
       </c>
     </row>
@@ -35963,7 +36140,7 @@
       <c r="D7" t="s">
         <v>47</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="6">
         <v>1</v>
       </c>
     </row>
@@ -35980,7 +36157,7 @@
       <c r="D8" t="s">
         <v>50</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="6">
         <v>0</v>
       </c>
     </row>
@@ -35997,7 +36174,7 @@
       <c r="D9" t="s">
         <v>53</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="6">
         <v>1</v>
       </c>
     </row>
@@ -36014,7 +36191,7 @@
       <c r="D10" t="s">
         <v>55</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="6">
         <v>0</v>
       </c>
     </row>
@@ -36031,7 +36208,7 @@
       <c r="D11" t="s">
         <v>57</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="6">
         <v>1</v>
       </c>
     </row>
@@ -36048,7 +36225,7 @@
       <c r="D12" t="s">
         <v>60</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="6">
         <v>1</v>
       </c>
     </row>
@@ -36065,7 +36242,7 @@
       <c r="D13" t="s">
         <v>63</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="6">
         <v>0</v>
       </c>
     </row>
@@ -36082,7 +36259,7 @@
       <c r="D14" t="s">
         <v>66</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="6">
         <v>1</v>
       </c>
     </row>
@@ -36099,7 +36276,7 @@
       <c r="D15" t="s">
         <v>68</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="6">
         <v>0</v>
       </c>
     </row>
@@ -36116,7 +36293,7 @@
       <c r="D16" t="s">
         <v>71</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="6">
         <v>1</v>
       </c>
     </row>
@@ -36124,16 +36301,16 @@
       <c r="A17">
         <v>15</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="6" t="s">
+        <v>1042</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" s="6" t="s">
         <v>1043</v>
       </c>
-      <c r="C17" t="s">
-        <v>65</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>1044</v>
-      </c>
-      <c r="E17">
+      <c r="E17" s="6">
         <v>1</v>
       </c>
     </row>
@@ -36150,7 +36327,7 @@
       <c r="D18" t="s">
         <v>74</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="6">
         <v>1</v>
       </c>
     </row>
@@ -36167,7 +36344,7 @@
       <c r="D19" t="s">
         <v>76</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E19" s="6">
         <v>0</v>
       </c>
     </row>
@@ -36184,7 +36361,7 @@
       <c r="D20" t="s">
         <v>78</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="6">
         <v>1</v>
       </c>
     </row>
@@ -36709,7 +36886,7 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
   </sheetData>
@@ -38752,7 +38929,7 @@
         <v>251</v>
       </c>
       <c r="B253" s="6" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.3">
@@ -38760,7 +38937,7 @@
         <v>252</v>
       </c>
       <c r="B254" s="5" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TFS 15465 - Additional changes to support wild card.
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C43629
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="132" windowWidth="22992" windowHeight="12840" firstSheet="26" activeTab="30"/>
+    <workbookView xWindow="480" yWindow="132" windowWidth="22992" windowHeight="12840"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_History" sheetId="14" r:id="rId1"/>
@@ -42,7 +42,7 @@
     <sheet name="ShortCalls_Behavior" sheetId="29" r:id="rId28"/>
     <sheet name="ShortCalls_Actions" sheetId="30" r:id="rId29"/>
     <sheet name="ShortCalls_BAL" sheetId="31" r:id="rId30"/>
-    <sheet name="Quality_Now_Bingo_Images" sheetId="32" r:id="rId31"/>
+    <sheet name="Bingo_Images" sheetId="32" r:id="rId31"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">Coaching_Reason_Selection!$A$1:$P$313</definedName>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3723" uniqueCount="1058">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3731" uniqueCount="1062">
   <si>
     <t>SourceID</t>
   </si>
@@ -3189,9 +3189,6 @@
     <t>FL - Tampa</t>
   </si>
   <si>
-    <t>New column and records to Quality_Now_Bingo_Images tab</t>
-  </si>
-  <si>
     <t>BingoType</t>
   </si>
   <si>
@@ -3229,6 +3226,21 @@
   </si>
   <si>
     <t>&lt;img border="20" src="cid:so_qm.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img border="20" src="cid:wc.png"&gt;</t>
+  </si>
+  <si>
+    <t>Wild Card</t>
+  </si>
+  <si>
+    <t>&lt;img border="20" src="cid:wc_qm.png"&gt;</t>
+  </si>
+  <si>
+    <t>New column and records to Bingo_Images tab</t>
+  </si>
+  <si>
+    <t>Added 2 new rows to Bingo_Images tab</t>
   </si>
 </sst>
 </file>
@@ -3615,10 +3627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L91"/>
+  <dimension ref="A1:L92"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="A91" sqref="A91:E91"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="A92" sqref="A92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5147,20 +5159,37 @@
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A91" s="5">
+      <c r="A91" s="8">
         <v>81</v>
       </c>
-      <c r="B91" s="11">
+      <c r="B91" s="9">
         <v>43731</v>
       </c>
-      <c r="C91" s="5" t="s">
+      <c r="C91" s="8" t="s">
         <v>429</v>
       </c>
-      <c r="D91" s="5">
+      <c r="D91" s="8">
         <v>15465</v>
       </c>
-      <c r="E91" s="5" t="s">
-        <v>1044</v>
+      <c r="E91" s="8" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A92" s="5">
+        <v>82</v>
+      </c>
+      <c r="B92" s="11">
+        <v>43739</v>
+      </c>
+      <c r="C92" s="5" t="s">
+        <v>429</v>
+      </c>
+      <c r="D92" s="5">
+        <v>15465</v>
+      </c>
+      <c r="E92" s="5" t="s">
+        <v>1061</v>
       </c>
     </row>
   </sheetData>
@@ -35781,10 +35810,10 @@
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -35804,8 +35833,8 @@
       <c r="C1" s="6" t="s">
         <v>1019</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>1045</v>
+      <c r="D1" s="6" t="s">
+        <v>1044</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -35818,8 +35847,8 @@
       <c r="C2" t="s">
         <v>1021</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>1046</v>
+      <c r="D2" s="6" t="s">
+        <v>1045</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -35832,8 +35861,8 @@
       <c r="C3" t="s">
         <v>1023</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>1046</v>
+      <c r="D3" s="6" t="s">
+        <v>1045</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -35846,8 +35875,8 @@
       <c r="C4" t="s">
         <v>1025</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>1046</v>
+      <c r="D4" s="6" t="s">
+        <v>1045</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -35855,13 +35884,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="C5" t="s">
         <v>1026</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>1046</v>
+      <c r="D5" s="6" t="s">
+        <v>1045</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -35874,8 +35903,8 @@
       <c r="C6" t="s">
         <v>1028</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>1046</v>
+      <c r="D6" s="6" t="s">
+        <v>1045</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -35888,8 +35917,8 @@
       <c r="C7" t="s">
         <v>1030</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>1046</v>
+      <c r="D7" s="6" t="s">
+        <v>1045</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -35902,106 +35931,134 @@
       <c r="C8" t="s">
         <v>1032</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="5">
+      <c r="D8" s="6" t="s">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="6">
         <v>8</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="6" t="s">
+        <v>1047</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>1021</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>1048</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>1021</v>
-      </c>
-      <c r="D9" s="5" t="s">
+    </row>
+    <row r="10" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="6">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>1049</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="5">
-        <v>9</v>
-      </c>
-      <c r="B10" s="5" t="s">
+      <c r="C10" s="6" t="s">
+        <v>1025</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="6">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>1050</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>1025</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>1049</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="5">
-        <v>10</v>
-      </c>
-      <c r="B11" s="5" t="s">
+      <c r="C11" s="6" t="s">
         <v>1051</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="D11" s="6" t="s">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="6">
+        <v>11</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>1052</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>1049</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="5">
-        <v>11</v>
-      </c>
-      <c r="B12" s="5" t="s">
+      <c r="C12" s="6" t="s">
+        <v>1028</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="6">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>1053</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>1028</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>1049</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="5">
-        <v>12</v>
-      </c>
-      <c r="B13" s="5" t="s">
+      <c r="C13" s="6" t="s">
+        <v>1030</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="6">
+        <v>13</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>1054</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>1030</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>1049</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="5">
-        <v>13</v>
-      </c>
-      <c r="B14" s="5" t="s">
+      <c r="C14" s="6" t="s">
         <v>1055</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="D14" s="6" t="s">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="6">
+        <v>14</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>1056</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>1049</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="5">
-        <v>14</v>
-      </c>
-      <c r="B15" s="5" t="s">
+      <c r="C15" s="6" t="s">
+        <v>1032</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="5">
+        <v>15</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>1057</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>1032</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>1049</v>
+      <c r="C16" s="5" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="5">
+        <v>16</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>1059</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>1048</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TFS 15859 - Added WPOP12 to ARC Role
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C43842
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="132" windowWidth="22992" windowHeight="12840"/>
+    <workbookView xWindow="480" yWindow="132" windowWidth="22992" windowHeight="12840" firstSheet="19" activeTab="23"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_History" sheetId="14" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3731" uniqueCount="1062">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3733" uniqueCount="1063">
   <si>
     <t>SourceID</t>
   </si>
@@ -2895,9 +2895,6 @@
     <t>WACS0% and No ARC Role in ACL</t>
   </si>
   <si>
-    <t>WACS0% and ARC Role in ACL</t>
-  </si>
-  <si>
     <t>SRM in ACL</t>
   </si>
   <si>
@@ -3241,6 +3238,12 @@
   </si>
   <si>
     <t>Added 2 new rows to Bingo_Images tab</t>
+  </si>
+  <si>
+    <t>(WACS0% OR WPOP12) and ARC Role in ACL</t>
+  </si>
+  <si>
+    <t>Add WPOP12 job code to ARC Role. Update ARC Role description in UI_User_Role</t>
   </si>
 </sst>
 </file>
@@ -3627,10 +3630,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L92"/>
+  <dimension ref="A1:L93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="A92" sqref="A92"/>
+    <sheetView topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="E93" sqref="E93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4808,7 +4811,7 @@
         <v>7137</v>
       </c>
       <c r="E70" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.3">
@@ -4825,7 +4828,7 @@
         <v>11500</v>
       </c>
       <c r="E71" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.3">
@@ -4842,7 +4845,7 @@
         <v>11451</v>
       </c>
       <c r="E72" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.3">
@@ -4859,7 +4862,7 @@
         <v>12308</v>
       </c>
       <c r="E73" s="8" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.3">
@@ -4876,7 +4879,7 @@
         <v>12308</v>
       </c>
       <c r="E74" s="8" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="75" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -4893,7 +4896,7 @@
         <v>12316</v>
       </c>
       <c r="E75" s="6" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="76" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -4910,7 +4913,7 @@
         <v>12455</v>
       </c>
       <c r="E76" s="6" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="F76" s="6"/>
       <c r="G76" s="10"/>
@@ -4934,7 +4937,7 @@
         <v>12467</v>
       </c>
       <c r="E77" s="6" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
     <row r="78" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -4951,7 +4954,7 @@
         <v>12591</v>
       </c>
       <c r="E78" s="8" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
     </row>
     <row r="79" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -4968,7 +4971,7 @@
         <v>12591</v>
       </c>
       <c r="E79" s="8" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.3">
@@ -4985,7 +4988,7 @@
         <v>13334</v>
       </c>
       <c r="E80" s="6" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
@@ -5002,7 +5005,7 @@
         <v>13643</v>
       </c>
       <c r="E81" s="6" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="82" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -5019,7 +5022,7 @@
         <v>13332</v>
       </c>
       <c r="E82" s="8" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
     </row>
     <row r="83" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -5036,7 +5039,7 @@
         <v>14178</v>
       </c>
       <c r="E83" s="8" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="84" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -5053,7 +5056,7 @@
         <v>14108</v>
       </c>
       <c r="E84" s="6" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
@@ -5070,7 +5073,7 @@
         <v>15063</v>
       </c>
       <c r="E85" s="6" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
@@ -5087,7 +5090,7 @@
         <v>15144</v>
       </c>
       <c r="E86" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
@@ -5104,7 +5107,7 @@
         <v>15095</v>
       </c>
       <c r="E87" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="88" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -5121,7 +5124,7 @@
         <v>13644</v>
       </c>
       <c r="E88" s="6" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
@@ -5138,7 +5141,7 @@
         <v>15621</v>
       </c>
       <c r="E89" s="8" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
@@ -5155,7 +5158,7 @@
         <v>15450</v>
       </c>
       <c r="E90" s="12" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
@@ -5172,24 +5175,41 @@
         <v>15465</v>
       </c>
       <c r="E91" s="8" t="s">
+        <v>1059</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="6">
+        <v>82</v>
+      </c>
+      <c r="B92" s="10">
+        <v>43739</v>
+      </c>
+      <c r="C92" s="6" t="s">
+        <v>429</v>
+      </c>
+      <c r="D92" s="6">
+        <v>15465</v>
+      </c>
+      <c r="E92" s="6" t="s">
         <v>1060</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A92" s="5">
-        <v>82</v>
-      </c>
-      <c r="B92" s="11">
-        <v>43739</v>
-      </c>
-      <c r="C92" s="5" t="s">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A93" s="5">
+        <v>83</v>
+      </c>
+      <c r="B93" s="11">
+        <v>43766</v>
+      </c>
+      <c r="C93" s="5" t="s">
         <v>429</v>
       </c>
-      <c r="D92" s="5">
-        <v>15465</v>
-      </c>
-      <c r="E92" s="5" t="s">
-        <v>1061</v>
+      <c r="D93" s="5">
+        <v>15859</v>
+      </c>
+      <c r="E93" s="5" t="s">
+        <v>1062</v>
       </c>
     </row>
   </sheetData>
@@ -6544,10 +6564,10 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="6" t="s">
+        <v>965</v>
+      </c>
+      <c r="B59" s="6" t="s">
         <v>966</v>
-      </c>
-      <c r="B59" s="6" t="s">
-        <v>967</v>
       </c>
       <c r="C59" s="6">
         <v>1</v>
@@ -6592,7 +6612,7 @@
         <v>172</v>
       </c>
       <c r="D1" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -6614,7 +6634,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -6744,7 +6764,7 @@
         <v>251</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="E2" s="5">
         <v>1</v>
@@ -7044,7 +7064,7 @@
         <v>251</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="E8" s="5">
         <v>1</v>
@@ -7344,7 +7364,7 @@
         <v>251</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="E14" s="5">
         <v>1</v>
@@ -21794,7 +21814,7 @@
         <v>245</v>
       </c>
       <c r="D303" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="E303">
         <v>0</v>
@@ -21844,7 +21864,7 @@
         <v>246</v>
       </c>
       <c r="D304" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="E304">
         <v>1</v>
@@ -21894,7 +21914,7 @@
         <v>247</v>
       </c>
       <c r="D305" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="E305">
         <v>1</v>
@@ -21944,7 +21964,7 @@
         <v>248</v>
       </c>
       <c r="D306" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="E306">
         <v>1</v>
@@ -21994,7 +22014,7 @@
         <v>246</v>
       </c>
       <c r="D307" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="E307">
         <v>1</v>
@@ -22044,7 +22064,7 @@
         <v>247</v>
       </c>
       <c r="D308" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="E308">
         <v>1</v>
@@ -22094,7 +22114,7 @@
         <v>248</v>
       </c>
       <c r="D309" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="E309">
         <v>1</v>
@@ -22144,7 +22164,7 @@
         <v>246</v>
       </c>
       <c r="D310" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="E310">
         <v>1</v>
@@ -22194,7 +22214,7 @@
         <v>247</v>
       </c>
       <c r="D311" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="E311">
         <v>1</v>
@@ -22244,7 +22264,7 @@
         <v>248</v>
       </c>
       <c r="D312" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="E312">
         <v>1</v>
@@ -22294,7 +22314,7 @@
         <v>249</v>
       </c>
       <c r="D313" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="E313">
         <v>1</v>
@@ -22338,7 +22358,7 @@
         <v>59</v>
       </c>
       <c r="B314" s="6" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="C314" s="6">
         <v>42</v>
@@ -28641,7 +28661,7 @@
         <v>3</v>
       </c>
       <c r="D175" s="6" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="E175" s="6">
         <v>0</v>
@@ -29471,7 +29491,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="C8" s="6">
         <v>98</v>
@@ -29817,7 +29837,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="C20" s="6">
         <v>1</v>
@@ -29831,7 +29851,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="C21" s="6">
         <v>1</v>
@@ -29845,7 +29865,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="C22" s="6">
         <v>1</v>
@@ -29859,7 +29879,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="C23" s="6">
         <v>1</v>
@@ -29873,7 +29893,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="C24" s="6">
         <v>1</v>
@@ -29887,7 +29907,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="C25" s="6">
         <v>1</v>
@@ -29901,7 +29921,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="C26" s="6">
         <v>1</v>
@@ -30980,7 +31000,7 @@
         <v>5</v>
       </c>
       <c r="C37" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -31009,7 +31029,7 @@
         <v>5</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="D38" s="6">
         <v>1</v>
@@ -31038,7 +31058,7 @@
         <v>5</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="D39" s="6">
         <v>1</v>
@@ -32024,7 +32044,7 @@
         <v>3</v>
       </c>
       <c r="C73" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="D73">
         <v>1</v>
@@ -32053,7 +32073,7 @@
         <v>3</v>
       </c>
       <c r="C74" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="D74">
         <v>1</v>
@@ -32082,7 +32102,7 @@
         <v>3</v>
       </c>
       <c r="C75" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="D75">
         <v>1</v>
@@ -33160,7 +33180,7 @@
         <v>18</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="F26" s="6" t="s">
         <v>727</v>
@@ -33201,7 +33221,7 @@
         <v>19</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>727</v>
@@ -33242,7 +33262,7 @@
         <v>20</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="F28" s="6" t="s">
         <v>727</v>
@@ -33283,7 +33303,7 @@
         <v>21</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="F29" s="6" t="s">
         <v>727</v>
@@ -33324,7 +33344,7 @@
         <v>22</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="F30" s="6" t="s">
         <v>727</v>
@@ -33365,7 +33385,7 @@
         <v>23</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="F31" s="6" t="s">
         <v>727</v>
@@ -33406,7 +33426,7 @@
         <v>24</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="F32" s="6" t="s">
         <v>727</v>
@@ -34153,7 +34173,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -34185,14 +34207,14 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="A3" s="5">
         <v>102</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C3" t="s">
-        <v>946</v>
+      <c r="C3" s="5" t="s">
+        <v>1061</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -34203,7 +34225,7 @@
         <v>174</v>
       </c>
       <c r="C4" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -34214,7 +34236,7 @@
         <v>378</v>
       </c>
       <c r="C5" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -34225,7 +34247,7 @@
         <v>915</v>
       </c>
       <c r="C6" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -34236,7 +34258,7 @@
         <v>916</v>
       </c>
       <c r="C7" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -34247,7 +34269,7 @@
         <v>422</v>
       </c>
       <c r="C8" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -34258,7 +34280,7 @@
         <v>917</v>
       </c>
       <c r="C9" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -34269,7 +34291,7 @@
         <v>918</v>
       </c>
       <c r="C10" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -34277,10 +34299,10 @@
         <v>110</v>
       </c>
       <c r="B11" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="C11" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
     </row>
   </sheetData>
@@ -34479,7 +34501,7 @@
         <v>110</v>
       </c>
       <c r="B11" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -34542,7 +34564,7 @@
         <v>927</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -34811,7 +34833,7 @@
         <v>110</v>
       </c>
       <c r="B11" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -35074,10 +35096,10 @@
         <v>502</v>
       </c>
       <c r="C1" t="s">
+        <v>992</v>
+      </c>
+      <c r="D1" t="s">
         <v>993</v>
-      </c>
-      <c r="D1" t="s">
-        <v>994</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -35085,7 +35107,7 @@
         <v>101</v>
       </c>
       <c r="B2" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -35099,7 +35121,7 @@
         <v>102</v>
       </c>
       <c r="B3" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -35113,7 +35135,7 @@
         <v>103</v>
       </c>
       <c r="B4" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -35127,7 +35149,7 @@
         <v>104</v>
       </c>
       <c r="B5" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -35141,7 +35163,7 @@
         <v>105</v>
       </c>
       <c r="B6" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -35155,7 +35177,7 @@
         <v>106</v>
       </c>
       <c r="B7" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -35169,7 +35191,7 @@
         <v>107</v>
       </c>
       <c r="B8" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -35183,7 +35205,7 @@
         <v>108</v>
       </c>
       <c r="B9" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -35197,7 +35219,7 @@
         <v>109</v>
       </c>
       <c r="B10" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -35211,7 +35233,7 @@
         <v>110</v>
       </c>
       <c r="B11" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -35225,7 +35247,7 @@
         <v>111</v>
       </c>
       <c r="B12" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -35254,10 +35276,10 @@
         <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="C1" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -35265,7 +35287,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -35276,7 +35298,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -35287,7 +35309,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -35298,7 +35320,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -35309,7 +35331,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -35320,7 +35342,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -35331,7 +35353,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -35449,7 +35471,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
   </sheetData>
@@ -35469,16 +35491,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>1013</v>
+      </c>
+      <c r="B1" t="s">
         <v>1014</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1015</v>
       </c>
       <c r="C1" t="s">
         <v>731</v>
       </c>
       <c r="D1" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -35825,16 +35847,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
+        <v>1016</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>1017</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
         <v>1018</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>1019</v>
-      </c>
       <c r="D1" s="6" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -35842,13 +35864,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>1019</v>
+      </c>
+      <c r="C2" t="s">
         <v>1020</v>
       </c>
-      <c r="C2" t="s">
-        <v>1021</v>
-      </c>
       <c r="D2" s="6" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -35856,13 +35878,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>1021</v>
+      </c>
+      <c r="C3" t="s">
         <v>1022</v>
       </c>
-      <c r="C3" t="s">
-        <v>1023</v>
-      </c>
       <c r="D3" s="6" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -35870,13 +35892,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>1023</v>
+      </c>
+      <c r="C4" t="s">
         <v>1024</v>
       </c>
-      <c r="C4" t="s">
-        <v>1025</v>
-      </c>
       <c r="D4" s="6" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -35884,13 +35906,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="C5" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -35898,13 +35920,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>1026</v>
+      </c>
+      <c r="C6" t="s">
         <v>1027</v>
       </c>
-      <c r="C6" t="s">
-        <v>1028</v>
-      </c>
       <c r="D6" s="6" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -35912,13 +35934,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>1028</v>
+      </c>
+      <c r="C7" t="s">
         <v>1029</v>
       </c>
-      <c r="C7" t="s">
-        <v>1030</v>
-      </c>
       <c r="D7" s="6" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -35926,13 +35948,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>1030</v>
+      </c>
+      <c r="C8" t="s">
         <v>1031</v>
       </c>
-      <c r="C8" t="s">
-        <v>1032</v>
-      </c>
       <c r="D8" s="6" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -35940,13 +35962,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>1046</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>1020</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>1047</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>1021</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>1048</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -35954,13 +35976,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -35968,13 +35990,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>1049</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>1050</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>1051</v>
-      </c>
       <c r="D11" s="6" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -35982,13 +36004,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -35996,13 +36018,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -36010,13 +36032,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
+        <v>1053</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>1054</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>1055</v>
-      </c>
       <c r="D14" s="6" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -36024,13 +36046,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -36038,13 +36060,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
+        <v>1056</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>1057</v>
       </c>
-      <c r="C16" s="5" t="s">
-        <v>1058</v>
-      </c>
       <c r="D16" s="5" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -36052,13 +36074,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
   </sheetData>
@@ -36359,13 +36381,13 @@
         <v>15</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>65</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="E17" s="6">
         <v>1</v>
@@ -36927,7 +36949,7 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
@@ -36935,7 +36957,7 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
@@ -36943,7 +36965,7 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
   </sheetData>
@@ -38938,7 +38960,7 @@
         <v>245</v>
       </c>
       <c r="B247" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.3">
@@ -38946,7 +38968,7 @@
         <v>246</v>
       </c>
       <c r="B248" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.3">
@@ -38954,7 +38976,7 @@
         <v>247</v>
       </c>
       <c r="B249" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.3">
@@ -38962,7 +38984,7 @@
         <v>248</v>
       </c>
       <c r="B250" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.3">
@@ -38970,7 +38992,7 @@
         <v>249</v>
       </c>
       <c r="B251" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.3">
@@ -38978,7 +39000,7 @@
         <v>250</v>
       </c>
       <c r="B252" s="6" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.3">
@@ -38986,7 +39008,7 @@
         <v>251</v>
       </c>
       <c r="B253" s="6" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.3">
@@ -38994,7 +39016,7 @@
         <v>252</v>
       </c>
       <c r="B254" s="5" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TFS 15989 - change to London surveys
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C43932
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="132" windowWidth="22992" windowHeight="12840" firstSheet="19" activeTab="23"/>
+    <workbookView xWindow="480" yWindow="132" windowWidth="22992" windowHeight="12840"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_History" sheetId="14" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3733" uniqueCount="1063">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3735" uniqueCount="1064">
   <si>
     <t>SourceID</t>
   </si>
@@ -3244,6 +3244,9 @@
   </si>
   <si>
     <t>Add WPOP12 job code to ARC Role. Update ARC Role description in UI_User_Role</t>
+  </si>
+  <si>
+    <t>Change to London surveys. Updated Survey_Sites and Survey_DIM_Question tabs</t>
   </si>
 </sst>
 </file>
@@ -3308,7 +3311,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -3326,6 +3329,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3630,10 +3634,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L93"/>
+  <dimension ref="A1:L94"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="E93" sqref="E93"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="A94" sqref="A94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5196,20 +5200,37 @@
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A93" s="5">
+      <c r="A93" s="8">
         <v>83</v>
       </c>
-      <c r="B93" s="11">
+      <c r="B93" s="9">
         <v>43766</v>
       </c>
-      <c r="C93" s="5" t="s">
+      <c r="C93" s="8" t="s">
         <v>429</v>
       </c>
-      <c r="D93" s="5">
+      <c r="D93" s="8">
         <v>15859</v>
       </c>
-      <c r="E93" s="5" t="s">
+      <c r="E93" s="8" t="s">
         <v>1062</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A94" s="5">
+        <v>84</v>
+      </c>
+      <c r="B94" s="11">
+        <v>43774</v>
+      </c>
+      <c r="C94" s="5" t="s">
+        <v>429</v>
+      </c>
+      <c r="D94" s="5">
+        <v>15989</v>
+      </c>
+      <c r="E94" s="5" t="s">
+        <v>1063</v>
       </c>
     </row>
   </sheetData>
@@ -29270,7 +29291,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:I9"/>
+      <selection activeCell="I8" sqref="A8:I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -29487,31 +29508,31 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="6">
+      <c r="A8" s="5">
         <v>6</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>983</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="5">
         <v>98</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="5">
         <v>20190501</v>
       </c>
-      <c r="E8" s="6">
-        <v>20190731</v>
-      </c>
-      <c r="F8" s="6">
-        <v>1</v>
-      </c>
-      <c r="G8" s="6">
-        <v>1</v>
-      </c>
-      <c r="H8" s="7">
+      <c r="E8" s="5">
+        <v>20191031</v>
+      </c>
+      <c r="F8" s="5">
+        <v>1</v>
+      </c>
+      <c r="G8" s="5">
+        <v>0</v>
+      </c>
+      <c r="H8" s="13">
         <v>43577.559065011577</v>
       </c>
-      <c r="I8" s="6">
+      <c r="I8" s="5">
         <v>1</v>
       </c>
     </row>
@@ -29555,7 +29576,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:D26"/>
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -33463,7 +33484,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:E11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -33638,19 +33661,19 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11">
+      <c r="A11" s="5">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11">
+      <c r="C11" s="5">
+        <v>1</v>
+      </c>
+      <c r="D11" s="5">
+        <v>0</v>
+      </c>
+      <c r="E11" s="5">
         <v>0</v>
       </c>
     </row>
@@ -34173,8 +34196,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -34207,13 +34230,13 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="5">
+      <c r="A3" s="8">
         <v>102</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="8" t="s">
         <v>1061</v>
       </c>
     </row>

</xml_diff>

<commit_message>
TFS 15989 - change to London surveys. Additional update from V&V.
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C43935
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="132" windowWidth="22992" windowHeight="12840"/>
+    <workbookView xWindow="480" yWindow="132" windowWidth="22992" windowHeight="12840" firstSheet="17" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_History" sheetId="14" r:id="rId1"/>
@@ -3636,7 +3636,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+    <sheetView topLeftCell="A85" workbookViewId="0">
       <selection activeCell="A94" sqref="A94"/>
     </sheetView>
   </sheetViews>
@@ -33484,9 +33484,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:E11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -33559,19 +33557,19 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="A5" s="5">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
+      <c r="C5" s="5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5">
         <v>0</v>
       </c>
     </row>
@@ -33610,19 +33608,19 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="A8" s="5">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
+      <c r="C8" s="5">
+        <v>0</v>
+      </c>
+      <c r="D8" s="5">
+        <v>0</v>
+      </c>
+      <c r="E8" s="5">
         <v>0</v>
       </c>
     </row>
@@ -33797,19 +33795,19 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19">
+      <c r="A19" s="5">
         <v>17</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
+      <c r="C19" s="5">
+        <v>0</v>
+      </c>
+      <c r="D19" s="5">
+        <v>0</v>
+      </c>
+      <c r="E19" s="5">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
TFS 16389 - Historical dashboard access to amy job code WPSM%
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C44394
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="132" windowWidth="22992" windowHeight="12840"/>
+    <workbookView xWindow="480" yWindow="132" windowWidth="22992" windowHeight="12840" firstSheet="19" activeTab="23"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_History" sheetId="14" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3893" uniqueCount="1085">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3895" uniqueCount="1086">
   <si>
     <t>SourceID</t>
   </si>
@@ -2960,9 +2960,6 @@
   </si>
   <si>
     <t>Assign Manager Role to WPPM job codes . Updated RoleDescription in UI_User_Role tab for Analyst and Manager roles.</t>
-  </si>
-  <si>
-    <t>%50 or %60 or %70 or WEEX% or WISO% or WISY% or WPWL% or WSTE% or WPPM%</t>
   </si>
   <si>
     <t>Added new source 'Quality Alignment' in DIM_Source tab and new record in Email Notification tab for Quality Module and Quality Alignment source</t>
@@ -3339,6 +3336,12 @@
   </si>
   <si>
     <t>WPOP12</t>
+  </si>
+  <si>
+    <t>Add WPSM% job code to Manager Role. Update Mgr Role descriptions in UI_User_Role</t>
+  </si>
+  <si>
+    <t>%50 or %60 or %70 or WEEX% or WISO% or WISY% or WPWL% or WSTE% or WPPM% or WPSM%</t>
   </si>
 </sst>
 </file>
@@ -3403,7 +3406,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -3422,6 +3425,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3726,10 +3732,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L97"/>
+  <dimension ref="A1:L98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="A97" sqref="A97"/>
+    <sheetView topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="E98" sqref="E98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5050,7 +5056,7 @@
         <v>12591</v>
       </c>
       <c r="E78" s="8" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
     </row>
     <row r="79" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -5067,7 +5073,7 @@
         <v>12591</v>
       </c>
       <c r="E79" s="8" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.3">
@@ -5084,7 +5090,7 @@
         <v>13334</v>
       </c>
       <c r="E80" s="6" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
@@ -5101,7 +5107,7 @@
         <v>13643</v>
       </c>
       <c r="E81" s="6" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="82" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -5118,7 +5124,7 @@
         <v>13332</v>
       </c>
       <c r="E82" s="8" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="83" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -5135,7 +5141,7 @@
         <v>14178</v>
       </c>
       <c r="E83" s="8" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="84" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -5152,7 +5158,7 @@
         <v>14108</v>
       </c>
       <c r="E84" s="6" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
@@ -5169,7 +5175,7 @@
         <v>15063</v>
       </c>
       <c r="E85" s="6" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
@@ -5186,7 +5192,7 @@
         <v>15144</v>
       </c>
       <c r="E86" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
@@ -5203,7 +5209,7 @@
         <v>15095</v>
       </c>
       <c r="E87" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="88" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -5220,7 +5226,7 @@
         <v>13644</v>
       </c>
       <c r="E88" s="6" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
@@ -5237,7 +5243,7 @@
         <v>15621</v>
       </c>
       <c r="E89" s="8" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
@@ -5254,7 +5260,7 @@
         <v>15450</v>
       </c>
       <c r="E90" s="12" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
@@ -5271,7 +5277,7 @@
         <v>15465</v>
       </c>
       <c r="E91" s="8" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="92" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -5288,7 +5294,7 @@
         <v>15465</v>
       </c>
       <c r="E92" s="6" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.3">
@@ -5305,7 +5311,7 @@
         <v>15859</v>
       </c>
       <c r="E93" s="8" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
@@ -5322,7 +5328,7 @@
         <v>15989</v>
       </c>
       <c r="E94" s="8" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="95" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -5339,7 +5345,7 @@
         <v>15803</v>
       </c>
       <c r="E95" s="8" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="96" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -5356,25 +5362,43 @@
         <v>15803</v>
       </c>
       <c r="E96" s="8" t="s">
-        <v>1077</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A97" s="5">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="8">
         <v>86</v>
       </c>
-      <c r="B97" s="11">
+      <c r="B97" s="9">
         <v>43811</v>
       </c>
-      <c r="C97" s="5" t="s">
+      <c r="C97" s="8" t="s">
         <v>429</v>
       </c>
-      <c r="D97" s="5">
+      <c r="D97" s="8">
         <v>16261</v>
       </c>
-      <c r="E97" s="5" t="s">
-        <v>1082</v>
-      </c>
+      <c r="E97" s="8" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A98" s="5">
+        <v>87</v>
+      </c>
+      <c r="B98" s="11">
+        <v>43844</v>
+      </c>
+      <c r="C98" s="5" t="s">
+        <v>429</v>
+      </c>
+      <c r="D98" s="5">
+        <v>16389</v>
+      </c>
+      <c r="E98" s="5" t="s">
+        <v>1084</v>
+      </c>
+      <c r="F98" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6751,7 +6775,7 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="B60" s="5" t="s">
         <v>963</v>
@@ -6799,7 +6823,7 @@
         <v>172</v>
       </c>
       <c r="D1" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -6821,7 +6845,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -6952,7 +6976,7 @@
         <v>251</v>
       </c>
       <c r="D2" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -7252,7 +7276,7 @@
         <v>251</v>
       </c>
       <c r="D8" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -7552,7 +7576,7 @@
         <v>251</v>
       </c>
       <c r="D14" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -15696,7 +15720,7 @@
         <v>59</v>
       </c>
       <c r="B177" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="C177">
         <v>42</v>
@@ -15852,7 +15876,7 @@
         <v>253</v>
       </c>
       <c r="D180" s="8" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="E180" s="8">
         <v>1</v>
@@ -15902,7 +15926,7 @@
         <v>254</v>
       </c>
       <c r="D181" s="8" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="E181" s="8">
         <v>1</v>
@@ -15952,7 +15976,7 @@
         <v>255</v>
       </c>
       <c r="D182" s="8" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="E182" s="8">
         <v>1</v>
@@ -16002,7 +16026,7 @@
         <v>256</v>
       </c>
       <c r="D183" s="8" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="E183" s="8">
         <v>1</v>
@@ -16052,7 +16076,7 @@
         <v>257</v>
       </c>
       <c r="D184" s="8" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="E184" s="8">
         <v>1</v>
@@ -16102,7 +16126,7 @@
         <v>258</v>
       </c>
       <c r="D185" s="8" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="E185" s="8">
         <v>1</v>
@@ -16152,7 +16176,7 @@
         <v>259</v>
       </c>
       <c r="D186" s="8" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="E186" s="8">
         <v>1</v>
@@ -16202,7 +16226,7 @@
         <v>260</v>
       </c>
       <c r="D187" s="8" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="E187" s="8">
         <v>1</v>
@@ -16252,7 +16276,7 @@
         <v>261</v>
       </c>
       <c r="D188" s="8" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="E188" s="8">
         <v>1</v>
@@ -16302,7 +16326,7 @@
         <v>262</v>
       </c>
       <c r="D189" s="8" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="E189" s="8">
         <v>1</v>
@@ -16352,7 +16376,7 @@
         <v>263</v>
       </c>
       <c r="D190" s="8" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="E190" s="8">
         <v>1</v>
@@ -16452,7 +16476,7 @@
         <v>265</v>
       </c>
       <c r="D192" s="8" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="E192" s="8">
         <v>1</v>
@@ -16602,7 +16626,7 @@
         <v>253</v>
       </c>
       <c r="D195" s="8" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="E195" s="8">
         <v>1</v>
@@ -16652,7 +16676,7 @@
         <v>254</v>
       </c>
       <c r="D196" s="8" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="E196" s="8">
         <v>1</v>
@@ -16702,7 +16726,7 @@
         <v>255</v>
       </c>
       <c r="D197" s="8" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="E197" s="8">
         <v>1</v>
@@ -16752,7 +16776,7 @@
         <v>256</v>
       </c>
       <c r="D198" s="8" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="E198" s="8">
         <v>1</v>
@@ -16802,7 +16826,7 @@
         <v>257</v>
       </c>
       <c r="D199" s="8" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="E199" s="8">
         <v>1</v>
@@ -16852,7 +16876,7 @@
         <v>258</v>
       </c>
       <c r="D200" s="8" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="E200" s="8">
         <v>1</v>
@@ -16902,7 +16926,7 @@
         <v>259</v>
       </c>
       <c r="D201" s="8" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="E201" s="8">
         <v>1</v>
@@ -16952,7 +16976,7 @@
         <v>260</v>
       </c>
       <c r="D202" s="8" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="E202" s="8">
         <v>1</v>
@@ -17002,7 +17026,7 @@
         <v>261</v>
       </c>
       <c r="D203" s="8" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="E203" s="8">
         <v>1</v>
@@ -17052,7 +17076,7 @@
         <v>262</v>
       </c>
       <c r="D204" s="8" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="E204" s="8">
         <v>1</v>
@@ -17102,7 +17126,7 @@
         <v>263</v>
       </c>
       <c r="D205" s="8" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="E205" s="8">
         <v>1</v>
@@ -17202,7 +17226,7 @@
         <v>265</v>
       </c>
       <c r="D207" s="8" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="E207" s="8">
         <v>1</v>
@@ -17352,7 +17376,7 @@
         <v>253</v>
       </c>
       <c r="D210" s="8" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="E210" s="8">
         <v>1</v>
@@ -17402,7 +17426,7 @@
         <v>254</v>
       </c>
       <c r="D211" s="8" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="E211" s="8">
         <v>1</v>
@@ -17452,7 +17476,7 @@
         <v>255</v>
       </c>
       <c r="D212" s="8" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="E212" s="8">
         <v>1</v>
@@ -17502,7 +17526,7 @@
         <v>256</v>
       </c>
       <c r="D213" s="8" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="E213" s="8">
         <v>1</v>
@@ -17552,7 +17576,7 @@
         <v>257</v>
       </c>
       <c r="D214" s="8" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="E214" s="8">
         <v>1</v>
@@ -17602,7 +17626,7 @@
         <v>258</v>
       </c>
       <c r="D215" s="8" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="E215" s="8">
         <v>1</v>
@@ -17652,7 +17676,7 @@
         <v>259</v>
       </c>
       <c r="D216" s="8" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="E216" s="8">
         <v>1</v>
@@ -17702,7 +17726,7 @@
         <v>260</v>
       </c>
       <c r="D217" s="8" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="E217" s="8">
         <v>1</v>
@@ -17752,7 +17776,7 @@
         <v>261</v>
       </c>
       <c r="D218" s="8" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="E218" s="8">
         <v>1</v>
@@ -17802,7 +17826,7 @@
         <v>262</v>
       </c>
       <c r="D219" s="8" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="E219" s="8">
         <v>1</v>
@@ -17852,7 +17876,7 @@
         <v>263</v>
       </c>
       <c r="D220" s="8" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="E220" s="8">
         <v>1</v>
@@ -17952,7 +17976,7 @@
         <v>265</v>
       </c>
       <c r="D222" s="8" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="E222" s="8">
         <v>1</v>
@@ -17996,7 +18020,7 @@
         <v>60</v>
       </c>
       <c r="B223" s="8" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="C223" s="8">
         <v>95</v>
@@ -18046,7 +18070,7 @@
         <v>60</v>
       </c>
       <c r="B224" s="8" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="C224" s="8">
         <v>155</v>
@@ -18096,7 +18120,7 @@
         <v>60</v>
       </c>
       <c r="B225" s="8" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="C225" s="8">
         <v>178</v>
@@ -18146,13 +18170,13 @@
         <v>60</v>
       </c>
       <c r="B226" s="8" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="C226" s="8">
         <v>253</v>
       </c>
       <c r="D226" s="8" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="E226" s="8">
         <v>1</v>
@@ -18196,13 +18220,13 @@
         <v>60</v>
       </c>
       <c r="B227" s="8" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="C227" s="8">
         <v>254</v>
       </c>
       <c r="D227" s="8" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="E227" s="8">
         <v>1</v>
@@ -18246,13 +18270,13 @@
         <v>60</v>
       </c>
       <c r="B228" s="8" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="C228" s="8">
         <v>255</v>
       </c>
       <c r="D228" s="8" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="E228" s="8">
         <v>1</v>
@@ -18296,13 +18320,13 @@
         <v>60</v>
       </c>
       <c r="B229" s="8" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="C229" s="8">
         <v>256</v>
       </c>
       <c r="D229" s="8" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="E229" s="8">
         <v>1</v>
@@ -18346,13 +18370,13 @@
         <v>60</v>
       </c>
       <c r="B230" s="8" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="C230" s="8">
         <v>257</v>
       </c>
       <c r="D230" s="8" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="E230" s="8">
         <v>1</v>
@@ -18396,13 +18420,13 @@
         <v>60</v>
       </c>
       <c r="B231" s="8" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="C231" s="8">
         <v>258</v>
       </c>
       <c r="D231" s="8" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="E231" s="8">
         <v>1</v>
@@ -18446,13 +18470,13 @@
         <v>60</v>
       </c>
       <c r="B232" s="8" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="C232" s="8">
         <v>259</v>
       </c>
       <c r="D232" s="8" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="E232" s="8">
         <v>1</v>
@@ -18496,13 +18520,13 @@
         <v>60</v>
       </c>
       <c r="B233" s="8" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="C233" s="8">
         <v>260</v>
       </c>
       <c r="D233" s="8" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="E233" s="8">
         <v>1</v>
@@ -18546,13 +18570,13 @@
         <v>60</v>
       </c>
       <c r="B234" s="8" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="C234" s="8">
         <v>261</v>
       </c>
       <c r="D234" s="8" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="E234" s="8">
         <v>1</v>
@@ -18596,13 +18620,13 @@
         <v>60</v>
       </c>
       <c r="B235" s="8" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="C235" s="8">
         <v>262</v>
       </c>
       <c r="D235" s="8" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="E235" s="8">
         <v>1</v>
@@ -18646,13 +18670,13 @@
         <v>60</v>
       </c>
       <c r="B236" s="8" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="C236" s="8">
         <v>263</v>
       </c>
       <c r="D236" s="8" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="E236" s="8">
         <v>1</v>
@@ -18696,7 +18720,7 @@
         <v>60</v>
       </c>
       <c r="B237" s="8" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="C237" s="8">
         <v>264</v>
@@ -18746,13 +18770,13 @@
         <v>60</v>
       </c>
       <c r="B238" s="8" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="C238" s="8">
         <v>265</v>
       </c>
       <c r="D238" s="8" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="E238" s="8">
         <v>1</v>
@@ -31756,7 +31780,7 @@
         <v>3</v>
       </c>
       <c r="D170" s="6" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="E170" s="6">
         <v>0</v>
@@ -31806,7 +31830,7 @@
         <v>381</v>
       </c>
       <c r="I171" s="8" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="J171" s="5">
         <v>0</v>
@@ -31841,7 +31865,7 @@
         <v>381</v>
       </c>
       <c r="I172" s="8" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="J172" s="5">
         <v>0</v>
@@ -31876,7 +31900,7 @@
         <v>381</v>
       </c>
       <c r="I173" s="8" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="J173" s="5">
         <v>0</v>
@@ -31911,7 +31935,7 @@
         <v>381</v>
       </c>
       <c r="I174" s="8" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="J174" s="5">
         <v>0</v>
@@ -31946,7 +31970,7 @@
         <v>381</v>
       </c>
       <c r="I175" s="8" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="J175" s="5">
         <v>0</v>
@@ -32762,7 +32786,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="C8" s="8">
         <v>98</v>
@@ -33108,7 +33132,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="C20" s="6">
         <v>1</v>
@@ -33122,7 +33146,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="C21" s="6">
         <v>1</v>
@@ -33136,7 +33160,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="C22" s="6">
         <v>1</v>
@@ -33150,7 +33174,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="C23" s="6">
         <v>1</v>
@@ -33164,7 +33188,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="C24" s="6">
         <v>1</v>
@@ -33178,7 +33202,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="C25" s="6">
         <v>1</v>
@@ -33192,7 +33216,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="C26" s="6">
         <v>1</v>
@@ -34271,7 +34295,7 @@
         <v>5</v>
       </c>
       <c r="C37" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -34300,7 +34324,7 @@
         <v>5</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="D38" s="6">
         <v>1</v>
@@ -34329,7 +34353,7 @@
         <v>5</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="D39" s="6">
         <v>1</v>
@@ -35315,7 +35339,7 @@
         <v>3</v>
       </c>
       <c r="C73" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="D73">
         <v>1</v>
@@ -35344,7 +35368,7 @@
         <v>3</v>
       </c>
       <c r="C74" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="D74">
         <v>1</v>
@@ -35373,7 +35397,7 @@
         <v>3</v>
       </c>
       <c r="C75" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="D75">
         <v>1</v>
@@ -36451,7 +36475,7 @@
         <v>18</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="F26" s="6" t="s">
         <v>727</v>
@@ -36492,7 +36516,7 @@
         <v>19</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>727</v>
@@ -36533,7 +36557,7 @@
         <v>20</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="F28" s="6" t="s">
         <v>727</v>
@@ -36574,7 +36598,7 @@
         <v>21</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="F29" s="6" t="s">
         <v>727</v>
@@ -36615,7 +36639,7 @@
         <v>22</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="F30" s="6" t="s">
         <v>727</v>
@@ -36656,7 +36680,7 @@
         <v>23</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="F31" s="6" t="s">
         <v>727</v>
@@ -36697,7 +36721,7 @@
         <v>24</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="F32" s="6" t="s">
         <v>727</v>
@@ -37446,9 +37470,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:C11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -37480,14 +37502,14 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="5">
+      <c r="A3">
         <v>102</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>1083</v>
+      <c r="C3" t="s">
+        <v>1082</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -37501,15 +37523,15 @@
         <v>950</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5">
+    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="5">
         <v>104</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="5" t="s">
         <v>378</v>
       </c>
-      <c r="C5" t="s">
-        <v>968</v>
+      <c r="C5" s="14" t="s">
+        <v>1085</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -37568,14 +37590,14 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="5">
+      <c r="A11">
         <v>110</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" t="s">
         <v>963</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>1084</v>
+      <c r="C11" t="s">
+        <v>1083</v>
       </c>
     </row>
   </sheetData>
@@ -37837,7 +37859,7 @@
         <v>927</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -38369,10 +38391,10 @@
         <v>502</v>
       </c>
       <c r="C1" t="s">
+        <v>990</v>
+      </c>
+      <c r="D1" t="s">
         <v>991</v>
-      </c>
-      <c r="D1" t="s">
-        <v>992</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -38380,7 +38402,7 @@
         <v>101</v>
       </c>
       <c r="B2" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -38394,7 +38416,7 @@
         <v>102</v>
       </c>
       <c r="B3" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -38408,7 +38430,7 @@
         <v>103</v>
       </c>
       <c r="B4" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -38422,7 +38444,7 @@
         <v>104</v>
       </c>
       <c r="B5" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -38436,7 +38458,7 @@
         <v>105</v>
       </c>
       <c r="B6" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -38450,7 +38472,7 @@
         <v>106</v>
       </c>
       <c r="B7" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -38464,7 +38486,7 @@
         <v>107</v>
       </c>
       <c r="B8" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -38478,7 +38500,7 @@
         <v>108</v>
       </c>
       <c r="B9" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -38492,7 +38514,7 @@
         <v>109</v>
       </c>
       <c r="B10" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -38506,7 +38528,7 @@
         <v>110</v>
       </c>
       <c r="B11" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -38520,7 +38542,7 @@
         <v>111</v>
       </c>
       <c r="B12" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -38549,10 +38571,10 @@
         <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="C1" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -38560,7 +38582,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -38571,7 +38593,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -38582,7 +38604,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -38593,7 +38615,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -38604,7 +38626,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -38615,7 +38637,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -38626,7 +38648,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -38744,7 +38766,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
   </sheetData>
@@ -38764,16 +38786,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>1011</v>
+      </c>
+      <c r="B1" t="s">
         <v>1012</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1013</v>
       </c>
       <c r="C1" t="s">
         <v>731</v>
       </c>
       <c r="D1" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -39120,16 +39142,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
+        <v>1014</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>1015</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
         <v>1016</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>1017</v>
-      </c>
       <c r="D1" s="6" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -39137,13 +39159,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>1017</v>
+      </c>
+      <c r="C2" t="s">
         <v>1018</v>
       </c>
-      <c r="C2" t="s">
-        <v>1019</v>
-      </c>
       <c r="D2" s="6" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -39151,13 +39173,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>1019</v>
+      </c>
+      <c r="C3" t="s">
         <v>1020</v>
       </c>
-      <c r="C3" t="s">
-        <v>1021</v>
-      </c>
       <c r="D3" s="6" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -39165,13 +39187,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>1021</v>
+      </c>
+      <c r="C4" t="s">
         <v>1022</v>
       </c>
-      <c r="C4" t="s">
-        <v>1023</v>
-      </c>
       <c r="D4" s="6" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -39179,13 +39201,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="C5" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -39193,13 +39215,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>1024</v>
+      </c>
+      <c r="C6" t="s">
         <v>1025</v>
       </c>
-      <c r="C6" t="s">
-        <v>1026</v>
-      </c>
       <c r="D6" s="6" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -39207,13 +39229,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>1026</v>
+      </c>
+      <c r="C7" t="s">
         <v>1027</v>
       </c>
-      <c r="C7" t="s">
-        <v>1028</v>
-      </c>
       <c r="D7" s="6" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -39221,13 +39243,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>1028</v>
+      </c>
+      <c r="C8" t="s">
         <v>1029</v>
       </c>
-      <c r="C8" t="s">
-        <v>1030</v>
-      </c>
       <c r="D8" s="6" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -39235,13 +39257,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>1044</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>1018</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>1045</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>1019</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>1046</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -39249,13 +39271,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -39263,13 +39285,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>1047</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>1048</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>1049</v>
-      </c>
       <c r="D11" s="6" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -39277,13 +39299,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -39291,13 +39313,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -39305,13 +39327,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
+        <v>1051</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>1052</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>1053</v>
-      </c>
       <c r="D14" s="6" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -39319,13 +39341,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -39333,13 +39355,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
+        <v>1054</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>1055</v>
       </c>
-      <c r="C16" s="5" t="s">
-        <v>1056</v>
-      </c>
       <c r="D16" s="5" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -39347,13 +39369,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
     </row>
   </sheetData>
@@ -39374,13 +39396,13 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>1077</v>
+      </c>
+      <c r="B1" t="s">
         <v>1078</v>
       </c>
-      <c r="B1" t="s">
-        <v>1079</v>
-      </c>
       <c r="C1" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="D1" t="s">
         <v>81</v>
@@ -39415,7 +39437,7 @@
         <v>101</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -39453,7 +39475,7 @@
         <v>102</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -39785,13 +39807,13 @@
         <v>15</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>65</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="E17" s="6">
         <v>1</v>
@@ -40353,7 +40375,7 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
@@ -40361,7 +40383,7 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
@@ -40369,7 +40391,7 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
@@ -40377,7 +40399,7 @@
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
     </row>
   </sheetData>
@@ -42412,7 +42434,7 @@
         <v>250</v>
       </c>
       <c r="B252" s="6" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.3">
@@ -42420,7 +42442,7 @@
         <v>251</v>
       </c>
       <c r="B253" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.3">
@@ -42428,7 +42450,7 @@
         <v>252</v>
       </c>
       <c r="B254" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.3">
@@ -42436,7 +42458,7 @@
         <v>253</v>
       </c>
       <c r="B255" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.3">
@@ -42444,7 +42466,7 @@
         <v>254</v>
       </c>
       <c r="B256" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.3">
@@ -42452,7 +42474,7 @@
         <v>255</v>
       </c>
       <c r="B257" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.3">
@@ -42460,7 +42482,7 @@
         <v>256</v>
       </c>
       <c r="B258" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.3">
@@ -42468,7 +42490,7 @@
         <v>257</v>
       </c>
       <c r="B259" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.3">
@@ -42476,7 +42498,7 @@
         <v>258</v>
       </c>
       <c r="B260" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.3">
@@ -42484,7 +42506,7 @@
         <v>259</v>
       </c>
       <c r="B261" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.3">
@@ -42492,7 +42514,7 @@
         <v>260</v>
       </c>
       <c r="B262" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.3">
@@ -42500,7 +42522,7 @@
         <v>261</v>
       </c>
       <c r="B263" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.3">
@@ -42508,7 +42530,7 @@
         <v>262</v>
       </c>
       <c r="B264" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.3">
@@ -42516,7 +42538,7 @@
         <v>263</v>
       </c>
       <c r="B265" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.3">
@@ -42532,7 +42554,7 @@
         <v>265</v>
       </c>
       <c r="B267" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TFS 17263 - Work at Home Coaching Reason
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C46050
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3931" uniqueCount="1099">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3934" uniqueCount="1101">
   <si>
     <t>SourceID</t>
   </si>
@@ -3381,6 +3381,12 @@
   </si>
   <si>
     <t>Added Security &amp; Privacy coaching reason and sub-reasons. Updated DIM_Coaching_Reason, DIM_SubCoaching_Reason and Coaching_Reason_Selection tabs</t>
+  </si>
+  <si>
+    <t>Added Work at Home in DIM_Coaching_Reason tab</t>
+  </si>
+  <si>
+    <t>Work at Home</t>
   </si>
 </sst>
 </file>
@@ -3771,10 +3777,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L99"/>
+  <dimension ref="A1:L100"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="A99" sqref="A99"/>
+      <selection activeCell="A100" sqref="A100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5438,21 +5444,38 @@
         <v>1084</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A99" s="5">
+    <row r="99" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="8">
         <v>88</v>
       </c>
-      <c r="B99" s="11">
+      <c r="B99" s="9">
         <v>43957</v>
       </c>
-      <c r="C99" s="5" t="s">
+      <c r="C99" s="8" t="s">
         <v>429</v>
       </c>
-      <c r="D99" s="5">
+      <c r="D99" s="8">
         <v>17066</v>
       </c>
-      <c r="E99" s="5" t="s">
+      <c r="E99" s="8" t="s">
         <v>1098</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" s="5">
+        <v>89</v>
+      </c>
+      <c r="B100" s="11">
+        <v>43980</v>
+      </c>
+      <c r="C100" s="5" t="s">
+        <v>429</v>
+      </c>
+      <c r="D100" s="5">
+        <v>17263</v>
+      </c>
+      <c r="E100" s="5" t="s">
+        <v>1099</v>
       </c>
     </row>
   </sheetData>
@@ -40481,10 +40504,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B63"/>
+  <dimension ref="A1:B64"/>
   <sheetViews>
     <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A63" sqref="A63:B63"/>
+      <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40990,11 +41013,19 @@
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="5">
+      <c r="A63" s="8">
         <v>61</v>
       </c>
-      <c r="B63" s="5" t="s">
+      <c r="B63" s="8" t="s">
         <v>1086</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="5">
+        <v>62</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>1100</v>
       </c>
     </row>
   </sheetData>
@@ -41007,7 +41038,7 @@
   <dimension ref="A1:B278"/>
   <sheetViews>
     <sheetView topLeftCell="A246" workbookViewId="0">
-      <selection activeCell="A268" sqref="A268:B278"/>
+      <selection activeCell="A267" sqref="A267"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43153,90 +43184,90 @@
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A268" s="5">
+      <c r="A268" s="8">
         <v>266</v>
       </c>
-      <c r="B268" s="5" t="s">
+      <c r="B268" s="8" t="s">
         <v>1087</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A269" s="5">
+      <c r="A269" s="8">
         <v>267</v>
       </c>
-      <c r="B269" s="5" t="s">
+      <c r="B269" s="8" t="s">
         <v>1088</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A270" s="5">
+      <c r="A270" s="8">
         <v>268</v>
       </c>
-      <c r="B270" s="5" t="s">
+      <c r="B270" s="8" t="s">
         <v>1089</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A271" s="5">
+      <c r="A271" s="8">
         <v>269</v>
       </c>
-      <c r="B271" s="5" t="s">
+      <c r="B271" s="8" t="s">
         <v>1090</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A272" s="5">
+      <c r="A272" s="8">
         <v>270</v>
       </c>
-      <c r="B272" s="5" t="s">
+      <c r="B272" s="8" t="s">
         <v>1091</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A273" s="5">
+      <c r="A273" s="8">
         <v>271</v>
       </c>
-      <c r="B273" s="5" t="s">
+      <c r="B273" s="8" t="s">
         <v>1092</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A274" s="5">
+      <c r="A274" s="8">
         <v>272</v>
       </c>
-      <c r="B274" s="5" t="s">
+      <c r="B274" s="8" t="s">
         <v>1093</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A275" s="5">
+      <c r="A275" s="8">
         <v>273</v>
       </c>
-      <c r="B275" s="5" t="s">
+      <c r="B275" s="8" t="s">
         <v>1094</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A276" s="5">
+      <c r="A276" s="8">
         <v>274</v>
       </c>
-      <c r="B276" s="5" t="s">
+      <c r="B276" s="8" t="s">
         <v>1095</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A277" s="5">
+      <c r="A277" s="8">
         <v>275</v>
       </c>
-      <c r="B277" s="5" t="s">
+      <c r="B277" s="8" t="s">
         <v>1096</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A278" s="5">
+      <c r="A278" s="8">
         <v>276</v>
       </c>
-      <c r="B278" s="5" t="s">
+      <c r="B278" s="8" t="s">
         <v>1097</v>
       </c>
     </row>

</xml_diff>

<commit_message>
TFS 18255 - Changes to support WAH return to site
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C46921
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="22995" windowHeight="12840"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="22995" windowHeight="12840" firstSheet="5" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_History" sheetId="14" r:id="rId1"/>
@@ -46,7 +46,7 @@
     <sheet name="Warning_Log_StaticText" sheetId="33" r:id="rId32"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">Coaching_Reason_Selection!$A$1:$P$375</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">Coaching_Reason_Selection!$A$1:$P$386</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">DIM_Source!$A$1:$H$58</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">Email_Notifications!$A$1:$K$175</definedName>
   </definedNames>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3934" uniqueCount="1101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3951" uniqueCount="1107">
   <si>
     <t>SourceID</t>
   </si>
@@ -3387,6 +3387,24 @@
   </si>
   <si>
     <t>Work at Home</t>
+  </si>
+  <si>
+    <t>Discretionary Approved by Ops</t>
+  </si>
+  <si>
+    <t>Employee Accepted an On-Site Position</t>
+  </si>
+  <si>
+    <t>Employee Did not Meet Equipment Requirements</t>
+  </si>
+  <si>
+    <t>Employee Requested to Return to the Site</t>
+  </si>
+  <si>
+    <t>Added 1 new coaching Reason and 4 new subcoaching reasons and Updated DIM_Coaching_Reason, DIM_SubCoaching_Reason and Coaching_Reason_Selection tabs</t>
+  </si>
+  <si>
+    <t>Work at Home (Return to Site Only)</t>
   </si>
 </sst>
 </file>
@@ -3777,10 +3795,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L100"/>
+  <dimension ref="A1:L101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="A100" sqref="A100"/>
+    <sheetView topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="A101" sqref="A101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5461,21 +5479,38 @@
         <v>1098</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A100" s="5">
+    <row r="100" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="8">
         <v>89</v>
       </c>
-      <c r="B100" s="11">
+      <c r="B100" s="9">
         <v>43980</v>
       </c>
-      <c r="C100" s="5" t="s">
+      <c r="C100" s="8" t="s">
         <v>429</v>
       </c>
-      <c r="D100" s="5">
+      <c r="D100" s="8">
         <v>17263</v>
       </c>
-      <c r="E100" s="5" t="s">
+      <c r="E100" s="8" t="s">
         <v>1099</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" s="5">
+        <v>90</v>
+      </c>
+      <c r="B101" s="11">
+        <v>44069</v>
+      </c>
+      <c r="C101" s="5" t="s">
+        <v>429</v>
+      </c>
+      <c r="D101" s="5">
+        <v>18255</v>
+      </c>
+      <c r="E101" s="5" t="s">
+        <v>1105</v>
       </c>
     </row>
   </sheetData>
@@ -5489,7 +5524,7 @@
   <dimension ref="A1:G60"/>
   <sheetViews>
     <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60"/>
+      <selection activeCell="A60" sqref="A60:G60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6852,25 +6887,25 @@
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="5" t="s">
+      <c r="A60" s="8" t="s">
         <v>1083</v>
       </c>
-      <c r="B60" s="5" t="s">
+      <c r="B60" s="8" t="s">
         <v>963</v>
       </c>
-      <c r="C60" s="5">
-        <v>1</v>
-      </c>
-      <c r="D60" s="5">
-        <v>1</v>
-      </c>
-      <c r="E60" s="5">
-        <v>0</v>
-      </c>
-      <c r="F60" s="5">
-        <v>0</v>
-      </c>
-      <c r="G60" s="5">
+      <c r="C60" s="8">
+        <v>1</v>
+      </c>
+      <c r="D60" s="8">
+        <v>1</v>
+      </c>
+      <c r="E60" s="8">
+        <v>0</v>
+      </c>
+      <c r="F60" s="8">
+        <v>0</v>
+      </c>
+      <c r="G60" s="8">
         <v>0</v>
       </c>
     </row>
@@ -6982,14 +7017,15 @@
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:P386"/>
+  <dimension ref="A1:P391"/>
   <sheetViews>
-    <sheetView topLeftCell="A220" workbookViewId="0">
-      <selection activeCell="A377" sqref="A377:P386"/>
+    <sheetView tabSelected="1" topLeftCell="A357" workbookViewId="0">
+      <selection activeCell="B388" sqref="B388:B391"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="22.85546875" customWidth="1"/>
     <col min="4" max="4" width="44.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7943,7 +7979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>9</v>
       </c>
@@ -7993,7 +8029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>10</v>
       </c>
@@ -8043,7 +8079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>10</v>
       </c>
@@ -8093,7 +8129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>10</v>
       </c>
@@ -8143,7 +8179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>10</v>
       </c>
@@ -8193,7 +8229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>10</v>
       </c>
@@ -8243,7 +8279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>11</v>
       </c>
@@ -8293,7 +8329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>20</v>
       </c>
@@ -8343,7 +8379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>20</v>
       </c>
@@ -8393,7 +8429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>20</v>
       </c>
@@ -8443,7 +8479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>20</v>
       </c>
@@ -8493,7 +8529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>20</v>
       </c>
@@ -8543,7 +8579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1</v>
       </c>
@@ -8593,7 +8629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>1</v>
       </c>
@@ -8643,7 +8679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>1</v>
       </c>
@@ -8693,7 +8729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>1</v>
       </c>
@@ -8743,7 +8779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1</v>
       </c>
@@ -8793,7 +8829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>3</v>
       </c>
@@ -8843,7 +8879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>3</v>
       </c>
@@ -8893,7 +8929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>3</v>
       </c>
@@ -8943,7 +8979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>3</v>
       </c>
@@ -8993,7 +9029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>31</v>
       </c>
@@ -9043,7 +9079,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>31</v>
       </c>
@@ -9093,7 +9129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>32</v>
       </c>
@@ -9143,7 +9179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>32</v>
       </c>
@@ -9193,7 +9229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>32</v>
       </c>
@@ -9243,7 +9279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>32</v>
       </c>
@@ -9293,7 +9329,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>32</v>
       </c>
@@ -9343,7 +9379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>32</v>
       </c>
@@ -9393,7 +9429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>32</v>
       </c>
@@ -9443,7 +9479,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>32</v>
       </c>
@@ -9493,7 +9529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>32</v>
       </c>
@@ -9543,7 +9579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>32</v>
       </c>
@@ -9593,7 +9629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>32</v>
       </c>
@@ -9643,7 +9679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>33</v>
       </c>
@@ -9693,7 +9729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>33</v>
       </c>
@@ -9743,7 +9779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>33</v>
       </c>
@@ -9793,7 +9829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>33</v>
       </c>
@@ -9843,7 +9879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>34</v>
       </c>
@@ -9893,7 +9929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>34</v>
       </c>
@@ -9943,7 +9979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>34</v>
       </c>
@@ -9993,7 +10029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>35</v>
       </c>
@@ -10043,7 +10079,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>35</v>
       </c>
@@ -10093,7 +10129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>36</v>
       </c>
@@ -10143,7 +10179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>36</v>
       </c>
@@ -10193,7 +10229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>36</v>
       </c>
@@ -10243,7 +10279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>37</v>
       </c>
@@ -10293,7 +10329,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>37</v>
       </c>
@@ -10343,7 +10379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>38</v>
       </c>
@@ -10393,7 +10429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>38</v>
       </c>
@@ -10443,7 +10479,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>39</v>
       </c>
@@ -10493,7 +10529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>39</v>
       </c>
@@ -10543,7 +10579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>44</v>
       </c>
@@ -10593,7 +10629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>44</v>
       </c>
@@ -10643,7 +10679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>44</v>
       </c>
@@ -10693,7 +10729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>44</v>
       </c>
@@ -10743,7 +10779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>44</v>
       </c>
@@ -10793,7 +10829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>44</v>
       </c>
@@ -10843,7 +10879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>45</v>
       </c>
@@ -10893,7 +10929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>45</v>
       </c>
@@ -10943,7 +10979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>46</v>
       </c>
@@ -10993,7 +11029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>46</v>
       </c>
@@ -11043,7 +11079,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>46</v>
       </c>
@@ -11093,7 +11129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>46</v>
       </c>
@@ -11143,7 +11179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>11</v>
       </c>
@@ -11193,7 +11229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>11</v>
       </c>
@@ -11243,7 +11279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>11</v>
       </c>
@@ -11293,7 +11329,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>11</v>
       </c>
@@ -11343,7 +11379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>11</v>
       </c>
@@ -11393,7 +11429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>11</v>
       </c>
@@ -11443,7 +11479,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>11</v>
       </c>
@@ -11493,7 +11529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>11</v>
       </c>
@@ -11543,7 +11579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>11</v>
       </c>
@@ -11593,7 +11629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>11</v>
       </c>
@@ -11643,7 +11679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>11</v>
       </c>
@@ -11693,7 +11729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>11</v>
       </c>
@@ -11743,7 +11779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>11</v>
       </c>
@@ -11793,7 +11829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>11</v>
       </c>
@@ -11843,7 +11879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>11</v>
       </c>
@@ -11893,7 +11929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>11</v>
       </c>
@@ -11943,7 +11979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>47</v>
       </c>
@@ -11993,7 +12029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>47</v>
       </c>
@@ -12043,7 +12079,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>47</v>
       </c>
@@ -12093,7 +12129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>13</v>
       </c>
@@ -12143,7 +12179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>13</v>
       </c>
@@ -12193,7 +12229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>13</v>
       </c>
@@ -12243,7 +12279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>13</v>
       </c>
@@ -12293,7 +12329,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>13</v>
       </c>
@@ -12343,7 +12379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>13</v>
       </c>
@@ -12393,7 +12429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>13</v>
       </c>
@@ -12443,7 +12479,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>13</v>
       </c>
@@ -12493,7 +12529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>49</v>
       </c>
@@ -12543,7 +12579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>49</v>
       </c>
@@ -12593,7 +12629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>49</v>
       </c>
@@ -12643,7 +12679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>49</v>
       </c>
@@ -12693,7 +12729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>50</v>
       </c>
@@ -12743,7 +12779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>50</v>
       </c>
@@ -12793,7 +12829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>50</v>
       </c>
@@ -12843,7 +12879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>51</v>
       </c>
@@ -12893,7 +12929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>51</v>
       </c>
@@ -12943,7 +12979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>51</v>
       </c>
@@ -12993,7 +13029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>51</v>
       </c>
@@ -13043,7 +13079,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>51</v>
       </c>
@@ -13093,7 +13129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>51</v>
       </c>
@@ -13143,7 +13179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>51</v>
       </c>
@@ -13193,7 +13229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>51</v>
       </c>
@@ -13243,7 +13279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>51</v>
       </c>
@@ -13293,7 +13329,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>52</v>
       </c>
@@ -13343,7 +13379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>52</v>
       </c>
@@ -13393,7 +13429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>52</v>
       </c>
@@ -13443,7 +13479,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>52</v>
       </c>
@@ -13493,7 +13529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>52</v>
       </c>
@@ -13543,7 +13579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>52</v>
       </c>
@@ -13593,7 +13629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>52</v>
       </c>
@@ -13643,7 +13679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>52</v>
       </c>
@@ -13693,7 +13729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>52</v>
       </c>
@@ -13743,7 +13779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>53</v>
       </c>
@@ -13793,7 +13829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>53</v>
       </c>
@@ -13843,7 +13879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>54</v>
       </c>
@@ -13893,7 +13929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>54</v>
       </c>
@@ -13943,7 +13979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>54</v>
       </c>
@@ -13993,7 +14029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>6</v>
       </c>
@@ -14043,7 +14079,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>6</v>
       </c>
@@ -14093,7 +14129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>6</v>
       </c>
@@ -14143,7 +14179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>6</v>
       </c>
@@ -14193,7 +14229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>6</v>
       </c>
@@ -14243,7 +14279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>6</v>
       </c>
@@ -14293,7 +14329,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>6</v>
       </c>
@@ -14343,7 +14379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>6</v>
       </c>
@@ -14393,7 +14429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>6</v>
       </c>
@@ -14443,7 +14479,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>1</v>
       </c>
@@ -14493,7 +14529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>5</v>
       </c>
@@ -14543,7 +14579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>5</v>
       </c>
@@ -14593,7 +14629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>9</v>
       </c>
@@ -14643,7 +14679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>11</v>
       </c>
@@ -14693,7 +14729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>9</v>
       </c>
@@ -14743,7 +14779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>10</v>
       </c>
@@ -14793,7 +14829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>55</v>
       </c>
@@ -14843,7 +14879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>55</v>
       </c>
@@ -14893,7 +14929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>55</v>
       </c>
@@ -14943,7 +14979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>55</v>
       </c>
@@ -14993,7 +15029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>55</v>
       </c>
@@ -15043,7 +15079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>55</v>
       </c>
@@ -15093,7 +15129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>55</v>
       </c>
@@ -15143,7 +15179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>3</v>
       </c>
@@ -15193,7 +15229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>4</v>
       </c>
@@ -15743,7 +15779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>25</v>
       </c>
@@ -15793,7 +15829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>59</v>
       </c>
@@ -18943,7 +18979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>1</v>
       </c>
@@ -18993,7 +19029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>2</v>
       </c>
@@ -19043,7 +19079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>2</v>
       </c>
@@ -19093,7 +19129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>2</v>
       </c>
@@ -19143,7 +19179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>2</v>
       </c>
@@ -19193,7 +19229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>2</v>
       </c>
@@ -19243,7 +19279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>2</v>
       </c>
@@ -19293,7 +19329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>2</v>
       </c>
@@ -19343,7 +19379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>2</v>
       </c>
@@ -19393,7 +19429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>3</v>
       </c>
@@ -19443,7 +19479,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="250" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>4</v>
       </c>
@@ -19493,7 +19529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A251">
         <v>4</v>
       </c>
@@ -19543,7 +19579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A252">
         <v>5</v>
       </c>
@@ -19593,7 +19629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A253">
         <v>6</v>
       </c>
@@ -19643,7 +19679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A254">
         <v>6</v>
       </c>
@@ -19693,7 +19729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="255" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A255">
         <v>6</v>
       </c>
@@ -19743,7 +19779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A256">
         <v>6</v>
       </c>
@@ -19793,7 +19829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A257">
         <v>6</v>
       </c>
@@ -19843,7 +19879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A258">
         <v>6</v>
       </c>
@@ -19893,7 +19929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A259">
         <v>6</v>
       </c>
@@ -19943,7 +19979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A260">
         <v>6</v>
       </c>
@@ -19993,7 +20029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A261">
         <v>6</v>
       </c>
@@ -20043,7 +20079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A262">
         <v>6</v>
       </c>
@@ -20093,7 +20129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A263">
         <v>6</v>
       </c>
@@ -20143,7 +20179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="264" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A264">
         <v>7</v>
       </c>
@@ -20193,7 +20229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A265">
         <v>7</v>
       </c>
@@ -20243,7 +20279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A266">
         <v>8</v>
       </c>
@@ -20293,7 +20329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="267" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A267">
         <v>9</v>
       </c>
@@ -20343,7 +20379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A268">
         <v>9</v>
       </c>
@@ -20393,7 +20429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A269">
         <v>9</v>
       </c>
@@ -20443,7 +20479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="270" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A270">
         <v>9</v>
       </c>
@@ -20493,7 +20529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A271">
         <v>9</v>
       </c>
@@ -20543,7 +20579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A272">
         <v>9</v>
       </c>
@@ -20593,7 +20629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="273" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A273">
         <v>9</v>
       </c>
@@ -20643,7 +20679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="274" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A274">
         <v>9</v>
       </c>
@@ -20693,7 +20729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="275" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A275">
         <v>9</v>
       </c>
@@ -20743,7 +20779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="276" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A276">
         <v>9</v>
       </c>
@@ -20793,7 +20829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="277" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A277">
         <v>9</v>
       </c>
@@ -20843,7 +20879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="278" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A278">
         <v>9</v>
       </c>
@@ -20893,7 +20929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="279" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A279">
         <v>9</v>
       </c>
@@ -20943,7 +20979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="280" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A280">
         <v>10</v>
       </c>
@@ -20993,7 +21029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="281" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A281">
         <v>10</v>
       </c>
@@ -21043,7 +21079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="282" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A282">
         <v>10</v>
       </c>
@@ -21093,7 +21129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="283" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A283">
         <v>10</v>
       </c>
@@ -21143,7 +21179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="284" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A284">
         <v>10</v>
       </c>
@@ -21193,7 +21229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="285" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A285">
         <v>10</v>
       </c>
@@ -21243,7 +21279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="286" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A286">
         <v>11</v>
       </c>
@@ -21293,7 +21329,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="287" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A287">
         <v>11</v>
       </c>
@@ -21343,7 +21379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="288" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A288">
         <v>11</v>
       </c>
@@ -21393,7 +21429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="289" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A289">
         <v>12</v>
       </c>
@@ -21443,7 +21479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="290" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A290">
         <v>13</v>
       </c>
@@ -21493,7 +21529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="291" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A291">
         <v>14</v>
       </c>
@@ -21543,7 +21579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="292" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A292">
         <v>15</v>
       </c>
@@ -21593,7 +21629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="293" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A293">
         <v>15</v>
       </c>
@@ -21643,7 +21679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="294" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A294">
         <v>15</v>
       </c>
@@ -21693,7 +21729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="295" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A295">
         <v>15</v>
       </c>
@@ -21743,7 +21779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="296" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A296">
         <v>15</v>
       </c>
@@ -21793,7 +21829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="297" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A297">
         <v>15</v>
       </c>
@@ -21843,7 +21879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="298" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A298">
         <v>15</v>
       </c>
@@ -21893,7 +21929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="299" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A299">
         <v>15</v>
       </c>
@@ -21943,7 +21979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="300" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A300">
         <v>15</v>
       </c>
@@ -21993,7 +22029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="301" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A301">
         <v>15</v>
       </c>
@@ -22043,7 +22079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="302" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A302">
         <v>16</v>
       </c>
@@ -22093,7 +22129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="303" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A303">
         <v>16</v>
       </c>
@@ -22143,7 +22179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="304" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A304">
         <v>16</v>
       </c>
@@ -22193,7 +22229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="305" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A305">
         <v>17</v>
       </c>
@@ -22243,7 +22279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="306" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A306">
         <v>17</v>
       </c>
@@ -22293,7 +22329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="307" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A307">
         <v>17</v>
       </c>
@@ -22343,7 +22379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="308" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A308">
         <v>17</v>
       </c>
@@ -22393,7 +22429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="309" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A309">
         <v>17</v>
       </c>
@@ -22443,7 +22479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="310" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A310">
         <v>18</v>
       </c>
@@ -22493,7 +22529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="311" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A311">
         <v>19</v>
       </c>
@@ -22543,7 +22579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="312" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A312">
         <v>19</v>
       </c>
@@ -22593,7 +22629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="313" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A313">
         <v>20</v>
       </c>
@@ -22643,7 +22679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="314" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A314">
         <v>20</v>
       </c>
@@ -22693,7 +22729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="315" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A315">
         <v>20</v>
       </c>
@@ -22743,7 +22779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="316" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A316">
         <v>20</v>
       </c>
@@ -22793,7 +22829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="317" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A317">
         <v>20</v>
       </c>
@@ -22843,7 +22879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="318" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A318">
         <v>20</v>
       </c>
@@ -22893,7 +22929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="319" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A319">
         <v>21</v>
       </c>
@@ -22943,7 +22979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="320" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A320">
         <v>21</v>
       </c>
@@ -22993,7 +23029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="321" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A321">
         <v>21</v>
       </c>
@@ -23043,7 +23079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="322" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A322">
         <v>23</v>
       </c>
@@ -23093,7 +23129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="323" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A323">
         <v>23</v>
       </c>
@@ -23143,7 +23179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="324" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A324">
         <v>23</v>
       </c>
@@ -23193,7 +23229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="325" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A325">
         <v>23</v>
       </c>
@@ -23243,7 +23279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="326" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A326">
         <v>23</v>
       </c>
@@ -23293,7 +23329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="327" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A327">
         <v>23</v>
       </c>
@@ -23343,7 +23379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="328" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A328">
         <v>23</v>
       </c>
@@ -23393,7 +23429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="329" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A329">
         <v>23</v>
       </c>
@@ -23443,7 +23479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="330" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A330">
         <v>24</v>
       </c>
@@ -23493,7 +23529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="331" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A331">
         <v>25</v>
       </c>
@@ -23543,7 +23579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="332" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A332">
         <v>25</v>
       </c>
@@ -23593,7 +23629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="333" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A333">
         <v>25</v>
       </c>
@@ -23643,7 +23679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="334" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A334">
         <v>25</v>
       </c>
@@ -23693,7 +23729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="335" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A335">
         <v>25</v>
       </c>
@@ -23743,7 +23779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="336" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A336">
         <v>26</v>
       </c>
@@ -23793,7 +23829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="337" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A337">
         <v>26</v>
       </c>
@@ -23843,7 +23879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="338" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A338">
         <v>26</v>
       </c>
@@ -23893,7 +23929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="339" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A339">
         <v>26</v>
       </c>
@@ -23943,7 +23979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="340" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A340">
         <v>27</v>
       </c>
@@ -23993,7 +24029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="341" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A341">
         <v>27</v>
       </c>
@@ -24043,7 +24079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="342" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A342">
         <v>27</v>
       </c>
@@ -24093,7 +24129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="343" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A343">
         <v>27</v>
       </c>
@@ -24143,7 +24179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="344" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A344">
         <v>27</v>
       </c>
@@ -24193,7 +24229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="345" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A345">
         <v>27</v>
       </c>
@@ -24243,7 +24279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="346" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A346">
         <v>27</v>
       </c>
@@ -24293,7 +24329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="347" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A347">
         <v>27</v>
       </c>
@@ -24343,7 +24379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="348" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A348">
         <v>27</v>
       </c>
@@ -24393,7 +24429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="349" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A349">
         <v>27</v>
       </c>
@@ -24443,7 +24479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="350" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A350">
         <v>27</v>
       </c>
@@ -24493,7 +24529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="351" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A351">
         <v>27</v>
       </c>
@@ -24543,7 +24579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="352" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A352">
         <v>4</v>
       </c>
@@ -24593,7 +24629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="353" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A353">
         <v>4</v>
       </c>
@@ -24643,7 +24679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="354" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A354">
         <v>4</v>
       </c>
@@ -24693,7 +24729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="355" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A355">
         <v>13</v>
       </c>
@@ -24743,7 +24779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="356" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A356">
         <v>40</v>
       </c>
@@ -24793,7 +24829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="357" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A357">
         <v>40</v>
       </c>
@@ -24843,7 +24879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="358" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A358">
         <v>40</v>
       </c>
@@ -24893,7 +24929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="359" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A359">
         <v>40</v>
       </c>
@@ -24943,7 +24979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="360" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A360">
         <v>41</v>
       </c>
@@ -24993,7 +25029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="361" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A361">
         <v>41</v>
       </c>
@@ -25043,7 +25079,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="362" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A362">
         <v>41</v>
       </c>
@@ -25093,7 +25129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="363" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A363">
         <v>41</v>
       </c>
@@ -25143,7 +25179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="364" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A364">
         <v>42</v>
       </c>
@@ -25193,7 +25229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="365" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A365">
         <v>42</v>
       </c>
@@ -25243,7 +25279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="366" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A366">
         <v>42</v>
       </c>
@@ -25293,7 +25329,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="367" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A367">
         <v>42</v>
       </c>
@@ -25343,7 +25379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="368" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A368">
         <v>42</v>
       </c>
@@ -25393,7 +25429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="369" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A369">
         <v>42</v>
       </c>
@@ -25443,7 +25479,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="370" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A370">
         <v>42</v>
       </c>
@@ -25493,7 +25529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="371" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A371">
         <v>43</v>
       </c>
@@ -25543,7 +25579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="372" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A372">
         <v>43</v>
       </c>
@@ -25593,7 +25629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="373" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A373">
         <v>44</v>
       </c>
@@ -25643,7 +25679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="374" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A374">
         <v>44</v>
       </c>
@@ -25693,7 +25729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="375" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A375">
         <v>44</v>
       </c>
@@ -25744,565 +25780,807 @@
       </c>
     </row>
     <row r="376" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A376" s="5">
+      <c r="A376">
         <v>61</v>
       </c>
-      <c r="B376" s="5" t="s">
+      <c r="B376" t="s">
         <v>1086</v>
       </c>
-      <c r="C376" s="5">
+      <c r="C376">
         <v>266</v>
       </c>
-      <c r="D376" s="5" t="s">
+      <c r="D376" t="s">
         <v>1087</v>
       </c>
-      <c r="E376" s="5">
-        <v>1</v>
-      </c>
-      <c r="F376" s="5">
-        <v>1</v>
-      </c>
-      <c r="G376" s="5">
-        <v>1</v>
-      </c>
-      <c r="H376" s="5">
-        <v>1</v>
-      </c>
-      <c r="I376" s="5">
-        <v>1</v>
-      </c>
-      <c r="J376" s="5">
-        <v>1</v>
-      </c>
-      <c r="K376" s="5">
-        <v>1</v>
-      </c>
-      <c r="L376" s="5">
-        <v>1</v>
-      </c>
-      <c r="M376" s="5">
-        <v>0</v>
-      </c>
-      <c r="N376" s="5">
-        <v>0</v>
-      </c>
-      <c r="O376" s="5">
-        <v>1</v>
-      </c>
-      <c r="P376" s="5">
+      <c r="E376">
+        <v>1</v>
+      </c>
+      <c r="F376">
+        <v>1</v>
+      </c>
+      <c r="G376">
+        <v>1</v>
+      </c>
+      <c r="H376">
+        <v>1</v>
+      </c>
+      <c r="I376">
+        <v>1</v>
+      </c>
+      <c r="J376">
+        <v>1</v>
+      </c>
+      <c r="K376">
+        <v>1</v>
+      </c>
+      <c r="L376">
+        <v>1</v>
+      </c>
+      <c r="M376">
+        <v>0</v>
+      </c>
+      <c r="N376">
+        <v>0</v>
+      </c>
+      <c r="O376">
+        <v>1</v>
+      </c>
+      <c r="P376">
         <v>1</v>
       </c>
     </row>
     <row r="377" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A377" s="5">
+      <c r="A377">
         <v>61</v>
       </c>
-      <c r="B377" s="5" t="s">
+      <c r="B377" t="s">
         <v>1086</v>
       </c>
-      <c r="C377" s="5">
+      <c r="C377">
         <v>267</v>
       </c>
-      <c r="D377" s="5" t="s">
+      <c r="D377" t="s">
         <v>1088</v>
       </c>
-      <c r="E377" s="5">
-        <v>1</v>
-      </c>
-      <c r="F377" s="5">
-        <v>1</v>
-      </c>
-      <c r="G377" s="5">
-        <v>1</v>
-      </c>
-      <c r="H377" s="5">
-        <v>1</v>
-      </c>
-      <c r="I377" s="5">
-        <v>1</v>
-      </c>
-      <c r="J377" s="5">
-        <v>1</v>
-      </c>
-      <c r="K377" s="5">
-        <v>1</v>
-      </c>
-      <c r="L377" s="5">
-        <v>1</v>
-      </c>
-      <c r="M377" s="5">
-        <v>0</v>
-      </c>
-      <c r="N377" s="5">
-        <v>0</v>
-      </c>
-      <c r="O377" s="5">
-        <v>1</v>
-      </c>
-      <c r="P377" s="5">
+      <c r="E377">
+        <v>1</v>
+      </c>
+      <c r="F377">
+        <v>1</v>
+      </c>
+      <c r="G377">
+        <v>1</v>
+      </c>
+      <c r="H377">
+        <v>1</v>
+      </c>
+      <c r="I377">
+        <v>1</v>
+      </c>
+      <c r="J377">
+        <v>1</v>
+      </c>
+      <c r="K377">
+        <v>1</v>
+      </c>
+      <c r="L377">
+        <v>1</v>
+      </c>
+      <c r="M377">
+        <v>0</v>
+      </c>
+      <c r="N377">
+        <v>0</v>
+      </c>
+      <c r="O377">
+        <v>1</v>
+      </c>
+      <c r="P377">
         <v>1</v>
       </c>
     </row>
     <row r="378" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A378" s="5">
+      <c r="A378">
         <v>61</v>
       </c>
-      <c r="B378" s="5" t="s">
+      <c r="B378" t="s">
         <v>1086</v>
       </c>
-      <c r="C378" s="5">
+      <c r="C378">
         <v>268</v>
       </c>
-      <c r="D378" s="5" t="s">
+      <c r="D378" t="s">
         <v>1089</v>
       </c>
-      <c r="E378" s="5">
-        <v>1</v>
-      </c>
-      <c r="F378" s="5">
-        <v>1</v>
-      </c>
-      <c r="G378" s="5">
-        <v>1</v>
-      </c>
-      <c r="H378" s="5">
-        <v>1</v>
-      </c>
-      <c r="I378" s="5">
-        <v>1</v>
-      </c>
-      <c r="J378" s="5">
-        <v>1</v>
-      </c>
-      <c r="K378" s="5">
-        <v>1</v>
-      </c>
-      <c r="L378" s="5">
-        <v>1</v>
-      </c>
-      <c r="M378" s="5">
-        <v>0</v>
-      </c>
-      <c r="N378" s="5">
-        <v>0</v>
-      </c>
-      <c r="O378" s="5">
-        <v>1</v>
-      </c>
-      <c r="P378" s="5">
+      <c r="E378">
+        <v>1</v>
+      </c>
+      <c r="F378">
+        <v>1</v>
+      </c>
+      <c r="G378">
+        <v>1</v>
+      </c>
+      <c r="H378">
+        <v>1</v>
+      </c>
+      <c r="I378">
+        <v>1</v>
+      </c>
+      <c r="J378">
+        <v>1</v>
+      </c>
+      <c r="K378">
+        <v>1</v>
+      </c>
+      <c r="L378">
+        <v>1</v>
+      </c>
+      <c r="M378">
+        <v>0</v>
+      </c>
+      <c r="N378">
+        <v>0</v>
+      </c>
+      <c r="O378">
+        <v>1</v>
+      </c>
+      <c r="P378">
         <v>1</v>
       </c>
     </row>
     <row r="379" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A379" s="5">
+      <c r="A379">
         <v>61</v>
       </c>
-      <c r="B379" s="5" t="s">
+      <c r="B379" t="s">
         <v>1086</v>
       </c>
-      <c r="C379" s="5">
+      <c r="C379">
         <v>269</v>
       </c>
-      <c r="D379" s="5" t="s">
+      <c r="D379" t="s">
         <v>1090</v>
       </c>
-      <c r="E379" s="5">
-        <v>1</v>
-      </c>
-      <c r="F379" s="5">
-        <v>1</v>
-      </c>
-      <c r="G379" s="5">
-        <v>1</v>
-      </c>
-      <c r="H379" s="5">
-        <v>1</v>
-      </c>
-      <c r="I379" s="5">
-        <v>1</v>
-      </c>
-      <c r="J379" s="5">
-        <v>1</v>
-      </c>
-      <c r="K379" s="5">
-        <v>1</v>
-      </c>
-      <c r="L379" s="5">
-        <v>1</v>
-      </c>
-      <c r="M379" s="5">
-        <v>0</v>
-      </c>
-      <c r="N379" s="5">
-        <v>0</v>
-      </c>
-      <c r="O379" s="5">
-        <v>1</v>
-      </c>
-      <c r="P379" s="5">
+      <c r="E379">
+        <v>1</v>
+      </c>
+      <c r="F379">
+        <v>1</v>
+      </c>
+      <c r="G379">
+        <v>1</v>
+      </c>
+      <c r="H379">
+        <v>1</v>
+      </c>
+      <c r="I379">
+        <v>1</v>
+      </c>
+      <c r="J379">
+        <v>1</v>
+      </c>
+      <c r="K379">
+        <v>1</v>
+      </c>
+      <c r="L379">
+        <v>1</v>
+      </c>
+      <c r="M379">
+        <v>0</v>
+      </c>
+      <c r="N379">
+        <v>0</v>
+      </c>
+      <c r="O379">
+        <v>1</v>
+      </c>
+      <c r="P379">
         <v>1</v>
       </c>
     </row>
     <row r="380" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A380" s="5">
+      <c r="A380">
         <v>61</v>
       </c>
-      <c r="B380" s="5" t="s">
+      <c r="B380" t="s">
         <v>1086</v>
       </c>
-      <c r="C380" s="5">
+      <c r="C380">
         <v>270</v>
       </c>
-      <c r="D380" s="5" t="s">
+      <c r="D380" t="s">
         <v>1091</v>
       </c>
-      <c r="E380" s="5">
-        <v>1</v>
-      </c>
-      <c r="F380" s="5">
-        <v>1</v>
-      </c>
-      <c r="G380" s="5">
-        <v>1</v>
-      </c>
-      <c r="H380" s="5">
-        <v>1</v>
-      </c>
-      <c r="I380" s="5">
-        <v>1</v>
-      </c>
-      <c r="J380" s="5">
-        <v>1</v>
-      </c>
-      <c r="K380" s="5">
-        <v>1</v>
-      </c>
-      <c r="L380" s="5">
-        <v>1</v>
-      </c>
-      <c r="M380" s="5">
-        <v>0</v>
-      </c>
-      <c r="N380" s="5">
-        <v>0</v>
-      </c>
-      <c r="O380" s="5">
-        <v>1</v>
-      </c>
-      <c r="P380" s="5">
+      <c r="E380">
+        <v>1</v>
+      </c>
+      <c r="F380">
+        <v>1</v>
+      </c>
+      <c r="G380">
+        <v>1</v>
+      </c>
+      <c r="H380">
+        <v>1</v>
+      </c>
+      <c r="I380">
+        <v>1</v>
+      </c>
+      <c r="J380">
+        <v>1</v>
+      </c>
+      <c r="K380">
+        <v>1</v>
+      </c>
+      <c r="L380">
+        <v>1</v>
+      </c>
+      <c r="M380">
+        <v>0</v>
+      </c>
+      <c r="N380">
+        <v>0</v>
+      </c>
+      <c r="O380">
+        <v>1</v>
+      </c>
+      <c r="P380">
         <v>1</v>
       </c>
     </row>
     <row r="381" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A381" s="5">
+      <c r="A381">
         <v>61</v>
       </c>
-      <c r="B381" s="5" t="s">
+      <c r="B381" t="s">
         <v>1086</v>
       </c>
-      <c r="C381" s="5">
+      <c r="C381">
         <v>271</v>
       </c>
-      <c r="D381" s="5" t="s">
+      <c r="D381" t="s">
         <v>1092</v>
       </c>
-      <c r="E381" s="5">
-        <v>1</v>
-      </c>
-      <c r="F381" s="5">
-        <v>1</v>
-      </c>
-      <c r="G381" s="5">
-        <v>1</v>
-      </c>
-      <c r="H381" s="5">
-        <v>1</v>
-      </c>
-      <c r="I381" s="5">
-        <v>1</v>
-      </c>
-      <c r="J381" s="5">
-        <v>1</v>
-      </c>
-      <c r="K381" s="5">
-        <v>1</v>
-      </c>
-      <c r="L381" s="5">
-        <v>1</v>
-      </c>
-      <c r="M381" s="5">
-        <v>0</v>
-      </c>
-      <c r="N381" s="5">
-        <v>0</v>
-      </c>
-      <c r="O381" s="5">
-        <v>1</v>
-      </c>
-      <c r="P381" s="5">
+      <c r="E381">
+        <v>1</v>
+      </c>
+      <c r="F381">
+        <v>1</v>
+      </c>
+      <c r="G381">
+        <v>1</v>
+      </c>
+      <c r="H381">
+        <v>1</v>
+      </c>
+      <c r="I381">
+        <v>1</v>
+      </c>
+      <c r="J381">
+        <v>1</v>
+      </c>
+      <c r="K381">
+        <v>1</v>
+      </c>
+      <c r="L381">
+        <v>1</v>
+      </c>
+      <c r="M381">
+        <v>0</v>
+      </c>
+      <c r="N381">
+        <v>0</v>
+      </c>
+      <c r="O381">
+        <v>1</v>
+      </c>
+      <c r="P381">
         <v>1</v>
       </c>
     </row>
     <row r="382" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A382" s="5">
+      <c r="A382">
         <v>61</v>
       </c>
-      <c r="B382" s="5" t="s">
+      <c r="B382" t="s">
         <v>1086</v>
       </c>
-      <c r="C382" s="5">
+      <c r="C382">
         <v>272</v>
       </c>
-      <c r="D382" s="5" t="s">
+      <c r="D382" t="s">
         <v>1093</v>
       </c>
-      <c r="E382" s="5">
-        <v>1</v>
-      </c>
-      <c r="F382" s="5">
-        <v>1</v>
-      </c>
-      <c r="G382" s="5">
-        <v>1</v>
-      </c>
-      <c r="H382" s="5">
-        <v>1</v>
-      </c>
-      <c r="I382" s="5">
-        <v>1</v>
-      </c>
-      <c r="J382" s="5">
-        <v>1</v>
-      </c>
-      <c r="K382" s="5">
-        <v>1</v>
-      </c>
-      <c r="L382" s="5">
-        <v>1</v>
-      </c>
-      <c r="M382" s="5">
-        <v>0</v>
-      </c>
-      <c r="N382" s="5">
-        <v>0</v>
-      </c>
-      <c r="O382" s="5">
-        <v>1</v>
-      </c>
-      <c r="P382" s="5">
+      <c r="E382">
+        <v>1</v>
+      </c>
+      <c r="F382">
+        <v>1</v>
+      </c>
+      <c r="G382">
+        <v>1</v>
+      </c>
+      <c r="H382">
+        <v>1</v>
+      </c>
+      <c r="I382">
+        <v>1</v>
+      </c>
+      <c r="J382">
+        <v>1</v>
+      </c>
+      <c r="K382">
+        <v>1</v>
+      </c>
+      <c r="L382">
+        <v>1</v>
+      </c>
+      <c r="M382">
+        <v>0</v>
+      </c>
+      <c r="N382">
+        <v>0</v>
+      </c>
+      <c r="O382">
+        <v>1</v>
+      </c>
+      <c r="P382">
         <v>1</v>
       </c>
     </row>
     <row r="383" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A383" s="5">
+      <c r="A383">
         <v>61</v>
       </c>
-      <c r="B383" s="5" t="s">
+      <c r="B383" t="s">
         <v>1086</v>
       </c>
-      <c r="C383" s="5">
+      <c r="C383">
         <v>273</v>
       </c>
-      <c r="D383" s="5" t="s">
+      <c r="D383" t="s">
         <v>1094</v>
       </c>
-      <c r="E383" s="5">
-        <v>1</v>
-      </c>
-      <c r="F383" s="5">
-        <v>1</v>
-      </c>
-      <c r="G383" s="5">
-        <v>1</v>
-      </c>
-      <c r="H383" s="5">
-        <v>1</v>
-      </c>
-      <c r="I383" s="5">
-        <v>1</v>
-      </c>
-      <c r="J383" s="5">
-        <v>1</v>
-      </c>
-      <c r="K383" s="5">
-        <v>1</v>
-      </c>
-      <c r="L383" s="5">
-        <v>1</v>
-      </c>
-      <c r="M383" s="5">
-        <v>0</v>
-      </c>
-      <c r="N383" s="5">
-        <v>0</v>
-      </c>
-      <c r="O383" s="5">
-        <v>1</v>
-      </c>
-      <c r="P383" s="5">
+      <c r="E383">
+        <v>1</v>
+      </c>
+      <c r="F383">
+        <v>1</v>
+      </c>
+      <c r="G383">
+        <v>1</v>
+      </c>
+      <c r="H383">
+        <v>1</v>
+      </c>
+      <c r="I383">
+        <v>1</v>
+      </c>
+      <c r="J383">
+        <v>1</v>
+      </c>
+      <c r="K383">
+        <v>1</v>
+      </c>
+      <c r="L383">
+        <v>1</v>
+      </c>
+      <c r="M383">
+        <v>0</v>
+      </c>
+      <c r="N383">
+        <v>0</v>
+      </c>
+      <c r="O383">
+        <v>1</v>
+      </c>
+      <c r="P383">
         <v>1</v>
       </c>
     </row>
     <row r="384" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A384" s="5">
+      <c r="A384">
         <v>61</v>
       </c>
-      <c r="B384" s="5" t="s">
+      <c r="B384" t="s">
         <v>1086</v>
       </c>
-      <c r="C384" s="5">
+      <c r="C384">
         <v>274</v>
       </c>
-      <c r="D384" s="5" t="s">
+      <c r="D384" t="s">
         <v>1095</v>
       </c>
-      <c r="E384" s="5">
-        <v>1</v>
-      </c>
-      <c r="F384" s="5">
-        <v>1</v>
-      </c>
-      <c r="G384" s="5">
-        <v>1</v>
-      </c>
-      <c r="H384" s="5">
-        <v>1</v>
-      </c>
-      <c r="I384" s="5">
-        <v>1</v>
-      </c>
-      <c r="J384" s="5">
-        <v>1</v>
-      </c>
-      <c r="K384" s="5">
-        <v>1</v>
-      </c>
-      <c r="L384" s="5">
-        <v>1</v>
-      </c>
-      <c r="M384" s="5">
-        <v>0</v>
-      </c>
-      <c r="N384" s="5">
-        <v>0</v>
-      </c>
-      <c r="O384" s="5">
-        <v>1</v>
-      </c>
-      <c r="P384" s="5">
+      <c r="E384">
+        <v>1</v>
+      </c>
+      <c r="F384">
+        <v>1</v>
+      </c>
+      <c r="G384">
+        <v>1</v>
+      </c>
+      <c r="H384">
+        <v>1</v>
+      </c>
+      <c r="I384">
+        <v>1</v>
+      </c>
+      <c r="J384">
+        <v>1</v>
+      </c>
+      <c r="K384">
+        <v>1</v>
+      </c>
+      <c r="L384">
+        <v>1</v>
+      </c>
+      <c r="M384">
+        <v>0</v>
+      </c>
+      <c r="N384">
+        <v>0</v>
+      </c>
+      <c r="O384">
+        <v>1</v>
+      </c>
+      <c r="P384">
         <v>1</v>
       </c>
     </row>
     <row r="385" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A385" s="5">
+      <c r="A385">
         <v>61</v>
       </c>
-      <c r="B385" s="5" t="s">
+      <c r="B385" t="s">
         <v>1086</v>
       </c>
-      <c r="C385" s="5">
+      <c r="C385">
         <v>275</v>
       </c>
-      <c r="D385" s="5" t="s">
+      <c r="D385" t="s">
         <v>1096</v>
       </c>
-      <c r="E385" s="5">
-        <v>1</v>
-      </c>
-      <c r="F385" s="5">
-        <v>1</v>
-      </c>
-      <c r="G385" s="5">
-        <v>1</v>
-      </c>
-      <c r="H385" s="5">
-        <v>1</v>
-      </c>
-      <c r="I385" s="5">
-        <v>1</v>
-      </c>
-      <c r="J385" s="5">
-        <v>1</v>
-      </c>
-      <c r="K385" s="5">
-        <v>1</v>
-      </c>
-      <c r="L385" s="5">
-        <v>1</v>
-      </c>
-      <c r="M385" s="5">
-        <v>0</v>
-      </c>
-      <c r="N385" s="5">
-        <v>0</v>
-      </c>
-      <c r="O385" s="5">
-        <v>1</v>
-      </c>
-      <c r="P385" s="5">
+      <c r="E385">
+        <v>1</v>
+      </c>
+      <c r="F385">
+        <v>1</v>
+      </c>
+      <c r="G385">
+        <v>1</v>
+      </c>
+      <c r="H385">
+        <v>1</v>
+      </c>
+      <c r="I385">
+        <v>1</v>
+      </c>
+      <c r="J385">
+        <v>1</v>
+      </c>
+      <c r="K385">
+        <v>1</v>
+      </c>
+      <c r="L385">
+        <v>1</v>
+      </c>
+      <c r="M385">
+        <v>0</v>
+      </c>
+      <c r="N385">
+        <v>0</v>
+      </c>
+      <c r="O385">
+        <v>1</v>
+      </c>
+      <c r="P385">
         <v>1</v>
       </c>
     </row>
     <row r="386" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A386" s="5">
+      <c r="A386">
         <v>61</v>
       </c>
-      <c r="B386" s="5" t="s">
+      <c r="B386" t="s">
         <v>1086</v>
       </c>
-      <c r="C386" s="5">
+      <c r="C386">
         <v>276</v>
       </c>
-      <c r="D386" s="5" t="s">
+      <c r="D386" t="s">
         <v>1097</v>
       </c>
-      <c r="E386" s="5">
-        <v>1</v>
-      </c>
-      <c r="F386" s="5">
-        <v>1</v>
-      </c>
-      <c r="G386" s="5">
-        <v>1</v>
-      </c>
-      <c r="H386" s="5">
-        <v>1</v>
-      </c>
-      <c r="I386" s="5">
-        <v>1</v>
-      </c>
-      <c r="J386" s="5">
-        <v>1</v>
-      </c>
-      <c r="K386" s="5">
-        <v>1</v>
-      </c>
-      <c r="L386" s="5">
-        <v>1</v>
-      </c>
-      <c r="M386" s="5">
-        <v>0</v>
-      </c>
-      <c r="N386" s="5">
-        <v>0</v>
-      </c>
-      <c r="O386" s="5">
-        <v>1</v>
-      </c>
-      <c r="P386" s="5">
-        <v>1</v>
+      <c r="E386">
+        <v>1</v>
+      </c>
+      <c r="F386">
+        <v>1</v>
+      </c>
+      <c r="G386">
+        <v>1</v>
+      </c>
+      <c r="H386">
+        <v>1</v>
+      </c>
+      <c r="I386">
+        <v>1</v>
+      </c>
+      <c r="J386">
+        <v>1</v>
+      </c>
+      <c r="K386">
+        <v>1</v>
+      </c>
+      <c r="L386">
+        <v>1</v>
+      </c>
+      <c r="M386">
+        <v>0</v>
+      </c>
+      <c r="N386">
+        <v>0</v>
+      </c>
+      <c r="O386">
+        <v>1</v>
+      </c>
+      <c r="P386">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="387" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A387" s="8">
+        <v>62</v>
+      </c>
+      <c r="B387" s="8" t="s">
+        <v>1100</v>
+      </c>
+      <c r="C387" s="8">
+        <v>42</v>
+      </c>
+      <c r="D387" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="E387" s="8">
+        <v>1</v>
+      </c>
+      <c r="F387" s="8">
+        <v>1</v>
+      </c>
+      <c r="G387" s="8">
+        <v>1</v>
+      </c>
+      <c r="H387" s="8">
+        <v>1</v>
+      </c>
+      <c r="I387" s="8">
+        <v>1</v>
+      </c>
+      <c r="J387" s="8">
+        <v>1</v>
+      </c>
+      <c r="K387" s="8">
+        <v>1</v>
+      </c>
+      <c r="L387" s="8">
+        <v>1</v>
+      </c>
+      <c r="M387" s="8">
+        <v>0</v>
+      </c>
+      <c r="N387" s="8">
+        <v>0</v>
+      </c>
+      <c r="O387" s="8">
+        <v>0</v>
+      </c>
+      <c r="P387" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="388" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A388" s="5">
+        <v>63</v>
+      </c>
+      <c r="B388" s="5" t="s">
+        <v>1106</v>
+      </c>
+      <c r="C388" s="5">
+        <v>277</v>
+      </c>
+      <c r="D388" s="5" t="s">
+        <v>1101</v>
+      </c>
+      <c r="E388" s="5">
+        <v>1</v>
+      </c>
+      <c r="F388" s="5">
+        <v>1</v>
+      </c>
+      <c r="G388" s="5">
+        <v>1</v>
+      </c>
+      <c r="H388" s="5">
+        <v>1</v>
+      </c>
+      <c r="I388" s="5">
+        <v>1</v>
+      </c>
+      <c r="J388" s="5">
+        <v>1</v>
+      </c>
+      <c r="K388" s="5">
+        <v>0</v>
+      </c>
+      <c r="L388" s="5">
+        <v>0</v>
+      </c>
+      <c r="M388" s="5">
+        <v>0</v>
+      </c>
+      <c r="N388" s="5">
+        <v>0</v>
+      </c>
+      <c r="O388" s="5">
+        <v>0</v>
+      </c>
+      <c r="P388" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="389" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A389" s="5">
+        <v>63</v>
+      </c>
+      <c r="B389" s="5" t="s">
+        <v>1106</v>
+      </c>
+      <c r="C389" s="5">
+        <v>278</v>
+      </c>
+      <c r="D389" s="5" t="s">
+        <v>1102</v>
+      </c>
+      <c r="E389" s="5">
+        <v>1</v>
+      </c>
+      <c r="F389" s="5">
+        <v>1</v>
+      </c>
+      <c r="G389" s="5">
+        <v>1</v>
+      </c>
+      <c r="H389" s="5">
+        <v>1</v>
+      </c>
+      <c r="I389" s="5">
+        <v>1</v>
+      </c>
+      <c r="J389" s="5">
+        <v>1</v>
+      </c>
+      <c r="K389" s="5">
+        <v>0</v>
+      </c>
+      <c r="L389" s="5">
+        <v>0</v>
+      </c>
+      <c r="M389" s="5">
+        <v>0</v>
+      </c>
+      <c r="N389" s="5">
+        <v>0</v>
+      </c>
+      <c r="O389" s="5">
+        <v>0</v>
+      </c>
+      <c r="P389" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="390" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A390" s="5">
+        <v>63</v>
+      </c>
+      <c r="B390" s="5" t="s">
+        <v>1106</v>
+      </c>
+      <c r="C390" s="5">
+        <v>279</v>
+      </c>
+      <c r="D390" s="5" t="s">
+        <v>1103</v>
+      </c>
+      <c r="E390" s="5">
+        <v>1</v>
+      </c>
+      <c r="F390" s="5">
+        <v>1</v>
+      </c>
+      <c r="G390" s="5">
+        <v>1</v>
+      </c>
+      <c r="H390" s="5">
+        <v>1</v>
+      </c>
+      <c r="I390" s="5">
+        <v>1</v>
+      </c>
+      <c r="J390" s="5">
+        <v>1</v>
+      </c>
+      <c r="K390" s="5">
+        <v>0</v>
+      </c>
+      <c r="L390" s="5">
+        <v>0</v>
+      </c>
+      <c r="M390" s="5">
+        <v>0</v>
+      </c>
+      <c r="N390" s="5">
+        <v>0</v>
+      </c>
+      <c r="O390" s="5">
+        <v>0</v>
+      </c>
+      <c r="P390" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="391" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A391" s="5">
+        <v>63</v>
+      </c>
+      <c r="B391" s="5" t="s">
+        <v>1106</v>
+      </c>
+      <c r="C391" s="5">
+        <v>280</v>
+      </c>
+      <c r="D391" s="5" t="s">
+        <v>1104</v>
+      </c>
+      <c r="E391" s="5">
+        <v>1</v>
+      </c>
+      <c r="F391" s="5">
+        <v>1</v>
+      </c>
+      <c r="G391" s="5">
+        <v>1</v>
+      </c>
+      <c r="H391" s="5">
+        <v>1</v>
+      </c>
+      <c r="I391" s="5">
+        <v>1</v>
+      </c>
+      <c r="J391" s="5">
+        <v>1</v>
+      </c>
+      <c r="K391" s="5">
+        <v>0</v>
+      </c>
+      <c r="L391" s="5">
+        <v>0</v>
+      </c>
+      <c r="M391" s="5">
+        <v>0</v>
+      </c>
+      <c r="N391" s="5">
+        <v>0</v>
+      </c>
+      <c r="O391" s="5">
+        <v>0</v>
+      </c>
+      <c r="P391" s="5">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P375">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="28"/>
-        <filter val="29"/>
-        <filter val="30"/>
-        <filter val="60"/>
-      </filters>
-    </filterColumn>
+  <autoFilter ref="A1:P386">
     <filterColumn colId="4">
       <filters>
         <filter val="1"/>
@@ -40504,16 +40782,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B64"/>
+  <dimension ref="A1:B65"/>
   <sheetViews>
     <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -41013,19 +41291,27 @@
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="8">
+      <c r="A63">
         <v>61</v>
       </c>
-      <c r="B63" s="8" t="s">
+      <c r="B63" t="s">
         <v>1086</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="5">
+      <c r="A64">
         <v>62</v>
       </c>
-      <c r="B64" s="5" t="s">
+      <c r="B64" t="s">
         <v>1100</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="5">
+        <v>63</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>1106</v>
       </c>
     </row>
   </sheetData>
@@ -41035,10 +41321,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B278"/>
+  <dimension ref="A1:B282"/>
   <sheetViews>
-    <sheetView topLeftCell="A246" workbookViewId="0">
-      <selection activeCell="A267" sqref="A267"/>
+    <sheetView topLeftCell="A255" workbookViewId="0">
+      <selection activeCell="A279" sqref="A279:B282"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43184,95 +43470,128 @@
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A268" s="8">
+      <c r="A268">
         <v>266</v>
       </c>
-      <c r="B268" s="8" t="s">
+      <c r="B268" t="s">
         <v>1087</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A269" s="8">
+      <c r="A269">
         <v>267</v>
       </c>
-      <c r="B269" s="8" t="s">
+      <c r="B269" t="s">
         <v>1088</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A270" s="8">
+      <c r="A270">
         <v>268</v>
       </c>
-      <c r="B270" s="8" t="s">
+      <c r="B270" t="s">
         <v>1089</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A271" s="8">
+      <c r="A271">
         <v>269</v>
       </c>
-      <c r="B271" s="8" t="s">
+      <c r="B271" t="s">
         <v>1090</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A272" s="8">
+      <c r="A272">
         <v>270</v>
       </c>
-      <c r="B272" s="8" t="s">
+      <c r="B272" t="s">
         <v>1091</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A273" s="8">
+      <c r="A273">
         <v>271</v>
       </c>
-      <c r="B273" s="8" t="s">
+      <c r="B273" t="s">
         <v>1092</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A274" s="8">
+      <c r="A274">
         <v>272</v>
       </c>
-      <c r="B274" s="8" t="s">
+      <c r="B274" t="s">
         <v>1093</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A275" s="8">
+      <c r="A275">
         <v>273</v>
       </c>
-      <c r="B275" s="8" t="s">
+      <c r="B275" t="s">
         <v>1094</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A276" s="8">
+      <c r="A276">
         <v>274</v>
       </c>
-      <c r="B276" s="8" t="s">
+      <c r="B276" t="s">
         <v>1095</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A277" s="8">
+      <c r="A277">
         <v>275</v>
       </c>
-      <c r="B277" s="8" t="s">
+      <c r="B277" t="s">
         <v>1096</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A278" s="8">
+      <c r="A278">
         <v>276</v>
       </c>
-      <c r="B278" s="8" t="s">
+      <c r="B278" t="s">
         <v>1097</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A279" s="5">
+        <v>277</v>
+      </c>
+      <c r="B279" s="5" t="s">
+        <v>1101</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A280" s="5">
+        <v>278</v>
+      </c>
+      <c r="B280" s="5" t="s">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A281" s="5">
+        <v>279</v>
+      </c>
+      <c r="B281" s="5" t="s">
+        <v>1103</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A282" s="5">
+        <v>280</v>
+      </c>
+      <c r="B282" s="5" t="s">
+        <v>1104</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
TFS 18154 - CSR Incentive Discrepancy feed
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C47162
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="22995" windowHeight="12840" firstSheet="5" activeTab="11"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="22995" windowHeight="12840"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_History" sheetId="14" r:id="rId1"/>
@@ -47,7 +47,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">Coaching_Reason_Selection!$A$1:$P$386</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">DIM_Source!$A$1:$H$58</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">DIM_Source!$A$1:$H$59</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">Email_Notifications!$A$1:$K$175</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3951" uniqueCount="1107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3994" uniqueCount="1111">
   <si>
     <t>SourceID</t>
   </si>
@@ -3405,6 +3405,18 @@
   </si>
   <si>
     <t>Work at Home (Return to Site Only)</t>
+  </si>
+  <si>
+    <t>CSR Incentive Data Feed. Updated DIM_Source and DIM_SubCoaching_Reason, Email_Notifications tabs</t>
+  </si>
+  <si>
+    <t>Internal PRM-O (Incentives Team)</t>
+  </si>
+  <si>
+    <t>OMR: Incentives Data Discrepancy</t>
+  </si>
+  <si>
+    <t>A new eCoaching Log has been entered on your behalf. Please click on the link below to review and verify the coaching opportunity received on &lt;strong&gt;strDateTime&lt;/strong&gt;.</t>
   </si>
 </sst>
 </file>
@@ -3469,7 +3481,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -3484,9 +3496,6 @@
     <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3795,10 +3804,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L101"/>
+  <dimension ref="A1:L104"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="A101" sqref="A101"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="A102" sqref="A102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5276,70 +5285,70 @@
       </c>
     </row>
     <row r="88" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="6">
+      <c r="A88" s="8">
         <v>78</v>
       </c>
-      <c r="B88" s="10">
+      <c r="B88" s="9">
         <v>43714</v>
       </c>
-      <c r="C88" s="6" t="s">
+      <c r="C88" s="8" t="s">
         <v>429</v>
       </c>
-      <c r="D88" s="6">
+      <c r="D88" s="8">
         <v>13644</v>
       </c>
-      <c r="E88" s="6" t="s">
+      <c r="E88" s="8" t="s">
         <v>1035</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" s="8">
+      <c r="A89" s="6">
         <v>79</v>
       </c>
-      <c r="B89" s="9">
+      <c r="B89" s="10">
         <v>43725</v>
       </c>
-      <c r="C89" s="8" t="s">
+      <c r="C89" s="6" t="s">
         <v>429</v>
       </c>
-      <c r="D89" s="8">
+      <c r="D89" s="6">
         <v>15621</v>
       </c>
-      <c r="E89" s="8" t="s">
+      <c r="E89" s="6" t="s">
         <v>1037</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90" s="8">
+      <c r="A90" s="6">
         <v>80</v>
       </c>
-      <c r="B90" s="9">
+      <c r="B90" s="10">
         <v>43731</v>
       </c>
-      <c r="C90" s="8" t="s">
+      <c r="C90" s="6" t="s">
         <v>429</v>
       </c>
-      <c r="D90" s="8">
+      <c r="D90" s="6">
         <v>15450</v>
       </c>
-      <c r="E90" s="12" t="s">
+      <c r="E90" s="6" t="s">
         <v>1038</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A91" s="8">
+      <c r="A91" s="6">
         <v>81</v>
       </c>
-      <c r="B91" s="9">
+      <c r="B91" s="1">
         <v>43731</v>
       </c>
-      <c r="C91" s="8" t="s">
+      <c r="C91" s="6" t="s">
         <v>429</v>
       </c>
-      <c r="D91" s="8">
+      <c r="D91">
         <v>15465</v>
       </c>
-      <c r="E91" s="8" t="s">
+      <c r="E91" t="s">
         <v>1057</v>
       </c>
     </row>
@@ -5347,16 +5356,16 @@
       <c r="A92" s="6">
         <v>82</v>
       </c>
-      <c r="B92" s="10">
+      <c r="B92" s="1">
         <v>43739</v>
       </c>
       <c r="C92" s="6" t="s">
         <v>429</v>
       </c>
-      <c r="D92" s="6">
+      <c r="D92">
         <v>15465</v>
       </c>
-      <c r="E92" s="6" t="s">
+      <c r="E92" t="s">
         <v>1058</v>
       </c>
     </row>
@@ -5378,70 +5387,70 @@
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94" s="8">
+      <c r="A94" s="6">
         <v>84</v>
       </c>
-      <c r="B94" s="9">
+      <c r="B94" s="10">
         <v>43774</v>
       </c>
-      <c r="C94" s="8" t="s">
+      <c r="C94" s="6" t="s">
         <v>429</v>
       </c>
-      <c r="D94" s="8">
+      <c r="D94" s="6">
         <v>15989</v>
       </c>
-      <c r="E94" s="8" t="s">
+      <c r="E94" s="6" t="s">
         <v>1060</v>
       </c>
     </row>
     <row r="95" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="8">
+      <c r="A95" s="6">
         <v>85</v>
       </c>
-      <c r="B95" s="9">
+      <c r="B95" s="10">
         <v>43787</v>
       </c>
-      <c r="C95" s="8" t="s">
+      <c r="C95" s="6" t="s">
         <v>429</v>
       </c>
-      <c r="D95" s="8">
+      <c r="D95" s="6">
         <v>15803</v>
       </c>
-      <c r="E95" s="8" t="s">
+      <c r="E95" s="6" t="s">
         <v>1061</v>
       </c>
     </row>
     <row r="96" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="8">
+      <c r="A96" s="6">
         <v>85.1</v>
       </c>
-      <c r="B96" s="9">
+      <c r="B96" s="1">
         <v>43803</v>
       </c>
-      <c r="C96" s="8" t="s">
+      <c r="C96" s="6" t="s">
         <v>429</v>
       </c>
-      <c r="D96" s="8">
+      <c r="D96">
         <v>15803</v>
       </c>
-      <c r="E96" s="8" t="s">
+      <c r="E96" t="s">
         <v>1076</v>
       </c>
     </row>
     <row r="97" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="8">
+      <c r="A97" s="6">
         <v>86</v>
       </c>
-      <c r="B97" s="9">
+      <c r="B97" s="1">
         <v>43811</v>
       </c>
-      <c r="C97" s="8" t="s">
+      <c r="C97" s="6" t="s">
         <v>429</v>
       </c>
-      <c r="D97" s="8">
+      <c r="D97">
         <v>16261</v>
       </c>
-      <c r="E97" s="8" t="s">
+      <c r="E97" t="s">
         <v>1081</v>
       </c>
     </row>
@@ -5463,55 +5472,84 @@
       </c>
     </row>
     <row r="99" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="8">
+      <c r="A99" s="6">
         <v>88</v>
       </c>
-      <c r="B99" s="9">
+      <c r="B99" s="10">
         <v>43957</v>
       </c>
-      <c r="C99" s="8" t="s">
+      <c r="C99" s="6" t="s">
         <v>429</v>
       </c>
-      <c r="D99" s="8">
+      <c r="D99" s="6">
         <v>17066</v>
       </c>
-      <c r="E99" s="8" t="s">
+      <c r="E99" s="6" t="s">
         <v>1098</v>
       </c>
     </row>
     <row r="100" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="8">
+      <c r="A100" s="6">
         <v>89</v>
       </c>
-      <c r="B100" s="9">
+      <c r="B100" s="10">
         <v>43980</v>
       </c>
-      <c r="C100" s="8" t="s">
+      <c r="C100" s="6" t="s">
         <v>429</v>
       </c>
-      <c r="D100" s="8">
+      <c r="D100" s="6">
         <v>17263</v>
       </c>
-      <c r="E100" s="8" t="s">
+      <c r="E100" s="6" t="s">
         <v>1099</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A101" s="5">
+      <c r="A101" s="6">
         <v>90</v>
       </c>
-      <c r="B101" s="11">
+      <c r="B101" s="1">
         <v>44069</v>
       </c>
-      <c r="C101" s="5" t="s">
+      <c r="C101" s="6" t="s">
         <v>429</v>
       </c>
-      <c r="D101" s="5">
+      <c r="D101">
         <v>18255</v>
       </c>
-      <c r="E101" s="5" t="s">
+      <c r="E101" t="s">
         <v>1105</v>
       </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" s="5">
+        <v>91</v>
+      </c>
+      <c r="B102" s="11">
+        <v>44092</v>
+      </c>
+      <c r="C102" s="5" t="s">
+        <v>429</v>
+      </c>
+      <c r="D102" s="5">
+        <v>18154</v>
+      </c>
+      <c r="E102" s="5" t="s">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" s="6"/>
+      <c r="B103" s="1"/>
+      <c r="C103" s="6"/>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" s="6"/>
+      <c r="B104" s="10"/>
+      <c r="C104" s="6"/>
+      <c r="D104" s="6"/>
+      <c r="E104" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7019,7 +7057,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:P391"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A357" workbookViewId="0">
+    <sheetView topLeftCell="A357" workbookViewId="0">
       <selection activeCell="B388" sqref="B388:B391"/>
     </sheetView>
   </sheetViews>
@@ -26721,10 +26759,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K175"/>
+  <dimension ref="A1:K179"/>
   <sheetViews>
-    <sheetView topLeftCell="A154" workbookViewId="0">
-      <selection activeCell="A171" sqref="A171:I175"/>
+    <sheetView topLeftCell="A160" workbookViewId="0">
+      <selection activeCell="A176" sqref="A176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32720,10 +32758,10 @@
       <c r="I171" s="8" t="s">
         <v>1075</v>
       </c>
-      <c r="J171" s="5">
-        <v>0</v>
-      </c>
-      <c r="K171" s="5" t="s">
+      <c r="J171" s="8">
+        <v>0</v>
+      </c>
+      <c r="K171" s="8" t="s">
         <v>377</v>
       </c>
     </row>
@@ -32755,10 +32793,10 @@
       <c r="I172" s="8" t="s">
         <v>1075</v>
       </c>
-      <c r="J172" s="5">
-        <v>0</v>
-      </c>
-      <c r="K172" s="5" t="s">
+      <c r="J172" s="8">
+        <v>0</v>
+      </c>
+      <c r="K172" s="8" t="s">
         <v>377</v>
       </c>
     </row>
@@ -32790,10 +32828,10 @@
       <c r="I173" s="8" t="s">
         <v>1075</v>
       </c>
-      <c r="J173" s="5">
-        <v>0</v>
-      </c>
-      <c r="K173" s="5" t="s">
+      <c r="J173" s="8">
+        <v>0</v>
+      </c>
+      <c r="K173" s="8" t="s">
         <v>377</v>
       </c>
     </row>
@@ -32825,10 +32863,10 @@
       <c r="I174" s="8" t="s">
         <v>1075</v>
       </c>
-      <c r="J174" s="5">
-        <v>0</v>
-      </c>
-      <c r="K174" s="5" t="s">
+      <c r="J174" s="8">
+        <v>0</v>
+      </c>
+      <c r="K174" s="8" t="s">
         <v>377</v>
       </c>
     </row>
@@ -32860,10 +32898,150 @@
       <c r="I175" s="8" t="s">
         <v>1075</v>
       </c>
-      <c r="J175" s="5">
-        <v>0</v>
-      </c>
-      <c r="K175" s="5" t="s">
+      <c r="J175" s="8">
+        <v>0</v>
+      </c>
+      <c r="K175" s="8" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A176" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="B176" s="5" t="s">
+        <v>383</v>
+      </c>
+      <c r="C176" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D176" s="5" t="s">
+        <v>1108</v>
+      </c>
+      <c r="E176" s="5">
+        <v>0</v>
+      </c>
+      <c r="F176" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="G176" s="5" t="s">
+        <v>422</v>
+      </c>
+      <c r="H176" s="5" t="s">
+        <v>381</v>
+      </c>
+      <c r="I176" s="5" t="s">
+        <v>1110</v>
+      </c>
+      <c r="J176" s="5">
+        <v>0</v>
+      </c>
+      <c r="K176" s="5" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A177" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B177" s="5" t="s">
+        <v>383</v>
+      </c>
+      <c r="C177" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D177" s="5" t="s">
+        <v>1108</v>
+      </c>
+      <c r="E177" s="5">
+        <v>0</v>
+      </c>
+      <c r="F177" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="G177" s="5" t="s">
+        <v>422</v>
+      </c>
+      <c r="H177" s="5" t="s">
+        <v>381</v>
+      </c>
+      <c r="I177" s="5" t="s">
+        <v>1110</v>
+      </c>
+      <c r="J177" s="5">
+        <v>0</v>
+      </c>
+      <c r="K177" s="5" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A178" s="5" t="s">
+        <v>476</v>
+      </c>
+      <c r="B178" s="5" t="s">
+        <v>383</v>
+      </c>
+      <c r="C178" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D178" s="5" t="s">
+        <v>1108</v>
+      </c>
+      <c r="E178" s="5">
+        <v>0</v>
+      </c>
+      <c r="F178" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="G178" s="5" t="s">
+        <v>422</v>
+      </c>
+      <c r="H178" s="5" t="s">
+        <v>381</v>
+      </c>
+      <c r="I178" s="5" t="s">
+        <v>1110</v>
+      </c>
+      <c r="J178" s="5">
+        <v>0</v>
+      </c>
+      <c r="K178" s="5" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A179" s="5" t="s">
+        <v>545</v>
+      </c>
+      <c r="B179" s="5" t="s">
+        <v>383</v>
+      </c>
+      <c r="C179" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D179" s="5" t="s">
+        <v>1108</v>
+      </c>
+      <c r="E179" s="5">
+        <v>0</v>
+      </c>
+      <c r="F179" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="G179" s="5" t="s">
+        <v>422</v>
+      </c>
+      <c r="H179" s="5" t="s">
+        <v>381</v>
+      </c>
+      <c r="I179" s="5" t="s">
+        <v>1110</v>
+      </c>
+      <c r="J179" s="5">
+        <v>0</v>
+      </c>
+      <c r="K179" s="5" t="s">
         <v>377</v>
       </c>
     </row>
@@ -33691,7 +33869,7 @@
       <c r="G8" s="5">
         <v>0</v>
       </c>
-      <c r="H8" s="13">
+      <c r="H8" s="12">
         <v>43577.559065011577</v>
       </c>
       <c r="I8" s="5">
@@ -34120,9 +34298,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I75"/>
+  <dimension ref="A1:I77"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -35262,44 +35442,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>201</v>
-      </c>
-      <c r="B40" t="s">
-        <v>3</v>
-      </c>
-      <c r="C40" t="s">
-        <v>6</v>
-      </c>
-      <c r="D40">
-        <v>1</v>
-      </c>
-      <c r="E40">
-        <v>1</v>
-      </c>
-      <c r="F40">
-        <v>0</v>
-      </c>
-      <c r="G40">
-        <v>0</v>
-      </c>
-      <c r="H40">
-        <v>0</v>
-      </c>
-      <c r="I40">
+    <row r="40" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="5">
+        <v>137</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>1108</v>
+      </c>
+      <c r="D40" s="5">
+        <v>1</v>
+      </c>
+      <c r="E40" s="5">
+        <v>0</v>
+      </c>
+      <c r="F40" s="5">
+        <v>0</v>
+      </c>
+      <c r="G40" s="5">
+        <v>0</v>
+      </c>
+      <c r="H40" s="5">
+        <v>0</v>
+      </c>
+      <c r="I40" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B41" t="s">
         <v>3</v>
       </c>
       <c r="C41" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D41">
         <v>1</v>
@@ -35311,24 +35491,24 @@
         <v>0</v>
       </c>
       <c r="G41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H41">
         <v>0</v>
       </c>
       <c r="I41">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B42" t="s">
         <v>3</v>
       </c>
       <c r="C42" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D42">
         <v>1</v>
@@ -35343,7 +35523,7 @@
         <v>1</v>
       </c>
       <c r="H42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I42">
         <v>1</v>
@@ -35351,13 +35531,13 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B43" t="s">
         <v>3</v>
       </c>
       <c r="C43" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D43">
         <v>1</v>
@@ -35372,21 +35552,21 @@
         <v>1</v>
       </c>
       <c r="H43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I43">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B44" t="s">
         <v>3</v>
       </c>
       <c r="C44" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D44">
         <v>1</v>
@@ -35404,18 +35584,18 @@
         <v>0</v>
       </c>
       <c r="I44">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B45" t="s">
         <v>3</v>
       </c>
       <c r="C45" t="s">
-        <v>169</v>
+        <v>10</v>
       </c>
       <c r="D45">
         <v>1</v>
@@ -35430,7 +35610,7 @@
         <v>1</v>
       </c>
       <c r="H45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I45">
         <v>1</v>
@@ -35438,13 +35618,13 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B46" t="s">
         <v>3</v>
       </c>
       <c r="C46" t="s">
-        <v>11</v>
+        <v>169</v>
       </c>
       <c r="D46">
         <v>1</v>
@@ -35459,7 +35639,7 @@
         <v>1</v>
       </c>
       <c r="H46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I46">
         <v>1</v>
@@ -35467,13 +35647,13 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B47" t="s">
         <v>3</v>
       </c>
       <c r="C47" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D47">
         <v>1</v>
@@ -35482,27 +35662,27 @@
         <v>1</v>
       </c>
       <c r="F47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G47">
         <v>1</v>
       </c>
       <c r="H47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I47">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B48" t="s">
         <v>3</v>
       </c>
       <c r="C48" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D48">
         <v>1</v>
@@ -35517,21 +35697,21 @@
         <v>1</v>
       </c>
       <c r="H48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I48">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B49" t="s">
         <v>3</v>
       </c>
       <c r="C49" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D49">
         <v>1</v>
@@ -35549,30 +35729,30 @@
         <v>0</v>
       </c>
       <c r="I49">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B50" t="s">
         <v>3</v>
       </c>
       <c r="C50" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D50">
         <v>1</v>
       </c>
       <c r="E50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H50">
         <v>0</v>
@@ -35583,13 +35763,13 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B51" t="s">
         <v>3</v>
       </c>
       <c r="C51" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D51">
         <v>1</v>
@@ -35612,13 +35792,13 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B52" t="s">
         <v>3</v>
       </c>
       <c r="C52" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D52">
         <v>1</v>
@@ -35641,13 +35821,13 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B53" t="s">
         <v>3</v>
       </c>
       <c r="C53" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D53">
         <v>1</v>
@@ -35670,13 +35850,13 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B54" t="s">
         <v>3</v>
       </c>
       <c r="C54" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D54">
         <v>1</v>
@@ -35699,13 +35879,13 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B55" t="s">
         <v>3</v>
       </c>
       <c r="C55" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D55">
         <v>1</v>
@@ -35728,13 +35908,13 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B56" t="s">
         <v>3</v>
       </c>
       <c r="C56" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D56">
         <v>1</v>
@@ -35757,71 +35937,71 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B57" t="s">
         <v>3</v>
       </c>
       <c r="C57" t="s">
-        <v>170</v>
+        <v>21</v>
       </c>
       <c r="D57">
         <v>1</v>
       </c>
       <c r="E57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H57">
         <v>0</v>
       </c>
       <c r="I57">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B58" t="s">
         <v>3</v>
       </c>
       <c r="C58" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="D58">
         <v>1</v>
       </c>
       <c r="E58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F58">
         <v>1</v>
       </c>
       <c r="G58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H58">
         <v>0</v>
       </c>
       <c r="I58">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B59" t="s">
         <v>3</v>
       </c>
       <c r="C59" t="s">
-        <v>436</v>
+        <v>175</v>
       </c>
       <c r="D59">
         <v>1</v>
@@ -35830,7 +36010,7 @@
         <v>0</v>
       </c>
       <c r="F59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G59">
         <v>0</v>
@@ -35844,13 +36024,13 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B60" t="s">
         <v>3</v>
       </c>
       <c r="C60" t="s">
-        <v>171</v>
+        <v>436</v>
       </c>
       <c r="D60">
         <v>1</v>
@@ -35873,13 +36053,13 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B61" t="s">
         <v>3</v>
       </c>
       <c r="C61" t="s">
-        <v>469</v>
+        <v>171</v>
       </c>
       <c r="D61">
         <v>1</v>
@@ -35902,13 +36082,13 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B62" t="s">
         <v>3</v>
       </c>
       <c r="C62" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="D62">
         <v>1</v>
@@ -35931,13 +36111,13 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B63" t="s">
         <v>3</v>
       </c>
       <c r="C63" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D63">
         <v>1</v>
@@ -35960,13 +36140,13 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B64" t="s">
         <v>3</v>
       </c>
       <c r="C64" t="s">
-        <v>486</v>
+        <v>468</v>
       </c>
       <c r="D64">
         <v>1</v>
@@ -35981,7 +36161,7 @@
         <v>0</v>
       </c>
       <c r="H64">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I64">
         <v>0</v>
@@ -35989,16 +36169,16 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B65" t="s">
         <v>3</v>
       </c>
       <c r="C65" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="D65">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E65">
         <v>0</v>
@@ -36010,7 +36190,7 @@
         <v>0</v>
       </c>
       <c r="H65">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I65">
         <v>0</v>
@@ -36018,16 +36198,16 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B66" t="s">
         <v>3</v>
       </c>
       <c r="C66" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D66">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E66">
         <v>0</v>
@@ -36039,7 +36219,7 @@
         <v>0</v>
       </c>
       <c r="H66">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I66">
         <v>0</v>
@@ -36047,13 +36227,13 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B67" t="s">
         <v>3</v>
       </c>
       <c r="C67" t="s">
-        <v>547</v>
+        <v>488</v>
       </c>
       <c r="D67">
         <v>1</v>
@@ -36068,21 +36248,21 @@
         <v>0</v>
       </c>
       <c r="H67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I67">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B68" t="s">
         <v>3</v>
       </c>
       <c r="C68" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="D68">
         <v>1</v>
@@ -36105,13 +36285,13 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B69" t="s">
         <v>3</v>
       </c>
       <c r="C69" t="s">
-        <v>691</v>
+        <v>548</v>
       </c>
       <c r="D69">
         <v>1</v>
@@ -36129,105 +36309,105 @@
         <v>0</v>
       </c>
       <c r="I69">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B70" t="s">
         <v>3</v>
       </c>
       <c r="C70" t="s">
+        <v>691</v>
+      </c>
+      <c r="D70">
+        <v>1</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
+      </c>
+      <c r="F70">
+        <v>0</v>
+      </c>
+      <c r="G70">
+        <v>0</v>
+      </c>
+      <c r="H70">
+        <v>0</v>
+      </c>
+      <c r="I70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>231</v>
+      </c>
+      <c r="B71" t="s">
+        <v>3</v>
+      </c>
+      <c r="C71" t="s">
         <v>739</v>
       </c>
-      <c r="D70">
-        <v>0</v>
-      </c>
-      <c r="E70">
-        <v>0</v>
-      </c>
-      <c r="F70">
-        <v>0</v>
-      </c>
-      <c r="G70">
-        <v>0</v>
-      </c>
-      <c r="H70">
-        <v>0</v>
-      </c>
-      <c r="I70">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="8">
+      <c r="D71">
+        <v>0</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
+      </c>
+      <c r="F71">
+        <v>0</v>
+      </c>
+      <c r="G71">
+        <v>0</v>
+      </c>
+      <c r="H71">
+        <v>0</v>
+      </c>
+      <c r="I71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="8">
         <v>232</v>
       </c>
-      <c r="B71" s="8" t="s">
+      <c r="B72" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C71" s="8" t="s">
+      <c r="C72" s="8" t="s">
         <v>822</v>
       </c>
-      <c r="D71" s="8">
-        <v>1</v>
-      </c>
-      <c r="E71" s="8">
-        <v>0</v>
-      </c>
-      <c r="F71" s="8">
-        <v>0</v>
-      </c>
-      <c r="G71" s="8">
-        <v>0</v>
-      </c>
-      <c r="H71" s="8">
-        <v>0</v>
-      </c>
-      <c r="I71" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A72">
-        <v>233</v>
-      </c>
-      <c r="B72" t="s">
-        <v>3</v>
-      </c>
-      <c r="C72" t="s">
-        <v>825</v>
-      </c>
-      <c r="D72">
-        <v>1</v>
-      </c>
-      <c r="E72">
-        <v>0</v>
-      </c>
-      <c r="F72">
-        <v>0</v>
-      </c>
-      <c r="G72">
-        <v>0</v>
-      </c>
-      <c r="H72">
-        <v>0</v>
-      </c>
-      <c r="I72">
+      <c r="D72" s="8">
+        <v>1</v>
+      </c>
+      <c r="E72" s="8">
+        <v>0</v>
+      </c>
+      <c r="F72" s="8">
+        <v>0</v>
+      </c>
+      <c r="G72" s="8">
+        <v>0</v>
+      </c>
+      <c r="H72" s="8">
+        <v>0</v>
+      </c>
+      <c r="I72" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B73" t="s">
         <v>3</v>
       </c>
       <c r="C73" t="s">
-        <v>969</v>
+        <v>825</v>
       </c>
       <c r="D73">
         <v>1</v>
@@ -36250,13 +36430,13 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B74" t="s">
         <v>3</v>
       </c>
       <c r="C74" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
       <c r="D74">
         <v>1</v>
@@ -36279,30 +36459,88 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B75" t="s">
         <v>3</v>
       </c>
       <c r="C75" t="s">
+        <v>971</v>
+      </c>
+      <c r="D75">
+        <v>1</v>
+      </c>
+      <c r="E75">
+        <v>0</v>
+      </c>
+      <c r="F75">
+        <v>0</v>
+      </c>
+      <c r="G75">
+        <v>0</v>
+      </c>
+      <c r="H75">
+        <v>0</v>
+      </c>
+      <c r="I75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>236</v>
+      </c>
+      <c r="B76" t="s">
+        <v>3</v>
+      </c>
+      <c r="C76" t="s">
         <v>972</v>
       </c>
-      <c r="D75">
-        <v>1</v>
-      </c>
-      <c r="E75">
-        <v>0</v>
-      </c>
-      <c r="F75">
-        <v>0</v>
-      </c>
-      <c r="G75">
-        <v>0</v>
-      </c>
-      <c r="H75">
-        <v>0</v>
-      </c>
-      <c r="I75">
+      <c r="D76">
+        <v>1</v>
+      </c>
+      <c r="E76">
+        <v>0</v>
+      </c>
+      <c r="F76">
+        <v>0</v>
+      </c>
+      <c r="G76">
+        <v>0</v>
+      </c>
+      <c r="H76">
+        <v>0</v>
+      </c>
+      <c r="I76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" s="5">
+        <v>237</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>1108</v>
+      </c>
+      <c r="D77" s="5">
+        <v>1</v>
+      </c>
+      <c r="E77" s="5">
+        <v>0</v>
+      </c>
+      <c r="F77" s="5">
+        <v>0</v>
+      </c>
+      <c r="G77" s="5">
+        <v>0</v>
+      </c>
+      <c r="H77" s="5">
+        <v>0</v>
+      </c>
+      <c r="I77" s="5">
         <v>0</v>
       </c>
     </row>
@@ -38418,7 +38656,7 @@
       <c r="B5" s="5" t="s">
         <v>378</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="13" t="s">
         <v>1085</v>
       </c>
     </row>
@@ -40785,7 +41023,7 @@
   <dimension ref="A1:B65"/>
   <sheetViews>
     <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+      <selection activeCell="A65" sqref="A65:B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -41307,10 +41545,10 @@
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="5">
+      <c r="A65" s="8">
         <v>63</v>
       </c>
-      <c r="B65" s="5" t="s">
+      <c r="B65" s="8" t="s">
         <v>1106</v>
       </c>
     </row>
@@ -41321,10 +41559,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B282"/>
+  <dimension ref="A1:B283"/>
   <sheetViews>
     <sheetView topLeftCell="A255" workbookViewId="0">
-      <selection activeCell="A279" sqref="A279:B282"/>
+      <selection activeCell="B283" sqref="B283"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43558,35 +43796,43 @@
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A279" s="5">
+      <c r="A279" s="8">
         <v>277</v>
       </c>
-      <c r="B279" s="5" t="s">
+      <c r="B279" s="8" t="s">
         <v>1101</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A280" s="5">
+      <c r="A280" s="8">
         <v>278</v>
       </c>
-      <c r="B280" s="5" t="s">
+      <c r="B280" s="8" t="s">
         <v>1102</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A281" s="5">
+      <c r="A281" s="8">
         <v>279</v>
       </c>
-      <c r="B281" s="5" t="s">
+      <c r="B281" s="8" t="s">
         <v>1103</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A282" s="5">
+      <c r="A282" s="8">
         <v>280</v>
       </c>
-      <c r="B282" s="5" t="s">
+      <c r="B282" s="8" t="s">
         <v>1104</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A283" s="5">
+        <v>281</v>
+      </c>
+      <c r="B283" s="5" t="s">
+        <v>1109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TFS 19937 - Generate coaching log for CSRs regarding credit card policy
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C48401
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OmniCloud\eCoaching_V2\Design\DD\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C04D7982-0A0C-4466-A6A3-40FCCD027A43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B6F0911-ED96-4E03-B742-22D145EFEB53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="204" yWindow="0" windowWidth="22974" windowHeight="12360" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_History" sheetId="14" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3997" uniqueCount="1113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4017" uniqueCount="1114">
   <si>
     <t>SourceID</t>
   </si>
@@ -3424,6 +3424,9 @@
   </si>
   <si>
     <t>Attendance Earn Back Day</t>
+  </si>
+  <si>
+    <t>Generate coaching log for CSRs regarding credit card policy. Added rows to Email_Notifications Table</t>
   </si>
 </sst>
 </file>
@@ -3847,8 +3850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L104"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="A103" sqref="A103:E103"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="E104" sqref="E104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -5581,28 +5584,38 @@
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A103" s="5">
+      <c r="A103" s="8">
         <v>92</v>
       </c>
-      <c r="B103" s="11">
+      <c r="B103" s="9">
         <v>44165</v>
       </c>
-      <c r="C103" s="5" t="s">
+      <c r="C103" s="8" t="s">
         <v>429</v>
       </c>
-      <c r="D103" s="5">
+      <c r="D103" s="8">
         <v>19502</v>
       </c>
-      <c r="E103" s="5" t="s">
+      <c r="E103" s="8" t="s">
         <v>1111</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A104" s="6"/>
-      <c r="B104" s="10"/>
-      <c r="C104" s="6"/>
-      <c r="D104" s="6"/>
-      <c r="E104" s="6"/>
+      <c r="A104" s="5">
+        <v>93</v>
+      </c>
+      <c r="B104" s="11">
+        <v>44222</v>
+      </c>
+      <c r="C104" s="5" t="s">
+        <v>429</v>
+      </c>
+      <c r="D104" s="5">
+        <v>19937</v>
+      </c>
+      <c r="E104" s="5" t="s">
+        <v>1113</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -26812,10 +26825,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:K179"/>
+  <dimension ref="A1:K181"/>
   <sheetViews>
-    <sheetView topLeftCell="A160" workbookViewId="0">
-      <selection activeCell="A176" sqref="A176"/>
+    <sheetView topLeftCell="A169" workbookViewId="0">
+      <selection activeCell="A180" sqref="A180:K181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -32958,143 +32971,213 @@
         <v>377</v>
       </c>
     </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A176" s="5" t="s">
+    <row r="176" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A176" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="B176" s="5" t="s">
+      <c r="B176" s="8" t="s">
         <v>383</v>
       </c>
-      <c r="C176" s="5" t="s">
+      <c r="C176" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D176" s="5" t="s">
+      <c r="D176" s="8" t="s">
         <v>1108</v>
       </c>
-      <c r="E176" s="5">
-        <v>0</v>
-      </c>
-      <c r="F176" s="5" t="s">
+      <c r="E176" s="8">
+        <v>0</v>
+      </c>
+      <c r="F176" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="G176" s="5" t="s">
+      <c r="G176" s="8" t="s">
         <v>422</v>
       </c>
-      <c r="H176" s="5" t="s">
+      <c r="H176" s="8" t="s">
         <v>381</v>
       </c>
-      <c r="I176" s="5" t="s">
+      <c r="I176" s="8" t="s">
         <v>1110</v>
       </c>
-      <c r="J176" s="5">
-        <v>0</v>
-      </c>
-      <c r="K176" s="5" t="s">
+      <c r="J176" s="8">
+        <v>0</v>
+      </c>
+      <c r="K176" s="8" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A177" s="5" t="s">
+    <row r="177" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A177" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="B177" s="5" t="s">
+      <c r="B177" s="8" t="s">
         <v>383</v>
       </c>
-      <c r="C177" s="5" t="s">
+      <c r="C177" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D177" s="5" t="s">
+      <c r="D177" s="8" t="s">
         <v>1108</v>
       </c>
-      <c r="E177" s="5">
-        <v>0</v>
-      </c>
-      <c r="F177" s="5" t="s">
+      <c r="E177" s="8">
+        <v>0</v>
+      </c>
+      <c r="F177" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="G177" s="5" t="s">
+      <c r="G177" s="8" t="s">
         <v>422</v>
       </c>
-      <c r="H177" s="5" t="s">
+      <c r="H177" s="8" t="s">
         <v>381</v>
       </c>
-      <c r="I177" s="5" t="s">
+      <c r="I177" s="8" t="s">
         <v>1110</v>
       </c>
-      <c r="J177" s="5">
-        <v>0</v>
-      </c>
-      <c r="K177" s="5" t="s">
+      <c r="J177" s="8">
+        <v>0</v>
+      </c>
+      <c r="K177" s="8" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A178" s="5" t="s">
+    <row r="178" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A178" s="8" t="s">
         <v>476</v>
       </c>
-      <c r="B178" s="5" t="s">
+      <c r="B178" s="8" t="s">
         <v>383</v>
       </c>
-      <c r="C178" s="5" t="s">
+      <c r="C178" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D178" s="5" t="s">
+      <c r="D178" s="8" t="s">
         <v>1108</v>
       </c>
-      <c r="E178" s="5">
-        <v>0</v>
-      </c>
-      <c r="F178" s="5" t="s">
+      <c r="E178" s="8">
+        <v>0</v>
+      </c>
+      <c r="F178" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="G178" s="5" t="s">
+      <c r="G178" s="8" t="s">
         <v>422</v>
       </c>
-      <c r="H178" s="5" t="s">
+      <c r="H178" s="8" t="s">
         <v>381</v>
       </c>
-      <c r="I178" s="5" t="s">
+      <c r="I178" s="8" t="s">
         <v>1110</v>
       </c>
-      <c r="J178" s="5">
-        <v>0</v>
-      </c>
-      <c r="K178" s="5" t="s">
+      <c r="J178" s="8">
+        <v>0</v>
+      </c>
+      <c r="K178" s="8" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A179" s="5" t="s">
+    <row r="179" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A179" s="8" t="s">
         <v>545</v>
       </c>
-      <c r="B179" s="5" t="s">
+      <c r="B179" s="8" t="s">
         <v>383</v>
       </c>
-      <c r="C179" s="5" t="s">
+      <c r="C179" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D179" s="5" t="s">
+      <c r="D179" s="8" t="s">
         <v>1108</v>
       </c>
-      <c r="E179" s="5">
-        <v>0</v>
-      </c>
-      <c r="F179" s="5" t="s">
+      <c r="E179" s="8">
+        <v>0</v>
+      </c>
+      <c r="F179" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="G179" s="5" t="s">
+      <c r="G179" s="8" t="s">
         <v>422</v>
       </c>
-      <c r="H179" s="5" t="s">
+      <c r="H179" s="8" t="s">
         <v>381</v>
       </c>
-      <c r="I179" s="5" t="s">
+      <c r="I179" s="8" t="s">
         <v>1110</v>
       </c>
-      <c r="J179" s="5">
-        <v>0</v>
-      </c>
-      <c r="K179" s="5" t="s">
+      <c r="J179" s="8">
+        <v>0</v>
+      </c>
+      <c r="K179" s="8" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="180" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A180" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="B180" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C180" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D180" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E180" s="5">
+        <v>0</v>
+      </c>
+      <c r="F180" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="G180" s="5" t="s">
+        <v>422</v>
+      </c>
+      <c r="H180" s="5" t="s">
+        <v>381</v>
+      </c>
+      <c r="I180" s="5" t="s">
+        <v>1110</v>
+      </c>
+      <c r="J180" s="5">
+        <v>0</v>
+      </c>
+      <c r="K180" s="5" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="181" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A181" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B181" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C181" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D181" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E181" s="5">
+        <v>0</v>
+      </c>
+      <c r="F181" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="G181" s="5" t="s">
+        <v>422</v>
+      </c>
+      <c r="H181" s="5" t="s">
+        <v>381</v>
+      </c>
+      <c r="I181" s="5" t="s">
+        <v>1110</v>
+      </c>
+      <c r="J181" s="5">
+        <v>0</v>
+      </c>
+      <c r="K181" s="5" t="s">
         <v>377</v>
       </c>
     </row>
@@ -41614,7 +41697,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B284"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A282" workbookViewId="0">
+    <sheetView topLeftCell="A282" workbookViewId="0">
       <selection activeCell="A284" sqref="A284"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
TFS 20256 -  Add Quality Now surveys for additional sites
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C48880
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OmniCloud\eCoaching_V2\Design\DD\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B6F0911-ED96-4E03-B742-22D145EFEB53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D05A721-330C-48C6-B0E1-314BFB5172A3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_History" sheetId="14" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4017" uniqueCount="1114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4019" uniqueCount="1115">
   <si>
     <t>SourceID</t>
   </si>
@@ -2757,9 +2757,6 @@
   </si>
   <si>
     <t>isPilot</t>
-  </si>
-  <si>
-    <t>How prepared was your supervisor during your coaching session?| Please explain below.</t>
   </si>
   <si>
     <t>1 - Very Unprepared</t>
@@ -3427,6 +3424,13 @@
   </si>
   <si>
     <t>Generate coaching log for CSRs regarding credit card policy. Added rows to Email_Notifications Table</t>
+  </si>
+  <si>
+    <t>How prepared was your supervisor during your coaching session? | Please explain below.</t>
+  </si>
+  <si>
+    <t>Set additional sites as isPilot = 1 and Activated the Extra HotTopic question for the duration of the QN Survey pilot for additional saites.
+*isPilot for Bogalusa, Brownsville, Lawrence, Phoenix, Sandy(Phase III sites) set as Active but will be Updated in database via admin task afterMay 1st.</t>
   </si>
 </sst>
 </file>
@@ -3453,7 +3457,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3478,6 +3482,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -3491,7 +3501,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -3510,6 +3520,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3848,10 +3860,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L104"/>
+  <dimension ref="A1:L105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="E104" sqref="E104"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="A105" sqref="A105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -4961,7 +4973,7 @@
         <v>9511</v>
       </c>
       <c r="E66" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -4978,7 +4990,7 @@
         <v>7136</v>
       </c>
       <c r="E67" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -4995,7 +5007,7 @@
         <v>10890</v>
       </c>
       <c r="E68" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -5012,7 +5024,7 @@
         <v>7137</v>
       </c>
       <c r="E69" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -5029,7 +5041,7 @@
         <v>7137</v>
       </c>
       <c r="E70" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -5046,7 +5058,7 @@
         <v>11500</v>
       </c>
       <c r="E71" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -5063,7 +5075,7 @@
         <v>11451</v>
       </c>
       <c r="E72" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -5080,7 +5092,7 @@
         <v>12308</v>
       </c>
       <c r="E73" s="8" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -5097,7 +5109,7 @@
         <v>12308</v>
       </c>
       <c r="E74" s="8" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="75" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -5114,7 +5126,7 @@
         <v>12316</v>
       </c>
       <c r="E75" s="6" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="76" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -5131,7 +5143,7 @@
         <v>12455</v>
       </c>
       <c r="E76" s="6" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="F76" s="6"/>
       <c r="G76" s="10"/>
@@ -5155,7 +5167,7 @@
         <v>12467</v>
       </c>
       <c r="E77" s="6" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
     </row>
     <row r="78" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -5172,7 +5184,7 @@
         <v>12591</v>
       </c>
       <c r="E78" s="8" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
     <row r="79" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -5189,7 +5201,7 @@
         <v>12591</v>
       </c>
       <c r="E79" s="8" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -5206,7 +5218,7 @@
         <v>13334</v>
       </c>
       <c r="E80" s="6" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -5223,7 +5235,7 @@
         <v>13643</v>
       </c>
       <c r="E81" s="6" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="82" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -5240,7 +5252,7 @@
         <v>13332</v>
       </c>
       <c r="E82" s="8" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="83" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -5257,7 +5269,7 @@
         <v>14178</v>
       </c>
       <c r="E83" s="8" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="84" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -5274,7 +5286,7 @@
         <v>14108</v>
       </c>
       <c r="E84" s="6" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -5291,7 +5303,7 @@
         <v>15063</v>
       </c>
       <c r="E85" s="6" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -5308,7 +5320,7 @@
         <v>15144</v>
       </c>
       <c r="E86" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -5325,7 +5337,7 @@
         <v>15095</v>
       </c>
       <c r="E87" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="88" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -5342,7 +5354,7 @@
         <v>13644</v>
       </c>
       <c r="E88" s="8" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -5359,7 +5371,7 @@
         <v>15621</v>
       </c>
       <c r="E89" s="6" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -5376,7 +5388,7 @@
         <v>15450</v>
       </c>
       <c r="E90" s="6" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -5393,7 +5405,7 @@
         <v>15465</v>
       </c>
       <c r="E91" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="92" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -5410,7 +5422,7 @@
         <v>15465</v>
       </c>
       <c r="E92" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -5427,7 +5439,7 @@
         <v>15859</v>
       </c>
       <c r="E93" s="8" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -5444,7 +5456,7 @@
         <v>15989</v>
       </c>
       <c r="E94" s="6" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="95" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -5461,7 +5473,7 @@
         <v>15803</v>
       </c>
       <c r="E95" s="6" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="96" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -5478,7 +5490,7 @@
         <v>15803</v>
       </c>
       <c r="E96" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="97" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -5495,7 +5507,7 @@
         <v>16261</v>
       </c>
       <c r="E97" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="98" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -5512,7 +5524,7 @@
         <v>16389</v>
       </c>
       <c r="E98" s="8" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="99" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -5529,7 +5541,7 @@
         <v>17066</v>
       </c>
       <c r="E99" s="6" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="100" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -5546,7 +5558,7 @@
         <v>17263</v>
       </c>
       <c r="E100" s="6" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -5563,7 +5575,7 @@
         <v>18255</v>
       </c>
       <c r="E101" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="102" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -5580,7 +5592,7 @@
         <v>18154</v>
       </c>
       <c r="E102" s="6" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -5597,24 +5609,41 @@
         <v>19502</v>
       </c>
       <c r="E103" s="8" t="s">
-        <v>1111</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A104" s="5">
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A104" s="8">
         <v>93</v>
       </c>
-      <c r="B104" s="11">
+      <c r="B104" s="9">
         <v>44222</v>
       </c>
-      <c r="C104" s="5" t="s">
+      <c r="C104" s="8" t="s">
         <v>429</v>
       </c>
-      <c r="D104" s="5">
+      <c r="D104" s="8">
         <v>19937</v>
       </c>
-      <c r="E104" s="5" t="s">
-        <v>1113</v>
+      <c r="E104" s="8" t="s">
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A105" s="5">
+        <v>94</v>
+      </c>
+      <c r="B105" s="11">
+        <v>44277</v>
+      </c>
+      <c r="C105" s="5" t="s">
+        <v>429</v>
+      </c>
+      <c r="D105" s="5">
+        <v>20256</v>
+      </c>
+      <c r="E105" s="13" t="s">
+        <v>1114</v>
       </c>
     </row>
   </sheetData>
@@ -6969,10 +6998,10 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="6" t="s">
+        <v>964</v>
+      </c>
+      <c r="B59" s="6" t="s">
         <v>965</v>
-      </c>
-      <c r="B59" s="6" t="s">
-        <v>966</v>
       </c>
       <c r="C59" s="6">
         <v>1</v>
@@ -6992,10 +7021,10 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="8" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="C60" s="8">
         <v>1</v>
@@ -7040,7 +7069,7 @@
         <v>172</v>
       </c>
       <c r="D1" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -7062,7 +7091,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -7194,7 +7223,7 @@
         <v>251</v>
       </c>
       <c r="D2" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -7494,7 +7523,7 @@
         <v>251</v>
       </c>
       <c r="D8" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -7794,7 +7823,7 @@
         <v>251</v>
       </c>
       <c r="D14" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -15394,7 +15423,7 @@
         <v>245</v>
       </c>
       <c r="D166" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="E166">
         <v>0</v>
@@ -15444,7 +15473,7 @@
         <v>246</v>
       </c>
       <c r="D167" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="E167">
         <v>0</v>
@@ -15494,7 +15523,7 @@
         <v>247</v>
       </c>
       <c r="D168" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="E168">
         <v>0</v>
@@ -15544,7 +15573,7 @@
         <v>248</v>
       </c>
       <c r="D169" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="E169">
         <v>0</v>
@@ -15594,7 +15623,7 @@
         <v>246</v>
       </c>
       <c r="D170" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="E170">
         <v>0</v>
@@ -15644,7 +15673,7 @@
         <v>247</v>
       </c>
       <c r="D171" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="E171">
         <v>0</v>
@@ -15694,7 +15723,7 @@
         <v>248</v>
       </c>
       <c r="D172" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="E172">
         <v>0</v>
@@ -15744,7 +15773,7 @@
         <v>246</v>
       </c>
       <c r="D173" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="E173">
         <v>0</v>
@@ -15794,7 +15823,7 @@
         <v>247</v>
       </c>
       <c r="D174" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="E174">
         <v>0</v>
@@ -15844,7 +15873,7 @@
         <v>248</v>
       </c>
       <c r="D175" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="E175">
         <v>0</v>
@@ -15894,7 +15923,7 @@
         <v>249</v>
       </c>
       <c r="D176" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="E176">
         <v>1</v>
@@ -15938,7 +15967,7 @@
         <v>59</v>
       </c>
       <c r="B177" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="C177">
         <v>42</v>
@@ -16094,7 +16123,7 @@
         <v>253</v>
       </c>
       <c r="D180" s="8" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="E180" s="8">
         <v>1</v>
@@ -16144,7 +16173,7 @@
         <v>254</v>
       </c>
       <c r="D181" s="8" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="E181" s="8">
         <v>1</v>
@@ -16194,7 +16223,7 @@
         <v>255</v>
       </c>
       <c r="D182" s="8" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="E182" s="8">
         <v>1</v>
@@ -16244,7 +16273,7 @@
         <v>256</v>
       </c>
       <c r="D183" s="8" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="E183" s="8">
         <v>1</v>
@@ -16294,7 +16323,7 @@
         <v>257</v>
       </c>
       <c r="D184" s="8" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="E184" s="8">
         <v>1</v>
@@ -16344,7 +16373,7 @@
         <v>258</v>
       </c>
       <c r="D185" s="8" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="E185" s="8">
         <v>1</v>
@@ -16394,7 +16423,7 @@
         <v>259</v>
       </c>
       <c r="D186" s="8" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="E186" s="8">
         <v>1</v>
@@ -16444,7 +16473,7 @@
         <v>260</v>
       </c>
       <c r="D187" s="8" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="E187" s="8">
         <v>1</v>
@@ -16494,7 +16523,7 @@
         <v>261</v>
       </c>
       <c r="D188" s="8" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="E188" s="8">
         <v>1</v>
@@ -16544,7 +16573,7 @@
         <v>262</v>
       </c>
       <c r="D189" s="8" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="E189" s="8">
         <v>1</v>
@@ -16594,7 +16623,7 @@
         <v>263</v>
       </c>
       <c r="D190" s="8" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="E190" s="8">
         <v>1</v>
@@ -16694,7 +16723,7 @@
         <v>265</v>
       </c>
       <c r="D192" s="8" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="E192" s="8">
         <v>1</v>
@@ -16844,7 +16873,7 @@
         <v>253</v>
       </c>
       <c r="D195" s="8" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="E195" s="8">
         <v>1</v>
@@ -16894,7 +16923,7 @@
         <v>254</v>
       </c>
       <c r="D196" s="8" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="E196" s="8">
         <v>1</v>
@@ -16944,7 +16973,7 @@
         <v>255</v>
       </c>
       <c r="D197" s="8" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="E197" s="8">
         <v>1</v>
@@ -16994,7 +17023,7 @@
         <v>256</v>
       </c>
       <c r="D198" s="8" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="E198" s="8">
         <v>1</v>
@@ -17044,7 +17073,7 @@
         <v>257</v>
       </c>
       <c r="D199" s="8" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="E199" s="8">
         <v>1</v>
@@ -17094,7 +17123,7 @@
         <v>258</v>
       </c>
       <c r="D200" s="8" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="E200" s="8">
         <v>1</v>
@@ -17144,7 +17173,7 @@
         <v>259</v>
       </c>
       <c r="D201" s="8" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="E201" s="8">
         <v>1</v>
@@ -17194,7 +17223,7 @@
         <v>260</v>
       </c>
       <c r="D202" s="8" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="E202" s="8">
         <v>1</v>
@@ -17244,7 +17273,7 @@
         <v>261</v>
       </c>
       <c r="D203" s="8" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="E203" s="8">
         <v>1</v>
@@ -17294,7 +17323,7 @@
         <v>262</v>
       </c>
       <c r="D204" s="8" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="E204" s="8">
         <v>1</v>
@@ -17344,7 +17373,7 @@
         <v>263</v>
       </c>
       <c r="D205" s="8" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="E205" s="8">
         <v>1</v>
@@ -17444,7 +17473,7 @@
         <v>265</v>
       </c>
       <c r="D207" s="8" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="E207" s="8">
         <v>1</v>
@@ -17594,7 +17623,7 @@
         <v>253</v>
       </c>
       <c r="D210" s="8" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="E210" s="8">
         <v>1</v>
@@ -17644,7 +17673,7 @@
         <v>254</v>
       </c>
       <c r="D211" s="8" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="E211" s="8">
         <v>1</v>
@@ -17694,7 +17723,7 @@
         <v>255</v>
       </c>
       <c r="D212" s="8" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="E212" s="8">
         <v>1</v>
@@ -17744,7 +17773,7 @@
         <v>256</v>
       </c>
       <c r="D213" s="8" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="E213" s="8">
         <v>1</v>
@@ -17794,7 +17823,7 @@
         <v>257</v>
       </c>
       <c r="D214" s="8" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="E214" s="8">
         <v>1</v>
@@ -17844,7 +17873,7 @@
         <v>258</v>
       </c>
       <c r="D215" s="8" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="E215" s="8">
         <v>1</v>
@@ -17894,7 +17923,7 @@
         <v>259</v>
       </c>
       <c r="D216" s="8" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="E216" s="8">
         <v>1</v>
@@ -17944,7 +17973,7 @@
         <v>260</v>
       </c>
       <c r="D217" s="8" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="E217" s="8">
         <v>1</v>
@@ -17994,7 +18023,7 @@
         <v>261</v>
       </c>
       <c r="D218" s="8" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="E218" s="8">
         <v>1</v>
@@ -18044,7 +18073,7 @@
         <v>262</v>
       </c>
       <c r="D219" s="8" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="E219" s="8">
         <v>1</v>
@@ -18094,7 +18123,7 @@
         <v>263</v>
       </c>
       <c r="D220" s="8" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="E220" s="8">
         <v>1</v>
@@ -18194,7 +18223,7 @@
         <v>265</v>
       </c>
       <c r="D222" s="8" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="E222" s="8">
         <v>1</v>
@@ -18238,7 +18267,7 @@
         <v>60</v>
       </c>
       <c r="B223" s="8" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="C223" s="8">
         <v>95</v>
@@ -18288,7 +18317,7 @@
         <v>60</v>
       </c>
       <c r="B224" s="8" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="C224" s="8">
         <v>155</v>
@@ -18338,7 +18367,7 @@
         <v>60</v>
       </c>
       <c r="B225" s="8" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="C225" s="8">
         <v>178</v>
@@ -18388,13 +18417,13 @@
         <v>60</v>
       </c>
       <c r="B226" s="8" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="C226" s="8">
         <v>253</v>
       </c>
       <c r="D226" s="8" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="E226" s="8">
         <v>1</v>
@@ -18438,13 +18467,13 @@
         <v>60</v>
       </c>
       <c r="B227" s="8" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="C227" s="8">
         <v>254</v>
       </c>
       <c r="D227" s="8" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="E227" s="8">
         <v>1</v>
@@ -18488,13 +18517,13 @@
         <v>60</v>
       </c>
       <c r="B228" s="8" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="C228" s="8">
         <v>255</v>
       </c>
       <c r="D228" s="8" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="E228" s="8">
         <v>1</v>
@@ -18538,13 +18567,13 @@
         <v>60</v>
       </c>
       <c r="B229" s="8" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="C229" s="8">
         <v>256</v>
       </c>
       <c r="D229" s="8" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="E229" s="8">
         <v>1</v>
@@ -18588,13 +18617,13 @@
         <v>60</v>
       </c>
       <c r="B230" s="8" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="C230" s="8">
         <v>257</v>
       </c>
       <c r="D230" s="8" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="E230" s="8">
         <v>1</v>
@@ -18638,13 +18667,13 @@
         <v>60</v>
       </c>
       <c r="B231" s="8" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="C231" s="8">
         <v>258</v>
       </c>
       <c r="D231" s="8" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="E231" s="8">
         <v>1</v>
@@ -18688,13 +18717,13 @@
         <v>60</v>
       </c>
       <c r="B232" s="8" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="C232" s="8">
         <v>259</v>
       </c>
       <c r="D232" s="8" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="E232" s="8">
         <v>1</v>
@@ -18738,13 +18767,13 @@
         <v>60</v>
       </c>
       <c r="B233" s="8" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="C233" s="8">
         <v>260</v>
       </c>
       <c r="D233" s="8" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="E233" s="8">
         <v>1</v>
@@ -18788,13 +18817,13 @@
         <v>60</v>
       </c>
       <c r="B234" s="8" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="C234" s="8">
         <v>261</v>
       </c>
       <c r="D234" s="8" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="E234" s="8">
         <v>1</v>
@@ -18838,13 +18867,13 @@
         <v>60</v>
       </c>
       <c r="B235" s="8" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="C235" s="8">
         <v>262</v>
       </c>
       <c r="D235" s="8" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="E235" s="8">
         <v>1</v>
@@ -18888,13 +18917,13 @@
         <v>60</v>
       </c>
       <c r="B236" s="8" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="C236" s="8">
         <v>263</v>
       </c>
       <c r="D236" s="8" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="E236" s="8">
         <v>1</v>
@@ -18938,7 +18967,7 @@
         <v>60</v>
       </c>
       <c r="B237" s="8" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="C237" s="8">
         <v>264</v>
@@ -18988,13 +19017,13 @@
         <v>60</v>
       </c>
       <c r="B238" s="8" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="C238" s="8">
         <v>265</v>
       </c>
       <c r="D238" s="8" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="E238" s="8">
         <v>1</v>
@@ -25888,13 +25917,13 @@
         <v>61</v>
       </c>
       <c r="B376" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="C376">
         <v>266</v>
       </c>
       <c r="D376" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="E376">
         <v>1</v>
@@ -25938,13 +25967,13 @@
         <v>61</v>
       </c>
       <c r="B377" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="C377">
         <v>267</v>
       </c>
       <c r="D377" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="E377">
         <v>1</v>
@@ -25988,13 +26017,13 @@
         <v>61</v>
       </c>
       <c r="B378" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="C378">
         <v>268</v>
       </c>
       <c r="D378" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="E378">
         <v>1</v>
@@ -26038,13 +26067,13 @@
         <v>61</v>
       </c>
       <c r="B379" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="C379">
         <v>269</v>
       </c>
       <c r="D379" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="E379">
         <v>1</v>
@@ -26088,13 +26117,13 @@
         <v>61</v>
       </c>
       <c r="B380" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="C380">
         <v>270</v>
       </c>
       <c r="D380" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="E380">
         <v>1</v>
@@ -26138,13 +26167,13 @@
         <v>61</v>
       </c>
       <c r="B381" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="C381">
         <v>271</v>
       </c>
       <c r="D381" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="E381">
         <v>1</v>
@@ -26188,13 +26217,13 @@
         <v>61</v>
       </c>
       <c r="B382" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="C382">
         <v>272</v>
       </c>
       <c r="D382" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="E382">
         <v>1</v>
@@ -26238,13 +26267,13 @@
         <v>61</v>
       </c>
       <c r="B383" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="C383">
         <v>273</v>
       </c>
       <c r="D383" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="E383">
         <v>1</v>
@@ -26288,13 +26317,13 @@
         <v>61</v>
       </c>
       <c r="B384" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="C384">
         <v>274</v>
       </c>
       <c r="D384" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="E384">
         <v>1</v>
@@ -26338,13 +26367,13 @@
         <v>61</v>
       </c>
       <c r="B385" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="C385">
         <v>275</v>
       </c>
       <c r="D385" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="E385">
         <v>1</v>
@@ -26388,13 +26417,13 @@
         <v>61</v>
       </c>
       <c r="B386" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="C386">
         <v>276</v>
       </c>
       <c r="D386" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="E386">
         <v>1</v>
@@ -26438,7 +26467,7 @@
         <v>62</v>
       </c>
       <c r="B387" s="8" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="C387" s="8">
         <v>42</v>
@@ -26488,13 +26517,13 @@
         <v>63</v>
       </c>
       <c r="B388" s="5" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="C388" s="5">
         <v>277</v>
       </c>
       <c r="D388" s="5" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="E388" s="5">
         <v>1</v>
@@ -26538,13 +26567,13 @@
         <v>63</v>
       </c>
       <c r="B389" s="5" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="C389" s="5">
         <v>278</v>
       </c>
       <c r="D389" s="5" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="E389" s="5">
         <v>1</v>
@@ -26588,13 +26617,13 @@
         <v>63</v>
       </c>
       <c r="B390" s="5" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="C390" s="5">
         <v>279</v>
       </c>
       <c r="D390" s="5" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="E390" s="5">
         <v>1</v>
@@ -26638,13 +26667,13 @@
         <v>63</v>
       </c>
       <c r="B391" s="5" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="C391" s="5">
         <v>280</v>
       </c>
       <c r="D391" s="5" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="E391" s="5">
         <v>1</v>
@@ -26751,7 +26780,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="B3" t="s">
         <v>362</v>
@@ -26828,7 +26857,7 @@
   <dimension ref="A1:K181"/>
   <sheetViews>
     <sheetView topLeftCell="A169" workbookViewId="0">
-      <selection activeCell="A180" sqref="A180:K181"/>
+      <selection activeCell="A180" sqref="A180:XFD181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -32772,7 +32801,7 @@
         <v>3</v>
       </c>
       <c r="D170" s="6" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="E170" s="6">
         <v>0</v>
@@ -32822,7 +32851,7 @@
         <v>381</v>
       </c>
       <c r="I171" s="8" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="J171" s="8">
         <v>0</v>
@@ -32857,7 +32886,7 @@
         <v>381</v>
       </c>
       <c r="I172" s="8" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="J172" s="8">
         <v>0</v>
@@ -32892,7 +32921,7 @@
         <v>381</v>
       </c>
       <c r="I173" s="8" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="J173" s="8">
         <v>0</v>
@@ -32927,7 +32956,7 @@
         <v>381</v>
       </c>
       <c r="I174" s="8" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="J174" s="8">
         <v>0</v>
@@ -32962,7 +32991,7 @@
         <v>381</v>
       </c>
       <c r="I175" s="8" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="J175" s="8">
         <v>0</v>
@@ -32982,7 +33011,7 @@
         <v>3</v>
       </c>
       <c r="D176" s="8" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="E176" s="8">
         <v>0</v>
@@ -32997,7 +33026,7 @@
         <v>381</v>
       </c>
       <c r="I176" s="8" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="J176" s="8">
         <v>0</v>
@@ -33017,7 +33046,7 @@
         <v>3</v>
       </c>
       <c r="D177" s="8" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="E177" s="8">
         <v>0</v>
@@ -33032,7 +33061,7 @@
         <v>381</v>
       </c>
       <c r="I177" s="8" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="J177" s="8">
         <v>0</v>
@@ -33052,7 +33081,7 @@
         <v>3</v>
       </c>
       <c r="D178" s="8" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="E178" s="8">
         <v>0</v>
@@ -33067,7 +33096,7 @@
         <v>381</v>
       </c>
       <c r="I178" s="8" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="J178" s="8">
         <v>0</v>
@@ -33087,7 +33116,7 @@
         <v>3</v>
       </c>
       <c r="D179" s="8" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="E179" s="8">
         <v>0</v>
@@ -33102,7 +33131,7 @@
         <v>381</v>
       </c>
       <c r="I179" s="8" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="J179" s="8">
         <v>0</v>
@@ -33111,73 +33140,73 @@
         <v>377</v>
       </c>
     </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A180" s="5" t="s">
+    <row r="180" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A180" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="B180" s="5" t="s">
+      <c r="B180" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C180" s="5" t="s">
+      <c r="C180" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D180" s="5" t="s">
+      <c r="D180" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E180" s="5">
-        <v>0</v>
-      </c>
-      <c r="F180" s="5" t="s">
+      <c r="E180" s="8">
+        <v>0</v>
+      </c>
+      <c r="F180" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="G180" s="5" t="s">
+      <c r="G180" s="8" t="s">
         <v>422</v>
       </c>
-      <c r="H180" s="5" t="s">
+      <c r="H180" s="8" t="s">
         <v>381</v>
       </c>
-      <c r="I180" s="5" t="s">
-        <v>1110</v>
-      </c>
-      <c r="J180" s="5">
-        <v>0</v>
-      </c>
-      <c r="K180" s="5" t="s">
+      <c r="I180" s="8" t="s">
+        <v>1109</v>
+      </c>
+      <c r="J180" s="8">
+        <v>0</v>
+      </c>
+      <c r="K180" s="8" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A181" s="5" t="s">
+    <row r="181" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A181" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="B181" s="5" t="s">
+      <c r="B181" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C181" s="5" t="s">
+      <c r="C181" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D181" s="5" t="s">
+      <c r="D181" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E181" s="5">
-        <v>0</v>
-      </c>
-      <c r="F181" s="5" t="s">
+      <c r="E181" s="8">
+        <v>0</v>
+      </c>
+      <c r="F181" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="G181" s="5" t="s">
+      <c r="G181" s="8" t="s">
         <v>422</v>
       </c>
-      <c r="H181" s="5" t="s">
+      <c r="H181" s="8" t="s">
         <v>381</v>
       </c>
-      <c r="I181" s="5" t="s">
-        <v>1110</v>
-      </c>
-      <c r="J181" s="5">
-        <v>0</v>
-      </c>
-      <c r="K181" s="5" t="s">
+      <c r="I181" s="8" t="s">
+        <v>1109</v>
+      </c>
+      <c r="J181" s="8">
+        <v>0</v>
+      </c>
+      <c r="K181" s="8" t="s">
         <v>377</v>
       </c>
     </row>
@@ -33766,14 +33795,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:E8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="169.578125" customWidth="1"/>
+    <col min="2" max="2" width="148.68359375" customWidth="1"/>
     <col min="3" max="3" width="9.26171875" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="9" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="9.26171875" bestFit="1" customWidth="1"/>
@@ -33955,89 +33982,89 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7">
+      <c r="A7" s="8">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="8" t="s">
         <v>734</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="8">
         <v>5</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="8">
         <v>20150901</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="8">
         <v>99991231</v>
       </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7" s="4">
+      <c r="F7" s="8">
+        <v>0</v>
+      </c>
+      <c r="G7" s="8">
+        <v>1</v>
+      </c>
+      <c r="H7" s="14">
         <v>42248</v>
       </c>
-      <c r="I7" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="8">
+      <c r="I7" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="5">
         <v>6</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>981</v>
-      </c>
-      <c r="C8" s="8">
+      <c r="B8" s="5" t="s">
+        <v>980</v>
+      </c>
+      <c r="C8" s="5">
         <v>98</v>
       </c>
-      <c r="D8" s="8">
-        <v>20190501</v>
-      </c>
-      <c r="E8" s="8">
-        <v>20191031</v>
+      <c r="D8" s="5">
+        <v>20210401</v>
+      </c>
+      <c r="E8" s="5">
+        <v>20210731</v>
       </c>
       <c r="F8" s="5">
         <v>1</v>
       </c>
       <c r="G8" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8" s="12">
-        <v>43577.559065011577</v>
+        <v>44275.455153935189</v>
       </c>
       <c r="I8" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="6">
+    <row r="9" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="8">
         <v>7</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>900</v>
-      </c>
-      <c r="C9" s="6">
+      <c r="B9" s="8" t="s">
+        <v>1113</v>
+      </c>
+      <c r="C9" s="8">
         <v>7</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="8">
         <v>20180201</v>
       </c>
-      <c r="E9" s="6">
-        <v>99991231</v>
-      </c>
-      <c r="F9" s="6">
-        <v>0</v>
-      </c>
-      <c r="G9" s="6">
-        <v>0</v>
-      </c>
-      <c r="H9" s="7">
-        <v>43577.559065011577</v>
-      </c>
-      <c r="I9" s="6">
+      <c r="E9" s="8">
+        <v>20190422</v>
+      </c>
+      <c r="F9" s="8">
+        <v>0</v>
+      </c>
+      <c r="G9" s="8">
+        <v>0</v>
+      </c>
+      <c r="H9" s="14">
+        <v>43577.412575810187</v>
+      </c>
+      <c r="I9" s="8">
         <v>0</v>
       </c>
     </row>
@@ -34264,7 +34291,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="C15" s="6">
         <v>1</v>
@@ -34278,7 +34305,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="C16" s="6">
         <v>1</v>
@@ -34292,7 +34319,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="C17" s="6">
         <v>1</v>
@@ -34306,7 +34333,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="C18" s="6">
         <v>1</v>
@@ -34320,7 +34347,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="C19" s="6">
         <v>1</v>
@@ -34334,7 +34361,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="C20" s="6">
         <v>1</v>
@@ -34348,7 +34375,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="C21" s="6">
         <v>1</v>
@@ -34362,7 +34389,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="C22" s="6">
         <v>1</v>
@@ -34376,7 +34403,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="C23" s="6">
         <v>1</v>
@@ -34390,7 +34417,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="C24" s="6">
         <v>1</v>
@@ -34404,7 +34431,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="C25" s="6">
         <v>1</v>
@@ -34418,7 +34445,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="C26" s="6">
         <v>1</v>
@@ -35499,7 +35526,7 @@
         <v>5</v>
       </c>
       <c r="C37" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -35528,7 +35555,7 @@
         <v>5</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="D38" s="6">
         <v>1</v>
@@ -35557,7 +35584,7 @@
         <v>5</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="D39" s="6">
         <v>1</v>
@@ -35586,7 +35613,7 @@
         <v>5</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="D40" s="5">
         <v>1</v>
@@ -36572,7 +36599,7 @@
         <v>3</v>
       </c>
       <c r="C74" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="D74">
         <v>1</v>
@@ -36601,7 +36628,7 @@
         <v>3</v>
       </c>
       <c r="C75" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="D75">
         <v>1</v>
@@ -36630,7 +36657,7 @@
         <v>3</v>
       </c>
       <c r="C76" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="D76">
         <v>1</v>
@@ -36659,7 +36686,7 @@
         <v>3</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="D77" s="5">
         <v>1</v>
@@ -36736,7 +36763,7 @@
         <v>899</v>
       </c>
       <c r="M1" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -37532,7 +37559,7 @@
         <v>13</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="F21" s="6" t="s">
         <v>727</v>
@@ -37573,7 +37600,7 @@
         <v>14</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>727</v>
@@ -37614,7 +37641,7 @@
         <v>15</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="F23" s="6" t="s">
         <v>727</v>
@@ -37655,7 +37682,7 @@
         <v>16</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="F24" s="6" t="s">
         <v>727</v>
@@ -37696,7 +37723,7 @@
         <v>17</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="F25" s="6" t="s">
         <v>727</v>
@@ -37737,7 +37764,7 @@
         <v>18</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="F26" s="6" t="s">
         <v>727</v>
@@ -37778,7 +37805,7 @@
         <v>19</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>727</v>
@@ -37819,7 +37846,7 @@
         <v>20</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="F28" s="6" t="s">
         <v>727</v>
@@ -37860,7 +37887,7 @@
         <v>21</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="F29" s="6" t="s">
         <v>727</v>
@@ -37901,7 +37928,7 @@
         <v>22</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="F30" s="6" t="s">
         <v>727</v>
@@ -37942,7 +37969,7 @@
         <v>23</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="F31" s="6" t="s">
         <v>727</v>
@@ -37983,7 +38010,7 @@
         <v>24</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="F32" s="6" t="s">
         <v>727</v>
@@ -38021,7 +38048,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:E5"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -38061,19 +38088,19 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="A3" s="15">
+        <v>1</v>
+      </c>
+      <c r="B3" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
+      <c r="C3" s="15">
+        <v>1</v>
+      </c>
+      <c r="D3" s="15">
+        <v>1</v>
+      </c>
+      <c r="E3" s="15">
         <v>0</v>
       </c>
     </row>
@@ -38095,36 +38122,36 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="8">
+      <c r="A5" s="15">
         <v>3</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="8">
-        <v>1</v>
-      </c>
-      <c r="D5" s="8">
-        <v>0</v>
-      </c>
-      <c r="E5" s="8">
+      <c r="C5" s="15">
+        <v>1</v>
+      </c>
+      <c r="D5" s="15">
+        <v>1</v>
+      </c>
+      <c r="E5" s="15">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6">
+      <c r="A6" s="5">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
+      <c r="C6" s="5">
+        <v>1</v>
+      </c>
+      <c r="D6" s="5">
+        <v>1</v>
+      </c>
+      <c r="E6" s="5">
         <v>0</v>
       </c>
     </row>
@@ -38163,19 +38190,19 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9">
+      <c r="A9" s="5">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
+      <c r="C9" s="5">
+        <v>1</v>
+      </c>
+      <c r="D9" s="5">
+        <v>1</v>
+      </c>
+      <c r="E9" s="5">
         <v>0</v>
       </c>
     </row>
@@ -38207,26 +38234,26 @@
         <v>1</v>
       </c>
       <c r="D11" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12">
+      <c r="A12" s="15">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12" s="6">
-        <v>0</v>
-      </c>
-      <c r="E12">
+      <c r="C12" s="15">
+        <v>1</v>
+      </c>
+      <c r="D12" s="15">
+        <v>1</v>
+      </c>
+      <c r="E12" s="15">
         <v>0</v>
       </c>
     </row>
@@ -38248,19 +38275,19 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14">
+      <c r="A14" s="5">
         <v>12</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
+      <c r="C14" s="5">
+        <v>1</v>
+      </c>
+      <c r="D14" s="5">
+        <v>1</v>
+      </c>
+      <c r="E14" s="5">
         <v>0</v>
       </c>
     </row>
@@ -38282,53 +38309,53 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16">
+      <c r="A16" s="15">
         <v>14</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
+      <c r="C16" s="15">
+        <v>1</v>
+      </c>
+      <c r="D16" s="15">
+        <v>1</v>
+      </c>
+      <c r="E16" s="15">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17">
+      <c r="A17" s="5">
         <v>15</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17">
+      <c r="C17" s="5">
+        <v>1</v>
+      </c>
+      <c r="D17" s="5">
+        <v>1</v>
+      </c>
+      <c r="E17" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18">
+      <c r="A18" s="15">
         <v>16</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
+      <c r="C18" s="15">
+        <v>1</v>
+      </c>
+      <c r="D18" s="15">
+        <v>1</v>
+      </c>
+      <c r="E18" s="15">
         <v>0</v>
       </c>
     </row>
@@ -38350,19 +38377,19 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20">
+      <c r="A20" s="5">
         <v>18</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
+      <c r="C20" s="5">
+        <v>1</v>
+      </c>
+      <c r="D20" s="5">
+        <v>1</v>
+      </c>
+      <c r="E20" s="5">
         <v>0</v>
       </c>
     </row>
@@ -38743,13 +38770,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
+        <v>911</v>
+      </c>
+      <c r="B1" t="s">
         <v>912</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>913</v>
-      </c>
-      <c r="C1" t="s">
-        <v>914</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -38760,7 +38787,7 @@
         <v>173</v>
       </c>
       <c r="C2" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -38771,7 +38798,7 @@
         <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -38782,7 +38809,7 @@
         <v>174</v>
       </c>
       <c r="C4" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -38793,7 +38820,7 @@
         <v>378</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -38801,10 +38828,10 @@
         <v>105</v>
       </c>
       <c r="B6" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="C6" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -38812,10 +38839,10 @@
         <v>106</v>
       </c>
       <c r="B7" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="C7" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -38826,7 +38853,7 @@
         <v>422</v>
       </c>
       <c r="C8" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -38834,10 +38861,10 @@
         <v>108</v>
       </c>
       <c r="B9" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="C9" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -38845,10 +38872,10 @@
         <v>109</v>
       </c>
       <c r="B10" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="C10" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -38856,10 +38883,10 @@
         <v>110</v>
       </c>
       <c r="B11" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="C11" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
     </row>
   </sheetData>
@@ -38885,19 +38912,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
+        <v>918</v>
+      </c>
+      <c r="B1" t="s">
+        <v>912</v>
+      </c>
+      <c r="C1" t="s">
         <v>919</v>
-      </c>
-      <c r="B1" t="s">
-        <v>913</v>
-      </c>
-      <c r="C1" t="s">
-        <v>920</v>
       </c>
       <c r="D1" t="s">
         <v>757</v>
       </c>
       <c r="E1" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -38973,7 +39000,7 @@
         <v>105</v>
       </c>
       <c r="B6" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -38990,7 +39017,7 @@
         <v>106</v>
       </c>
       <c r="B7" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -39024,7 +39051,7 @@
         <v>108</v>
       </c>
       <c r="B9" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -39041,7 +39068,7 @@
         <v>109</v>
       </c>
       <c r="B10" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -39058,7 +39085,7 @@
         <v>110</v>
       </c>
       <c r="B11" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -39097,31 +39124,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
+        <v>911</v>
+      </c>
+      <c r="B1" t="s">
         <v>912</v>
       </c>
-      <c r="B1" t="s">
-        <v>913</v>
-      </c>
       <c r="C1" t="s">
+        <v>921</v>
+      </c>
+      <c r="D1" t="s">
         <v>922</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>923</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>924</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>925</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>926</v>
       </c>
-      <c r="H1" t="s">
-        <v>927</v>
-      </c>
       <c r="I1" s="6" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -39245,7 +39272,7 @@
         <v>105</v>
       </c>
       <c r="B6" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -39274,7 +39301,7 @@
         <v>106</v>
       </c>
       <c r="B7" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -39332,7 +39359,7 @@
         <v>108</v>
       </c>
       <c r="B9" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -39361,7 +39388,7 @@
         <v>109</v>
       </c>
       <c r="B10" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -39390,7 +39417,7 @@
         <v>110</v>
       </c>
       <c r="B11" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -39437,7 +39464,7 @@
         <v>500</v>
       </c>
       <c r="B1" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>731</v>
@@ -39445,10 +39472,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
+        <v>928</v>
+      </c>
+      <c r="B2" t="s">
         <v>929</v>
-      </c>
-      <c r="B2" t="s">
-        <v>930</v>
       </c>
       <c r="C2" s="6">
         <v>101</v>
@@ -39456,7 +39483,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="B3" t="s">
         <v>17</v>
@@ -39467,10 +39494,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="B4" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="C4" s="6">
         <v>201</v>
@@ -39478,7 +39505,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="B5" t="s">
         <v>17</v>
@@ -39489,10 +39516,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
+        <v>931</v>
+      </c>
+      <c r="B6" t="s">
         <v>932</v>
-      </c>
-      <c r="B6" t="s">
-        <v>933</v>
       </c>
       <c r="C6" s="6">
         <v>301</v>
@@ -39500,10 +39527,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="B7" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="C7" s="6">
         <v>302</v>
@@ -39511,10 +39538,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="B8" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="C8" s="6">
         <v>303</v>
@@ -39522,10 +39549,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="B9" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="C9" s="6">
         <v>304</v>
@@ -39533,7 +39560,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="B10" t="s">
         <v>17</v>
@@ -39555,10 +39582,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
+        <v>936</v>
+      </c>
+      <c r="B12" t="s">
         <v>937</v>
-      </c>
-      <c r="B12" t="s">
-        <v>938</v>
       </c>
       <c r="C12" s="6">
         <v>401</v>
@@ -39566,10 +39593,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="B13" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="C13" s="6">
         <v>402</v>
@@ -39577,10 +39604,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="B14" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="C14" s="6">
         <v>403</v>
@@ -39588,10 +39615,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="B15" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="C15" s="6">
         <v>404</v>
@@ -39599,10 +39626,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="B16" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="C16" s="6">
         <v>405</v>
@@ -39610,10 +39637,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="B17" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="C17" s="6">
         <v>406</v>
@@ -39621,10 +39648,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="B18" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="C18" s="6">
         <v>407</v>
@@ -39653,10 +39680,10 @@
         <v>502</v>
       </c>
       <c r="C1" t="s">
+        <v>989</v>
+      </c>
+      <c r="D1" t="s">
         <v>990</v>
-      </c>
-      <c r="D1" t="s">
-        <v>991</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -39664,7 +39691,7 @@
         <v>101</v>
       </c>
       <c r="B2" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -39678,7 +39705,7 @@
         <v>102</v>
       </c>
       <c r="B3" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -39692,7 +39719,7 @@
         <v>103</v>
       </c>
       <c r="B4" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -39706,7 +39733,7 @@
         <v>104</v>
       </c>
       <c r="B5" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -39720,7 +39747,7 @@
         <v>105</v>
       </c>
       <c r="B6" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -39734,7 +39761,7 @@
         <v>106</v>
       </c>
       <c r="B7" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -39748,7 +39775,7 @@
         <v>107</v>
       </c>
       <c r="B8" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -39762,7 +39789,7 @@
         <v>108</v>
       </c>
       <c r="B9" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -39776,7 +39803,7 @@
         <v>109</v>
       </c>
       <c r="B10" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -39790,7 +39817,7 @@
         <v>110</v>
       </c>
       <c r="B11" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -39804,7 +39831,7 @@
         <v>111</v>
       </c>
       <c r="B12" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -39833,10 +39860,10 @@
         <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="C1" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -39844,7 +39871,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -39855,7 +39882,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -39866,7 +39893,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -39877,7 +39904,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -39888,7 +39915,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -39899,7 +39926,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -39910,7 +39937,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -40028,7 +40055,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
   </sheetData>
@@ -40048,16 +40075,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
+        <v>1010</v>
+      </c>
+      <c r="B1" t="s">
         <v>1011</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1012</v>
       </c>
       <c r="C1" t="s">
         <v>731</v>
       </c>
       <c r="D1" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -40404,16 +40431,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="6" t="s">
+        <v>1013</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>1014</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
         <v>1015</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>1016</v>
-      </c>
       <c r="D1" s="6" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -40421,13 +40448,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>1016</v>
+      </c>
+      <c r="C2" t="s">
         <v>1017</v>
       </c>
-      <c r="C2" t="s">
-        <v>1018</v>
-      </c>
       <c r="D2" s="6" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -40435,13 +40462,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>1018</v>
+      </c>
+      <c r="C3" t="s">
         <v>1019</v>
       </c>
-      <c r="C3" t="s">
-        <v>1020</v>
-      </c>
       <c r="D3" s="6" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -40449,13 +40476,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>1020</v>
+      </c>
+      <c r="C4" t="s">
         <v>1021</v>
       </c>
-      <c r="C4" t="s">
-        <v>1022</v>
-      </c>
       <c r="D4" s="6" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -40463,13 +40490,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="C5" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -40477,13 +40504,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>1023</v>
+      </c>
+      <c r="C6" t="s">
         <v>1024</v>
       </c>
-      <c r="C6" t="s">
-        <v>1025</v>
-      </c>
       <c r="D6" s="6" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -40491,13 +40518,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>1025</v>
+      </c>
+      <c r="C7" t="s">
         <v>1026</v>
       </c>
-      <c r="C7" t="s">
-        <v>1027</v>
-      </c>
       <c r="D7" s="6" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -40505,13 +40532,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>1027</v>
+      </c>
+      <c r="C8" t="s">
         <v>1028</v>
       </c>
-      <c r="C8" t="s">
-        <v>1029</v>
-      </c>
       <c r="D8" s="6" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -40519,13 +40546,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>1043</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>1017</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>1044</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>1018</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>1045</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -40533,13 +40560,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -40547,13 +40574,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>1046</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>1047</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>1048</v>
-      </c>
       <c r="D11" s="6" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -40561,13 +40588,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -40575,13 +40602,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -40589,13 +40616,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
+        <v>1050</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>1051</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>1052</v>
-      </c>
       <c r="D14" s="6" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -40603,13 +40630,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -40617,13 +40644,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
+        <v>1053</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>1054</v>
       </c>
-      <c r="C16" s="5" t="s">
-        <v>1055</v>
-      </c>
       <c r="D16" s="5" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -40631,13 +40658,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
   </sheetData>
@@ -40658,13 +40685,13 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1" t="s">
         <v>1077</v>
       </c>
-      <c r="B1" t="s">
-        <v>1078</v>
-      </c>
       <c r="C1" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="D1" t="s">
         <v>81</v>
@@ -40699,7 +40726,7 @@
         <v>101</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -40737,7 +40764,7 @@
         <v>102</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -41069,13 +41096,13 @@
         <v>15</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>65</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="E17" s="6">
         <v>1</v>
@@ -41637,7 +41664,7 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -41645,7 +41672,7 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -41653,7 +41680,7 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -41661,7 +41688,7 @@
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -41669,7 +41696,7 @@
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -41677,7 +41704,7 @@
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -41685,7 +41712,7 @@
         <v>63</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
     </row>
   </sheetData>
@@ -43680,7 +43707,7 @@
         <v>245</v>
       </c>
       <c r="B247" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -43688,7 +43715,7 @@
         <v>246</v>
       </c>
       <c r="B248" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -43696,7 +43723,7 @@
         <v>247</v>
       </c>
       <c r="B249" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -43704,7 +43731,7 @@
         <v>248</v>
       </c>
       <c r="B250" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -43712,7 +43739,7 @@
         <v>249</v>
       </c>
       <c r="B251" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -43720,7 +43747,7 @@
         <v>250</v>
       </c>
       <c r="B252" s="6" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -43728,7 +43755,7 @@
         <v>251</v>
       </c>
       <c r="B253" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -43736,7 +43763,7 @@
         <v>252</v>
       </c>
       <c r="B254" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -43744,7 +43771,7 @@
         <v>253</v>
       </c>
       <c r="B255" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -43752,7 +43779,7 @@
         <v>254</v>
       </c>
       <c r="B256" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -43760,7 +43787,7 @@
         <v>255</v>
       </c>
       <c r="B257" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -43768,7 +43795,7 @@
         <v>256</v>
       </c>
       <c r="B258" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -43776,7 +43803,7 @@
         <v>257</v>
       </c>
       <c r="B259" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -43784,7 +43811,7 @@
         <v>258</v>
       </c>
       <c r="B260" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -43792,7 +43819,7 @@
         <v>259</v>
       </c>
       <c r="B261" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -43800,7 +43827,7 @@
         <v>260</v>
       </c>
       <c r="B262" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -43808,7 +43835,7 @@
         <v>261</v>
       </c>
       <c r="B263" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -43816,7 +43843,7 @@
         <v>262</v>
       </c>
       <c r="B264" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -43824,7 +43851,7 @@
         <v>263</v>
       </c>
       <c r="B265" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -43840,7 +43867,7 @@
         <v>265</v>
       </c>
       <c r="B267" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -43848,7 +43875,7 @@
         <v>266</v>
       </c>
       <c r="B268" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -43856,7 +43883,7 @@
         <v>267</v>
       </c>
       <c r="B269" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -43864,7 +43891,7 @@
         <v>268</v>
       </c>
       <c r="B270" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -43872,7 +43899,7 @@
         <v>269</v>
       </c>
       <c r="B271" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -43880,7 +43907,7 @@
         <v>270</v>
       </c>
       <c r="B272" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -43888,7 +43915,7 @@
         <v>271</v>
       </c>
       <c r="B273" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -43896,7 +43923,7 @@
         <v>272</v>
       </c>
       <c r="B274" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -43904,7 +43931,7 @@
         <v>273</v>
       </c>
       <c r="B275" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -43912,7 +43939,7 @@
         <v>274</v>
       </c>
       <c r="B276" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -43920,7 +43947,7 @@
         <v>275</v>
       </c>
       <c r="B277" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -43928,7 +43955,7 @@
         <v>276</v>
       </c>
       <c r="B278" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -43936,7 +43963,7 @@
         <v>277</v>
       </c>
       <c r="B279" s="8" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -43944,7 +43971,7 @@
         <v>278</v>
       </c>
       <c r="B280" s="8" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -43952,7 +43979,7 @@
         <v>279</v>
       </c>
       <c r="B281" s="8" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -43960,7 +43987,7 @@
         <v>280</v>
       </c>
       <c r="B282" s="8" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -43968,7 +43995,7 @@
         <v>281</v>
       </c>
       <c r="B283" s="6" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -43976,7 +44003,7 @@
         <v>282</v>
       </c>
       <c r="B284" s="5" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TFS 21493 - Written Corr Bingo records in bingo feeds
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C49592
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OmniCloud\eCoaching_V2\Design\DD\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D05A721-330C-48C6-B0E1-314BFB5172A3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1890687-53B0-4533-A9EE-0045EFC5F41E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4019" uniqueCount="1115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4033" uniqueCount="1121">
   <si>
     <t>SourceID</t>
   </si>
@@ -3431,6 +3431,24 @@
   <si>
     <t>Set additional sites as isPilot = 1 and Activated the Extra HotTopic question for the duration of the QN Survey pilot for additional saites.
 *isPilot for Bogalusa, Brownsville, Lawrence, Phoenix, Sandy(Phase III sites) set as Active but will be Updated in database via admin task afterMay 1st.</t>
+  </si>
+  <si>
+    <t>&lt;img border="20" src="cid:qc.png"&gt;</t>
+  </si>
+  <si>
+    <t>Quality Correspondent 1</t>
+  </si>
+  <si>
+    <t>Quality Correspondent 2</t>
+  </si>
+  <si>
+    <t>Quality Correspondent 3</t>
+  </si>
+  <si>
+    <t>Quality Correspondent 4</t>
+  </si>
+  <si>
+    <t>Added Images for Quality Correpondence Competencies in Bingo images tab.</t>
   </si>
 </sst>
 </file>
@@ -3501,7 +3519,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -3522,6 +3540,9 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3860,10 +3881,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L105"/>
+  <dimension ref="A1:L106"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="A105" sqref="A105"/>
+      <selection activeCell="A106" sqref="A106:E106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -5629,21 +5650,38 @@
         <v>1112</v>
       </c>
     </row>
-    <row r="105" spans="1:5" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A105" s="5">
+    <row r="105" spans="1:5" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A105" s="8">
         <v>94</v>
       </c>
-      <c r="B105" s="11">
+      <c r="B105" s="9">
         <v>44277</v>
       </c>
-      <c r="C105" s="5" t="s">
+      <c r="C105" s="8" t="s">
         <v>429</v>
       </c>
-      <c r="D105" s="5">
+      <c r="D105" s="8">
         <v>20256</v>
       </c>
-      <c r="E105" s="13" t="s">
+      <c r="E105" s="16" t="s">
         <v>1114</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A106" s="5">
+        <v>95</v>
+      </c>
+      <c r="B106" s="11">
+        <v>44357</v>
+      </c>
+      <c r="C106" s="5" t="s">
+        <v>429</v>
+      </c>
+      <c r="D106" s="5">
+        <v>21493</v>
+      </c>
+      <c r="E106" s="5" t="s">
+        <v>1120</v>
       </c>
     </row>
   </sheetData>
@@ -40416,10 +40454,10 @@
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A18" sqref="A18:D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -40640,31 +40678,87 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="5">
+      <c r="A16" s="8">
         <v>15</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="8" t="s">
         <v>1053</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="8" t="s">
         <v>1054</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="8" t="s">
         <v>1041</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="5">
+      <c r="A17" s="8">
         <v>16</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="8" t="s">
         <v>1055</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="8" t="s">
         <v>1054</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="8" t="s">
         <v>1044</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="5">
+        <v>17</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>1115</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>1116</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="5">
+        <v>18</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>1115</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>1117</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="5">
+        <v>19</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>1115</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>1118</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="5">
+        <v>20</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>1115</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>1119</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>1041</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TFS 22187 - Quality Now Workflow Enhancements. Additional Changes.
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C50419
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OmniCloud\eCoaching_V2\Design\DD\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1890687-53B0-4533-A9EE-0045EFC5F41E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9F142DA-2F92-4854-BA64-9ACFFAC9B425}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4033" uniqueCount="1121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4044" uniqueCount="1132">
   <si>
     <t>SourceID</t>
   </si>
@@ -3449,6 +3449,39 @@
   </si>
   <si>
     <t>Added Images for Quality Correpondence Competencies in Bingo images tab.</t>
+  </si>
+  <si>
+    <t>Pending Follow-up Preparation</t>
+  </si>
+  <si>
+    <t>Pending Follow-up Coaching</t>
+  </si>
+  <si>
+    <t>Pending Follow-up Employee Review</t>
+  </si>
+  <si>
+    <t>MyCompletedQN</t>
+  </si>
+  <si>
+    <t>MySubmissionQN</t>
+  </si>
+  <si>
+    <t>MyPendingQN</t>
+  </si>
+  <si>
+    <t>MyPendingFollowupPrepQN</t>
+  </si>
+  <si>
+    <t>MyPendingFollowupCoachQN</t>
+  </si>
+  <si>
+    <t>MyTeamPendingQN</t>
+  </si>
+  <si>
+    <t>MyTeamcompletedQN</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Quality Now Workflow Enhancements. Added 3 new Statuses in DIM_Status table. Added new values to UI_Dashboard_Summary_Display</t>
   </si>
 </sst>
 </file>
@@ -3475,7 +3508,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3500,12 +3533,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -3519,7 +3546,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -3534,12 +3561,7 @@
     <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -3881,10 +3903,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L106"/>
+  <dimension ref="A1:L107"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="A106" sqref="A106:E106"/>
+      <selection activeCell="E107" sqref="E107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -5663,25 +5685,42 @@
       <c r="D105" s="8">
         <v>20256</v>
       </c>
-      <c r="E105" s="16" t="s">
+      <c r="E105" s="13" t="s">
         <v>1114</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A106" s="5">
+    <row r="106" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A106" s="8">
         <v>95</v>
       </c>
-      <c r="B106" s="11">
+      <c r="B106" s="9">
         <v>44357</v>
       </c>
-      <c r="C106" s="5" t="s">
+      <c r="C106" s="8" t="s">
         <v>429</v>
       </c>
-      <c r="D106" s="5">
+      <c r="D106" s="8">
         <v>21493</v>
       </c>
-      <c r="E106" s="5" t="s">
+      <c r="E106" s="8" t="s">
         <v>1120</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A107" s="5">
+        <v>96</v>
+      </c>
+      <c r="B107" s="11">
+        <v>44454</v>
+      </c>
+      <c r="C107" s="5" t="s">
+        <v>429</v>
+      </c>
+      <c r="D107" s="5">
+        <v>22187</v>
+      </c>
+      <c r="E107" s="5" t="s">
+        <v>1131</v>
       </c>
     </row>
   </sheetData>
@@ -33833,7 +33872,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -34041,39 +34082,39 @@
       <c r="G7" s="8">
         <v>1</v>
       </c>
-      <c r="H7" s="14">
+      <c r="H7" s="12">
         <v>42248</v>
       </c>
       <c r="I7" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="5">
+    <row r="8" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="8">
         <v>6</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="8" t="s">
         <v>980</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="8">
         <v>98</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="8">
         <v>20210401</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="8">
         <v>20210731</v>
       </c>
-      <c r="F8" s="5">
-        <v>1</v>
-      </c>
-      <c r="G8" s="5">
+      <c r="F8" s="8">
+        <v>1</v>
+      </c>
+      <c r="G8" s="8">
         <v>1</v>
       </c>
       <c r="H8" s="12">
         <v>44275.455153935189</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="8">
         <v>1</v>
       </c>
     </row>
@@ -34099,7 +34140,7 @@
       <c r="G9" s="8">
         <v>0</v>
       </c>
-      <c r="H9" s="14">
+      <c r="H9" s="12">
         <v>43577.412575810187</v>
       </c>
       <c r="I9" s="8">
@@ -38086,7 +38127,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="A3" sqref="A3:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -38125,92 +38166,92 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="15">
-        <v>1</v>
-      </c>
-      <c r="B3" s="15" t="s">
+    <row r="3" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="8">
+        <v>1</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="15">
-        <v>1</v>
-      </c>
-      <c r="D3" s="15">
-        <v>1</v>
-      </c>
-      <c r="E3" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4">
+      <c r="C3" s="8">
+        <v>1</v>
+      </c>
+      <c r="D3" s="8">
+        <v>1</v>
+      </c>
+      <c r="E3" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="8">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="15">
+      <c r="C4" s="8">
+        <v>0</v>
+      </c>
+      <c r="D4" s="8">
+        <v>0</v>
+      </c>
+      <c r="E4" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="8">
         <v>3</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="15">
-        <v>1</v>
-      </c>
-      <c r="D5" s="15">
-        <v>1</v>
-      </c>
-      <c r="E5" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="5">
+      <c r="C5" s="8">
+        <v>1</v>
+      </c>
+      <c r="D5" s="8">
+        <v>1</v>
+      </c>
+      <c r="E5" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="8">
         <v>4</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="5">
-        <v>1</v>
-      </c>
-      <c r="D6" s="5">
-        <v>1</v>
-      </c>
-      <c r="E6" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7">
+      <c r="C6" s="8">
+        <v>1</v>
+      </c>
+      <c r="D6" s="8">
+        <v>1</v>
+      </c>
+      <c r="E6" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="8">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C7" s="8">
+        <v>1</v>
+      </c>
+      <c r="D7" s="8">
+        <v>0</v>
+      </c>
+      <c r="E7" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="8">
         <v>6</v>
       </c>
@@ -38227,41 +38268,41 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="5">
+    <row r="9" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="8">
         <v>7</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="5">
-        <v>1</v>
-      </c>
-      <c r="D9" s="5">
-        <v>1</v>
-      </c>
-      <c r="E9" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10">
+      <c r="C9" s="8">
+        <v>1</v>
+      </c>
+      <c r="D9" s="8">
+        <v>1</v>
+      </c>
+      <c r="E9" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="8">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C10" s="8">
+        <v>0</v>
+      </c>
+      <c r="D10" s="8">
+        <v>0</v>
+      </c>
+      <c r="E10" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="8">
         <v>9</v>
       </c>
@@ -38278,126 +38319,126 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="15">
+    <row r="12" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="8">
         <v>10</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="15">
-        <v>1</v>
-      </c>
-      <c r="D12" s="15">
-        <v>1</v>
-      </c>
-      <c r="E12" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13">
+      <c r="C12" s="8">
+        <v>1</v>
+      </c>
+      <c r="D12" s="8">
+        <v>1</v>
+      </c>
+      <c r="E12" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="8">
         <v>11</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="5">
+      <c r="C13" s="8">
+        <v>0</v>
+      </c>
+      <c r="D13" s="8">
+        <v>0</v>
+      </c>
+      <c r="E13" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="8">
         <v>12</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="C14" s="5">
-        <v>1</v>
-      </c>
-      <c r="D14" s="5">
-        <v>1</v>
-      </c>
-      <c r="E14" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15">
+      <c r="C14" s="8">
+        <v>1</v>
+      </c>
+      <c r="D14" s="8">
+        <v>1</v>
+      </c>
+      <c r="E14" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="8">
         <v>13</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="15">
+      <c r="C15" s="8">
+        <v>0</v>
+      </c>
+      <c r="D15" s="8">
+        <v>0</v>
+      </c>
+      <c r="E15" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="8">
         <v>14</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="C16" s="15">
-        <v>1</v>
-      </c>
-      <c r="D16" s="15">
-        <v>1</v>
-      </c>
-      <c r="E16" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="5">
+      <c r="C16" s="8">
+        <v>1</v>
+      </c>
+      <c r="D16" s="8">
+        <v>1</v>
+      </c>
+      <c r="E16" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="8">
         <v>15</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="C17" s="5">
-        <v>1</v>
-      </c>
-      <c r="D17" s="5">
-        <v>1</v>
-      </c>
-      <c r="E17" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="15">
+      <c r="C17" s="8">
+        <v>1</v>
+      </c>
+      <c r="D17" s="8">
+        <v>1</v>
+      </c>
+      <c r="E17" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="8">
         <v>16</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="C18" s="15">
-        <v>1</v>
-      </c>
-      <c r="D18" s="15">
-        <v>1</v>
-      </c>
-      <c r="E18" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C18" s="8">
+        <v>1</v>
+      </c>
+      <c r="D18" s="8">
+        <v>1</v>
+      </c>
+      <c r="E18" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="8">
         <v>17</v>
       </c>
@@ -38414,37 +38455,37 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="5">
+    <row r="20" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="8">
         <v>18</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="C20" s="5">
-        <v>1</v>
-      </c>
-      <c r="D20" s="5">
-        <v>1</v>
-      </c>
-      <c r="E20" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21">
+      <c r="C20" s="8">
+        <v>1</v>
+      </c>
+      <c r="D20" s="8">
+        <v>1</v>
+      </c>
+      <c r="E20" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="8">
         <v>19</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
+      <c r="C21" s="8">
+        <v>0</v>
+      </c>
+      <c r="D21" s="8">
+        <v>0</v>
+      </c>
+      <c r="E21" s="8">
         <v>0</v>
       </c>
     </row>
@@ -38797,7 +38838,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -38851,10 +38894,10 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="5">
+      <c r="A5" s="8">
         <v>104</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="8" t="s">
         <v>378</v>
       </c>
       <c r="C5" s="13" t="s">
@@ -39142,10 +39185,10 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I11"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -39160,7 +39203,7 @@
     <col min="8" max="8" width="12.578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>911</v>
       </c>
@@ -39188,8 +39231,29 @@
       <c r="I1" s="6" t="s">
         <v>1035</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J1" s="5" t="s">
+        <v>1124</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>1125</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>1126</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>1127</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>1128</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>1129</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>1130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>101</v>
       </c>
@@ -39217,8 +39281,29 @@
       <c r="I2" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J2" s="5">
+        <v>1</v>
+      </c>
+      <c r="K2" s="5">
+        <v>0</v>
+      </c>
+      <c r="L2" s="5">
+        <v>1</v>
+      </c>
+      <c r="M2" s="5">
+        <v>0</v>
+      </c>
+      <c r="N2" s="5">
+        <v>0</v>
+      </c>
+      <c r="O2" s="5">
+        <v>0</v>
+      </c>
+      <c r="P2" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>102</v>
       </c>
@@ -39246,8 +39331,29 @@
       <c r="I3" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J3" s="5">
+        <v>1</v>
+      </c>
+      <c r="K3" s="5">
+        <v>1</v>
+      </c>
+      <c r="L3" s="5">
+        <v>1</v>
+      </c>
+      <c r="M3" s="5">
+        <v>0</v>
+      </c>
+      <c r="N3" s="5">
+        <v>0</v>
+      </c>
+      <c r="O3" s="5">
+        <v>0</v>
+      </c>
+      <c r="P3" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>103</v>
       </c>
@@ -39275,8 +39381,29 @@
       <c r="I4" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J4" s="5">
+        <v>1</v>
+      </c>
+      <c r="K4" s="5">
+        <v>1</v>
+      </c>
+      <c r="L4" s="5">
+        <v>1</v>
+      </c>
+      <c r="M4" s="5">
+        <v>1</v>
+      </c>
+      <c r="N4" s="5">
+        <v>1</v>
+      </c>
+      <c r="O4" s="5">
+        <v>1</v>
+      </c>
+      <c r="P4" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>104</v>
       </c>
@@ -39304,19 +39431,40 @@
       <c r="I5" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J5" s="5">
+        <v>0</v>
+      </c>
+      <c r="K5" s="5">
+        <v>1</v>
+      </c>
+      <c r="L5" s="5">
+        <v>0</v>
+      </c>
+      <c r="M5" s="5">
+        <v>0</v>
+      </c>
+      <c r="N5" s="5">
+        <v>0</v>
+      </c>
+      <c r="O5" s="5">
+        <v>1</v>
+      </c>
+      <c r="P5" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B6" t="s">
-        <v>914</v>
+        <v>915</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -39328,53 +39476,95 @@
         <v>1</v>
       </c>
       <c r="H6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I6" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J6" s="5">
+        <v>0</v>
+      </c>
+      <c r="K6" s="5">
+        <v>0</v>
+      </c>
+      <c r="L6" s="5">
+        <v>0</v>
+      </c>
+      <c r="M6" s="5">
+        <v>0</v>
+      </c>
+      <c r="N6" s="5">
+        <v>0</v>
+      </c>
+      <c r="O6" s="5">
+        <v>0</v>
+      </c>
+      <c r="P6" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B7" t="s">
-        <v>915</v>
+        <v>422</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J7" s="5">
+        <v>1</v>
+      </c>
+      <c r="K7" s="5">
+        <v>1</v>
+      </c>
+      <c r="L7" s="5">
+        <v>1</v>
+      </c>
+      <c r="M7" s="5">
+        <v>0</v>
+      </c>
+      <c r="N7" s="5">
+        <v>0</v>
+      </c>
+      <c r="O7" s="5">
+        <v>0</v>
+      </c>
+      <c r="P7" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B8" t="s">
-        <v>422</v>
+        <v>916</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -39386,18 +39576,39 @@
         <v>0</v>
       </c>
       <c r="H8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I8" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J8" s="5">
+        <v>0</v>
+      </c>
+      <c r="K8" s="5">
+        <v>0</v>
+      </c>
+      <c r="L8" s="5">
+        <v>0</v>
+      </c>
+      <c r="M8" s="5">
+        <v>0</v>
+      </c>
+      <c r="N8" s="5">
+        <v>0</v>
+      </c>
+      <c r="O8" s="5">
+        <v>0</v>
+      </c>
+      <c r="P8" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B9" t="s">
-        <v>916</v>
+        <v>917</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -39420,13 +39631,34 @@
       <c r="I9" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J9" s="5">
+        <v>0</v>
+      </c>
+      <c r="K9" s="5">
+        <v>0</v>
+      </c>
+      <c r="L9" s="5">
+        <v>0</v>
+      </c>
+      <c r="M9" s="5">
+        <v>0</v>
+      </c>
+      <c r="N9" s="5">
+        <v>0</v>
+      </c>
+      <c r="O9" s="5">
+        <v>0</v>
+      </c>
+      <c r="P9" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B10" t="s">
-        <v>917</v>
+        <v>962</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -39449,33 +39681,25 @@
       <c r="I10" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11">
-        <v>110</v>
-      </c>
-      <c r="B11" t="s">
-        <v>962</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>1</v>
-      </c>
-      <c r="I11" s="6">
+      <c r="J10" s="5">
+        <v>0</v>
+      </c>
+      <c r="K10" s="5">
+        <v>1</v>
+      </c>
+      <c r="L10" s="5">
+        <v>0</v>
+      </c>
+      <c r="M10" s="5">
+        <v>0</v>
+      </c>
+      <c r="N10" s="5">
+        <v>0</v>
+      </c>
+      <c r="O10" s="5">
+        <v>0</v>
+      </c>
+      <c r="P10" s="5">
         <v>0</v>
       </c>
     </row>
@@ -39988,10 +40212,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:B12"/>
+      <selection activeCell="A13" sqref="A13:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -40094,6 +40318,30 @@
       </c>
       <c r="B12" s="6" t="s">
         <v>1033</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="5">
+        <v>11</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="5">
+        <v>12</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>1122</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="5">
+        <v>13</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>1123</v>
       </c>
     </row>
   </sheetData>
@@ -40706,58 +40954,58 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="5">
+      <c r="A18" s="8">
         <v>17</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="8" t="s">
         <v>1115</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="8" t="s">
         <v>1116</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="8" t="s">
         <v>1041</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="5">
+      <c r="A19" s="8">
         <v>18</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="8" t="s">
         <v>1115</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="8" t="s">
         <v>1117</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="8" t="s">
         <v>1041</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="5">
+      <c r="A20" s="8">
         <v>19</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="8" t="s">
         <v>1115</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="8" t="s">
         <v>1118</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="8" t="s">
         <v>1041</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="5">
+      <c r="A21" s="8">
         <v>20</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="8" t="s">
         <v>1115</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="8" t="s">
         <v>1119</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="8" t="s">
         <v>1041</v>
       </c>
     </row>

</xml_diff>

<commit_message>
TFS 24631 - Removal of Sandy from eCoaching log
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C51486
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OmniCloud\eCoaching_V2\Design\DD\DB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TFS\eCoaching_V2\Design\DD\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70FE1272-3DF6-4AFB-AA2B-A57097DCD42D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABC79102-DEDC-490C-8F9E-13B31692ED79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="5" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57504" yWindow="1932" windowWidth="28992" windowHeight="15792" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_History" sheetId="14" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4144" uniqueCount="1156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4146" uniqueCount="1157">
   <si>
     <t>SourceID</t>
   </si>
@@ -3490,9 +3490,6 @@
     <t>Added New Coaching Reason, Updated DIM Source,new entry in Coaching Reason Selection and Emai8l Notification tables</t>
   </si>
   <si>
-    <t>TFS 24083 - Updates to LSA Module DIM_Coaching_Reason, DIM_Sub_SubCoaching_Reason and Coaching_Reason_Selection tables for changes to LSA Module.</t>
-  </si>
-  <si>
     <t>Flag Entries</t>
   </si>
   <si>
@@ -3554,6 +3551,12 @@
   </si>
   <si>
     <t>UAT Reminders</t>
+  </si>
+  <si>
+    <t>Updates to LSA Module DIM_Coaching_Reason, DIM_Sub_SubCoaching_Reason and Coaching_Reason_Selection tables for changes to LSA Module.</t>
+  </si>
+  <si>
+    <t>Set Sandy to Inactive in DIM_Site and Survey_Sites tabs</t>
   </si>
 </sst>
 </file>
@@ -3632,11 +3635,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3975,10 +3978,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L109"/>
+  <dimension ref="A1:L110"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="E109" sqref="E109"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="A110" sqref="A110:E110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -5813,20 +5816,37 @@
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A109" s="5">
+      <c r="A109" s="6">
         <v>99</v>
       </c>
-      <c r="B109" s="11">
+      <c r="B109" s="10">
         <v>44641</v>
       </c>
-      <c r="C109" s="5" t="s">
+      <c r="C109" s="6" t="s">
         <v>428</v>
       </c>
-      <c r="D109" s="5">
+      <c r="D109" s="6">
         <v>24083</v>
       </c>
-      <c r="E109" s="11" t="s">
-        <v>1134</v>
+      <c r="E109" s="10" t="s">
+        <v>1155</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A110" s="5">
+        <v>100</v>
+      </c>
+      <c r="B110" s="13">
+        <v>44698</v>
+      </c>
+      <c r="C110" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="D110" s="5">
+        <v>24631</v>
+      </c>
+      <c r="E110" s="13" t="s">
+        <v>1156</v>
       </c>
     </row>
   </sheetData>
@@ -7334,8 +7354,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:P416"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A381" workbookViewId="0">
-      <selection activeCell="A416" sqref="A416"/>
+    <sheetView topLeftCell="A381" workbookViewId="0">
+      <selection activeCell="A398" sqref="A398:P416"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -8505,7 +8525,7 @@
         <v>291</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="E24" s="5">
         <v>1</v>
@@ -8555,7 +8575,7 @@
         <v>293</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="E25" s="5">
         <v>1</v>
@@ -8605,7 +8625,7 @@
         <v>295</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="E26" s="5">
         <v>1</v>
@@ -10155,7 +10175,7 @@
         <v>292</v>
       </c>
       <c r="D57" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="E57">
         <v>1</v>
@@ -13355,7 +13375,7 @@
         <v>284</v>
       </c>
       <c r="D121" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="E121">
         <v>1</v>
@@ -27195,952 +27215,952 @@
       </c>
     </row>
     <row r="398" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A398" s="5">
+      <c r="A398">
         <v>65</v>
       </c>
-      <c r="B398" s="5" t="s">
+      <c r="B398" t="s">
+        <v>1134</v>
+      </c>
+      <c r="C398">
+        <v>42</v>
+      </c>
+      <c r="D398" t="s">
+        <v>205</v>
+      </c>
+      <c r="E398">
+        <v>1</v>
+      </c>
+      <c r="F398">
+        <v>1</v>
+      </c>
+      <c r="G398">
+        <v>1</v>
+      </c>
+      <c r="H398">
+        <v>1</v>
+      </c>
+      <c r="I398">
+        <v>1</v>
+      </c>
+      <c r="J398">
+        <v>0</v>
+      </c>
+      <c r="K398">
+        <v>0</v>
+      </c>
+      <c r="L398">
+        <v>0</v>
+      </c>
+      <c r="M398">
+        <v>0</v>
+      </c>
+      <c r="N398">
+        <v>0</v>
+      </c>
+      <c r="O398">
+        <v>1</v>
+      </c>
+      <c r="P398">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="399" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A399">
+        <v>66</v>
+      </c>
+      <c r="B399" t="s">
         <v>1135</v>
       </c>
-      <c r="C398" s="5">
+      <c r="C399">
+        <v>296</v>
+      </c>
+      <c r="D399" t="s">
+        <v>1153</v>
+      </c>
+      <c r="E399">
+        <v>1</v>
+      </c>
+      <c r="F399">
+        <v>1</v>
+      </c>
+      <c r="G399">
+        <v>1</v>
+      </c>
+      <c r="H399">
+        <v>1</v>
+      </c>
+      <c r="I399">
+        <v>1</v>
+      </c>
+      <c r="J399">
+        <v>0</v>
+      </c>
+      <c r="K399">
+        <v>0</v>
+      </c>
+      <c r="L399">
+        <v>0</v>
+      </c>
+      <c r="M399">
+        <v>0</v>
+      </c>
+      <c r="N399">
+        <v>0</v>
+      </c>
+      <c r="O399">
+        <v>1</v>
+      </c>
+      <c r="P399">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="400" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A400">
+        <v>66</v>
+      </c>
+      <c r="B400" t="s">
+        <v>1135</v>
+      </c>
+      <c r="C400">
+        <v>297</v>
+      </c>
+      <c r="D400" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E400">
+        <v>1</v>
+      </c>
+      <c r="F400">
+        <v>1</v>
+      </c>
+      <c r="G400">
+        <v>1</v>
+      </c>
+      <c r="H400">
+        <v>1</v>
+      </c>
+      <c r="I400">
+        <v>1</v>
+      </c>
+      <c r="J400">
+        <v>0</v>
+      </c>
+      <c r="K400">
+        <v>0</v>
+      </c>
+      <c r="L400">
+        <v>0</v>
+      </c>
+      <c r="M400">
+        <v>0</v>
+      </c>
+      <c r="N400">
+        <v>0</v>
+      </c>
+      <c r="O400">
+        <v>1</v>
+      </c>
+      <c r="P400">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="401" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A401">
+        <v>66</v>
+      </c>
+      <c r="B401" t="s">
+        <v>1135</v>
+      </c>
+      <c r="C401">
         <v>42</v>
       </c>
-      <c r="D398" s="5" t="s">
+      <c r="D401" t="s">
         <v>205</v>
       </c>
-      <c r="E398" s="5">
-        <v>1</v>
-      </c>
-      <c r="F398" s="5">
-        <v>1</v>
-      </c>
-      <c r="G398" s="5">
-        <v>1</v>
-      </c>
-      <c r="H398" s="5">
-        <v>1</v>
-      </c>
-      <c r="I398" s="5">
-        <v>1</v>
-      </c>
-      <c r="J398" s="5">
-        <v>0</v>
-      </c>
-      <c r="K398" s="5">
-        <v>0</v>
-      </c>
-      <c r="L398" s="5">
-        <v>0</v>
-      </c>
-      <c r="M398" s="5">
-        <v>0</v>
-      </c>
-      <c r="N398" s="5">
-        <v>0</v>
-      </c>
-      <c r="O398" s="5">
-        <v>1</v>
-      </c>
-      <c r="P398" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="399" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A399" s="5">
+      <c r="E401">
+        <v>1</v>
+      </c>
+      <c r="F401">
+        <v>1</v>
+      </c>
+      <c r="G401">
+        <v>1</v>
+      </c>
+      <c r="H401">
+        <v>1</v>
+      </c>
+      <c r="I401">
+        <v>1</v>
+      </c>
+      <c r="J401">
+        <v>0</v>
+      </c>
+      <c r="K401">
+        <v>0</v>
+      </c>
+      <c r="L401">
+        <v>0</v>
+      </c>
+      <c r="M401">
+        <v>0</v>
+      </c>
+      <c r="N401">
+        <v>0</v>
+      </c>
+      <c r="O401">
+        <v>1</v>
+      </c>
+      <c r="P401">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="402" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A402">
         <v>66</v>
       </c>
-      <c r="B399" s="5" t="s">
+      <c r="B402" t="s">
+        <v>1135</v>
+      </c>
+      <c r="C402">
+        <v>286</v>
+      </c>
+      <c r="D402" t="s">
+        <v>1143</v>
+      </c>
+      <c r="E402">
+        <v>1</v>
+      </c>
+      <c r="F402">
+        <v>1</v>
+      </c>
+      <c r="G402">
+        <v>1</v>
+      </c>
+      <c r="H402">
+        <v>1</v>
+      </c>
+      <c r="I402">
+        <v>1</v>
+      </c>
+      <c r="J402">
+        <v>0</v>
+      </c>
+      <c r="K402">
+        <v>0</v>
+      </c>
+      <c r="L402">
+        <v>0</v>
+      </c>
+      <c r="M402">
+        <v>0</v>
+      </c>
+      <c r="N402">
+        <v>0</v>
+      </c>
+      <c r="O402">
+        <v>1</v>
+      </c>
+      <c r="P402">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="403" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A403">
+        <v>66</v>
+      </c>
+      <c r="B403" t="s">
+        <v>1135</v>
+      </c>
+      <c r="C403">
+        <v>288</v>
+      </c>
+      <c r="D403" t="s">
+        <v>1145</v>
+      </c>
+      <c r="E403">
+        <v>1</v>
+      </c>
+      <c r="F403">
+        <v>1</v>
+      </c>
+      <c r="G403">
+        <v>1</v>
+      </c>
+      <c r="H403">
+        <v>1</v>
+      </c>
+      <c r="I403">
+        <v>1</v>
+      </c>
+      <c r="J403">
+        <v>0</v>
+      </c>
+      <c r="K403">
+        <v>0</v>
+      </c>
+      <c r="L403">
+        <v>0</v>
+      </c>
+      <c r="M403">
+        <v>0</v>
+      </c>
+      <c r="N403">
+        <v>0</v>
+      </c>
+      <c r="O403">
+        <v>1</v>
+      </c>
+      <c r="P403">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="404" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A404">
+        <v>66</v>
+      </c>
+      <c r="B404" t="s">
+        <v>1135</v>
+      </c>
+      <c r="C404">
+        <v>294</v>
+      </c>
+      <c r="D404" t="s">
+        <v>1151</v>
+      </c>
+      <c r="E404">
+        <v>1</v>
+      </c>
+      <c r="F404">
+        <v>1</v>
+      </c>
+      <c r="G404">
+        <v>1</v>
+      </c>
+      <c r="H404">
+        <v>1</v>
+      </c>
+      <c r="I404">
+        <v>1</v>
+      </c>
+      <c r="J404">
+        <v>0</v>
+      </c>
+      <c r="K404">
+        <v>0</v>
+      </c>
+      <c r="L404">
+        <v>0</v>
+      </c>
+      <c r="M404">
+        <v>0</v>
+      </c>
+      <c r="N404">
+        <v>0</v>
+      </c>
+      <c r="O404">
+        <v>1</v>
+      </c>
+      <c r="P404">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="405" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A405">
+        <v>66</v>
+      </c>
+      <c r="B405" t="s">
+        <v>1135</v>
+      </c>
+      <c r="C405">
+        <v>285</v>
+      </c>
+      <c r="D405" t="s">
+        <v>1142</v>
+      </c>
+      <c r="E405">
+        <v>1</v>
+      </c>
+      <c r="F405">
+        <v>1</v>
+      </c>
+      <c r="G405">
+        <v>1</v>
+      </c>
+      <c r="H405">
+        <v>1</v>
+      </c>
+      <c r="I405">
+        <v>1</v>
+      </c>
+      <c r="J405">
+        <v>0</v>
+      </c>
+      <c r="K405">
+        <v>0</v>
+      </c>
+      <c r="L405">
+        <v>0</v>
+      </c>
+      <c r="M405">
+        <v>0</v>
+      </c>
+      <c r="N405">
+        <v>0</v>
+      </c>
+      <c r="O405">
+        <v>1</v>
+      </c>
+      <c r="P405">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="406" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A406">
+        <v>67</v>
+      </c>
+      <c r="B406" t="s">
         <v>1136</v>
       </c>
-      <c r="C399" s="5">
-        <v>296</v>
-      </c>
-      <c r="D399" s="5" t="s">
-        <v>1154</v>
-      </c>
-      <c r="E399" s="5">
-        <v>1</v>
-      </c>
-      <c r="F399" s="5">
-        <v>1</v>
-      </c>
-      <c r="G399" s="5">
-        <v>1</v>
-      </c>
-      <c r="H399" s="5">
-        <v>1</v>
-      </c>
-      <c r="I399" s="5">
-        <v>1</v>
-      </c>
-      <c r="J399" s="5">
-        <v>0</v>
-      </c>
-      <c r="K399" s="5">
-        <v>0</v>
-      </c>
-      <c r="L399" s="5">
-        <v>0</v>
-      </c>
-      <c r="M399" s="5">
-        <v>0</v>
-      </c>
-      <c r="N399" s="5">
-        <v>0</v>
-      </c>
-      <c r="O399" s="5">
-        <v>1</v>
-      </c>
-      <c r="P399" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="400" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A400" s="5">
-        <v>66</v>
-      </c>
-      <c r="B400" s="5" t="s">
+      <c r="C406">
+        <v>113</v>
+      </c>
+      <c r="D406" t="s">
+        <v>491</v>
+      </c>
+      <c r="E406">
+        <v>1</v>
+      </c>
+      <c r="F406">
+        <v>1</v>
+      </c>
+      <c r="G406">
+        <v>1</v>
+      </c>
+      <c r="H406">
+        <v>1</v>
+      </c>
+      <c r="I406">
+        <v>1</v>
+      </c>
+      <c r="J406">
+        <v>0</v>
+      </c>
+      <c r="K406">
+        <v>0</v>
+      </c>
+      <c r="L406">
+        <v>0</v>
+      </c>
+      <c r="M406">
+        <v>0</v>
+      </c>
+      <c r="N406">
+        <v>0</v>
+      </c>
+      <c r="O406">
+        <v>1</v>
+      </c>
+      <c r="P406">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="407" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A407">
+        <v>67</v>
+      </c>
+      <c r="B407" t="s">
         <v>1136</v>
       </c>
-      <c r="C400" s="5">
-        <v>297</v>
-      </c>
-      <c r="D400" s="5" t="s">
-        <v>1155</v>
-      </c>
-      <c r="E400" s="5">
-        <v>1</v>
-      </c>
-      <c r="F400" s="5">
-        <v>1</v>
-      </c>
-      <c r="G400" s="5">
-        <v>1</v>
-      </c>
-      <c r="H400" s="5">
-        <v>1</v>
-      </c>
-      <c r="I400" s="5">
-        <v>1</v>
-      </c>
-      <c r="J400" s="5">
-        <v>0</v>
-      </c>
-      <c r="K400" s="5">
-        <v>0</v>
-      </c>
-      <c r="L400" s="5">
-        <v>0</v>
-      </c>
-      <c r="M400" s="5">
-        <v>0</v>
-      </c>
-      <c r="N400" s="5">
-        <v>0</v>
-      </c>
-      <c r="O400" s="5">
-        <v>1</v>
-      </c>
-      <c r="P400" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="401" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A401" s="5">
-        <v>66</v>
-      </c>
-      <c r="B401" s="5" t="s">
+      <c r="C407">
+        <v>287</v>
+      </c>
+      <c r="D407" t="s">
+        <v>1144</v>
+      </c>
+      <c r="E407">
+        <v>1</v>
+      </c>
+      <c r="F407">
+        <v>1</v>
+      </c>
+      <c r="G407">
+        <v>1</v>
+      </c>
+      <c r="H407">
+        <v>1</v>
+      </c>
+      <c r="I407">
+        <v>1</v>
+      </c>
+      <c r="J407">
+        <v>0</v>
+      </c>
+      <c r="K407">
+        <v>0</v>
+      </c>
+      <c r="L407">
+        <v>0</v>
+      </c>
+      <c r="M407">
+        <v>0</v>
+      </c>
+      <c r="N407">
+        <v>0</v>
+      </c>
+      <c r="O407">
+        <v>1</v>
+      </c>
+      <c r="P407">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="408" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A408">
+        <v>67</v>
+      </c>
+      <c r="B408" t="s">
         <v>1136</v>
       </c>
-      <c r="C401" s="5">
+      <c r="C408">
+        <v>290</v>
+      </c>
+      <c r="D408" t="s">
+        <v>1147</v>
+      </c>
+      <c r="E408">
+        <v>1</v>
+      </c>
+      <c r="F408">
+        <v>1</v>
+      </c>
+      <c r="G408">
+        <v>1</v>
+      </c>
+      <c r="H408">
+        <v>1</v>
+      </c>
+      <c r="I408">
+        <v>1</v>
+      </c>
+      <c r="J408">
+        <v>0</v>
+      </c>
+      <c r="K408">
+        <v>0</v>
+      </c>
+      <c r="L408">
+        <v>0</v>
+      </c>
+      <c r="M408">
+        <v>0</v>
+      </c>
+      <c r="N408">
+        <v>0</v>
+      </c>
+      <c r="O408">
+        <v>1</v>
+      </c>
+      <c r="P408">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="409" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A409">
+        <v>67</v>
+      </c>
+      <c r="B409" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C409">
         <v>42</v>
       </c>
-      <c r="D401" s="5" t="s">
+      <c r="D409" t="s">
         <v>205</v>
       </c>
-      <c r="E401" s="5">
-        <v>1</v>
-      </c>
-      <c r="F401" s="5">
-        <v>1</v>
-      </c>
-      <c r="G401" s="5">
-        <v>1</v>
-      </c>
-      <c r="H401" s="5">
-        <v>1</v>
-      </c>
-      <c r="I401" s="5">
-        <v>1</v>
-      </c>
-      <c r="J401" s="5">
-        <v>0</v>
-      </c>
-      <c r="K401" s="5">
-        <v>0</v>
-      </c>
-      <c r="L401" s="5">
-        <v>0</v>
-      </c>
-      <c r="M401" s="5">
-        <v>0</v>
-      </c>
-      <c r="N401" s="5">
-        <v>0</v>
-      </c>
-      <c r="O401" s="5">
-        <v>1</v>
-      </c>
-      <c r="P401" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="402" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A402" s="5">
-        <v>66</v>
-      </c>
-      <c r="B402" s="5" t="s">
-        <v>1136</v>
-      </c>
-      <c r="C402" s="5">
-        <v>286</v>
-      </c>
-      <c r="D402" s="5" t="s">
-        <v>1144</v>
-      </c>
-      <c r="E402" s="5">
-        <v>1</v>
-      </c>
-      <c r="F402" s="5">
-        <v>1</v>
-      </c>
-      <c r="G402" s="5">
-        <v>1</v>
-      </c>
-      <c r="H402" s="5">
-        <v>1</v>
-      </c>
-      <c r="I402" s="5">
-        <v>1</v>
-      </c>
-      <c r="J402" s="5">
-        <v>0</v>
-      </c>
-      <c r="K402" s="5">
-        <v>0</v>
-      </c>
-      <c r="L402" s="5">
-        <v>0</v>
-      </c>
-      <c r="M402" s="5">
-        <v>0</v>
-      </c>
-      <c r="N402" s="5">
-        <v>0</v>
-      </c>
-      <c r="O402" s="5">
-        <v>1</v>
-      </c>
-      <c r="P402" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="403" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A403" s="5">
-        <v>66</v>
-      </c>
-      <c r="B403" s="5" t="s">
-        <v>1136</v>
-      </c>
-      <c r="C403" s="5">
-        <v>288</v>
-      </c>
-      <c r="D403" s="5" t="s">
+      <c r="E409">
+        <v>1</v>
+      </c>
+      <c r="F409">
+        <v>1</v>
+      </c>
+      <c r="G409">
+        <v>1</v>
+      </c>
+      <c r="H409">
+        <v>1</v>
+      </c>
+      <c r="I409">
+        <v>1</v>
+      </c>
+      <c r="J409">
+        <v>0</v>
+      </c>
+      <c r="K409">
+        <v>0</v>
+      </c>
+      <c r="L409">
+        <v>0</v>
+      </c>
+      <c r="M409">
+        <v>0</v>
+      </c>
+      <c r="N409">
+        <v>0</v>
+      </c>
+      <c r="O409">
+        <v>1</v>
+      </c>
+      <c r="P409">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="410" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A410">
+        <v>68</v>
+      </c>
+      <c r="B410" t="s">
+        <v>112</v>
+      </c>
+      <c r="C410">
+        <v>289</v>
+      </c>
+      <c r="D410" t="s">
         <v>1146</v>
       </c>
-      <c r="E403" s="5">
-        <v>1</v>
-      </c>
-      <c r="F403" s="5">
-        <v>1</v>
-      </c>
-      <c r="G403" s="5">
-        <v>1</v>
-      </c>
-      <c r="H403" s="5">
-        <v>1</v>
-      </c>
-      <c r="I403" s="5">
-        <v>1</v>
-      </c>
-      <c r="J403" s="5">
-        <v>0</v>
-      </c>
-      <c r="K403" s="5">
-        <v>0</v>
-      </c>
-      <c r="L403" s="5">
-        <v>0</v>
-      </c>
-      <c r="M403" s="5">
-        <v>0</v>
-      </c>
-      <c r="N403" s="5">
-        <v>0</v>
-      </c>
-      <c r="O403" s="5">
-        <v>1</v>
-      </c>
-      <c r="P403" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="404" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A404" s="5">
-        <v>66</v>
-      </c>
-      <c r="B404" s="5" t="s">
-        <v>1136</v>
-      </c>
-      <c r="C404" s="5">
-        <v>294</v>
-      </c>
-      <c r="D404" s="5" t="s">
-        <v>1152</v>
-      </c>
-      <c r="E404" s="5">
-        <v>1</v>
-      </c>
-      <c r="F404" s="5">
-        <v>1</v>
-      </c>
-      <c r="G404" s="5">
-        <v>1</v>
-      </c>
-      <c r="H404" s="5">
-        <v>1</v>
-      </c>
-      <c r="I404" s="5">
-        <v>1</v>
-      </c>
-      <c r="J404" s="5">
-        <v>0</v>
-      </c>
-      <c r="K404" s="5">
-        <v>0</v>
-      </c>
-      <c r="L404" s="5">
-        <v>0</v>
-      </c>
-      <c r="M404" s="5">
-        <v>0</v>
-      </c>
-      <c r="N404" s="5">
-        <v>0</v>
-      </c>
-      <c r="O404" s="5">
-        <v>1</v>
-      </c>
-      <c r="P404" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="405" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A405" s="5">
-        <v>66</v>
-      </c>
-      <c r="B405" s="5" t="s">
-        <v>1136</v>
-      </c>
-      <c r="C405" s="5">
-        <v>285</v>
-      </c>
-      <c r="D405" s="5" t="s">
-        <v>1143</v>
-      </c>
-      <c r="E405" s="5">
-        <v>1</v>
-      </c>
-      <c r="F405" s="5">
-        <v>1</v>
-      </c>
-      <c r="G405" s="5">
-        <v>1</v>
-      </c>
-      <c r="H405" s="5">
-        <v>1</v>
-      </c>
-      <c r="I405" s="5">
-        <v>1</v>
-      </c>
-      <c r="J405" s="5">
-        <v>0</v>
-      </c>
-      <c r="K405" s="5">
-        <v>0</v>
-      </c>
-      <c r="L405" s="5">
-        <v>0</v>
-      </c>
-      <c r="M405" s="5">
-        <v>0</v>
-      </c>
-      <c r="N405" s="5">
-        <v>0</v>
-      </c>
-      <c r="O405" s="5">
-        <v>1</v>
-      </c>
-      <c r="P405" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="406" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A406" s="5">
-        <v>67</v>
-      </c>
-      <c r="B406" s="5" t="s">
+      <c r="E410">
+        <v>1</v>
+      </c>
+      <c r="F410">
+        <v>1</v>
+      </c>
+      <c r="G410">
+        <v>1</v>
+      </c>
+      <c r="H410">
+        <v>1</v>
+      </c>
+      <c r="I410">
+        <v>1</v>
+      </c>
+      <c r="J410">
+        <v>0</v>
+      </c>
+      <c r="K410">
+        <v>0</v>
+      </c>
+      <c r="L410">
+        <v>0</v>
+      </c>
+      <c r="M410">
+        <v>0</v>
+      </c>
+      <c r="N410">
+        <v>0</v>
+      </c>
+      <c r="O410">
+        <v>1</v>
+      </c>
+      <c r="P410">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="411" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A411">
+        <v>68</v>
+      </c>
+      <c r="B411" t="s">
+        <v>112</v>
+      </c>
+      <c r="C411">
+        <v>283</v>
+      </c>
+      <c r="D411" t="s">
+        <v>1140</v>
+      </c>
+      <c r="E411">
+        <v>1</v>
+      </c>
+      <c r="F411">
+        <v>1</v>
+      </c>
+      <c r="G411">
+        <v>1</v>
+      </c>
+      <c r="H411">
+        <v>1</v>
+      </c>
+      <c r="I411">
+        <v>1</v>
+      </c>
+      <c r="J411">
+        <v>0</v>
+      </c>
+      <c r="K411">
+        <v>0</v>
+      </c>
+      <c r="L411">
+        <v>0</v>
+      </c>
+      <c r="M411">
+        <v>0</v>
+      </c>
+      <c r="N411">
+        <v>0</v>
+      </c>
+      <c r="O411">
+        <v>1</v>
+      </c>
+      <c r="P411">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="412" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A412">
+        <v>68</v>
+      </c>
+      <c r="B412" t="s">
+        <v>112</v>
+      </c>
+      <c r="C412">
+        <v>42</v>
+      </c>
+      <c r="D412" t="s">
+        <v>205</v>
+      </c>
+      <c r="E412">
+        <v>1</v>
+      </c>
+      <c r="F412">
+        <v>1</v>
+      </c>
+      <c r="G412">
+        <v>1</v>
+      </c>
+      <c r="H412">
+        <v>1</v>
+      </c>
+      <c r="I412">
+        <v>1</v>
+      </c>
+      <c r="J412">
+        <v>0</v>
+      </c>
+      <c r="K412">
+        <v>0</v>
+      </c>
+      <c r="L412">
+        <v>0</v>
+      </c>
+      <c r="M412">
+        <v>0</v>
+      </c>
+      <c r="N412">
+        <v>0</v>
+      </c>
+      <c r="O412">
+        <v>1</v>
+      </c>
+      <c r="P412">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="413" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A413">
+        <v>69</v>
+      </c>
+      <c r="B413" t="s">
         <v>1137</v>
       </c>
-      <c r="C406" s="5">
-        <v>113</v>
-      </c>
-      <c r="D406" s="5" t="s">
-        <v>491</v>
-      </c>
-      <c r="E406" s="5">
-        <v>1</v>
-      </c>
-      <c r="F406" s="5">
-        <v>1</v>
-      </c>
-      <c r="G406" s="5">
-        <v>1</v>
-      </c>
-      <c r="H406" s="5">
-        <v>1</v>
-      </c>
-      <c r="I406" s="5">
-        <v>1</v>
-      </c>
-      <c r="J406" s="5">
-        <v>0</v>
-      </c>
-      <c r="K406" s="5">
-        <v>0</v>
-      </c>
-      <c r="L406" s="5">
-        <v>0</v>
-      </c>
-      <c r="M406" s="5">
-        <v>0</v>
-      </c>
-      <c r="N406" s="5">
-        <v>0</v>
-      </c>
-      <c r="O406" s="5">
-        <v>1</v>
-      </c>
-      <c r="P406" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="407" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A407" s="5">
-        <v>67</v>
-      </c>
-      <c r="B407" s="5" t="s">
-        <v>1137</v>
-      </c>
-      <c r="C407" s="5">
-        <v>287</v>
-      </c>
-      <c r="D407" s="5" t="s">
-        <v>1145</v>
-      </c>
-      <c r="E407" s="5">
-        <v>1</v>
-      </c>
-      <c r="F407" s="5">
-        <v>1</v>
-      </c>
-      <c r="G407" s="5">
-        <v>1</v>
-      </c>
-      <c r="H407" s="5">
-        <v>1</v>
-      </c>
-      <c r="I407" s="5">
-        <v>1</v>
-      </c>
-      <c r="J407" s="5">
-        <v>0</v>
-      </c>
-      <c r="K407" s="5">
-        <v>0</v>
-      </c>
-      <c r="L407" s="5">
-        <v>0</v>
-      </c>
-      <c r="M407" s="5">
-        <v>0</v>
-      </c>
-      <c r="N407" s="5">
-        <v>0</v>
-      </c>
-      <c r="O407" s="5">
-        <v>1</v>
-      </c>
-      <c r="P407" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="408" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A408" s="5">
-        <v>67</v>
-      </c>
-      <c r="B408" s="5" t="s">
-        <v>1137</v>
-      </c>
-      <c r="C408" s="5">
-        <v>290</v>
-      </c>
-      <c r="D408" s="5" t="s">
-        <v>1148</v>
-      </c>
-      <c r="E408" s="5">
-        <v>1</v>
-      </c>
-      <c r="F408" s="5">
-        <v>1</v>
-      </c>
-      <c r="G408" s="5">
-        <v>1</v>
-      </c>
-      <c r="H408" s="5">
-        <v>1</v>
-      </c>
-      <c r="I408" s="5">
-        <v>1</v>
-      </c>
-      <c r="J408" s="5">
-        <v>0</v>
-      </c>
-      <c r="K408" s="5">
-        <v>0</v>
-      </c>
-      <c r="L408" s="5">
-        <v>0</v>
-      </c>
-      <c r="M408" s="5">
-        <v>0</v>
-      </c>
-      <c r="N408" s="5">
-        <v>0</v>
-      </c>
-      <c r="O408" s="5">
-        <v>1</v>
-      </c>
-      <c r="P408" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="409" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A409" s="5">
-        <v>67</v>
-      </c>
-      <c r="B409" s="5" t="s">
-        <v>1137</v>
-      </c>
-      <c r="C409" s="5">
+      <c r="C413">
         <v>42</v>
       </c>
-      <c r="D409" s="5" t="s">
+      <c r="D413" t="s">
         <v>205</v>
       </c>
-      <c r="E409" s="5">
-        <v>1</v>
-      </c>
-      <c r="F409" s="5">
-        <v>1</v>
-      </c>
-      <c r="G409" s="5">
-        <v>1</v>
-      </c>
-      <c r="H409" s="5">
-        <v>1</v>
-      </c>
-      <c r="I409" s="5">
-        <v>1</v>
-      </c>
-      <c r="J409" s="5">
-        <v>0</v>
-      </c>
-      <c r="K409" s="5">
-        <v>0</v>
-      </c>
-      <c r="L409" s="5">
-        <v>0</v>
-      </c>
-      <c r="M409" s="5">
-        <v>0</v>
-      </c>
-      <c r="N409" s="5">
-        <v>0</v>
-      </c>
-      <c r="O409" s="5">
-        <v>1</v>
-      </c>
-      <c r="P409" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="410" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A410" s="5">
-        <v>68</v>
-      </c>
-      <c r="B410" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="C410" s="5">
-        <v>289</v>
-      </c>
-      <c r="D410" s="5" t="s">
-        <v>1147</v>
-      </c>
-      <c r="E410" s="5">
-        <v>1</v>
-      </c>
-      <c r="F410" s="5">
-        <v>1</v>
-      </c>
-      <c r="G410" s="5">
-        <v>1</v>
-      </c>
-      <c r="H410" s="5">
-        <v>1</v>
-      </c>
-      <c r="I410" s="5">
-        <v>1</v>
-      </c>
-      <c r="J410" s="5">
-        <v>0</v>
-      </c>
-      <c r="K410" s="5">
-        <v>0</v>
-      </c>
-      <c r="L410" s="5">
-        <v>0</v>
-      </c>
-      <c r="M410" s="5">
-        <v>0</v>
-      </c>
-      <c r="N410" s="5">
-        <v>0</v>
-      </c>
-      <c r="O410" s="5">
-        <v>1</v>
-      </c>
-      <c r="P410" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="411" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A411" s="5">
-        <v>68</v>
-      </c>
-      <c r="B411" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="C411" s="5">
-        <v>283</v>
-      </c>
-      <c r="D411" s="5" t="s">
-        <v>1141</v>
-      </c>
-      <c r="E411" s="5">
-        <v>1</v>
-      </c>
-      <c r="F411" s="5">
-        <v>1</v>
-      </c>
-      <c r="G411" s="5">
-        <v>1</v>
-      </c>
-      <c r="H411" s="5">
-        <v>1</v>
-      </c>
-      <c r="I411" s="5">
-        <v>1</v>
-      </c>
-      <c r="J411" s="5">
-        <v>0</v>
-      </c>
-      <c r="K411" s="5">
-        <v>0</v>
-      </c>
-      <c r="L411" s="5">
-        <v>0</v>
-      </c>
-      <c r="M411" s="5">
-        <v>0</v>
-      </c>
-      <c r="N411" s="5">
-        <v>0</v>
-      </c>
-      <c r="O411" s="5">
-        <v>1</v>
-      </c>
-      <c r="P411" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="412" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A412" s="5">
-        <v>68</v>
-      </c>
-      <c r="B412" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="C412" s="5">
+      <c r="E413">
+        <v>1</v>
+      </c>
+      <c r="F413">
+        <v>1</v>
+      </c>
+      <c r="G413">
+        <v>1</v>
+      </c>
+      <c r="H413">
+        <v>1</v>
+      </c>
+      <c r="I413">
+        <v>1</v>
+      </c>
+      <c r="J413">
+        <v>0</v>
+      </c>
+      <c r="K413">
+        <v>0</v>
+      </c>
+      <c r="L413">
+        <v>0</v>
+      </c>
+      <c r="M413">
+        <v>0</v>
+      </c>
+      <c r="N413">
+        <v>0</v>
+      </c>
+      <c r="O413">
+        <v>1</v>
+      </c>
+      <c r="P413">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="414" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A414">
+        <v>70</v>
+      </c>
+      <c r="B414" t="s">
+        <v>1138</v>
+      </c>
+      <c r="C414">
         <v>42</v>
       </c>
-      <c r="D412" s="5" t="s">
+      <c r="D414" t="s">
         <v>205</v>
       </c>
-      <c r="E412" s="5">
-        <v>1</v>
-      </c>
-      <c r="F412" s="5">
-        <v>1</v>
-      </c>
-      <c r="G412" s="5">
-        <v>1</v>
-      </c>
-      <c r="H412" s="5">
-        <v>1</v>
-      </c>
-      <c r="I412" s="5">
-        <v>1</v>
-      </c>
-      <c r="J412" s="5">
-        <v>0</v>
-      </c>
-      <c r="K412" s="5">
-        <v>0</v>
-      </c>
-      <c r="L412" s="5">
-        <v>0</v>
-      </c>
-      <c r="M412" s="5">
-        <v>0</v>
-      </c>
-      <c r="N412" s="5">
-        <v>0</v>
-      </c>
-      <c r="O412" s="5">
-        <v>1</v>
-      </c>
-      <c r="P412" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="413" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A413" s="5">
-        <v>69</v>
-      </c>
-      <c r="B413" s="5" t="s">
-        <v>1138</v>
-      </c>
-      <c r="C413" s="5">
+      <c r="E414">
+        <v>1</v>
+      </c>
+      <c r="F414">
+        <v>1</v>
+      </c>
+      <c r="G414">
+        <v>1</v>
+      </c>
+      <c r="H414">
+        <v>1</v>
+      </c>
+      <c r="I414">
+        <v>1</v>
+      </c>
+      <c r="J414">
+        <v>0</v>
+      </c>
+      <c r="K414">
+        <v>0</v>
+      </c>
+      <c r="L414">
+        <v>0</v>
+      </c>
+      <c r="M414">
+        <v>0</v>
+      </c>
+      <c r="N414">
+        <v>0</v>
+      </c>
+      <c r="O414">
+        <v>1</v>
+      </c>
+      <c r="P414">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="415" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A415">
+        <v>71</v>
+      </c>
+      <c r="B415" t="s">
+        <v>544</v>
+      </c>
+      <c r="C415">
         <v>42</v>
       </c>
-      <c r="D413" s="5" t="s">
+      <c r="D415" t="s">
         <v>205</v>
       </c>
-      <c r="E413" s="5">
-        <v>1</v>
-      </c>
-      <c r="F413" s="5">
-        <v>1</v>
-      </c>
-      <c r="G413" s="5">
-        <v>1</v>
-      </c>
-      <c r="H413" s="5">
-        <v>1</v>
-      </c>
-      <c r="I413" s="5">
-        <v>1</v>
-      </c>
-      <c r="J413" s="5">
-        <v>0</v>
-      </c>
-      <c r="K413" s="5">
-        <v>0</v>
-      </c>
-      <c r="L413" s="5">
-        <v>0</v>
-      </c>
-      <c r="M413" s="5">
-        <v>0</v>
-      </c>
-      <c r="N413" s="5">
-        <v>0</v>
-      </c>
-      <c r="O413" s="5">
-        <v>1</v>
-      </c>
-      <c r="P413" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="414" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A414" s="5">
-        <v>70</v>
-      </c>
-      <c r="B414" s="5" t="s">
+      <c r="E415">
+        <v>1</v>
+      </c>
+      <c r="F415">
+        <v>1</v>
+      </c>
+      <c r="G415">
+        <v>1</v>
+      </c>
+      <c r="H415">
+        <v>1</v>
+      </c>
+      <c r="I415">
+        <v>1</v>
+      </c>
+      <c r="J415">
+        <v>0</v>
+      </c>
+      <c r="K415">
+        <v>0</v>
+      </c>
+      <c r="L415">
+        <v>0</v>
+      </c>
+      <c r="M415">
+        <v>0</v>
+      </c>
+      <c r="N415">
+        <v>0</v>
+      </c>
+      <c r="O415">
+        <v>1</v>
+      </c>
+      <c r="P415">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="416" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A416">
+        <v>72</v>
+      </c>
+      <c r="B416" t="s">
         <v>1139</v>
       </c>
-      <c r="C414" s="5">
+      <c r="C416">
         <v>42</v>
       </c>
-      <c r="D414" s="5" t="s">
+      <c r="D416" t="s">
         <v>205</v>
       </c>
-      <c r="E414" s="5">
-        <v>1</v>
-      </c>
-      <c r="F414" s="5">
-        <v>1</v>
-      </c>
-      <c r="G414" s="5">
-        <v>1</v>
-      </c>
-      <c r="H414" s="5">
-        <v>1</v>
-      </c>
-      <c r="I414" s="5">
-        <v>1</v>
-      </c>
-      <c r="J414" s="5">
-        <v>0</v>
-      </c>
-      <c r="K414" s="5">
-        <v>0</v>
-      </c>
-      <c r="L414" s="5">
-        <v>0</v>
-      </c>
-      <c r="M414" s="5">
-        <v>0</v>
-      </c>
-      <c r="N414" s="5">
-        <v>0</v>
-      </c>
-      <c r="O414" s="5">
-        <v>1</v>
-      </c>
-      <c r="P414" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="415" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A415" s="5">
-        <v>71</v>
-      </c>
-      <c r="B415" s="5" t="s">
-        <v>544</v>
-      </c>
-      <c r="C415" s="5">
-        <v>42</v>
-      </c>
-      <c r="D415" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="E415" s="5">
-        <v>1</v>
-      </c>
-      <c r="F415" s="5">
-        <v>1</v>
-      </c>
-      <c r="G415" s="5">
-        <v>1</v>
-      </c>
-      <c r="H415" s="5">
-        <v>1</v>
-      </c>
-      <c r="I415" s="5">
-        <v>1</v>
-      </c>
-      <c r="J415" s="5">
-        <v>0</v>
-      </c>
-      <c r="K415" s="5">
-        <v>0</v>
-      </c>
-      <c r="L415" s="5">
-        <v>0</v>
-      </c>
-      <c r="M415" s="5">
-        <v>0</v>
-      </c>
-      <c r="N415" s="5">
-        <v>0</v>
-      </c>
-      <c r="O415" s="5">
-        <v>1</v>
-      </c>
-      <c r="P415" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="416" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A416" s="5">
-        <v>72</v>
-      </c>
-      <c r="B416" s="5" t="s">
-        <v>1140</v>
-      </c>
-      <c r="C416" s="5">
-        <v>42</v>
-      </c>
-      <c r="D416" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="E416" s="5">
-        <v>1</v>
-      </c>
-      <c r="F416" s="5">
-        <v>1</v>
-      </c>
-      <c r="G416" s="5">
-        <v>1</v>
-      </c>
-      <c r="H416" s="5">
-        <v>1</v>
-      </c>
-      <c r="I416" s="5">
-        <v>1</v>
-      </c>
-      <c r="J416" s="5">
-        <v>0</v>
-      </c>
-      <c r="K416" s="5">
-        <v>0</v>
-      </c>
-      <c r="L416" s="5">
-        <v>0</v>
-      </c>
-      <c r="M416" s="5">
-        <v>0</v>
-      </c>
-      <c r="N416" s="5">
-        <v>0</v>
-      </c>
-      <c r="O416" s="5">
-        <v>1</v>
-      </c>
-      <c r="P416" s="5">
+      <c r="E416">
+        <v>1</v>
+      </c>
+      <c r="F416">
+        <v>1</v>
+      </c>
+      <c r="G416">
+        <v>1</v>
+      </c>
+      <c r="H416">
+        <v>1</v>
+      </c>
+      <c r="I416">
+        <v>1</v>
+      </c>
+      <c r="J416">
+        <v>0</v>
+      </c>
+      <c r="K416">
+        <v>0</v>
+      </c>
+      <c r="L416">
+        <v>0</v>
+      </c>
+      <c r="M416">
+        <v>0</v>
+      </c>
+      <c r="N416">
+        <v>0</v>
+      </c>
+      <c r="O416">
+        <v>1</v>
+      </c>
+      <c r="P416">
         <v>0</v>
       </c>
     </row>
@@ -35499,7 +35519,7 @@
       <c r="G7" s="8">
         <v>1</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H7" s="11">
         <v>42248</v>
       </c>
       <c r="I7" s="8">
@@ -35528,7 +35548,7 @@
       <c r="G8" s="8">
         <v>1</v>
       </c>
-      <c r="H8" s="12">
+      <c r="H8" s="11">
         <v>44275.455153935189</v>
       </c>
       <c r="I8" s="8">
@@ -35557,7 +35577,7 @@
       <c r="G9" s="8">
         <v>0</v>
       </c>
-      <c r="H9" s="12">
+      <c r="H9" s="11">
         <v>43577.412575810187</v>
       </c>
       <c r="I9" s="8">
@@ -35960,7 +35980,7 @@
   <dimension ref="A1:I79"/>
   <sheetViews>
     <sheetView topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="G75" sqref="G75"/>
+      <selection activeCell="A79" sqref="A78:I79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -38233,31 +38253,31 @@
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A79" s="5">
+      <c r="A79">
         <v>238</v>
       </c>
-      <c r="B79" s="5" t="s">
+      <c r="B79" t="s">
         <v>3</v>
       </c>
-      <c r="C79" s="5" t="s">
+      <c r="C79" t="s">
         <v>1131</v>
       </c>
-      <c r="D79" s="5">
-        <v>1</v>
-      </c>
-      <c r="E79" s="5">
-        <v>0</v>
-      </c>
-      <c r="F79" s="5">
-        <v>0</v>
-      </c>
-      <c r="G79" s="5">
-        <v>1</v>
-      </c>
-      <c r="H79" s="5">
-        <v>0</v>
-      </c>
-      <c r="I79" s="5">
+      <c r="D79">
+        <v>1</v>
+      </c>
+      <c r="E79">
+        <v>0</v>
+      </c>
+      <c r="F79">
+        <v>0</v>
+      </c>
+      <c r="G79">
+        <v>1</v>
+      </c>
+      <c r="H79">
+        <v>0</v>
+      </c>
+      <c r="I79">
         <v>0</v>
       </c>
     </row>
@@ -39602,7 +39622,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD21"/>
+      <selection activeCell="A18" sqref="A18:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -39642,325 +39662,325 @@
       </c>
     </row>
     <row r="3" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="8">
-        <v>1</v>
-      </c>
-      <c r="B3" s="8" t="s">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="8">
-        <v>1</v>
-      </c>
-      <c r="D3" s="8">
-        <v>1</v>
-      </c>
-      <c r="E3" s="8">
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="8">
+      <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="8">
-        <v>0</v>
-      </c>
-      <c r="D4" s="8">
-        <v>0</v>
-      </c>
-      <c r="E4" s="8">
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="8">
+      <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="8">
-        <v>1</v>
-      </c>
-      <c r="D5" s="8">
-        <v>1</v>
-      </c>
-      <c r="E5" s="8">
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="8">
+      <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="8">
-        <v>1</v>
-      </c>
-      <c r="D6" s="8">
-        <v>1</v>
-      </c>
-      <c r="E6" s="8">
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="8">
+      <c r="A7">
         <v>5</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="8">
-        <v>1</v>
-      </c>
-      <c r="D7" s="8">
-        <v>0</v>
-      </c>
-      <c r="E7" s="8">
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="8">
+      <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="8">
-        <v>0</v>
-      </c>
-      <c r="D8" s="8">
-        <v>0</v>
-      </c>
-      <c r="E8" s="8">
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="8">
+      <c r="A9">
         <v>7</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="8">
-        <v>1</v>
-      </c>
-      <c r="D9" s="8">
-        <v>1</v>
-      </c>
-      <c r="E9" s="8">
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="8">
+      <c r="A10">
         <v>8</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" t="s">
         <v>54</v>
       </c>
-      <c r="C10" s="8">
-        <v>0</v>
-      </c>
-      <c r="D10" s="8">
-        <v>0</v>
-      </c>
-      <c r="E10" s="8">
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="8">
+      <c r="A11">
         <v>9</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="8">
-        <v>1</v>
-      </c>
-      <c r="D11" s="8">
-        <v>1</v>
-      </c>
-      <c r="E11" s="8">
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="8">
+      <c r="A12">
         <v>10</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="8">
-        <v>1</v>
-      </c>
-      <c r="D12" s="8">
-        <v>1</v>
-      </c>
-      <c r="E12" s="8">
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="8">
+      <c r="A13">
         <v>11</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" t="s">
         <v>61</v>
       </c>
-      <c r="C13" s="8">
-        <v>0</v>
-      </c>
-      <c r="D13" s="8">
-        <v>0</v>
-      </c>
-      <c r="E13" s="8">
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="8">
+      <c r="A14">
         <v>12</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" t="s">
         <v>64</v>
       </c>
-      <c r="C14" s="8">
-        <v>1</v>
-      </c>
-      <c r="D14" s="8">
-        <v>1</v>
-      </c>
-      <c r="E14" s="8">
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="8">
+      <c r="A15">
         <v>13</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" t="s">
         <v>67</v>
       </c>
-      <c r="C15" s="8">
-        <v>0</v>
-      </c>
-      <c r="D15" s="8">
-        <v>0</v>
-      </c>
-      <c r="E15" s="8">
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="8">
+      <c r="A16">
         <v>14</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" t="s">
         <v>69</v>
       </c>
-      <c r="C16" s="8">
-        <v>1</v>
-      </c>
-      <c r="D16" s="8">
-        <v>1</v>
-      </c>
-      <c r="E16" s="8">
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="8">
+      <c r="A17">
         <v>15</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" t="s">
         <v>72</v>
       </c>
-      <c r="C17" s="8">
-        <v>1</v>
-      </c>
-      <c r="D17" s="8">
-        <v>1</v>
-      </c>
-      <c r="E17" s="8">
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="8">
+      <c r="A18" s="5">
         <v>16</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C18" s="8">
-        <v>1</v>
-      </c>
-      <c r="D18" s="8">
-        <v>1</v>
-      </c>
-      <c r="E18" s="8">
+      <c r="C18" s="5">
+        <v>0</v>
+      </c>
+      <c r="D18" s="5">
+        <v>0</v>
+      </c>
+      <c r="E18" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="8">
+      <c r="A19">
         <v>17</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" t="s">
         <v>75</v>
       </c>
-      <c r="C19" s="8">
-        <v>0</v>
-      </c>
-      <c r="D19" s="8">
-        <v>0</v>
-      </c>
-      <c r="E19" s="8">
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="8">
+      <c r="A20">
         <v>18</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" t="s">
         <v>77</v>
       </c>
-      <c r="C20" s="8">
-        <v>1</v>
-      </c>
-      <c r="D20" s="8">
-        <v>1</v>
-      </c>
-      <c r="E20" s="8">
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="8">
+      <c r="A21">
         <v>19</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" t="s">
         <v>79</v>
       </c>
-      <c r="C21" s="8">
-        <v>0</v>
-      </c>
-      <c r="D21" s="8">
-        <v>0</v>
-      </c>
-      <c r="E21" s="8">
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
         <v>0</v>
       </c>
     </row>
@@ -40375,7 +40395,7 @@
       <c r="B5" s="8" t="s">
         <v>377</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="12" t="s">
         <v>1083</v>
       </c>
     </row>
@@ -41796,26 +41816,26 @@
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="5">
+      <c r="A13">
         <v>11</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" t="s">
         <v>1120</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="5">
+      <c r="A14">
         <v>12</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" t="s">
         <v>1121</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="5">
+      <c r="A15">
         <v>13</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" t="s">
         <v>1122</v>
       </c>
     </row>
@@ -42625,7 +42645,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:D17"/>
+      <selection activeCell="A18" sqref="A18:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -42926,20 +42946,20 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18">
+      <c r="A18" s="5">
         <v>16</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="E18" s="6">
-        <v>1</v>
+      <c r="E18" s="5">
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -43541,67 +43561,67 @@
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A67" s="5">
+      <c r="A67">
         <v>65</v>
       </c>
-      <c r="B67" s="5" t="s">
+      <c r="B67" t="s">
+        <v>1134</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A68">
+        <v>66</v>
+      </c>
+      <c r="B68" t="s">
         <v>1135</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A68" s="5">
-        <v>66</v>
-      </c>
-      <c r="B68" s="5" t="s">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A69">
+        <v>67</v>
+      </c>
+      <c r="B69" t="s">
         <v>1136</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A69" s="5">
-        <v>67</v>
-      </c>
-      <c r="B69" s="5" t="s">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A70">
+        <v>68</v>
+      </c>
+      <c r="B70" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A71">
+        <v>69</v>
+      </c>
+      <c r="B71" t="s">
         <v>1137</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A70" s="5">
-        <v>68</v>
-      </c>
-      <c r="B70" s="5" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A71" s="5">
-        <v>69</v>
-      </c>
-      <c r="B71" s="5" t="s">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A72">
+        <v>70</v>
+      </c>
+      <c r="B72" t="s">
         <v>1138</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A72" s="5">
-        <v>70</v>
-      </c>
-      <c r="B72" s="5" t="s">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A73">
+        <v>71</v>
+      </c>
+      <c r="B73" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A74">
+        <v>72</v>
+      </c>
+      <c r="B74" t="s">
         <v>1139</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A73" s="5">
-        <v>71</v>
-      </c>
-      <c r="B73" s="5" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A74" s="5">
-        <v>72</v>
-      </c>
-      <c r="B74" s="5" t="s">
-        <v>1140</v>
       </c>
     </row>
   </sheetData>
@@ -43614,7 +43634,7 @@
   <dimension ref="A1:B299"/>
   <sheetViews>
     <sheetView topLeftCell="A271" workbookViewId="0">
-      <selection activeCell="A285" sqref="A285:B299"/>
+      <selection activeCell="B283" sqref="B282:B283"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -45896,123 +45916,123 @@
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A285" s="5">
+      <c r="A285">
         <v>283</v>
       </c>
-      <c r="B285" s="5" t="s">
+      <c r="B285" t="s">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A286">
+        <v>284</v>
+      </c>
+      <c r="B286" t="s">
         <v>1141</v>
       </c>
     </row>
-    <row r="286" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A286" s="5">
-        <v>284</v>
-      </c>
-      <c r="B286" s="5" t="s">
+    <row r="287" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A287">
+        <v>285</v>
+      </c>
+      <c r="B287" t="s">
         <v>1142</v>
       </c>
     </row>
-    <row r="287" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A287" s="5">
-        <v>285</v>
-      </c>
-      <c r="B287" s="5" t="s">
+    <row r="288" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A288">
+        <v>286</v>
+      </c>
+      <c r="B288" t="s">
         <v>1143</v>
       </c>
     </row>
-    <row r="288" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A288" s="5">
-        <v>286</v>
-      </c>
-      <c r="B288" s="5" t="s">
+    <row r="289" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A289">
+        <v>287</v>
+      </c>
+      <c r="B289" t="s">
         <v>1144</v>
       </c>
     </row>
-    <row r="289" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A289" s="5">
-        <v>287</v>
-      </c>
-      <c r="B289" s="5" t="s">
+    <row r="290" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A290">
+        <v>288</v>
+      </c>
+      <c r="B290" t="s">
         <v>1145</v>
       </c>
     </row>
-    <row r="290" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A290" s="5">
-        <v>288</v>
-      </c>
-      <c r="B290" s="5" t="s">
+    <row r="291" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A291">
+        <v>289</v>
+      </c>
+      <c r="B291" t="s">
         <v>1146</v>
       </c>
     </row>
-    <row r="291" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A291" s="5">
-        <v>289</v>
-      </c>
-      <c r="B291" s="5" t="s">
+    <row r="292" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A292">
+        <v>290</v>
+      </c>
+      <c r="B292" t="s">
         <v>1147</v>
       </c>
     </row>
-    <row r="292" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A292" s="5">
-        <v>290</v>
-      </c>
-      <c r="B292" s="5" t="s">
+    <row r="293" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A293">
+        <v>291</v>
+      </c>
+      <c r="B293" t="s">
         <v>1148</v>
       </c>
     </row>
-    <row r="293" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A293" s="5">
-        <v>291</v>
-      </c>
-      <c r="B293" s="5" t="s">
+    <row r="294" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A294">
+        <v>292</v>
+      </c>
+      <c r="B294" t="s">
         <v>1149</v>
       </c>
     </row>
-    <row r="294" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A294" s="5">
-        <v>292</v>
-      </c>
-      <c r="B294" s="5" t="s">
+    <row r="295" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A295">
+        <v>293</v>
+      </c>
+      <c r="B295" t="s">
         <v>1150</v>
       </c>
     </row>
-    <row r="295" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A295" s="5">
-        <v>293</v>
-      </c>
-      <c r="B295" s="5" t="s">
+    <row r="296" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A296">
+        <v>294</v>
+      </c>
+      <c r="B296" t="s">
         <v>1151</v>
       </c>
     </row>
-    <row r="296" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A296" s="5">
-        <v>294</v>
-      </c>
-      <c r="B296" s="5" t="s">
+    <row r="297" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A297">
+        <v>295</v>
+      </c>
+      <c r="B297" t="s">
         <v>1152</v>
       </c>
     </row>
-    <row r="297" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A297" s="5">
-        <v>295</v>
-      </c>
-      <c r="B297" s="5" t="s">
+    <row r="298" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A298">
+        <v>296</v>
+      </c>
+      <c r="B298" t="s">
         <v>1153</v>
       </c>
     </row>
-    <row r="298" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A298" s="5">
-        <v>296</v>
-      </c>
-      <c r="B298" s="5" t="s">
+    <row r="299" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A299">
+        <v>297</v>
+      </c>
+      <c r="B299" t="s">
         <v>1154</v>
-      </c>
-    </row>
-    <row r="299" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A299" s="5">
-        <v>297</v>
-      </c>
-      <c r="B299" s="5" t="s">
-        <v>1155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TFS 24715 - Updates to Warnings Reasons and Sub Reasons
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C51590
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TFS\eCoaching_V2\Design\DD\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABC79102-DEDC-490C-8F9E-13B31692ED79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F92C8171-FD67-4D72-B7F7-90DA7BE6C1E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57504" yWindow="1932" windowWidth="28992" windowHeight="15792" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4146" uniqueCount="1157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4178" uniqueCount="1162">
   <si>
     <t>SourceID</t>
   </si>
@@ -3557,6 +3557,21 @@
   </si>
   <si>
     <t>Set Sandy to Inactive in DIM_Site and Survey_Sites tabs</t>
+  </si>
+  <si>
+    <t>Updates to Warnings Reasons and Sub Reasons in DIM_Sub_Coaching_Reason and Coaching_Reason_Selection tabs</t>
+  </si>
+  <si>
+    <t>Quality-Business Process</t>
+  </si>
+  <si>
+    <t>Quality-Critical error</t>
+  </si>
+  <si>
+    <t>Quality-Information Accuracy</t>
+  </si>
+  <si>
+    <t>Quality-Privacy and Disclaimers</t>
   </si>
 </sst>
 </file>
@@ -3978,10 +3993,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L110"/>
+  <dimension ref="A1:L111"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="A110" sqref="A110:E110"/>
+      <selection activeCell="A111" sqref="A111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -5833,20 +5848,37 @@
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A110" s="5">
+      <c r="A110" s="8">
         <v>100</v>
       </c>
-      <c r="B110" s="13">
+      <c r="B110" s="9">
         <v>44698</v>
       </c>
-      <c r="C110" s="5" t="s">
+      <c r="C110" s="8" t="s">
         <v>428</v>
       </c>
-      <c r="D110" s="5">
+      <c r="D110" s="8">
         <v>24631</v>
       </c>
-      <c r="E110" s="13" t="s">
+      <c r="E110" s="9" t="s">
         <v>1156</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A111" s="5">
+        <v>101</v>
+      </c>
+      <c r="B111" s="13">
+        <v>44718</v>
+      </c>
+      <c r="C111" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="D111" s="5">
+        <v>24715</v>
+      </c>
+      <c r="E111" s="5" t="s">
+        <v>1157</v>
       </c>
     </row>
   </sheetData>
@@ -7352,10 +7384,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:P416"/>
+  <dimension ref="A1:P429"/>
   <sheetViews>
-    <sheetView topLeftCell="A381" workbookViewId="0">
-      <selection activeCell="A398" sqref="A398:P416"/>
+    <sheetView topLeftCell="A396" workbookViewId="0">
+      <selection activeCell="A417" sqref="A417:P429"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -28161,6 +28193,656 @@
         <v>1</v>
       </c>
       <c r="P416">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="417" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A417" s="5">
+        <v>28</v>
+      </c>
+      <c r="B417" s="5" t="s">
+        <v>436</v>
+      </c>
+      <c r="C417" s="5">
+        <v>298</v>
+      </c>
+      <c r="D417" s="5" t="s">
+        <v>1158</v>
+      </c>
+      <c r="E417" s="5">
+        <v>1</v>
+      </c>
+      <c r="F417" s="5">
+        <v>1</v>
+      </c>
+      <c r="G417" s="5">
+        <v>0</v>
+      </c>
+      <c r="H417" s="5">
+        <v>1</v>
+      </c>
+      <c r="I417" s="5">
+        <v>0</v>
+      </c>
+      <c r="J417" s="5">
+        <v>1</v>
+      </c>
+      <c r="K417" s="5">
+        <v>0</v>
+      </c>
+      <c r="L417" s="5">
+        <v>0</v>
+      </c>
+      <c r="M417" s="5">
+        <v>1</v>
+      </c>
+      <c r="N417" s="5">
+        <v>1</v>
+      </c>
+      <c r="O417" s="5">
+        <v>0</v>
+      </c>
+      <c r="P417" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="418" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A418" s="5">
+        <v>28</v>
+      </c>
+      <c r="B418" s="5" t="s">
+        <v>436</v>
+      </c>
+      <c r="C418" s="5">
+        <v>300</v>
+      </c>
+      <c r="D418" s="5" t="s">
+        <v>1160</v>
+      </c>
+      <c r="E418" s="5">
+        <v>1</v>
+      </c>
+      <c r="F418" s="5">
+        <v>1</v>
+      </c>
+      <c r="G418" s="5">
+        <v>0</v>
+      </c>
+      <c r="H418" s="5">
+        <v>1</v>
+      </c>
+      <c r="I418" s="5">
+        <v>0</v>
+      </c>
+      <c r="J418" s="5">
+        <v>1</v>
+      </c>
+      <c r="K418" s="5">
+        <v>0</v>
+      </c>
+      <c r="L418" s="5">
+        <v>0</v>
+      </c>
+      <c r="M418" s="5">
+        <v>1</v>
+      </c>
+      <c r="N418" s="5">
+        <v>1</v>
+      </c>
+      <c r="O418" s="5">
+        <v>0</v>
+      </c>
+      <c r="P418" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="419" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A419" s="5">
+        <v>28</v>
+      </c>
+      <c r="B419" s="5" t="s">
+        <v>436</v>
+      </c>
+      <c r="C419" s="5">
+        <v>301</v>
+      </c>
+      <c r="D419" s="5" t="s">
+        <v>1161</v>
+      </c>
+      <c r="E419" s="5">
+        <v>1</v>
+      </c>
+      <c r="F419" s="5">
+        <v>1</v>
+      </c>
+      <c r="G419" s="5">
+        <v>0</v>
+      </c>
+      <c r="H419" s="5">
+        <v>1</v>
+      </c>
+      <c r="I419" s="5">
+        <v>0</v>
+      </c>
+      <c r="J419" s="5">
+        <v>1</v>
+      </c>
+      <c r="K419" s="5">
+        <v>0</v>
+      </c>
+      <c r="L419" s="5">
+        <v>0</v>
+      </c>
+      <c r="M419" s="5">
+        <v>1</v>
+      </c>
+      <c r="N419" s="5">
+        <v>1</v>
+      </c>
+      <c r="O419" s="5">
+        <v>0</v>
+      </c>
+      <c r="P419" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="420" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A420" s="5">
+        <v>29</v>
+      </c>
+      <c r="B420" s="5" t="s">
+        <v>437</v>
+      </c>
+      <c r="C420" s="5">
+        <v>298</v>
+      </c>
+      <c r="D420" s="5" t="s">
+        <v>1158</v>
+      </c>
+      <c r="E420" s="5">
+        <v>1</v>
+      </c>
+      <c r="F420" s="5">
+        <v>1</v>
+      </c>
+      <c r="G420" s="5">
+        <v>0</v>
+      </c>
+      <c r="H420" s="5">
+        <v>1</v>
+      </c>
+      <c r="I420" s="5">
+        <v>0</v>
+      </c>
+      <c r="J420" s="5">
+        <v>1</v>
+      </c>
+      <c r="K420" s="5">
+        <v>0</v>
+      </c>
+      <c r="L420" s="5">
+        <v>0</v>
+      </c>
+      <c r="M420" s="5">
+        <v>1</v>
+      </c>
+      <c r="N420" s="5">
+        <v>1</v>
+      </c>
+      <c r="O420" s="5">
+        <v>0</v>
+      </c>
+      <c r="P420" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="421" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A421" s="5">
+        <v>29</v>
+      </c>
+      <c r="B421" s="5" t="s">
+        <v>437</v>
+      </c>
+      <c r="C421" s="5">
+        <v>299</v>
+      </c>
+      <c r="D421" s="5" t="s">
+        <v>1159</v>
+      </c>
+      <c r="E421" s="5">
+        <v>1</v>
+      </c>
+      <c r="F421" s="5">
+        <v>1</v>
+      </c>
+      <c r="G421" s="5">
+        <v>0</v>
+      </c>
+      <c r="H421" s="5">
+        <v>1</v>
+      </c>
+      <c r="I421" s="5">
+        <v>0</v>
+      </c>
+      <c r="J421" s="5">
+        <v>1</v>
+      </c>
+      <c r="K421" s="5">
+        <v>0</v>
+      </c>
+      <c r="L421" s="5">
+        <v>0</v>
+      </c>
+      <c r="M421" s="5">
+        <v>1</v>
+      </c>
+      <c r="N421" s="5">
+        <v>1</v>
+      </c>
+      <c r="O421" s="5">
+        <v>0</v>
+      </c>
+      <c r="P421" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="422" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A422" s="5">
+        <v>29</v>
+      </c>
+      <c r="B422" s="5" t="s">
+        <v>437</v>
+      </c>
+      <c r="C422" s="5">
+        <v>300</v>
+      </c>
+      <c r="D422" s="5" t="s">
+        <v>1160</v>
+      </c>
+      <c r="E422" s="5">
+        <v>1</v>
+      </c>
+      <c r="F422" s="5">
+        <v>1</v>
+      </c>
+      <c r="G422" s="5">
+        <v>0</v>
+      </c>
+      <c r="H422" s="5">
+        <v>1</v>
+      </c>
+      <c r="I422" s="5">
+        <v>0</v>
+      </c>
+      <c r="J422" s="5">
+        <v>1</v>
+      </c>
+      <c r="K422" s="5">
+        <v>0</v>
+      </c>
+      <c r="L422" s="5">
+        <v>0</v>
+      </c>
+      <c r="M422" s="5">
+        <v>1</v>
+      </c>
+      <c r="N422" s="5">
+        <v>1</v>
+      </c>
+      <c r="O422" s="5">
+        <v>0</v>
+      </c>
+      <c r="P422" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="423" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A423" s="5">
+        <v>29</v>
+      </c>
+      <c r="B423" s="5" t="s">
+        <v>437</v>
+      </c>
+      <c r="C423" s="5">
+        <v>301</v>
+      </c>
+      <c r="D423" s="5" t="s">
+        <v>1161</v>
+      </c>
+      <c r="E423" s="5">
+        <v>1</v>
+      </c>
+      <c r="F423" s="5">
+        <v>1</v>
+      </c>
+      <c r="G423" s="5">
+        <v>0</v>
+      </c>
+      <c r="H423" s="5">
+        <v>1</v>
+      </c>
+      <c r="I423" s="5">
+        <v>0</v>
+      </c>
+      <c r="J423" s="5">
+        <v>1</v>
+      </c>
+      <c r="K423" s="5">
+        <v>0</v>
+      </c>
+      <c r="L423" s="5">
+        <v>0</v>
+      </c>
+      <c r="M423" s="5">
+        <v>1</v>
+      </c>
+      <c r="N423" s="5">
+        <v>1</v>
+      </c>
+      <c r="O423" s="5">
+        <v>0</v>
+      </c>
+      <c r="P423" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="424" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A424" s="5">
+        <v>30</v>
+      </c>
+      <c r="B424" s="5" t="s">
+        <v>438</v>
+      </c>
+      <c r="C424" s="5">
+        <v>298</v>
+      </c>
+      <c r="D424" s="5" t="s">
+        <v>1158</v>
+      </c>
+      <c r="E424" s="5">
+        <v>1</v>
+      </c>
+      <c r="F424" s="5">
+        <v>1</v>
+      </c>
+      <c r="G424" s="5">
+        <v>0</v>
+      </c>
+      <c r="H424" s="5">
+        <v>1</v>
+      </c>
+      <c r="I424" s="5">
+        <v>0</v>
+      </c>
+      <c r="J424" s="5">
+        <v>1</v>
+      </c>
+      <c r="K424" s="5">
+        <v>0</v>
+      </c>
+      <c r="L424" s="5">
+        <v>0</v>
+      </c>
+      <c r="M424" s="5">
+        <v>1</v>
+      </c>
+      <c r="N424" s="5">
+        <v>1</v>
+      </c>
+      <c r="O424" s="5">
+        <v>0</v>
+      </c>
+      <c r="P424" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="425" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A425" s="5">
+        <v>30</v>
+      </c>
+      <c r="B425" s="5" t="s">
+        <v>438</v>
+      </c>
+      <c r="C425" s="5">
+        <v>299</v>
+      </c>
+      <c r="D425" s="5" t="s">
+        <v>1159</v>
+      </c>
+      <c r="E425" s="5">
+        <v>1</v>
+      </c>
+      <c r="F425" s="5">
+        <v>1</v>
+      </c>
+      <c r="G425" s="5">
+        <v>0</v>
+      </c>
+      <c r="H425" s="5">
+        <v>1</v>
+      </c>
+      <c r="I425" s="5">
+        <v>0</v>
+      </c>
+      <c r="J425" s="5">
+        <v>1</v>
+      </c>
+      <c r="K425" s="5">
+        <v>0</v>
+      </c>
+      <c r="L425" s="5">
+        <v>0</v>
+      </c>
+      <c r="M425" s="5">
+        <v>1</v>
+      </c>
+      <c r="N425" s="5">
+        <v>1</v>
+      </c>
+      <c r="O425" s="5">
+        <v>0</v>
+      </c>
+      <c r="P425" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="426" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A426" s="5">
+        <v>30</v>
+      </c>
+      <c r="B426" s="5" t="s">
+        <v>438</v>
+      </c>
+      <c r="C426" s="5">
+        <v>300</v>
+      </c>
+      <c r="D426" s="5" t="s">
+        <v>1160</v>
+      </c>
+      <c r="E426" s="5">
+        <v>1</v>
+      </c>
+      <c r="F426" s="5">
+        <v>1</v>
+      </c>
+      <c r="G426" s="5">
+        <v>0</v>
+      </c>
+      <c r="H426" s="5">
+        <v>1</v>
+      </c>
+      <c r="I426" s="5">
+        <v>0</v>
+      </c>
+      <c r="J426" s="5">
+        <v>1</v>
+      </c>
+      <c r="K426" s="5">
+        <v>0</v>
+      </c>
+      <c r="L426" s="5">
+        <v>0</v>
+      </c>
+      <c r="M426" s="5">
+        <v>1</v>
+      </c>
+      <c r="N426" s="5">
+        <v>1</v>
+      </c>
+      <c r="O426" s="5">
+        <v>0</v>
+      </c>
+      <c r="P426" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="427" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A427" s="5">
+        <v>30</v>
+      </c>
+      <c r="B427" s="5" t="s">
+        <v>438</v>
+      </c>
+      <c r="C427" s="5">
+        <v>301</v>
+      </c>
+      <c r="D427" s="5" t="s">
+        <v>1161</v>
+      </c>
+      <c r="E427" s="5">
+        <v>1</v>
+      </c>
+      <c r="F427" s="5">
+        <v>1</v>
+      </c>
+      <c r="G427" s="5">
+        <v>0</v>
+      </c>
+      <c r="H427" s="5">
+        <v>1</v>
+      </c>
+      <c r="I427" s="5">
+        <v>0</v>
+      </c>
+      <c r="J427" s="5">
+        <v>1</v>
+      </c>
+      <c r="K427" s="5">
+        <v>0</v>
+      </c>
+      <c r="L427" s="5">
+        <v>0</v>
+      </c>
+      <c r="M427" s="5">
+        <v>1</v>
+      </c>
+      <c r="N427" s="5">
+        <v>1</v>
+      </c>
+      <c r="O427" s="5">
+        <v>0</v>
+      </c>
+      <c r="P427" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="428" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A428" s="5">
+        <v>60</v>
+      </c>
+      <c r="B428" s="5" t="s">
+        <v>1060</v>
+      </c>
+      <c r="C428" s="5">
+        <v>298</v>
+      </c>
+      <c r="D428" s="5" t="s">
+        <v>1158</v>
+      </c>
+      <c r="E428" s="5">
+        <v>1</v>
+      </c>
+      <c r="F428" s="5">
+        <v>1</v>
+      </c>
+      <c r="G428" s="5">
+        <v>0</v>
+      </c>
+      <c r="H428" s="5">
+        <v>1</v>
+      </c>
+      <c r="I428" s="5">
+        <v>0</v>
+      </c>
+      <c r="J428" s="5">
+        <v>1</v>
+      </c>
+      <c r="K428" s="5">
+        <v>0</v>
+      </c>
+      <c r="L428" s="5">
+        <v>0</v>
+      </c>
+      <c r="M428" s="5">
+        <v>1</v>
+      </c>
+      <c r="N428" s="5">
+        <v>1</v>
+      </c>
+      <c r="O428" s="5">
+        <v>0</v>
+      </c>
+      <c r="P428" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="429" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A429" s="5">
+        <v>60</v>
+      </c>
+      <c r="B429" s="5" t="s">
+        <v>1060</v>
+      </c>
+      <c r="C429" s="5">
+        <v>300</v>
+      </c>
+      <c r="D429" s="5" t="s">
+        <v>1160</v>
+      </c>
+      <c r="E429" s="5">
+        <v>1</v>
+      </c>
+      <c r="F429" s="5">
+        <v>1</v>
+      </c>
+      <c r="G429" s="5">
+        <v>0</v>
+      </c>
+      <c r="H429" s="5">
+        <v>1</v>
+      </c>
+      <c r="I429" s="5">
+        <v>0</v>
+      </c>
+      <c r="J429" s="5">
+        <v>1</v>
+      </c>
+      <c r="K429" s="5">
+        <v>0</v>
+      </c>
+      <c r="L429" s="5">
+        <v>0</v>
+      </c>
+      <c r="M429" s="5">
+        <v>1</v>
+      </c>
+      <c r="N429" s="5">
+        <v>1</v>
+      </c>
+      <c r="O429" s="5">
+        <v>0</v>
+      </c>
+      <c r="P429" s="5">
         <v>0</v>
       </c>
     </row>
@@ -39917,19 +40599,19 @@
       </c>
     </row>
     <row r="18" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="5">
+      <c r="A18" s="8">
         <v>16</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="C18" s="5">
-        <v>0</v>
-      </c>
-      <c r="D18" s="5">
-        <v>0</v>
-      </c>
-      <c r="E18" s="5">
+      <c r="C18" s="8">
+        <v>0</v>
+      </c>
+      <c r="D18" s="8">
+        <v>0</v>
+      </c>
+      <c r="E18" s="8">
         <v>0</v>
       </c>
     </row>
@@ -42946,19 +43628,19 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="5">
+      <c r="A18" s="8">
         <v>16</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18" s="8">
         <v>0</v>
       </c>
     </row>
@@ -43631,10 +44313,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:B299"/>
+  <dimension ref="A1:B303"/>
   <sheetViews>
     <sheetView topLeftCell="A271" workbookViewId="0">
-      <selection activeCell="B283" sqref="B282:B283"/>
+      <selection activeCell="A300" sqref="A300:B303"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -46033,6 +46715,38 @@
       </c>
       <c r="B299" t="s">
         <v>1154</v>
+      </c>
+    </row>
+    <row r="300" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A300" s="5">
+        <v>298</v>
+      </c>
+      <c r="B300" s="5" t="s">
+        <v>1158</v>
+      </c>
+    </row>
+    <row r="301" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A301" s="5">
+        <v>299</v>
+      </c>
+      <c r="B301" s="5" t="s">
+        <v>1159</v>
+      </c>
+    </row>
+    <row r="302" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A302" s="5">
+        <v>300</v>
+      </c>
+      <c r="B302" s="5" t="s">
+        <v>1160</v>
+      </c>
+    </row>
+    <row r="303" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A303" s="5">
+        <v>301</v>
+      </c>
+      <c r="B303" s="5" t="s">
+        <v>1161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TFS 24711 - Update site to include Netpark and remove Coralville
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C51602
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TFS\eCoaching_V2\Design\DD\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F92C8171-FD67-4D72-B7F7-90DA7BE6C1E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A768D5C-557C-4EB6-A79B-039B02B22FBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57504" yWindow="1932" windowWidth="28992" windowHeight="15792" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4178" uniqueCount="1162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4183" uniqueCount="1165">
   <si>
     <t>SourceID</t>
   </si>
@@ -3168,12 +3168,6 @@
   </si>
   <si>
     <t>Integrate Brownsville into eCL.</t>
-  </si>
-  <si>
-    <t>Tampa</t>
-  </si>
-  <si>
-    <t>FL - Tampa</t>
   </si>
   <si>
     <t>BingoType</t>
@@ -3572,6 +3566,21 @@
   </si>
   <si>
     <t>Quality-Privacy and Disclaimers</t>
+  </si>
+  <si>
+    <t>Tampa Riverview</t>
+  </si>
+  <si>
+    <t>Tampa Netpark</t>
+  </si>
+  <si>
+    <t>FL - Tampa Riverview</t>
+  </si>
+  <si>
+    <t>FL - Tampa Netpark</t>
+  </si>
+  <si>
+    <t>Update site to include Netpark and remove Coralville. Changes in DIM_Site tab.</t>
   </si>
 </sst>
 </file>
@@ -3993,10 +4002,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L111"/>
+  <dimension ref="A1:L112"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="A111" sqref="A111"/>
+      <selection activeCell="E112" sqref="E112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -5538,7 +5547,7 @@
         <v>15465</v>
       </c>
       <c r="E91" t="s">
-        <v>1055</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="92" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -5555,7 +5564,7 @@
         <v>15465</v>
       </c>
       <c r="E92" t="s">
-        <v>1056</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -5572,7 +5581,7 @@
         <v>15859</v>
       </c>
       <c r="E93" s="8" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -5589,7 +5598,7 @@
         <v>15989</v>
       </c>
       <c r="E94" s="6" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="95" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -5606,7 +5615,7 @@
         <v>15803</v>
       </c>
       <c r="E95" s="10" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="96" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -5623,7 +5632,7 @@
         <v>15803</v>
       </c>
       <c r="E96" s="10" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="97" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -5640,7 +5649,7 @@
         <v>16261</v>
       </c>
       <c r="E97" s="10" t="s">
-        <v>1079</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="98" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -5657,7 +5666,7 @@
         <v>16389</v>
       </c>
       <c r="E98" s="10" t="s">
-        <v>1082</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="99" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -5674,7 +5683,7 @@
         <v>17066</v>
       </c>
       <c r="E99" s="10" t="s">
-        <v>1096</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="100" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -5691,7 +5700,7 @@
         <v>17263</v>
       </c>
       <c r="E100" s="10" t="s">
-        <v>1097</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -5708,7 +5717,7 @@
         <v>18255</v>
       </c>
       <c r="E101" s="10" t="s">
-        <v>1103</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="102" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -5725,7 +5734,7 @@
         <v>18154</v>
       </c>
       <c r="E102" s="10" t="s">
-        <v>1105</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -5742,7 +5751,7 @@
         <v>19502</v>
       </c>
       <c r="E103" s="10" t="s">
-        <v>1109</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="104" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -5759,7 +5768,7 @@
         <v>19937</v>
       </c>
       <c r="E104" s="10" t="s">
-        <v>1111</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="105" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -5776,7 +5785,7 @@
         <v>20256</v>
       </c>
       <c r="E105" s="10" t="s">
-        <v>1113</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="106" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -5793,7 +5802,7 @@
         <v>21493</v>
       </c>
       <c r="E106" s="10" t="s">
-        <v>1119</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -5810,7 +5819,7 @@
         <v>22187</v>
       </c>
       <c r="E107" s="10" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -5827,7 +5836,7 @@
         <v>23051</v>
       </c>
       <c r="E108" s="10" t="s">
-        <v>1133</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -5844,7 +5853,7 @@
         <v>24083</v>
       </c>
       <c r="E109" s="10" t="s">
-        <v>1155</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -5861,24 +5870,41 @@
         <v>24631</v>
       </c>
       <c r="E110" s="9" t="s">
-        <v>1156</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A111" s="5">
+        <v>1154</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A111" s="8">
         <v>101</v>
       </c>
-      <c r="B111" s="13">
+      <c r="B111" s="9">
         <v>44718</v>
       </c>
-      <c r="C111" s="5" t="s">
+      <c r="C111" s="8" t="s">
         <v>428</v>
       </c>
-      <c r="D111" s="5">
+      <c r="D111" s="8">
         <v>24715</v>
       </c>
-      <c r="E111" s="5" t="s">
-        <v>1157</v>
+      <c r="E111" s="8" t="s">
+        <v>1155</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A112" s="5">
+        <v>102</v>
+      </c>
+      <c r="B112" s="13">
+        <v>44719</v>
+      </c>
+      <c r="C112" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="D112" s="5">
+        <v>24711</v>
+      </c>
+      <c r="E112" s="5" t="s">
+        <v>1164</v>
       </c>
     </row>
   </sheetData>
@@ -7256,7 +7282,7 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="8" t="s">
-        <v>1081</v>
+        <v>1079</v>
       </c>
       <c r="B60" s="8" t="s">
         <v>961</v>
@@ -8557,7 +8583,7 @@
         <v>291</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="E24" s="5">
         <v>1</v>
@@ -8607,7 +8633,7 @@
         <v>293</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>1150</v>
+        <v>1148</v>
       </c>
       <c r="E25" s="5">
         <v>1</v>
@@ -8657,7 +8683,7 @@
         <v>295</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>1152</v>
+        <v>1150</v>
       </c>
       <c r="E26" s="5">
         <v>1</v>
@@ -10207,7 +10233,7 @@
         <v>292</v>
       </c>
       <c r="D57" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="E57">
         <v>1</v>
@@ -13407,7 +13433,7 @@
         <v>284</v>
       </c>
       <c r="D121" t="s">
-        <v>1141</v>
+        <v>1139</v>
       </c>
       <c r="E121">
         <v>1</v>
@@ -16907,7 +16933,7 @@
         <v>253</v>
       </c>
       <c r="D191" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
       <c r="E191">
         <v>1</v>
@@ -16957,7 +16983,7 @@
         <v>254</v>
       </c>
       <c r="D192" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
       <c r="E192">
         <v>1</v>
@@ -17007,7 +17033,7 @@
         <v>255</v>
       </c>
       <c r="D193" t="s">
-        <v>1063</v>
+        <v>1061</v>
       </c>
       <c r="E193">
         <v>1</v>
@@ -17057,7 +17083,7 @@
         <v>256</v>
       </c>
       <c r="D194" t="s">
-        <v>1064</v>
+        <v>1062</v>
       </c>
       <c r="E194">
         <v>1</v>
@@ -17107,7 +17133,7 @@
         <v>257</v>
       </c>
       <c r="D195" t="s">
-        <v>1065</v>
+        <v>1063</v>
       </c>
       <c r="E195">
         <v>1</v>
@@ -17157,7 +17183,7 @@
         <v>258</v>
       </c>
       <c r="D196" t="s">
-        <v>1066</v>
+        <v>1064</v>
       </c>
       <c r="E196">
         <v>1</v>
@@ -17207,7 +17233,7 @@
         <v>259</v>
       </c>
       <c r="D197" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
       <c r="E197">
         <v>1</v>
@@ -17257,7 +17283,7 @@
         <v>260</v>
       </c>
       <c r="D198" t="s">
-        <v>1068</v>
+        <v>1066</v>
       </c>
       <c r="E198">
         <v>1</v>
@@ -17307,7 +17333,7 @@
         <v>261</v>
       </c>
       <c r="D199" t="s">
-        <v>1069</v>
+        <v>1067</v>
       </c>
       <c r="E199">
         <v>1</v>
@@ -17357,7 +17383,7 @@
         <v>262</v>
       </c>
       <c r="D200" t="s">
-        <v>1070</v>
+        <v>1068</v>
       </c>
       <c r="E200">
         <v>1</v>
@@ -17407,7 +17433,7 @@
         <v>263</v>
       </c>
       <c r="D201" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
       <c r="E201">
         <v>1</v>
@@ -17507,7 +17533,7 @@
         <v>265</v>
       </c>
       <c r="D203" t="s">
-        <v>1072</v>
+        <v>1070</v>
       </c>
       <c r="E203">
         <v>1</v>
@@ -18557,7 +18583,7 @@
         <v>253</v>
       </c>
       <c r="D224" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
       <c r="E224">
         <v>1</v>
@@ -18607,7 +18633,7 @@
         <v>254</v>
       </c>
       <c r="D225" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
       <c r="E225">
         <v>1</v>
@@ -18657,7 +18683,7 @@
         <v>255</v>
       </c>
       <c r="D226" t="s">
-        <v>1063</v>
+        <v>1061</v>
       </c>
       <c r="E226">
         <v>1</v>
@@ -18707,7 +18733,7 @@
         <v>256</v>
       </c>
       <c r="D227" t="s">
-        <v>1064</v>
+        <v>1062</v>
       </c>
       <c r="E227">
         <v>1</v>
@@ -18757,7 +18783,7 @@
         <v>257</v>
       </c>
       <c r="D228" t="s">
-        <v>1065</v>
+        <v>1063</v>
       </c>
       <c r="E228">
         <v>1</v>
@@ -18807,7 +18833,7 @@
         <v>258</v>
       </c>
       <c r="D229" t="s">
-        <v>1066</v>
+        <v>1064</v>
       </c>
       <c r="E229">
         <v>1</v>
@@ -18857,7 +18883,7 @@
         <v>259</v>
       </c>
       <c r="D230" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
       <c r="E230">
         <v>1</v>
@@ -18907,7 +18933,7 @@
         <v>260</v>
       </c>
       <c r="D231" t="s">
-        <v>1068</v>
+        <v>1066</v>
       </c>
       <c r="E231">
         <v>1</v>
@@ -18957,7 +18983,7 @@
         <v>261</v>
       </c>
       <c r="D232" t="s">
-        <v>1069</v>
+        <v>1067</v>
       </c>
       <c r="E232">
         <v>1</v>
@@ -19007,7 +19033,7 @@
         <v>262</v>
       </c>
       <c r="D233" t="s">
-        <v>1070</v>
+        <v>1068</v>
       </c>
       <c r="E233">
         <v>1</v>
@@ -19057,7 +19083,7 @@
         <v>263</v>
       </c>
       <c r="D234" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
       <c r="E234">
         <v>1</v>
@@ -19157,7 +19183,7 @@
         <v>265</v>
       </c>
       <c r="D236" t="s">
-        <v>1072</v>
+        <v>1070</v>
       </c>
       <c r="E236">
         <v>1</v>
@@ -19307,7 +19333,7 @@
         <v>253</v>
       </c>
       <c r="D239" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
       <c r="E239">
         <v>1</v>
@@ -19357,7 +19383,7 @@
         <v>254</v>
       </c>
       <c r="D240" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
       <c r="E240">
         <v>1</v>
@@ -19407,7 +19433,7 @@
         <v>255</v>
       </c>
       <c r="D241" t="s">
-        <v>1063</v>
+        <v>1061</v>
       </c>
       <c r="E241">
         <v>1</v>
@@ -19457,7 +19483,7 @@
         <v>256</v>
       </c>
       <c r="D242" t="s">
-        <v>1064</v>
+        <v>1062</v>
       </c>
       <c r="E242">
         <v>1</v>
@@ -19507,7 +19533,7 @@
         <v>257</v>
       </c>
       <c r="D243" t="s">
-        <v>1065</v>
+        <v>1063</v>
       </c>
       <c r="E243">
         <v>1</v>
@@ -19557,7 +19583,7 @@
         <v>258</v>
       </c>
       <c r="D244" t="s">
-        <v>1066</v>
+        <v>1064</v>
       </c>
       <c r="E244">
         <v>1</v>
@@ -19607,7 +19633,7 @@
         <v>259</v>
       </c>
       <c r="D245" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
       <c r="E245">
         <v>1</v>
@@ -19657,7 +19683,7 @@
         <v>260</v>
       </c>
       <c r="D246" t="s">
-        <v>1068</v>
+        <v>1066</v>
       </c>
       <c r="E246">
         <v>1</v>
@@ -19707,7 +19733,7 @@
         <v>261</v>
       </c>
       <c r="D247" t="s">
-        <v>1069</v>
+        <v>1067</v>
       </c>
       <c r="E247">
         <v>1</v>
@@ -19757,7 +19783,7 @@
         <v>262</v>
       </c>
       <c r="D248" t="s">
-        <v>1070</v>
+        <v>1068</v>
       </c>
       <c r="E248">
         <v>1</v>
@@ -19807,7 +19833,7 @@
         <v>263</v>
       </c>
       <c r="D249" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
       <c r="E249">
         <v>1</v>
@@ -19907,7 +19933,7 @@
         <v>265</v>
       </c>
       <c r="D251" t="s">
-        <v>1072</v>
+        <v>1070</v>
       </c>
       <c r="E251">
         <v>1</v>
@@ -25601,7 +25627,7 @@
         <v>60</v>
       </c>
       <c r="B365" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
       <c r="C365">
         <v>95</v>
@@ -25651,7 +25677,7 @@
         <v>60</v>
       </c>
       <c r="B366" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
       <c r="C366">
         <v>155</v>
@@ -25701,7 +25727,7 @@
         <v>60</v>
       </c>
       <c r="B367" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
       <c r="C367">
         <v>178</v>
@@ -25751,13 +25777,13 @@
         <v>60</v>
       </c>
       <c r="B368" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
       <c r="C368">
         <v>253</v>
       </c>
       <c r="D368" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
       <c r="E368">
         <v>1</v>
@@ -25801,13 +25827,13 @@
         <v>60</v>
       </c>
       <c r="B369" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
       <c r="C369">
         <v>254</v>
       </c>
       <c r="D369" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
       <c r="E369">
         <v>1</v>
@@ -25851,13 +25877,13 @@
         <v>60</v>
       </c>
       <c r="B370" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
       <c r="C370">
         <v>255</v>
       </c>
       <c r="D370" t="s">
-        <v>1063</v>
+        <v>1061</v>
       </c>
       <c r="E370">
         <v>1</v>
@@ -25901,13 +25927,13 @@
         <v>60</v>
       </c>
       <c r="B371" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
       <c r="C371">
         <v>256</v>
       </c>
       <c r="D371" t="s">
-        <v>1064</v>
+        <v>1062</v>
       </c>
       <c r="E371">
         <v>1</v>
@@ -25951,13 +25977,13 @@
         <v>60</v>
       </c>
       <c r="B372" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
       <c r="C372">
         <v>257</v>
       </c>
       <c r="D372" t="s">
-        <v>1065</v>
+        <v>1063</v>
       </c>
       <c r="E372">
         <v>1</v>
@@ -26001,13 +26027,13 @@
         <v>60</v>
       </c>
       <c r="B373" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
       <c r="C373">
         <v>258</v>
       </c>
       <c r="D373" t="s">
-        <v>1066</v>
+        <v>1064</v>
       </c>
       <c r="E373">
         <v>1</v>
@@ -26051,13 +26077,13 @@
         <v>60</v>
       </c>
       <c r="B374" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
       <c r="C374">
         <v>259</v>
       </c>
       <c r="D374" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
       <c r="E374">
         <v>1</v>
@@ -26101,13 +26127,13 @@
         <v>60</v>
       </c>
       <c r="B375" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
       <c r="C375">
         <v>260</v>
       </c>
       <c r="D375" t="s">
-        <v>1068</v>
+        <v>1066</v>
       </c>
       <c r="E375">
         <v>1</v>
@@ -26151,13 +26177,13 @@
         <v>60</v>
       </c>
       <c r="B376" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
       <c r="C376">
         <v>261</v>
       </c>
       <c r="D376" t="s">
-        <v>1069</v>
+        <v>1067</v>
       </c>
       <c r="E376">
         <v>1</v>
@@ -26201,13 +26227,13 @@
         <v>60</v>
       </c>
       <c r="B377" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
       <c r="C377">
         <v>262</v>
       </c>
       <c r="D377" t="s">
-        <v>1070</v>
+        <v>1068</v>
       </c>
       <c r="E377">
         <v>1</v>
@@ -26251,13 +26277,13 @@
         <v>60</v>
       </c>
       <c r="B378" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
       <c r="C378">
         <v>263</v>
       </c>
       <c r="D378" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
       <c r="E378">
         <v>1</v>
@@ -26301,7 +26327,7 @@
         <v>60</v>
       </c>
       <c r="B379" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
       <c r="C379">
         <v>264</v>
@@ -26351,13 +26377,13 @@
         <v>60</v>
       </c>
       <c r="B380" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
       <c r="C380">
         <v>265</v>
       </c>
       <c r="D380" t="s">
-        <v>1072</v>
+        <v>1070</v>
       </c>
       <c r="E380">
         <v>1</v>
@@ -26401,13 +26427,13 @@
         <v>61</v>
       </c>
       <c r="B381" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="C381">
         <v>266</v>
       </c>
       <c r="D381" t="s">
-        <v>1085</v>
+        <v>1083</v>
       </c>
       <c r="E381">
         <v>1</v>
@@ -26451,13 +26477,13 @@
         <v>61</v>
       </c>
       <c r="B382" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="C382">
         <v>267</v>
       </c>
       <c r="D382" t="s">
-        <v>1086</v>
+        <v>1084</v>
       </c>
       <c r="E382">
         <v>1</v>
@@ -26501,13 +26527,13 @@
         <v>61</v>
       </c>
       <c r="B383" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="C383">
         <v>268</v>
       </c>
       <c r="D383" t="s">
-        <v>1087</v>
+        <v>1085</v>
       </c>
       <c r="E383">
         <v>1</v>
@@ -26551,13 +26577,13 @@
         <v>61</v>
       </c>
       <c r="B384" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="C384">
         <v>269</v>
       </c>
       <c r="D384" t="s">
-        <v>1088</v>
+        <v>1086</v>
       </c>
       <c r="E384">
         <v>1</v>
@@ -26601,13 +26627,13 @@
         <v>61</v>
       </c>
       <c r="B385" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="C385">
         <v>270</v>
       </c>
       <c r="D385" t="s">
-        <v>1089</v>
+        <v>1087</v>
       </c>
       <c r="E385">
         <v>1</v>
@@ -26651,13 +26677,13 @@
         <v>61</v>
       </c>
       <c r="B386" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="C386">
         <v>271</v>
       </c>
       <c r="D386" t="s">
-        <v>1090</v>
+        <v>1088</v>
       </c>
       <c r="E386">
         <v>1</v>
@@ -26701,13 +26727,13 @@
         <v>61</v>
       </c>
       <c r="B387" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="C387">
         <v>272</v>
       </c>
       <c r="D387" t="s">
-        <v>1091</v>
+        <v>1089</v>
       </c>
       <c r="E387">
         <v>1</v>
@@ -26751,13 +26777,13 @@
         <v>61</v>
       </c>
       <c r="B388" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="C388">
         <v>273</v>
       </c>
       <c r="D388" t="s">
-        <v>1092</v>
+        <v>1090</v>
       </c>
       <c r="E388">
         <v>1</v>
@@ -26801,13 +26827,13 @@
         <v>61</v>
       </c>
       <c r="B389" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="C389">
         <v>274</v>
       </c>
       <c r="D389" t="s">
-        <v>1093</v>
+        <v>1091</v>
       </c>
       <c r="E389">
         <v>1</v>
@@ -26851,13 +26877,13 @@
         <v>61</v>
       </c>
       <c r="B390" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="C390">
         <v>275</v>
       </c>
       <c r="D390" t="s">
-        <v>1094</v>
+        <v>1092</v>
       </c>
       <c r="E390">
         <v>1</v>
@@ -26901,13 +26927,13 @@
         <v>61</v>
       </c>
       <c r="B391" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="C391">
         <v>276</v>
       </c>
       <c r="D391" t="s">
-        <v>1095</v>
+        <v>1093</v>
       </c>
       <c r="E391">
         <v>1</v>
@@ -26951,7 +26977,7 @@
         <v>62</v>
       </c>
       <c r="B392" t="s">
-        <v>1098</v>
+        <v>1096</v>
       </c>
       <c r="C392">
         <v>42</v>
@@ -27001,13 +27027,13 @@
         <v>63</v>
       </c>
       <c r="B393" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="C393">
         <v>277</v>
       </c>
       <c r="D393" t="s">
-        <v>1099</v>
+        <v>1097</v>
       </c>
       <c r="E393">
         <v>1</v>
@@ -27051,13 +27077,13 @@
         <v>63</v>
       </c>
       <c r="B394" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="C394">
         <v>278</v>
       </c>
       <c r="D394" t="s">
-        <v>1100</v>
+        <v>1098</v>
       </c>
       <c r="E394">
         <v>1</v>
@@ -27101,13 +27127,13 @@
         <v>63</v>
       </c>
       <c r="B395" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="C395">
         <v>279</v>
       </c>
       <c r="D395" t="s">
-        <v>1101</v>
+        <v>1099</v>
       </c>
       <c r="E395">
         <v>1</v>
@@ -27151,13 +27177,13 @@
         <v>63</v>
       </c>
       <c r="B396" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="C396">
         <v>280</v>
       </c>
       <c r="D396" t="s">
-        <v>1102</v>
+        <v>1100</v>
       </c>
       <c r="E396">
         <v>1</v>
@@ -27201,7 +27227,7 @@
         <v>64</v>
       </c>
       <c r="B397" t="s">
-        <v>1132</v>
+        <v>1130</v>
       </c>
       <c r="C397">
         <v>42</v>
@@ -27251,7 +27277,7 @@
         <v>65</v>
       </c>
       <c r="B398" t="s">
-        <v>1134</v>
+        <v>1132</v>
       </c>
       <c r="C398">
         <v>42</v>
@@ -27301,13 +27327,13 @@
         <v>66</v>
       </c>
       <c r="B399" t="s">
-        <v>1135</v>
+        <v>1133</v>
       </c>
       <c r="C399">
         <v>296</v>
       </c>
       <c r="D399" t="s">
-        <v>1153</v>
+        <v>1151</v>
       </c>
       <c r="E399">
         <v>1</v>
@@ -27351,13 +27377,13 @@
         <v>66</v>
       </c>
       <c r="B400" t="s">
-        <v>1135</v>
+        <v>1133</v>
       </c>
       <c r="C400">
         <v>297</v>
       </c>
       <c r="D400" t="s">
-        <v>1154</v>
+        <v>1152</v>
       </c>
       <c r="E400">
         <v>1</v>
@@ -27401,7 +27427,7 @@
         <v>66</v>
       </c>
       <c r="B401" t="s">
-        <v>1135</v>
+        <v>1133</v>
       </c>
       <c r="C401">
         <v>42</v>
@@ -27451,13 +27477,13 @@
         <v>66</v>
       </c>
       <c r="B402" t="s">
-        <v>1135</v>
+        <v>1133</v>
       </c>
       <c r="C402">
         <v>286</v>
       </c>
       <c r="D402" t="s">
-        <v>1143</v>
+        <v>1141</v>
       </c>
       <c r="E402">
         <v>1</v>
@@ -27501,13 +27527,13 @@
         <v>66</v>
       </c>
       <c r="B403" t="s">
-        <v>1135</v>
+        <v>1133</v>
       </c>
       <c r="C403">
         <v>288</v>
       </c>
       <c r="D403" t="s">
-        <v>1145</v>
+        <v>1143</v>
       </c>
       <c r="E403">
         <v>1</v>
@@ -27551,13 +27577,13 @@
         <v>66</v>
       </c>
       <c r="B404" t="s">
-        <v>1135</v>
+        <v>1133</v>
       </c>
       <c r="C404">
         <v>294</v>
       </c>
       <c r="D404" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="E404">
         <v>1</v>
@@ -27601,13 +27627,13 @@
         <v>66</v>
       </c>
       <c r="B405" t="s">
-        <v>1135</v>
+        <v>1133</v>
       </c>
       <c r="C405">
         <v>285</v>
       </c>
       <c r="D405" t="s">
-        <v>1142</v>
+        <v>1140</v>
       </c>
       <c r="E405">
         <v>1</v>
@@ -27651,7 +27677,7 @@
         <v>67</v>
       </c>
       <c r="B406" t="s">
-        <v>1136</v>
+        <v>1134</v>
       </c>
       <c r="C406">
         <v>113</v>
@@ -27701,13 +27727,13 @@
         <v>67</v>
       </c>
       <c r="B407" t="s">
-        <v>1136</v>
+        <v>1134</v>
       </c>
       <c r="C407">
         <v>287</v>
       </c>
       <c r="D407" t="s">
-        <v>1144</v>
+        <v>1142</v>
       </c>
       <c r="E407">
         <v>1</v>
@@ -27751,13 +27777,13 @@
         <v>67</v>
       </c>
       <c r="B408" t="s">
-        <v>1136</v>
+        <v>1134</v>
       </c>
       <c r="C408">
         <v>290</v>
       </c>
       <c r="D408" t="s">
-        <v>1147</v>
+        <v>1145</v>
       </c>
       <c r="E408">
         <v>1</v>
@@ -27801,7 +27827,7 @@
         <v>67</v>
       </c>
       <c r="B409" t="s">
-        <v>1136</v>
+        <v>1134</v>
       </c>
       <c r="C409">
         <v>42</v>
@@ -27857,7 +27883,7 @@
         <v>289</v>
       </c>
       <c r="D410" t="s">
-        <v>1146</v>
+        <v>1144</v>
       </c>
       <c r="E410">
         <v>1</v>
@@ -27907,7 +27933,7 @@
         <v>283</v>
       </c>
       <c r="D411" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
       <c r="E411">
         <v>1</v>
@@ -28001,7 +28027,7 @@
         <v>69</v>
       </c>
       <c r="B413" t="s">
-        <v>1137</v>
+        <v>1135</v>
       </c>
       <c r="C413">
         <v>42</v>
@@ -28051,7 +28077,7 @@
         <v>70</v>
       </c>
       <c r="B414" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
       <c r="C414">
         <v>42</v>
@@ -28151,7 +28177,7 @@
         <v>72</v>
       </c>
       <c r="B416" t="s">
-        <v>1139</v>
+        <v>1137</v>
       </c>
       <c r="C416">
         <v>42</v>
@@ -28207,7 +28233,7 @@
         <v>298</v>
       </c>
       <c r="D417" s="5" t="s">
-        <v>1158</v>
+        <v>1156</v>
       </c>
       <c r="E417" s="5">
         <v>1</v>
@@ -28257,7 +28283,7 @@
         <v>300</v>
       </c>
       <c r="D418" s="5" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="E418" s="5">
         <v>1</v>
@@ -28307,7 +28333,7 @@
         <v>301</v>
       </c>
       <c r="D419" s="5" t="s">
-        <v>1161</v>
+        <v>1159</v>
       </c>
       <c r="E419" s="5">
         <v>1</v>
@@ -28357,7 +28383,7 @@
         <v>298</v>
       </c>
       <c r="D420" s="5" t="s">
-        <v>1158</v>
+        <v>1156</v>
       </c>
       <c r="E420" s="5">
         <v>1</v>
@@ -28407,7 +28433,7 @@
         <v>299</v>
       </c>
       <c r="D421" s="5" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="E421" s="5">
         <v>1</v>
@@ -28457,7 +28483,7 @@
         <v>300</v>
       </c>
       <c r="D422" s="5" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="E422" s="5">
         <v>1</v>
@@ -28507,7 +28533,7 @@
         <v>301</v>
       </c>
       <c r="D423" s="5" t="s">
-        <v>1161</v>
+        <v>1159</v>
       </c>
       <c r="E423" s="5">
         <v>1</v>
@@ -28557,7 +28583,7 @@
         <v>298</v>
       </c>
       <c r="D424" s="5" t="s">
-        <v>1158</v>
+        <v>1156</v>
       </c>
       <c r="E424" s="5">
         <v>1</v>
@@ -28607,7 +28633,7 @@
         <v>299</v>
       </c>
       <c r="D425" s="5" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="E425" s="5">
         <v>1</v>
@@ -28657,7 +28683,7 @@
         <v>300</v>
       </c>
       <c r="D426" s="5" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="E426" s="5">
         <v>1</v>
@@ -28707,7 +28733,7 @@
         <v>301</v>
       </c>
       <c r="D427" s="5" t="s">
-        <v>1161</v>
+        <v>1159</v>
       </c>
       <c r="E427" s="5">
         <v>1</v>
@@ -28751,13 +28777,13 @@
         <v>60</v>
       </c>
       <c r="B428" s="5" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
       <c r="C428" s="5">
         <v>298</v>
       </c>
       <c r="D428" s="5" t="s">
-        <v>1158</v>
+        <v>1156</v>
       </c>
       <c r="E428" s="5">
         <v>1</v>
@@ -28801,13 +28827,13 @@
         <v>60</v>
       </c>
       <c r="B429" s="5" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
       <c r="C429" s="5">
         <v>300</v>
       </c>
       <c r="D429" s="5" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="E429" s="5">
         <v>1</v>
@@ -34977,7 +35003,7 @@
         <v>380</v>
       </c>
       <c r="I171" s="8" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="J171" s="8">
         <v>0</v>
@@ -35012,7 +35038,7 @@
         <v>380</v>
       </c>
       <c r="I172" s="8" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="J172" s="8">
         <v>0</v>
@@ -35047,7 +35073,7 @@
         <v>380</v>
       </c>
       <c r="I173" s="8" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="J173" s="8">
         <v>0</v>
@@ -35082,7 +35108,7 @@
         <v>380</v>
       </c>
       <c r="I174" s="8" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="J174" s="8">
         <v>0</v>
@@ -35117,7 +35143,7 @@
         <v>380</v>
       </c>
       <c r="I175" s="8" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="J175" s="8">
         <v>0</v>
@@ -35137,7 +35163,7 @@
         <v>3</v>
       </c>
       <c r="D176" s="8" t="s">
-        <v>1106</v>
+        <v>1104</v>
       </c>
       <c r="E176" s="8">
         <v>0</v>
@@ -35152,7 +35178,7 @@
         <v>380</v>
       </c>
       <c r="I176" s="8" t="s">
-        <v>1108</v>
+        <v>1106</v>
       </c>
       <c r="J176" s="8">
         <v>0</v>
@@ -35172,7 +35198,7 @@
         <v>3</v>
       </c>
       <c r="D177" s="8" t="s">
-        <v>1106</v>
+        <v>1104</v>
       </c>
       <c r="E177" s="8">
         <v>0</v>
@@ -35187,7 +35213,7 @@
         <v>380</v>
       </c>
       <c r="I177" s="8" t="s">
-        <v>1108</v>
+        <v>1106</v>
       </c>
       <c r="J177" s="8">
         <v>0</v>
@@ -35207,7 +35233,7 @@
         <v>3</v>
       </c>
       <c r="D178" s="8" t="s">
-        <v>1106</v>
+        <v>1104</v>
       </c>
       <c r="E178" s="8">
         <v>0</v>
@@ -35222,7 +35248,7 @@
         <v>380</v>
       </c>
       <c r="I178" s="8" t="s">
-        <v>1108</v>
+        <v>1106</v>
       </c>
       <c r="J178" s="8">
         <v>0</v>
@@ -35242,7 +35268,7 @@
         <v>3</v>
       </c>
       <c r="D179" s="8" t="s">
-        <v>1106</v>
+        <v>1104</v>
       </c>
       <c r="E179" s="8">
         <v>0</v>
@@ -35257,7 +35283,7 @@
         <v>380</v>
       </c>
       <c r="I179" s="8" t="s">
-        <v>1108</v>
+        <v>1106</v>
       </c>
       <c r="J179" s="8">
         <v>0</v>
@@ -35292,7 +35318,7 @@
         <v>380</v>
       </c>
       <c r="I180" s="8" t="s">
-        <v>1108</v>
+        <v>1106</v>
       </c>
       <c r="J180" s="8">
         <v>0</v>
@@ -35327,7 +35353,7 @@
         <v>380</v>
       </c>
       <c r="I181" s="8" t="s">
-        <v>1108</v>
+        <v>1106</v>
       </c>
       <c r="J181" s="8">
         <v>0</v>
@@ -35362,7 +35388,7 @@
         <v>380</v>
       </c>
       <c r="I182" s="5" t="s">
-        <v>1108</v>
+        <v>1106</v>
       </c>
       <c r="J182" s="5">
         <v>0</v>
@@ -36242,7 +36268,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>1112</v>
+        <v>1110</v>
       </c>
       <c r="C9" s="8">
         <v>7</v>
@@ -37811,7 +37837,7 @@
         <v>5</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>1106</v>
+        <v>1104</v>
       </c>
       <c r="D40" s="6">
         <v>1</v>
@@ -37840,7 +37866,7 @@
         <v>5</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
       <c r="D41" s="5">
         <v>0</v>
@@ -38913,7 +38939,7 @@
         <v>3</v>
       </c>
       <c r="C78" t="s">
-        <v>1106</v>
+        <v>1104</v>
       </c>
       <c r="D78">
         <v>1</v>
@@ -38942,7 +38968,7 @@
         <v>3</v>
       </c>
       <c r="C79" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
       <c r="D79">
         <v>1</v>
@@ -41056,7 +41082,7 @@
         <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>1080</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -41078,7 +41104,7 @@
         <v>377</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>1083</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -41144,7 +41170,7 @@
         <v>961</v>
       </c>
       <c r="C11" t="s">
-        <v>1081</v>
+        <v>1079</v>
       </c>
     </row>
   </sheetData>
@@ -41409,25 +41435,25 @@
         <v>1034</v>
       </c>
       <c r="J1" s="5" t="s">
+        <v>1121</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>1122</v>
+      </c>
+      <c r="L1" s="5" t="s">
         <v>1123</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>1124</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>1125</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>1126</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>1127</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>1128</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>1129</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -42502,7 +42528,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>1120</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -42510,7 +42536,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>1121</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -42518,7 +42544,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>1122</v>
+        <v>1120</v>
       </c>
     </row>
   </sheetData>
@@ -42903,7 +42929,7 @@
         <v>1014</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -42917,7 +42943,7 @@
         <v>1016</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -42931,7 +42957,7 @@
         <v>1018</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -42945,7 +42971,7 @@
         <v>1020</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -42953,13 +42979,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>1041</v>
+        <v>1039</v>
       </c>
       <c r="C5" t="s">
         <v>1021</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -42973,7 +42999,7 @@
         <v>1023</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -42987,7 +43013,7 @@
         <v>1025</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -43001,7 +43027,7 @@
         <v>1027</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -43009,13 +43035,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>1016</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -43023,13 +43049,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>1044</v>
+        <v>1042</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>1020</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -43037,13 +43063,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>1045</v>
+        <v>1043</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -43051,13 +43077,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>1047</v>
+        <v>1045</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>1023</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -43065,13 +43091,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>1048</v>
+        <v>1046</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>1025</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -43079,13 +43105,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -43093,13 +43119,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>1027</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -43107,13 +43133,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>1052</v>
+        <v>1050</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>1053</v>
+        <v>1051</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -43121,13 +43147,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>1054</v>
+        <v>1052</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>1053</v>
+        <v>1051</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -43135,13 +43161,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>1114</v>
+        <v>1112</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>1115</v>
+        <v>1113</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -43149,13 +43175,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="8" t="s">
+        <v>1112</v>
+      </c>
+      <c r="C19" s="8" t="s">
         <v>1114</v>
       </c>
-      <c r="C19" s="8" t="s">
-        <v>1116</v>
-      </c>
       <c r="D19" s="8" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -43163,13 +43189,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>1114</v>
+        <v>1112</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>1117</v>
+        <v>1115</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -43177,13 +43203,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>1114</v>
+        <v>1112</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
     </row>
   </sheetData>
@@ -43204,10 +43230,10 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
       <c r="B1" t="s">
-        <v>1076</v>
+        <v>1074</v>
       </c>
       <c r="C1" t="s">
         <v>989</v>
@@ -43245,7 +43271,7 @@
         <v>101</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -43283,7 +43309,7 @@
         <v>102</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>1078</v>
+        <v>1076</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -43324,18 +43350,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:E18"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="6.26171875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.41796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.15625" customWidth="1"/>
     <col min="3" max="3" width="9.41796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.68359375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.89453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -43441,20 +43467,20 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7">
+      <c r="A7" s="5">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E7" s="6">
-        <v>1</v>
+      <c r="E7" s="5">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -43611,19 +43637,19 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17">
+      <c r="A17" s="5">
         <v>15</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>1037</v>
-      </c>
-      <c r="C17" s="6" t="s">
+      <c r="B17" s="5" t="s">
+        <v>1160</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D17" s="6" t="s">
-        <v>1038</v>
-      </c>
-      <c r="E17" s="6">
+      <c r="D17" s="5" t="s">
+        <v>1162</v>
+      </c>
+      <c r="E17" s="5">
         <v>1</v>
       </c>
     </row>
@@ -43693,6 +43719,23 @@
       </c>
       <c r="E21">
         <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="5">
+        <v>20</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>1161</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>1163</v>
+      </c>
+      <c r="E22" s="5">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -44207,7 +44250,7 @@
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -44215,7 +44258,7 @@
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -44223,7 +44266,7 @@
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>1098</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -44231,7 +44274,7 @@
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -44239,7 +44282,7 @@
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>1132</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -44247,7 +44290,7 @@
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>1134</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -44255,7 +44298,7 @@
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>1135</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -44263,7 +44306,7 @@
         <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>1136</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -44279,7 +44322,7 @@
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>1137</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -44287,7 +44330,7 @@
         <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -44303,7 +44346,7 @@
         <v>72</v>
       </c>
       <c r="B74" t="s">
-        <v>1139</v>
+        <v>1137</v>
       </c>
     </row>
   </sheetData>
@@ -46362,7 +46405,7 @@
         <v>253</v>
       </c>
       <c r="B255" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -46370,7 +46413,7 @@
         <v>254</v>
       </c>
       <c r="B256" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -46378,7 +46421,7 @@
         <v>255</v>
       </c>
       <c r="B257" t="s">
-        <v>1063</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -46386,7 +46429,7 @@
         <v>256</v>
       </c>
       <c r="B258" t="s">
-        <v>1064</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -46394,7 +46437,7 @@
         <v>257</v>
       </c>
       <c r="B259" t="s">
-        <v>1065</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -46402,7 +46445,7 @@
         <v>258</v>
       </c>
       <c r="B260" t="s">
-        <v>1066</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -46410,7 +46453,7 @@
         <v>259</v>
       </c>
       <c r="B261" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -46418,7 +46461,7 @@
         <v>260</v>
       </c>
       <c r="B262" t="s">
-        <v>1068</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -46426,7 +46469,7 @@
         <v>261</v>
       </c>
       <c r="B263" t="s">
-        <v>1069</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -46434,7 +46477,7 @@
         <v>262</v>
       </c>
       <c r="B264" t="s">
-        <v>1070</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -46442,7 +46485,7 @@
         <v>263</v>
       </c>
       <c r="B265" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -46458,7 +46501,7 @@
         <v>265</v>
       </c>
       <c r="B267" t="s">
-        <v>1072</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -46466,7 +46509,7 @@
         <v>266</v>
       </c>
       <c r="B268" t="s">
-        <v>1085</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -46474,7 +46517,7 @@
         <v>267</v>
       </c>
       <c r="B269" t="s">
-        <v>1086</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -46482,7 +46525,7 @@
         <v>268</v>
       </c>
       <c r="B270" t="s">
-        <v>1087</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -46490,7 +46533,7 @@
         <v>269</v>
       </c>
       <c r="B271" t="s">
-        <v>1088</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -46498,7 +46541,7 @@
         <v>270</v>
       </c>
       <c r="B272" t="s">
-        <v>1089</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -46506,7 +46549,7 @@
         <v>271</v>
       </c>
       <c r="B273" t="s">
-        <v>1090</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -46514,7 +46557,7 @@
         <v>272</v>
       </c>
       <c r="B274" t="s">
-        <v>1091</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -46522,7 +46565,7 @@
         <v>273</v>
       </c>
       <c r="B275" t="s">
-        <v>1092</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -46530,7 +46573,7 @@
         <v>274</v>
       </c>
       <c r="B276" t="s">
-        <v>1093</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -46538,7 +46581,7 @@
         <v>275</v>
       </c>
       <c r="B277" t="s">
-        <v>1094</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -46546,7 +46589,7 @@
         <v>276</v>
       </c>
       <c r="B278" t="s">
-        <v>1095</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -46554,7 +46597,7 @@
         <v>277</v>
       </c>
       <c r="B279" t="s">
-        <v>1099</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -46562,7 +46605,7 @@
         <v>278</v>
       </c>
       <c r="B280" t="s">
-        <v>1100</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -46570,7 +46613,7 @@
         <v>279</v>
       </c>
       <c r="B281" t="s">
-        <v>1101</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -46578,7 +46621,7 @@
         <v>280</v>
       </c>
       <c r="B282" t="s">
-        <v>1102</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -46586,7 +46629,7 @@
         <v>281</v>
       </c>
       <c r="B283" t="s">
-        <v>1107</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -46594,7 +46637,7 @@
         <v>282</v>
       </c>
       <c r="B284" t="s">
-        <v>1110</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -46602,7 +46645,7 @@
         <v>283</v>
       </c>
       <c r="B285" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -46610,7 +46653,7 @@
         <v>284</v>
       </c>
       <c r="B286" t="s">
-        <v>1141</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -46618,7 +46661,7 @@
         <v>285</v>
       </c>
       <c r="B287" t="s">
-        <v>1142</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -46626,7 +46669,7 @@
         <v>286</v>
       </c>
       <c r="B288" t="s">
-        <v>1143</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -46634,7 +46677,7 @@
         <v>287</v>
       </c>
       <c r="B289" t="s">
-        <v>1144</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -46642,7 +46685,7 @@
         <v>288</v>
       </c>
       <c r="B290" t="s">
-        <v>1145</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -46650,7 +46693,7 @@
         <v>289</v>
       </c>
       <c r="B291" t="s">
-        <v>1146</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -46658,7 +46701,7 @@
         <v>290</v>
       </c>
       <c r="B292" t="s">
-        <v>1147</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -46666,7 +46709,7 @@
         <v>291</v>
       </c>
       <c r="B293" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -46674,7 +46717,7 @@
         <v>292</v>
       </c>
       <c r="B294" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -46682,7 +46725,7 @@
         <v>293</v>
       </c>
       <c r="B295" t="s">
-        <v>1150</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -46690,7 +46733,7 @@
         <v>294</v>
       </c>
       <c r="B296" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -46698,7 +46741,7 @@
         <v>295</v>
       </c>
       <c r="B297" t="s">
-        <v>1152</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -46706,7 +46749,7 @@
         <v>296</v>
       </c>
       <c r="B298" t="s">
-        <v>1153</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -46714,7 +46757,7 @@
         <v>297</v>
       </c>
       <c r="B299" t="s">
-        <v>1154</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -46722,7 +46765,7 @@
         <v>298</v>
       </c>
       <c r="B300" s="5" t="s">
-        <v>1158</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -46730,7 +46773,7 @@
         <v>299</v>
       </c>
       <c r="B301" s="5" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -46738,7 +46781,7 @@
         <v>300</v>
       </c>
       <c r="B302" s="5" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -46746,7 +46789,7 @@
         <v>301</v>
       </c>
       <c r="B303" s="5" t="s">
-        <v>1161</v>
+        <v>1159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TFS 25124 - Documentation update allowing Quality PMs access to the Quality Module submissions and EWLS text updates
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C51928
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TFS\eCoaching_V2\Design\DD\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB07E0BD-5C31-4CC7-AE9C-45ECAF7B6996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{039A6DCB-8011-4D74-97F5-EE4940ADB422}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57504" yWindow="1932" windowWidth="28992" windowHeight="15792" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_History" sheetId="14" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4221" uniqueCount="1167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4223" uniqueCount="1169">
   <si>
     <t>SourceID</t>
   </si>
@@ -3586,7 +3586,33 @@
     <t>Report access for Early Work Life Supervisors. Added row(s) to DIM_Sub_Coaching_Reason and Coaching_Reason_Selection</t>
   </si>
   <si>
-    <t>Early Work Life</t>
+    <r>
+      <t>Early Work Life (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>For Use by Early Work Life Staff Only</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Doc cleanup for Quality Module Submission for Quality PM Job code (Module_Submission tab) and text update for EWLS Sub Coaching Reason (Dim_SubCoaching_Reason and Coaching_Reason_Selection tabs)</t>
+  </si>
+  <si>
+    <t>Early Work Life (For Use by Early Work Life Staff Only)</t>
   </si>
 </sst>
 </file>
@@ -3596,7 +3622,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss:mss"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3611,6 +3637,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -3651,7 +3689,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -3670,6 +3708,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4008,10 +4047,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L114"/>
+  <dimension ref="A1:L115"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="A114" sqref="A114"/>
+      <selection activeCell="A115" sqref="A115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -5913,7 +5952,7 @@
         <v>1163</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" s="6">
         <v>102.1</v>
       </c>
@@ -5930,22 +5969,42 @@
         <v>1164</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A114" s="5">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A114" s="8">
         <v>103</v>
       </c>
-      <c r="B114" s="13">
+      <c r="B114" s="9">
         <v>44762</v>
       </c>
-      <c r="C114" s="5" t="s">
+      <c r="C114" s="8" t="s">
         <v>427</v>
       </c>
-      <c r="D114" s="5">
+      <c r="D114" s="8">
         <v>24924</v>
       </c>
-      <c r="E114" s="5" t="s">
+      <c r="E114" s="8" t="s">
         <v>1165</v>
       </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A115" s="5">
+        <v>104</v>
+      </c>
+      <c r="B115" s="13">
+        <v>44816</v>
+      </c>
+      <c r="C115" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="D115" s="5">
+        <v>25124</v>
+      </c>
+      <c r="E115" s="5" t="s">
+        <v>1167</v>
+      </c>
+      <c r="F115" s="5"/>
+      <c r="G115" s="5"/>
+      <c r="H115" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5957,8 +6016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60:G60"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -6574,8 +6633,8 @@
       <c r="D27">
         <v>1</v>
       </c>
-      <c r="E27">
-        <v>0</v>
+      <c r="E27" s="5">
+        <v>1</v>
       </c>
       <c r="F27">
         <v>1</v>
@@ -7453,13 +7512,13 @@
   <dimension ref="A1:P445"/>
   <sheetViews>
     <sheetView topLeftCell="A411" workbookViewId="0">
-      <selection activeCell="A430" sqref="A430:XFD430"/>
+      <selection activeCell="D430" sqref="D430:D445"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="22.83984375" customWidth="1"/>
-    <col min="4" max="4" width="44.41796875" customWidth="1"/>
+    <col min="2" max="2" width="33.05078125" customWidth="1"/>
+    <col min="4" max="4" width="59.5234375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -28913,802 +28972,802 @@
       </c>
     </row>
     <row r="430" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A430" s="5">
+      <c r="A430" s="6">
         <v>2</v>
       </c>
-      <c r="B430" s="5" t="s">
+      <c r="B430" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="C430" s="5">
+      <c r="C430" s="6">
         <v>302</v>
       </c>
       <c r="D430" s="5" t="s">
-        <v>1166</v>
-      </c>
-      <c r="E430" s="5">
-        <v>1</v>
-      </c>
-      <c r="F430" s="5">
-        <v>1</v>
-      </c>
-      <c r="G430" s="5">
-        <v>1</v>
-      </c>
-      <c r="H430" s="5">
-        <v>1</v>
-      </c>
-      <c r="I430" s="5">
-        <v>1</v>
-      </c>
-      <c r="J430" s="5">
-        <v>1</v>
-      </c>
-      <c r="K430" s="5">
-        <v>0</v>
-      </c>
-      <c r="L430" s="5">
-        <v>0</v>
-      </c>
-      <c r="M430" s="5">
-        <v>0</v>
-      </c>
-      <c r="N430" s="5">
-        <v>0</v>
-      </c>
-      <c r="O430" s="5">
-        <v>0</v>
-      </c>
-      <c r="P430" s="5">
+        <v>1168</v>
+      </c>
+      <c r="E430" s="6">
+        <v>1</v>
+      </c>
+      <c r="F430" s="6">
+        <v>1</v>
+      </c>
+      <c r="G430" s="6">
+        <v>1</v>
+      </c>
+      <c r="H430" s="6">
+        <v>1</v>
+      </c>
+      <c r="I430" s="6">
+        <v>1</v>
+      </c>
+      <c r="J430" s="6">
+        <v>1</v>
+      </c>
+      <c r="K430" s="6">
+        <v>0</v>
+      </c>
+      <c r="L430" s="6">
+        <v>0</v>
+      </c>
+      <c r="M430" s="6">
+        <v>0</v>
+      </c>
+      <c r="N430" s="6">
+        <v>0</v>
+      </c>
+      <c r="O430" s="6">
+        <v>0</v>
+      </c>
+      <c r="P430" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="431" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A431" s="5">
+      <c r="A431" s="6">
         <v>3</v>
       </c>
-      <c r="B431" s="5" t="s">
+      <c r="B431" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C431" s="5">
+      <c r="C431" s="6">
         <v>302</v>
       </c>
       <c r="D431" s="5" t="s">
-        <v>1166</v>
-      </c>
-      <c r="E431" s="5">
-        <v>1</v>
-      </c>
-      <c r="F431" s="5">
-        <v>1</v>
-      </c>
-      <c r="G431" s="5">
-        <v>1</v>
-      </c>
-      <c r="H431" s="5">
-        <v>1</v>
-      </c>
-      <c r="I431" s="5">
-        <v>1</v>
-      </c>
-      <c r="J431" s="5">
-        <v>1</v>
-      </c>
-      <c r="K431" s="5">
-        <v>0</v>
-      </c>
-      <c r="L431" s="5">
-        <v>0</v>
-      </c>
-      <c r="M431" s="5">
-        <v>0</v>
-      </c>
-      <c r="N431" s="5">
-        <v>0</v>
-      </c>
-      <c r="O431" s="5">
-        <v>0</v>
-      </c>
-      <c r="P431" s="5">
+        <v>1168</v>
+      </c>
+      <c r="E431" s="6">
+        <v>1</v>
+      </c>
+      <c r="F431" s="6">
+        <v>1</v>
+      </c>
+      <c r="G431" s="6">
+        <v>1</v>
+      </c>
+      <c r="H431" s="6">
+        <v>1</v>
+      </c>
+      <c r="I431" s="6">
+        <v>1</v>
+      </c>
+      <c r="J431" s="6">
+        <v>1</v>
+      </c>
+      <c r="K431" s="6">
+        <v>0</v>
+      </c>
+      <c r="L431" s="6">
+        <v>0</v>
+      </c>
+      <c r="M431" s="6">
+        <v>0</v>
+      </c>
+      <c r="N431" s="6">
+        <v>0</v>
+      </c>
+      <c r="O431" s="6">
+        <v>0</v>
+      </c>
+      <c r="P431" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="432" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A432" s="5">
+      <c r="A432" s="6">
         <v>4</v>
       </c>
-      <c r="B432" s="5" t="s">
+      <c r="B432" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="C432" s="5">
+      <c r="C432" s="6">
         <v>302</v>
       </c>
       <c r="D432" s="5" t="s">
-        <v>1166</v>
-      </c>
-      <c r="E432" s="5">
-        <v>1</v>
-      </c>
-      <c r="F432" s="5">
-        <v>1</v>
-      </c>
-      <c r="G432" s="5">
-        <v>1</v>
-      </c>
-      <c r="H432" s="5">
-        <v>1</v>
-      </c>
-      <c r="I432" s="5">
-        <v>1</v>
-      </c>
-      <c r="J432" s="5">
-        <v>1</v>
-      </c>
-      <c r="K432" s="5">
-        <v>0</v>
-      </c>
-      <c r="L432" s="5">
-        <v>0</v>
-      </c>
-      <c r="M432" s="5">
-        <v>0</v>
-      </c>
-      <c r="N432" s="5">
-        <v>0</v>
-      </c>
-      <c r="O432" s="5">
-        <v>0</v>
-      </c>
-      <c r="P432" s="5">
+        <v>1168</v>
+      </c>
+      <c r="E432" s="6">
+        <v>1</v>
+      </c>
+      <c r="F432" s="6">
+        <v>1</v>
+      </c>
+      <c r="G432" s="6">
+        <v>1</v>
+      </c>
+      <c r="H432" s="6">
+        <v>1</v>
+      </c>
+      <c r="I432" s="6">
+        <v>1</v>
+      </c>
+      <c r="J432" s="6">
+        <v>1</v>
+      </c>
+      <c r="K432" s="6">
+        <v>0</v>
+      </c>
+      <c r="L432" s="6">
+        <v>0</v>
+      </c>
+      <c r="M432" s="6">
+        <v>0</v>
+      </c>
+      <c r="N432" s="6">
+        <v>0</v>
+      </c>
+      <c r="O432" s="6">
+        <v>0</v>
+      </c>
+      <c r="P432" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="433" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A433" s="5">
+      <c r="A433" s="6">
         <v>5</v>
       </c>
-      <c r="B433" s="5" t="s">
+      <c r="B433" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="C433" s="5">
+      <c r="C433" s="6">
         <v>302</v>
       </c>
       <c r="D433" s="5" t="s">
-        <v>1166</v>
-      </c>
-      <c r="E433" s="5">
-        <v>1</v>
-      </c>
-      <c r="F433" s="5">
-        <v>1</v>
-      </c>
-      <c r="G433" s="5">
-        <v>1</v>
-      </c>
-      <c r="H433" s="5">
-        <v>1</v>
-      </c>
-      <c r="I433" s="5">
-        <v>1</v>
-      </c>
-      <c r="J433" s="5">
-        <v>1</v>
-      </c>
-      <c r="K433" s="5">
-        <v>0</v>
-      </c>
-      <c r="L433" s="5">
-        <v>0</v>
-      </c>
-      <c r="M433" s="5">
-        <v>0</v>
-      </c>
-      <c r="N433" s="5">
-        <v>0</v>
-      </c>
-      <c r="O433" s="5">
-        <v>0</v>
-      </c>
-      <c r="P433" s="5">
+        <v>1168</v>
+      </c>
+      <c r="E433" s="6">
+        <v>1</v>
+      </c>
+      <c r="F433" s="6">
+        <v>1</v>
+      </c>
+      <c r="G433" s="6">
+        <v>1</v>
+      </c>
+      <c r="H433" s="6">
+        <v>1</v>
+      </c>
+      <c r="I433" s="6">
+        <v>1</v>
+      </c>
+      <c r="J433" s="6">
+        <v>1</v>
+      </c>
+      <c r="K433" s="6">
+        <v>0</v>
+      </c>
+      <c r="L433" s="6">
+        <v>0</v>
+      </c>
+      <c r="M433" s="6">
+        <v>0</v>
+      </c>
+      <c r="N433" s="6">
+        <v>0</v>
+      </c>
+      <c r="O433" s="6">
+        <v>0</v>
+      </c>
+      <c r="P433" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="434" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A434" s="5">
+      <c r="A434" s="6">
         <v>6</v>
       </c>
-      <c r="B434" s="5" t="s">
+      <c r="B434" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="C434" s="5">
+      <c r="C434" s="6">
         <v>302</v>
       </c>
       <c r="D434" s="5" t="s">
-        <v>1166</v>
-      </c>
-      <c r="E434" s="5">
-        <v>1</v>
-      </c>
-      <c r="F434" s="5">
-        <v>1</v>
-      </c>
-      <c r="G434" s="5">
-        <v>1</v>
-      </c>
-      <c r="H434" s="5">
-        <v>1</v>
-      </c>
-      <c r="I434" s="5">
-        <v>0</v>
-      </c>
-      <c r="J434" s="5">
-        <v>1</v>
-      </c>
-      <c r="K434" s="5">
-        <v>0</v>
-      </c>
-      <c r="L434" s="5">
-        <v>0</v>
-      </c>
-      <c r="M434" s="5">
-        <v>0</v>
-      </c>
-      <c r="N434" s="5">
-        <v>0</v>
-      </c>
-      <c r="O434" s="5">
-        <v>0</v>
-      </c>
-      <c r="P434" s="5">
+        <v>1168</v>
+      </c>
+      <c r="E434" s="6">
+        <v>1</v>
+      </c>
+      <c r="F434" s="6">
+        <v>1</v>
+      </c>
+      <c r="G434" s="6">
+        <v>1</v>
+      </c>
+      <c r="H434" s="6">
+        <v>1</v>
+      </c>
+      <c r="I434" s="6">
+        <v>0</v>
+      </c>
+      <c r="J434" s="6">
+        <v>1</v>
+      </c>
+      <c r="K434" s="6">
+        <v>0</v>
+      </c>
+      <c r="L434" s="6">
+        <v>0</v>
+      </c>
+      <c r="M434" s="6">
+        <v>0</v>
+      </c>
+      <c r="N434" s="6">
+        <v>0</v>
+      </c>
+      <c r="O434" s="6">
+        <v>0</v>
+      </c>
+      <c r="P434" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="435" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A435" s="5">
+      <c r="A435" s="6">
         <v>7</v>
       </c>
-      <c r="B435" s="5" t="s">
+      <c r="B435" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="C435" s="5">
+      <c r="C435" s="6">
         <v>302</v>
       </c>
       <c r="D435" s="5" t="s">
-        <v>1166</v>
-      </c>
-      <c r="E435" s="5">
-        <v>1</v>
-      </c>
-      <c r="F435" s="5">
-        <v>1</v>
-      </c>
-      <c r="G435" s="5">
-        <v>1</v>
-      </c>
-      <c r="H435" s="5">
-        <v>1</v>
-      </c>
-      <c r="I435" s="5">
-        <v>1</v>
-      </c>
-      <c r="J435" s="5">
-        <v>1</v>
-      </c>
-      <c r="K435" s="5">
-        <v>0</v>
-      </c>
-      <c r="L435" s="5">
-        <v>0</v>
-      </c>
-      <c r="M435" s="5">
-        <v>0</v>
-      </c>
-      <c r="N435" s="5">
-        <v>0</v>
-      </c>
-      <c r="O435" s="5">
-        <v>0</v>
-      </c>
-      <c r="P435" s="5">
+        <v>1168</v>
+      </c>
+      <c r="E435" s="6">
+        <v>1</v>
+      </c>
+      <c r="F435" s="6">
+        <v>1</v>
+      </c>
+      <c r="G435" s="6">
+        <v>1</v>
+      </c>
+      <c r="H435" s="6">
+        <v>1</v>
+      </c>
+      <c r="I435" s="6">
+        <v>1</v>
+      </c>
+      <c r="J435" s="6">
+        <v>1</v>
+      </c>
+      <c r="K435" s="6">
+        <v>0</v>
+      </c>
+      <c r="L435" s="6">
+        <v>0</v>
+      </c>
+      <c r="M435" s="6">
+        <v>0</v>
+      </c>
+      <c r="N435" s="6">
+        <v>0</v>
+      </c>
+      <c r="O435" s="6">
+        <v>0</v>
+      </c>
+      <c r="P435" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="436" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A436" s="5">
+      <c r="A436" s="6">
         <v>8</v>
       </c>
-      <c r="B436" s="5" t="s">
+      <c r="B436" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="C436" s="5">
+      <c r="C436" s="6">
         <v>302</v>
       </c>
       <c r="D436" s="5" t="s">
-        <v>1166</v>
-      </c>
-      <c r="E436" s="5">
-        <v>1</v>
-      </c>
-      <c r="F436" s="5">
-        <v>1</v>
-      </c>
-      <c r="G436" s="5">
-        <v>1</v>
-      </c>
-      <c r="H436" s="5">
-        <v>1</v>
-      </c>
-      <c r="I436" s="5">
-        <v>1</v>
-      </c>
-      <c r="J436" s="5">
-        <v>1</v>
-      </c>
-      <c r="K436" s="5">
-        <v>0</v>
-      </c>
-      <c r="L436" s="5">
-        <v>0</v>
-      </c>
-      <c r="M436" s="5">
-        <v>0</v>
-      </c>
-      <c r="N436" s="5">
-        <v>0</v>
-      </c>
-      <c r="O436" s="5">
-        <v>0</v>
-      </c>
-      <c r="P436" s="5">
+        <v>1168</v>
+      </c>
+      <c r="E436" s="6">
+        <v>1</v>
+      </c>
+      <c r="F436" s="6">
+        <v>1</v>
+      </c>
+      <c r="G436" s="6">
+        <v>1</v>
+      </c>
+      <c r="H436" s="6">
+        <v>1</v>
+      </c>
+      <c r="I436" s="6">
+        <v>1</v>
+      </c>
+      <c r="J436" s="6">
+        <v>1</v>
+      </c>
+      <c r="K436" s="6">
+        <v>0</v>
+      </c>
+      <c r="L436" s="6">
+        <v>0</v>
+      </c>
+      <c r="M436" s="6">
+        <v>0</v>
+      </c>
+      <c r="N436" s="6">
+        <v>0</v>
+      </c>
+      <c r="O436" s="6">
+        <v>0</v>
+      </c>
+      <c r="P436" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="437" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A437" s="5">
+      <c r="A437" s="6">
         <v>9</v>
       </c>
-      <c r="B437" s="5" t="s">
+      <c r="B437" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="C437" s="5">
+      <c r="C437" s="6">
         <v>302</v>
       </c>
       <c r="D437" s="5" t="s">
-        <v>1166</v>
-      </c>
-      <c r="E437" s="5">
-        <v>1</v>
-      </c>
-      <c r="F437" s="5">
-        <v>1</v>
-      </c>
-      <c r="G437" s="5">
-        <v>1</v>
-      </c>
-      <c r="H437" s="5">
-        <v>1</v>
-      </c>
-      <c r="I437" s="5">
-        <v>1</v>
-      </c>
-      <c r="J437" s="5">
-        <v>1</v>
-      </c>
-      <c r="K437" s="5">
-        <v>0</v>
-      </c>
-      <c r="L437" s="5">
-        <v>0</v>
-      </c>
-      <c r="M437" s="5">
-        <v>0</v>
-      </c>
-      <c r="N437" s="5">
-        <v>0</v>
-      </c>
-      <c r="O437" s="5">
-        <v>0</v>
-      </c>
-      <c r="P437" s="5">
+        <v>1168</v>
+      </c>
+      <c r="E437" s="6">
+        <v>1</v>
+      </c>
+      <c r="F437" s="6">
+        <v>1</v>
+      </c>
+      <c r="G437" s="6">
+        <v>1</v>
+      </c>
+      <c r="H437" s="6">
+        <v>1</v>
+      </c>
+      <c r="I437" s="6">
+        <v>1</v>
+      </c>
+      <c r="J437" s="6">
+        <v>1</v>
+      </c>
+      <c r="K437" s="6">
+        <v>0</v>
+      </c>
+      <c r="L437" s="6">
+        <v>0</v>
+      </c>
+      <c r="M437" s="6">
+        <v>0</v>
+      </c>
+      <c r="N437" s="6">
+        <v>0</v>
+      </c>
+      <c r="O437" s="6">
+        <v>0</v>
+      </c>
+      <c r="P437" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="438" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A438" s="5">
+      <c r="A438" s="6">
         <v>10</v>
       </c>
-      <c r="B438" s="5" t="s">
+      <c r="B438" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="C438" s="5">
+      <c r="C438" s="6">
         <v>302</v>
       </c>
       <c r="D438" s="5" t="s">
-        <v>1166</v>
-      </c>
-      <c r="E438" s="5">
-        <v>1</v>
-      </c>
-      <c r="F438" s="5">
-        <v>1</v>
-      </c>
-      <c r="G438" s="5">
-        <v>1</v>
-      </c>
-      <c r="H438" s="5">
-        <v>1</v>
-      </c>
-      <c r="I438" s="5">
-        <v>1</v>
-      </c>
-      <c r="J438" s="5">
-        <v>1</v>
-      </c>
-      <c r="K438" s="5">
-        <v>0</v>
-      </c>
-      <c r="L438" s="5">
-        <v>0</v>
-      </c>
-      <c r="M438" s="5">
-        <v>0</v>
-      </c>
-      <c r="N438" s="5">
-        <v>0</v>
-      </c>
-      <c r="O438" s="5">
-        <v>0</v>
-      </c>
-      <c r="P438" s="5">
+        <v>1168</v>
+      </c>
+      <c r="E438" s="6">
+        <v>1</v>
+      </c>
+      <c r="F438" s="6">
+        <v>1</v>
+      </c>
+      <c r="G438" s="6">
+        <v>1</v>
+      </c>
+      <c r="H438" s="6">
+        <v>1</v>
+      </c>
+      <c r="I438" s="6">
+        <v>1</v>
+      </c>
+      <c r="J438" s="6">
+        <v>1</v>
+      </c>
+      <c r="K438" s="6">
+        <v>0</v>
+      </c>
+      <c r="L438" s="6">
+        <v>0</v>
+      </c>
+      <c r="M438" s="6">
+        <v>0</v>
+      </c>
+      <c r="N438" s="6">
+        <v>0</v>
+      </c>
+      <c r="O438" s="6">
+        <v>0</v>
+      </c>
+      <c r="P438" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="439" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A439" s="5">
+      <c r="A439" s="6">
         <v>11</v>
       </c>
-      <c r="B439" s="5" t="s">
+      <c r="B439" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="C439" s="5">
+      <c r="C439" s="6">
         <v>302</v>
       </c>
       <c r="D439" s="5" t="s">
-        <v>1166</v>
-      </c>
-      <c r="E439" s="5">
-        <v>1</v>
-      </c>
-      <c r="F439" s="5">
-        <v>1</v>
-      </c>
-      <c r="G439" s="5">
-        <v>1</v>
-      </c>
-      <c r="H439" s="5">
-        <v>0</v>
-      </c>
-      <c r="I439" s="5">
-        <v>1</v>
-      </c>
-      <c r="J439" s="5">
-        <v>1</v>
-      </c>
-      <c r="K439" s="5">
-        <v>0</v>
-      </c>
-      <c r="L439" s="5">
-        <v>0</v>
-      </c>
-      <c r="M439" s="5">
-        <v>0</v>
-      </c>
-      <c r="N439" s="5">
-        <v>0</v>
-      </c>
-      <c r="O439" s="5">
-        <v>0</v>
-      </c>
-      <c r="P439" s="5">
+        <v>1168</v>
+      </c>
+      <c r="E439" s="6">
+        <v>1</v>
+      </c>
+      <c r="F439" s="6">
+        <v>1</v>
+      </c>
+      <c r="G439" s="6">
+        <v>1</v>
+      </c>
+      <c r="H439" s="6">
+        <v>0</v>
+      </c>
+      <c r="I439" s="6">
+        <v>1</v>
+      </c>
+      <c r="J439" s="6">
+        <v>1</v>
+      </c>
+      <c r="K439" s="6">
+        <v>0</v>
+      </c>
+      <c r="L439" s="6">
+        <v>0</v>
+      </c>
+      <c r="M439" s="6">
+        <v>0</v>
+      </c>
+      <c r="N439" s="6">
+        <v>0</v>
+      </c>
+      <c r="O439" s="6">
+        <v>0</v>
+      </c>
+      <c r="P439" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="440" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A440" s="5">
+      <c r="A440" s="6">
         <v>12</v>
       </c>
-      <c r="B440" s="5" t="s">
+      <c r="B440" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="C440" s="5">
+      <c r="C440" s="6">
         <v>302</v>
       </c>
       <c r="D440" s="5" t="s">
-        <v>1166</v>
-      </c>
-      <c r="E440" s="5">
-        <v>1</v>
-      </c>
-      <c r="F440" s="5">
-        <v>1</v>
-      </c>
-      <c r="G440" s="5">
-        <v>1</v>
-      </c>
-      <c r="H440" s="5">
-        <v>1</v>
-      </c>
-      <c r="I440" s="5">
-        <v>1</v>
-      </c>
-      <c r="J440" s="5">
-        <v>1</v>
-      </c>
-      <c r="K440" s="5">
-        <v>0</v>
-      </c>
-      <c r="L440" s="5">
-        <v>0</v>
-      </c>
-      <c r="M440" s="5">
-        <v>0</v>
-      </c>
-      <c r="N440" s="5">
-        <v>0</v>
-      </c>
-      <c r="O440" s="5">
-        <v>0</v>
-      </c>
-      <c r="P440" s="5">
+        <v>1168</v>
+      </c>
+      <c r="E440" s="6">
+        <v>1</v>
+      </c>
+      <c r="F440" s="6">
+        <v>1</v>
+      </c>
+      <c r="G440" s="6">
+        <v>1</v>
+      </c>
+      <c r="H440" s="6">
+        <v>1</v>
+      </c>
+      <c r="I440" s="6">
+        <v>1</v>
+      </c>
+      <c r="J440" s="6">
+        <v>1</v>
+      </c>
+      <c r="K440" s="6">
+        <v>0</v>
+      </c>
+      <c r="L440" s="6">
+        <v>0</v>
+      </c>
+      <c r="M440" s="6">
+        <v>0</v>
+      </c>
+      <c r="N440" s="6">
+        <v>0</v>
+      </c>
+      <c r="O440" s="6">
+        <v>0</v>
+      </c>
+      <c r="P440" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="441" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A441" s="5">
+      <c r="A441" s="6">
         <v>13</v>
       </c>
-      <c r="B441" s="5" t="s">
+      <c r="B441" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="C441" s="5">
+      <c r="C441" s="6">
         <v>302</v>
       </c>
       <c r="D441" s="5" t="s">
-        <v>1166</v>
-      </c>
-      <c r="E441" s="5">
-        <v>1</v>
-      </c>
-      <c r="F441" s="5">
-        <v>1</v>
-      </c>
-      <c r="G441" s="5">
-        <v>1</v>
-      </c>
-      <c r="H441" s="5">
-        <v>1</v>
-      </c>
-      <c r="I441" s="5">
-        <v>1</v>
-      </c>
-      <c r="J441" s="5">
-        <v>1</v>
-      </c>
-      <c r="K441" s="5">
-        <v>0</v>
-      </c>
-      <c r="L441" s="5">
-        <v>0</v>
-      </c>
-      <c r="M441" s="5">
-        <v>0</v>
-      </c>
-      <c r="N441" s="5">
-        <v>0</v>
-      </c>
-      <c r="O441" s="5">
-        <v>0</v>
-      </c>
-      <c r="P441" s="5">
+        <v>1168</v>
+      </c>
+      <c r="E441" s="6">
+        <v>1</v>
+      </c>
+      <c r="F441" s="6">
+        <v>1</v>
+      </c>
+      <c r="G441" s="6">
+        <v>1</v>
+      </c>
+      <c r="H441" s="6">
+        <v>1</v>
+      </c>
+      <c r="I441" s="6">
+        <v>1</v>
+      </c>
+      <c r="J441" s="6">
+        <v>1</v>
+      </c>
+      <c r="K441" s="6">
+        <v>0</v>
+      </c>
+      <c r="L441" s="6">
+        <v>0</v>
+      </c>
+      <c r="M441" s="6">
+        <v>0</v>
+      </c>
+      <c r="N441" s="6">
+        <v>0</v>
+      </c>
+      <c r="O441" s="6">
+        <v>0</v>
+      </c>
+      <c r="P441" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="442" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A442" s="5">
+      <c r="A442" s="6">
         <v>55</v>
       </c>
-      <c r="B442" s="5" t="s">
+      <c r="B442" s="6" t="s">
         <v>797</v>
       </c>
-      <c r="C442" s="5">
+      <c r="C442" s="6">
         <v>302</v>
       </c>
       <c r="D442" s="5" t="s">
-        <v>1166</v>
-      </c>
-      <c r="E442" s="5">
-        <v>1</v>
-      </c>
-      <c r="F442" s="5">
-        <v>1</v>
-      </c>
-      <c r="G442" s="5">
-        <v>1</v>
-      </c>
-      <c r="H442" s="5">
-        <v>1</v>
-      </c>
-      <c r="I442" s="5">
-        <v>1</v>
-      </c>
-      <c r="J442" s="5">
-        <v>1</v>
-      </c>
-      <c r="K442" s="5">
-        <v>0</v>
-      </c>
-      <c r="L442" s="5">
-        <v>0</v>
-      </c>
-      <c r="M442" s="5">
-        <v>0</v>
-      </c>
-      <c r="N442" s="5">
-        <v>0</v>
-      </c>
-      <c r="O442" s="5">
-        <v>0</v>
-      </c>
-      <c r="P442" s="5">
+        <v>1168</v>
+      </c>
+      <c r="E442" s="6">
+        <v>1</v>
+      </c>
+      <c r="F442" s="6">
+        <v>1</v>
+      </c>
+      <c r="G442" s="6">
+        <v>1</v>
+      </c>
+      <c r="H442" s="6">
+        <v>1</v>
+      </c>
+      <c r="I442" s="6">
+        <v>1</v>
+      </c>
+      <c r="J442" s="6">
+        <v>1</v>
+      </c>
+      <c r="K442" s="6">
+        <v>0</v>
+      </c>
+      <c r="L442" s="6">
+        <v>0</v>
+      </c>
+      <c r="M442" s="6">
+        <v>0</v>
+      </c>
+      <c r="N442" s="6">
+        <v>0</v>
+      </c>
+      <c r="O442" s="6">
+        <v>0</v>
+      </c>
+      <c r="P442" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="443" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A443" s="5">
+      <c r="A443" s="6">
         <v>61</v>
       </c>
-      <c r="B443" s="5" t="s">
+      <c r="B443" s="6" t="s">
         <v>1081</v>
       </c>
-      <c r="C443" s="5">
+      <c r="C443" s="6">
         <v>302</v>
       </c>
       <c r="D443" s="5" t="s">
-        <v>1166</v>
-      </c>
-      <c r="E443" s="5">
-        <v>1</v>
-      </c>
-      <c r="F443" s="5">
-        <v>1</v>
-      </c>
-      <c r="G443" s="5">
-        <v>1</v>
-      </c>
-      <c r="H443" s="5">
-        <v>1</v>
-      </c>
-      <c r="I443" s="5">
-        <v>1</v>
-      </c>
-      <c r="J443" s="5">
-        <v>1</v>
-      </c>
-      <c r="K443" s="5">
-        <v>0</v>
-      </c>
-      <c r="L443" s="5">
-        <v>0</v>
-      </c>
-      <c r="M443" s="5">
-        <v>0</v>
-      </c>
-      <c r="N443" s="5">
-        <v>0</v>
-      </c>
-      <c r="O443" s="5">
-        <v>0</v>
-      </c>
-      <c r="P443" s="5">
+        <v>1168</v>
+      </c>
+      <c r="E443" s="6">
+        <v>1</v>
+      </c>
+      <c r="F443" s="6">
+        <v>1</v>
+      </c>
+      <c r="G443" s="6">
+        <v>1</v>
+      </c>
+      <c r="H443" s="6">
+        <v>1</v>
+      </c>
+      <c r="I443" s="6">
+        <v>1</v>
+      </c>
+      <c r="J443" s="6">
+        <v>1</v>
+      </c>
+      <c r="K443" s="6">
+        <v>0</v>
+      </c>
+      <c r="L443" s="6">
+        <v>0</v>
+      </c>
+      <c r="M443" s="6">
+        <v>0</v>
+      </c>
+      <c r="N443" s="6">
+        <v>0</v>
+      </c>
+      <c r="O443" s="6">
+        <v>0</v>
+      </c>
+      <c r="P443" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="444" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A444" s="5">
+      <c r="A444" s="6">
         <v>62</v>
       </c>
-      <c r="B444" s="5" t="s">
+      <c r="B444" s="6" t="s">
         <v>1095</v>
       </c>
-      <c r="C444" s="5">
+      <c r="C444" s="6">
         <v>302</v>
       </c>
       <c r="D444" s="5" t="s">
-        <v>1166</v>
-      </c>
-      <c r="E444" s="5">
-        <v>1</v>
-      </c>
-      <c r="F444" s="5">
-        <v>1</v>
-      </c>
-      <c r="G444" s="5">
-        <v>1</v>
-      </c>
-      <c r="H444" s="5">
-        <v>1</v>
-      </c>
-      <c r="I444" s="5">
-        <v>1</v>
-      </c>
-      <c r="J444" s="5">
-        <v>1</v>
-      </c>
-      <c r="K444" s="5">
-        <v>0</v>
-      </c>
-      <c r="L444" s="5">
-        <v>0</v>
-      </c>
-      <c r="M444" s="5">
-        <v>0</v>
-      </c>
-      <c r="N444" s="5">
-        <v>0</v>
-      </c>
-      <c r="O444" s="5">
-        <v>0</v>
-      </c>
-      <c r="P444" s="5">
+        <v>1168</v>
+      </c>
+      <c r="E444" s="6">
+        <v>1</v>
+      </c>
+      <c r="F444" s="6">
+        <v>1</v>
+      </c>
+      <c r="G444" s="6">
+        <v>1</v>
+      </c>
+      <c r="H444" s="6">
+        <v>1</v>
+      </c>
+      <c r="I444" s="6">
+        <v>1</v>
+      </c>
+      <c r="J444" s="6">
+        <v>1</v>
+      </c>
+      <c r="K444" s="6">
+        <v>0</v>
+      </c>
+      <c r="L444" s="6">
+        <v>0</v>
+      </c>
+      <c r="M444" s="6">
+        <v>0</v>
+      </c>
+      <c r="N444" s="6">
+        <v>0</v>
+      </c>
+      <c r="O444" s="6">
+        <v>0</v>
+      </c>
+      <c r="P444" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="445" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A445" s="5">
+      <c r="A445" s="6">
         <v>63</v>
       </c>
-      <c r="B445" s="5" t="s">
+      <c r="B445" s="6" t="s">
         <v>1101</v>
       </c>
-      <c r="C445" s="5">
+      <c r="C445" s="6">
         <v>302</v>
       </c>
       <c r="D445" s="5" t="s">
-        <v>1166</v>
-      </c>
-      <c r="E445" s="5">
-        <v>1</v>
-      </c>
-      <c r="F445" s="5">
-        <v>1</v>
-      </c>
-      <c r="G445" s="5">
-        <v>1</v>
-      </c>
-      <c r="H445" s="5">
-        <v>1</v>
-      </c>
-      <c r="I445" s="5">
-        <v>1</v>
-      </c>
-      <c r="J445" s="5">
-        <v>1</v>
-      </c>
-      <c r="K445" s="5">
-        <v>0</v>
-      </c>
-      <c r="L445" s="5">
-        <v>0</v>
-      </c>
-      <c r="M445" s="5">
-        <v>0</v>
-      </c>
-      <c r="N445" s="5">
-        <v>0</v>
-      </c>
-      <c r="O445" s="5">
-        <v>0</v>
-      </c>
-      <c r="P445" s="5">
+        <v>1168</v>
+      </c>
+      <c r="E445" s="6">
+        <v>1</v>
+      </c>
+      <c r="F445" s="6">
+        <v>1</v>
+      </c>
+      <c r="G445" s="6">
+        <v>1</v>
+      </c>
+      <c r="H445" s="6">
+        <v>1</v>
+      </c>
+      <c r="I445" s="6">
+        <v>1</v>
+      </c>
+      <c r="J445" s="6">
+        <v>1</v>
+      </c>
+      <c r="K445" s="6">
+        <v>0</v>
+      </c>
+      <c r="L445" s="6">
+        <v>0</v>
+      </c>
+      <c r="M445" s="6">
+        <v>0</v>
+      </c>
+      <c r="N445" s="6">
+        <v>0</v>
+      </c>
+      <c r="O445" s="6">
+        <v>0</v>
+      </c>
+      <c r="P445" s="6">
         <v>0</v>
       </c>
     </row>
@@ -45219,7 +45278,7 @@
   <dimension ref="A1:B304"/>
   <sheetViews>
     <sheetView topLeftCell="A280" workbookViewId="0">
-      <selection activeCell="A304" sqref="A304:B304"/>
+      <selection activeCell="A304" sqref="A304"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -47653,10 +47712,10 @@
       </c>
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A304" s="5">
+      <c r="A304" s="6">
         <v>302</v>
       </c>
-      <c r="B304" s="5" t="s">
+      <c r="B304" s="14" t="s">
         <v>1166</v>
       </c>
     </row>

</xml_diff>

<commit_message>
TFS 25412 - eCL-Update Help dropdown link to report issues
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C52061
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TFS\eCoaching_V2\Design\DD\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{039A6DCB-8011-4D74-97F5-EE4940ADB422}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84CD8302-A8D5-48A4-A491-E6E3A2BC192B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57504" yWindow="1932" windowWidth="28992" windowHeight="15792" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_History" sheetId="14" r:id="rId1"/>
@@ -45,6 +45,7 @@
     <sheet name="ShortCalls_BAL" sheetId="31" r:id="rId30"/>
     <sheet name="Bingo_Images" sheetId="32" r:id="rId31"/>
     <sheet name="Warning_Log_StaticText" sheetId="33" r:id="rId32"/>
+    <sheet name="Coaching_Support_Urls" sheetId="34" r:id="rId33"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">Coaching_Reason_Selection!$A$1:$P$416</definedName>
@@ -56,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4223" uniqueCount="1169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4233" uniqueCount="1174">
   <si>
     <t>SourceID</t>
   </si>
@@ -3613,6 +3614,21 @@
   </si>
   <si>
     <t>Early Work Life (For Use by Early Work Life Staff Only)</t>
+  </si>
+  <si>
+    <t>Update Help dropdown link to report issues. Added tab for new table Coaching_Support_Urls</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Submit Ticket</t>
+  </si>
+  <si>
+    <t>Directs user to Cherwell to submit a ticket through Help menu.</t>
+  </si>
+  <si>
+    <t>https://itservicedesk.maximus.com/CherwellPortal/IT?</t>
   </si>
 </sst>
 </file>
@@ -4047,10 +4063,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L115"/>
+  <dimension ref="A1:L116"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="A115" sqref="A115"/>
+      <selection activeCell="A116" sqref="A116:E116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -5952,7 +5968,7 @@
         <v>1163</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" s="6">
         <v>102.1</v>
       </c>
@@ -5969,7 +5985,7 @@
         <v>1164</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" s="8">
         <v>103</v>
       </c>
@@ -5986,25 +6002,39 @@
         <v>1165</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A115" s="5">
+    <row r="115" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A115" s="8">
         <v>104</v>
       </c>
-      <c r="B115" s="13">
+      <c r="B115" s="9">
         <v>44816</v>
       </c>
-      <c r="C115" s="5" t="s">
+      <c r="C115" s="8" t="s">
         <v>427</v>
       </c>
-      <c r="D115" s="5">
+      <c r="D115" s="8">
         <v>25124</v>
       </c>
-      <c r="E115" s="5" t="s">
+      <c r="E115" s="8" t="s">
         <v>1167</v>
       </c>
-      <c r="F115" s="5"/>
-      <c r="G115" s="5"/>
-      <c r="H115" s="5"/>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A116" s="5">
+        <v>105</v>
+      </c>
+      <c r="B116" s="13">
+        <v>44841</v>
+      </c>
+      <c r="C116" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="D116" s="5">
+        <v>25412</v>
+      </c>
+      <c r="E116" s="5" t="s">
+        <v>1169</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -41229,7 +41259,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -41323,206 +41353,206 @@
       </c>
     </row>
     <row r="6" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6">
+      <c r="A6" s="8">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
+      <c r="C6" s="8">
+        <v>1</v>
+      </c>
+      <c r="D6" s="8">
+        <v>1</v>
+      </c>
+      <c r="E6" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="5">
+      <c r="A7" s="8">
         <v>5</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="5">
-        <v>0</v>
-      </c>
-      <c r="D7" s="5">
-        <v>0</v>
-      </c>
-      <c r="E7" s="5">
+      <c r="C7" s="8">
+        <v>0</v>
+      </c>
+      <c r="D7" s="8">
+        <v>0</v>
+      </c>
+      <c r="E7" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8">
+      <c r="A8" s="8">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
+      <c r="C8" s="8">
+        <v>0</v>
+      </c>
+      <c r="D8" s="8">
+        <v>0</v>
+      </c>
+      <c r="E8" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9">
+      <c r="A9" s="8">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
+      <c r="C9" s="8">
+        <v>1</v>
+      </c>
+      <c r="D9" s="8">
+        <v>1</v>
+      </c>
+      <c r="E9" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10">
+      <c r="A10" s="8">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
+      <c r="C10" s="8">
+        <v>0</v>
+      </c>
+      <c r="D10" s="8">
+        <v>0</v>
+      </c>
+      <c r="E10" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11">
+      <c r="A11" s="8">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11">
+      <c r="C11" s="8">
+        <v>1</v>
+      </c>
+      <c r="D11" s="8">
+        <v>1</v>
+      </c>
+      <c r="E11" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12">
+      <c r="A12" s="8">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12">
+      <c r="C12" s="8">
+        <v>1</v>
+      </c>
+      <c r="D12" s="8">
+        <v>1</v>
+      </c>
+      <c r="E12" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13">
+      <c r="A13" s="8">
         <v>11</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
+      <c r="C13" s="8">
+        <v>0</v>
+      </c>
+      <c r="D13" s="8">
+        <v>0</v>
+      </c>
+      <c r="E13" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14">
+      <c r="A14" s="8">
         <v>12</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14">
+      <c r="C14" s="8">
+        <v>1</v>
+      </c>
+      <c r="D14" s="8">
+        <v>1</v>
+      </c>
+      <c r="E14" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15">
+      <c r="A15" s="8">
         <v>13</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
+      <c r="C15" s="8">
+        <v>0</v>
+      </c>
+      <c r="D15" s="8">
+        <v>0</v>
+      </c>
+      <c r="E15" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16">
+      <c r="A16" s="8">
         <v>14</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16">
+      <c r="C16" s="8">
+        <v>1</v>
+      </c>
+      <c r="D16" s="8">
+        <v>1</v>
+      </c>
+      <c r="E16" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="5">
+      <c r="A17" s="8">
         <v>15</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="8" t="s">
         <v>1159</v>
       </c>
-      <c r="C17" s="5">
-        <v>1</v>
-      </c>
-      <c r="D17" s="5">
-        <v>1</v>
-      </c>
-      <c r="E17" s="5">
+      <c r="C17" s="8">
+        <v>1</v>
+      </c>
+      <c r="D17" s="8">
+        <v>1</v>
+      </c>
+      <c r="E17" s="8">
         <v>0</v>
       </c>
     </row>
@@ -41544,70 +41574,70 @@
       </c>
     </row>
     <row r="19" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19">
+      <c r="A19" s="8">
         <v>17</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
+      <c r="C19" s="8">
+        <v>0</v>
+      </c>
+      <c r="D19" s="8">
+        <v>0</v>
+      </c>
+      <c r="E19" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20">
+      <c r="A20" s="8">
         <v>18</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20">
+      <c r="C20" s="8">
+        <v>1</v>
+      </c>
+      <c r="D20" s="8">
+        <v>1</v>
+      </c>
+      <c r="E20" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21">
+      <c r="A21" s="8">
         <v>19</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="5">
+      <c r="C21" s="8">
+        <v>0</v>
+      </c>
+      <c r="D21" s="8">
+        <v>0</v>
+      </c>
+      <c r="E21" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="8">
         <v>20</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="8" t="s">
         <v>1160</v>
       </c>
-      <c r="C22" s="5">
-        <v>1</v>
-      </c>
-      <c r="D22" s="5">
-        <v>1</v>
-      </c>
-      <c r="E22" s="5">
+      <c r="C22" s="8">
+        <v>1</v>
+      </c>
+      <c r="D22" s="8">
+        <v>1</v>
+      </c>
+      <c r="E22" s="8">
         <v>0</v>
       </c>
     </row>
@@ -43827,7 +43857,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:D21"/>
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -44264,6 +44294,62 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1689E84-D0B7-41B8-A9A0-552D90EE4E14}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="2.3671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.3125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.1015625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.68359375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C1" t="s">
+        <v>500</v>
+      </c>
+      <c r="D1" t="s">
+        <v>708</v>
+      </c>
+      <c r="E1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>1171</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>1172</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>1173</v>
+      </c>
+      <c r="E2" s="5">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
TFS 25626 - Removal of Winchester from eCoaching log
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C52158
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TFS\eCoaching_V2\Design\DD\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84CD8302-A8D5-48A4-A491-E6E3A2BC192B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E22A16C2-1256-4362-A4FB-6FA3D03E4D7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4233" uniqueCount="1174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4235" uniqueCount="1175">
   <si>
     <t>SourceID</t>
   </si>
@@ -3629,6 +3629,9 @@
   </si>
   <si>
     <t>https://itservicedesk.maximus.com/CherwellPortal/IT?</t>
+  </si>
+  <si>
+    <t>Set Winchester to Inactive in DIM_Site and Survey_Sites tabs</t>
   </si>
 </sst>
 </file>
@@ -3724,7 +3727,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4063,10 +4066,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L116"/>
+  <dimension ref="A1:L117"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="A116" sqref="A116:E116"/>
+      <selection activeCell="A117" sqref="A117:E117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -6019,21 +6022,38 @@
         <v>1167</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A116" s="5">
+    <row r="116" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A116" s="8">
         <v>105</v>
       </c>
-      <c r="B116" s="13">
+      <c r="B116" s="9">
         <v>44841</v>
       </c>
-      <c r="C116" s="5" t="s">
+      <c r="C116" s="8" t="s">
         <v>427</v>
       </c>
-      <c r="D116" s="5">
+      <c r="D116" s="8">
         <v>25412</v>
       </c>
-      <c r="E116" s="5" t="s">
+      <c r="E116" s="8" t="s">
         <v>1169</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A117" s="5">
+        <v>106</v>
+      </c>
+      <c r="B117" s="13">
+        <v>44860</v>
+      </c>
+      <c r="C117" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="D117" s="5">
+        <v>25626</v>
+      </c>
+      <c r="E117" s="5" t="s">
+        <v>1174</v>
       </c>
     </row>
   </sheetData>
@@ -6046,8 +6066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -6663,7 +6683,7 @@
       <c r="D27">
         <v>1</v>
       </c>
-      <c r="E27" s="5">
+      <c r="E27" s="8">
         <v>1</v>
       </c>
       <c r="F27">
@@ -7441,7 +7461,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -7541,8 +7563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:P445"/>
   <sheetViews>
-    <sheetView topLeftCell="A411" workbookViewId="0">
-      <selection activeCell="D430" sqref="D430:D445"/>
+    <sheetView topLeftCell="A420" workbookViewId="0">
+      <selection activeCell="A446" sqref="A446"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -29011,7 +29033,7 @@
       <c r="C430" s="6">
         <v>302</v>
       </c>
-      <c r="D430" s="5" t="s">
+      <c r="D430" s="8" t="s">
         <v>1168</v>
       </c>
       <c r="E430" s="6">
@@ -29061,7 +29083,7 @@
       <c r="C431" s="6">
         <v>302</v>
       </c>
-      <c r="D431" s="5" t="s">
+      <c r="D431" s="8" t="s">
         <v>1168</v>
       </c>
       <c r="E431" s="6">
@@ -29111,7 +29133,7 @@
       <c r="C432" s="6">
         <v>302</v>
       </c>
-      <c r="D432" s="5" t="s">
+      <c r="D432" s="8" t="s">
         <v>1168</v>
       </c>
       <c r="E432" s="6">
@@ -29161,7 +29183,7 @@
       <c r="C433" s="6">
         <v>302</v>
       </c>
-      <c r="D433" s="5" t="s">
+      <c r="D433" s="8" t="s">
         <v>1168</v>
       </c>
       <c r="E433" s="6">
@@ -29211,7 +29233,7 @@
       <c r="C434" s="6">
         <v>302</v>
       </c>
-      <c r="D434" s="5" t="s">
+      <c r="D434" s="8" t="s">
         <v>1168</v>
       </c>
       <c r="E434" s="6">
@@ -29261,7 +29283,7 @@
       <c r="C435" s="6">
         <v>302</v>
       </c>
-      <c r="D435" s="5" t="s">
+      <c r="D435" s="8" t="s">
         <v>1168</v>
       </c>
       <c r="E435" s="6">
@@ -29311,7 +29333,7 @@
       <c r="C436" s="6">
         <v>302</v>
       </c>
-      <c r="D436" s="5" t="s">
+      <c r="D436" s="8" t="s">
         <v>1168</v>
       </c>
       <c r="E436" s="6">
@@ -29361,7 +29383,7 @@
       <c r="C437" s="6">
         <v>302</v>
       </c>
-      <c r="D437" s="5" t="s">
+      <c r="D437" s="8" t="s">
         <v>1168</v>
       </c>
       <c r="E437" s="6">
@@ -29411,7 +29433,7 @@
       <c r="C438" s="6">
         <v>302</v>
       </c>
-      <c r="D438" s="5" t="s">
+      <c r="D438" s="8" t="s">
         <v>1168</v>
       </c>
       <c r="E438" s="6">
@@ -29461,7 +29483,7 @@
       <c r="C439" s="6">
         <v>302</v>
       </c>
-      <c r="D439" s="5" t="s">
+      <c r="D439" s="8" t="s">
         <v>1168</v>
       </c>
       <c r="E439" s="6">
@@ -29511,7 +29533,7 @@
       <c r="C440" s="6">
         <v>302</v>
       </c>
-      <c r="D440" s="5" t="s">
+      <c r="D440" s="8" t="s">
         <v>1168</v>
       </c>
       <c r="E440" s="6">
@@ -29561,7 +29583,7 @@
       <c r="C441" s="6">
         <v>302</v>
       </c>
-      <c r="D441" s="5" t="s">
+      <c r="D441" s="8" t="s">
         <v>1168</v>
       </c>
       <c r="E441" s="6">
@@ -29611,7 +29633,7 @@
       <c r="C442" s="6">
         <v>302</v>
       </c>
-      <c r="D442" s="5" t="s">
+      <c r="D442" s="8" t="s">
         <v>1168</v>
       </c>
       <c r="E442" s="6">
@@ -29661,7 +29683,7 @@
       <c r="C443" s="6">
         <v>302</v>
       </c>
-      <c r="D443" s="5" t="s">
+      <c r="D443" s="8" t="s">
         <v>1168</v>
       </c>
       <c r="E443" s="6">
@@ -29711,7 +29733,7 @@
       <c r="C444" s="6">
         <v>302</v>
       </c>
-      <c r="D444" s="5" t="s">
+      <c r="D444" s="8" t="s">
         <v>1168</v>
       </c>
       <c r="E444" s="6">
@@ -29761,7 +29783,7 @@
       <c r="C445" s="6">
         <v>302</v>
       </c>
-      <c r="D445" s="5" t="s">
+      <c r="D445" s="8" t="s">
         <v>1168</v>
       </c>
       <c r="E445" s="6">
@@ -29811,7 +29833,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
@@ -29939,7 +29963,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:K183"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A175" workbookViewId="0">
+      <selection activeCell="A184" sqref="A184"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -36292,31 +36318,31 @@
       </c>
     </row>
     <row r="182" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A182" s="5" t="s">
+      <c r="A182" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="B182" s="5" t="s">
+      <c r="B182" s="8" t="s">
         <v>374</v>
       </c>
-      <c r="C182" s="5" t="s">
+      <c r="C182" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D182" s="5" t="s">
+      <c r="D182" s="8" t="s">
         <v>966</v>
       </c>
-      <c r="E182" s="5">
-        <v>0</v>
-      </c>
-      <c r="F182" s="5" t="s">
+      <c r="E182" s="8">
+        <v>0</v>
+      </c>
+      <c r="F182" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="G182" s="5" t="s">
+      <c r="G182" s="8" t="s">
         <v>420</v>
       </c>
-      <c r="H182" s="5" t="s">
+      <c r="H182" s="8" t="s">
         <v>379</v>
       </c>
-      <c r="I182" s="5" t="s">
+      <c r="I182" s="8" t="s">
         <v>1105</v>
       </c>
       <c r="J182" s="5">
@@ -36327,31 +36353,31 @@
       </c>
     </row>
     <row r="183" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A183" s="5" t="s">
+      <c r="A183" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="B183" s="5" t="s">
+      <c r="B183" s="8" t="s">
         <v>374</v>
       </c>
-      <c r="C183" s="5" t="s">
+      <c r="C183" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D183" s="5" t="s">
+      <c r="D183" s="8" t="s">
         <v>966</v>
       </c>
-      <c r="E183" s="5">
-        <v>0</v>
-      </c>
-      <c r="F183" s="5" t="s">
+      <c r="E183" s="8">
+        <v>0</v>
+      </c>
+      <c r="F183" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="G183" s="5" t="s">
+      <c r="G183" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="H183" s="5" t="s">
+      <c r="H183" s="8" t="s">
         <v>386</v>
       </c>
-      <c r="I183" s="5" t="s">
+      <c r="I183" s="8" t="s">
         <v>418</v>
       </c>
       <c r="J183" s="5">
@@ -36815,7 +36841,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
@@ -36860,7 +36888,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -36947,7 +36977,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -37232,7 +37262,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -37617,7 +37647,7 @@
   <dimension ref="A1:I79"/>
   <sheetViews>
     <sheetView topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="A79" sqref="A78:I79"/>
+      <selection activeCell="A80" sqref="A80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -39928,7 +39958,7 @@
   <dimension ref="A1:M32"/>
   <sheetViews>
     <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:M32"/>
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -41259,7 +41289,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="A20" sqref="A20:E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -41591,19 +41621,19 @@
       </c>
     </row>
     <row r="20" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="8">
+      <c r="A20" s="5">
         <v>18</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C20" s="8">
-        <v>1</v>
-      </c>
-      <c r="D20" s="8">
-        <v>1</v>
-      </c>
-      <c r="E20" s="8">
+      <c r="C20" s="5">
+        <v>0</v>
+      </c>
+      <c r="D20" s="5">
+        <v>0</v>
+      </c>
+      <c r="E20" s="5">
         <v>0</v>
       </c>
     </row>
@@ -41650,7 +41680,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -41925,7 +41957,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -41991,7 +42025,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:C5"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -42132,7 +42166,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -42340,7 +42376,7 @@
   <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -42383,25 +42419,25 @@
       <c r="I1" s="6" t="s">
         <v>1033</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="8" t="s">
         <v>1120</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="8" t="s">
         <v>1121</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="8" t="s">
         <v>1122</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="8" t="s">
         <v>1123</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="8" t="s">
         <v>1124</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="O1" s="8" t="s">
         <v>1125</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="P1" s="8" t="s">
         <v>1126</v>
       </c>
     </row>
@@ -42433,25 +42469,25 @@
       <c r="I2" s="6">
         <v>1</v>
       </c>
-      <c r="J2" s="5">
-        <v>1</v>
-      </c>
-      <c r="K2" s="5">
-        <v>0</v>
-      </c>
-      <c r="L2" s="5">
-        <v>1</v>
-      </c>
-      <c r="M2" s="5">
-        <v>0</v>
-      </c>
-      <c r="N2" s="5">
-        <v>0</v>
-      </c>
-      <c r="O2" s="5">
-        <v>0</v>
-      </c>
-      <c r="P2" s="5">
+      <c r="J2" s="8">
+        <v>1</v>
+      </c>
+      <c r="K2" s="8">
+        <v>0</v>
+      </c>
+      <c r="L2" s="8">
+        <v>1</v>
+      </c>
+      <c r="M2" s="8">
+        <v>0</v>
+      </c>
+      <c r="N2" s="8">
+        <v>0</v>
+      </c>
+      <c r="O2" s="8">
+        <v>0</v>
+      </c>
+      <c r="P2" s="8">
         <v>0</v>
       </c>
     </row>
@@ -42483,25 +42519,25 @@
       <c r="I3" s="6">
         <v>1</v>
       </c>
-      <c r="J3" s="5">
-        <v>1</v>
-      </c>
-      <c r="K3" s="5">
-        <v>1</v>
-      </c>
-      <c r="L3" s="5">
-        <v>1</v>
-      </c>
-      <c r="M3" s="5">
-        <v>0</v>
-      </c>
-      <c r="N3" s="5">
-        <v>0</v>
-      </c>
-      <c r="O3" s="5">
-        <v>0</v>
-      </c>
-      <c r="P3" s="5">
+      <c r="J3" s="8">
+        <v>1</v>
+      </c>
+      <c r="K3" s="8">
+        <v>1</v>
+      </c>
+      <c r="L3" s="8">
+        <v>1</v>
+      </c>
+      <c r="M3" s="8">
+        <v>0</v>
+      </c>
+      <c r="N3" s="8">
+        <v>0</v>
+      </c>
+      <c r="O3" s="8">
+        <v>0</v>
+      </c>
+      <c r="P3" s="8">
         <v>0</v>
       </c>
     </row>
@@ -42533,25 +42569,25 @@
       <c r="I4" s="6">
         <v>0</v>
       </c>
-      <c r="J4" s="5">
-        <v>1</v>
-      </c>
-      <c r="K4" s="5">
-        <v>1</v>
-      </c>
-      <c r="L4" s="5">
-        <v>1</v>
-      </c>
-      <c r="M4" s="5">
-        <v>1</v>
-      </c>
-      <c r="N4" s="5">
-        <v>1</v>
-      </c>
-      <c r="O4" s="5">
-        <v>1</v>
-      </c>
-      <c r="P4" s="5">
+      <c r="J4" s="8">
+        <v>1</v>
+      </c>
+      <c r="K4" s="8">
+        <v>1</v>
+      </c>
+      <c r="L4" s="8">
+        <v>1</v>
+      </c>
+      <c r="M4" s="8">
+        <v>1</v>
+      </c>
+      <c r="N4" s="8">
+        <v>1</v>
+      </c>
+      <c r="O4" s="8">
+        <v>1</v>
+      </c>
+      <c r="P4" s="8">
         <v>1</v>
       </c>
     </row>
@@ -42583,25 +42619,25 @@
       <c r="I5" s="6">
         <v>0</v>
       </c>
-      <c r="J5" s="5">
-        <v>0</v>
-      </c>
-      <c r="K5" s="5">
-        <v>1</v>
-      </c>
-      <c r="L5" s="5">
-        <v>0</v>
-      </c>
-      <c r="M5" s="5">
-        <v>0</v>
-      </c>
-      <c r="N5" s="5">
-        <v>0</v>
-      </c>
-      <c r="O5" s="5">
-        <v>1</v>
-      </c>
-      <c r="P5" s="5">
+      <c r="J5" s="8">
+        <v>0</v>
+      </c>
+      <c r="K5" s="8">
+        <v>1</v>
+      </c>
+      <c r="L5" s="8">
+        <v>0</v>
+      </c>
+      <c r="M5" s="8">
+        <v>0</v>
+      </c>
+      <c r="N5" s="8">
+        <v>0</v>
+      </c>
+      <c r="O5" s="8">
+        <v>1</v>
+      </c>
+      <c r="P5" s="8">
         <v>1</v>
       </c>
     </row>
@@ -42633,25 +42669,25 @@
       <c r="I6" s="6">
         <v>0</v>
       </c>
-      <c r="J6" s="5">
-        <v>0</v>
-      </c>
-      <c r="K6" s="5">
-        <v>0</v>
-      </c>
-      <c r="L6" s="5">
-        <v>0</v>
-      </c>
-      <c r="M6" s="5">
-        <v>0</v>
-      </c>
-      <c r="N6" s="5">
-        <v>0</v>
-      </c>
-      <c r="O6" s="5">
-        <v>0</v>
-      </c>
-      <c r="P6" s="5">
+      <c r="J6" s="8">
+        <v>0</v>
+      </c>
+      <c r="K6" s="8">
+        <v>0</v>
+      </c>
+      <c r="L6" s="8">
+        <v>0</v>
+      </c>
+      <c r="M6" s="8">
+        <v>0</v>
+      </c>
+      <c r="N6" s="8">
+        <v>0</v>
+      </c>
+      <c r="O6" s="8">
+        <v>0</v>
+      </c>
+      <c r="P6" s="8">
         <v>0</v>
       </c>
     </row>
@@ -42683,25 +42719,25 @@
       <c r="I7" s="6">
         <v>0</v>
       </c>
-      <c r="J7" s="5">
-        <v>1</v>
-      </c>
-      <c r="K7" s="5">
-        <v>1</v>
-      </c>
-      <c r="L7" s="5">
-        <v>1</v>
-      </c>
-      <c r="M7" s="5">
-        <v>0</v>
-      </c>
-      <c r="N7" s="5">
-        <v>0</v>
-      </c>
-      <c r="O7" s="5">
-        <v>0</v>
-      </c>
-      <c r="P7" s="5">
+      <c r="J7" s="8">
+        <v>1</v>
+      </c>
+      <c r="K7" s="8">
+        <v>1</v>
+      </c>
+      <c r="L7" s="8">
+        <v>1</v>
+      </c>
+      <c r="M7" s="8">
+        <v>0</v>
+      </c>
+      <c r="N7" s="8">
+        <v>0</v>
+      </c>
+      <c r="O7" s="8">
+        <v>0</v>
+      </c>
+      <c r="P7" s="8">
         <v>0</v>
       </c>
     </row>
@@ -42733,25 +42769,25 @@
       <c r="I8" s="6">
         <v>0</v>
       </c>
-      <c r="J8" s="5">
-        <v>0</v>
-      </c>
-      <c r="K8" s="5">
-        <v>0</v>
-      </c>
-      <c r="L8" s="5">
-        <v>0</v>
-      </c>
-      <c r="M8" s="5">
-        <v>0</v>
-      </c>
-      <c r="N8" s="5">
-        <v>0</v>
-      </c>
-      <c r="O8" s="5">
-        <v>0</v>
-      </c>
-      <c r="P8" s="5">
+      <c r="J8" s="8">
+        <v>0</v>
+      </c>
+      <c r="K8" s="8">
+        <v>0</v>
+      </c>
+      <c r="L8" s="8">
+        <v>0</v>
+      </c>
+      <c r="M8" s="8">
+        <v>0</v>
+      </c>
+      <c r="N8" s="8">
+        <v>0</v>
+      </c>
+      <c r="O8" s="8">
+        <v>0</v>
+      </c>
+      <c r="P8" s="8">
         <v>0</v>
       </c>
     </row>
@@ -42783,25 +42819,25 @@
       <c r="I9" s="6">
         <v>0</v>
       </c>
-      <c r="J9" s="5">
-        <v>0</v>
-      </c>
-      <c r="K9" s="5">
-        <v>0</v>
-      </c>
-      <c r="L9" s="5">
-        <v>0</v>
-      </c>
-      <c r="M9" s="5">
-        <v>0</v>
-      </c>
-      <c r="N9" s="5">
-        <v>0</v>
-      </c>
-      <c r="O9" s="5">
-        <v>0</v>
-      </c>
-      <c r="P9" s="5">
+      <c r="J9" s="8">
+        <v>0</v>
+      </c>
+      <c r="K9" s="8">
+        <v>0</v>
+      </c>
+      <c r="L9" s="8">
+        <v>0</v>
+      </c>
+      <c r="M9" s="8">
+        <v>0</v>
+      </c>
+      <c r="N9" s="8">
+        <v>0</v>
+      </c>
+      <c r="O9" s="8">
+        <v>0</v>
+      </c>
+      <c r="P9" s="8">
         <v>0</v>
       </c>
     </row>
@@ -42833,25 +42869,25 @@
       <c r="I10" s="6">
         <v>0</v>
       </c>
-      <c r="J10" s="5">
-        <v>0</v>
-      </c>
-      <c r="K10" s="5">
-        <v>1</v>
-      </c>
-      <c r="L10" s="5">
-        <v>0</v>
-      </c>
-      <c r="M10" s="5">
-        <v>0</v>
-      </c>
-      <c r="N10" s="5">
-        <v>0</v>
-      </c>
-      <c r="O10" s="5">
-        <v>0</v>
-      </c>
-      <c r="P10" s="5">
+      <c r="J10" s="8">
+        <v>0</v>
+      </c>
+      <c r="K10" s="8">
+        <v>1</v>
+      </c>
+      <c r="L10" s="8">
+        <v>0</v>
+      </c>
+      <c r="M10" s="8">
+        <v>0</v>
+      </c>
+      <c r="N10" s="8">
+        <v>0</v>
+      </c>
+      <c r="O10" s="8">
+        <v>0</v>
+      </c>
+      <c r="P10" s="8">
         <v>0</v>
       </c>
     </row>
@@ -42864,7 +42900,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -43081,7 +43119,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -43264,7 +43302,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -43367,7 +43405,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:B15"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -43506,7 +43544,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -43857,7 +43895,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -44170,7 +44208,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -44302,7 +44342,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -44332,19 +44372,19 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="5">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5" t="s">
+      <c r="A2" s="8">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>1171</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="8" t="s">
         <v>1172</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="8" t="s">
         <v>1173</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="8">
         <v>1</v>
       </c>
     </row>
@@ -44358,7 +44398,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -44472,19 +44512,19 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="5">
+      <c r="A7" s="8">
         <v>5</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="8">
         <v>0</v>
       </c>
     </row>
@@ -44642,19 +44682,19 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="5">
+      <c r="A17" s="8">
         <v>15</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="8" t="s">
         <v>1159</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="8" t="s">
         <v>1161</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="8">
         <v>1</v>
       </c>
     </row>
@@ -44693,20 +44733,20 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20">
+      <c r="A20" s="5">
         <v>18</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="E20" s="6">
-        <v>1</v>
+      <c r="E20" s="5">
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -44727,19 +44767,19 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="5">
+      <c r="A22" s="8">
         <v>20</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="8" t="s">
         <v>1160</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="8" t="s">
         <v>1162</v>
       </c>
-      <c r="E22" s="5">
+      <c r="E22" s="8">
         <v>1</v>
       </c>
     </row>
@@ -44753,7 +44793,7 @@
   <dimension ref="A1:B74"/>
   <sheetViews>
     <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67:B74"/>
+      <selection activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -45364,7 +45404,7 @@
   <dimension ref="A1:B304"/>
   <sheetViews>
     <sheetView topLeftCell="A280" workbookViewId="0">
-      <selection activeCell="A304" sqref="A304"/>
+      <selection activeCell="A305" sqref="A305"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -48361,7 +48401,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
@@ -48594,7 +48636,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>

</xml_diff>

<commit_message>
TFS 26411 - New coaching reason for Claims View (Medicare Only)
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C52678
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TFS\eCoaching_V2\Design\DD\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E22A16C2-1256-4362-A4FB-6FA3D03E4D7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D693DFFF-EE05-4ED6-8F11-24AF8FE64E46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57504" yWindow="1932" windowWidth="28992" windowHeight="15792" firstSheet="3" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_History" sheetId="14" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4235" uniqueCount="1175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4273" uniqueCount="1188">
   <si>
     <t>SourceID</t>
   </si>
@@ -3632,6 +3632,45 @@
   </si>
   <si>
     <t>Set Winchester to Inactive in DIM_Site and Survey_Sites tabs</t>
+  </si>
+  <si>
+    <t>New coaching reason for Claims View (Medicare Only).Added row(s) to DIM_Coaching_Reason, DIM_Sub_Coaching_Reason and Coaching_Reason_Selection</t>
+  </si>
+  <si>
+    <t>Claims View (Medicare Only)</t>
+  </si>
+  <si>
+    <t>Old View</t>
+  </si>
+  <si>
+    <t>Claim Header</t>
+  </si>
+  <si>
+    <t>Claim Summary</t>
+  </si>
+  <si>
+    <t>Crossover</t>
+  </si>
+  <si>
+    <t>Patient Responsibility</t>
+  </si>
+  <si>
+    <t>Preventive Service Pop-Up</t>
+  </si>
+  <si>
+    <t>Benefit Period Pop-Up</t>
+  </si>
+  <si>
+    <t>Check Research</t>
+  </si>
+  <si>
+    <t>Provider Information</t>
+  </si>
+  <si>
+    <t>Undeliverable Address indicator</t>
+  </si>
+  <si>
+    <t>Claim Status</t>
   </si>
 </sst>
 </file>
@@ -4066,10 +4105,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L117"/>
+  <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="A117" sqref="A117:E117"/>
+    <sheetView topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="A118" sqref="A118:XFD118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -6039,21 +6078,38 @@
         <v>1169</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A117" s="5">
+    <row r="117" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A117" s="8">
         <v>106</v>
       </c>
-      <c r="B117" s="13">
+      <c r="B117" s="9">
         <v>44860</v>
       </c>
-      <c r="C117" s="5" t="s">
+      <c r="C117" s="8" t="s">
         <v>427</v>
       </c>
-      <c r="D117" s="5">
+      <c r="D117" s="8">
         <v>25626</v>
       </c>
-      <c r="E117" s="5" t="s">
+      <c r="E117" s="8" t="s">
         <v>1174</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A118" s="5">
+        <v>107</v>
+      </c>
+      <c r="B118" s="13">
+        <v>45019</v>
+      </c>
+      <c r="C118" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="D118" s="5">
+        <v>26411</v>
+      </c>
+      <c r="E118" s="5" t="s">
+        <v>1175</v>
       </c>
     </row>
   </sheetData>
@@ -7561,10 +7617,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:P445"/>
+  <dimension ref="A1:P457"/>
   <sheetViews>
-    <sheetView topLeftCell="A420" workbookViewId="0">
-      <selection activeCell="A446" sqref="A446"/>
+    <sheetView tabSelected="1" topLeftCell="A429" workbookViewId="0">
+      <selection activeCell="A446" sqref="A446:P457"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -29820,6 +29876,606 @@
         <v>0</v>
       </c>
       <c r="P445" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="446" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A446" s="5">
+        <v>73</v>
+      </c>
+      <c r="B446" s="5" t="s">
+        <v>1176</v>
+      </c>
+      <c r="C446" s="5">
+        <v>303</v>
+      </c>
+      <c r="D446" s="5" t="s">
+        <v>1177</v>
+      </c>
+      <c r="E446" s="5">
+        <v>1</v>
+      </c>
+      <c r="F446" s="5">
+        <v>1</v>
+      </c>
+      <c r="G446" s="5">
+        <v>1</v>
+      </c>
+      <c r="H446" s="5">
+        <v>1</v>
+      </c>
+      <c r="I446" s="5">
+        <v>1</v>
+      </c>
+      <c r="J446" s="5">
+        <v>1</v>
+      </c>
+      <c r="K446" s="5">
+        <v>0</v>
+      </c>
+      <c r="L446" s="5">
+        <v>0</v>
+      </c>
+      <c r="M446" s="5">
+        <v>0</v>
+      </c>
+      <c r="N446" s="5">
+        <v>0</v>
+      </c>
+      <c r="O446" s="5">
+        <v>0</v>
+      </c>
+      <c r="P446" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="447" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A447" s="5">
+        <v>73</v>
+      </c>
+      <c r="B447" s="5" t="s">
+        <v>1176</v>
+      </c>
+      <c r="C447" s="5">
+        <v>304</v>
+      </c>
+      <c r="D447" s="5" t="s">
+        <v>1178</v>
+      </c>
+      <c r="E447" s="5">
+        <v>1</v>
+      </c>
+      <c r="F447" s="5">
+        <v>1</v>
+      </c>
+      <c r="G447" s="5">
+        <v>1</v>
+      </c>
+      <c r="H447" s="5">
+        <v>1</v>
+      </c>
+      <c r="I447" s="5">
+        <v>1</v>
+      </c>
+      <c r="J447" s="5">
+        <v>1</v>
+      </c>
+      <c r="K447" s="5">
+        <v>0</v>
+      </c>
+      <c r="L447" s="5">
+        <v>0</v>
+      </c>
+      <c r="M447" s="5">
+        <v>0</v>
+      </c>
+      <c r="N447" s="5">
+        <v>0</v>
+      </c>
+      <c r="O447" s="5">
+        <v>0</v>
+      </c>
+      <c r="P447" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="448" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A448" s="5">
+        <v>73</v>
+      </c>
+      <c r="B448" s="5" t="s">
+        <v>1176</v>
+      </c>
+      <c r="C448" s="5">
+        <v>305</v>
+      </c>
+      <c r="D448" s="5" t="s">
+        <v>1179</v>
+      </c>
+      <c r="E448" s="5">
+        <v>1</v>
+      </c>
+      <c r="F448" s="5">
+        <v>1</v>
+      </c>
+      <c r="G448" s="5">
+        <v>1</v>
+      </c>
+      <c r="H448" s="5">
+        <v>1</v>
+      </c>
+      <c r="I448" s="5">
+        <v>1</v>
+      </c>
+      <c r="J448" s="5">
+        <v>1</v>
+      </c>
+      <c r="K448" s="5">
+        <v>0</v>
+      </c>
+      <c r="L448" s="5">
+        <v>0</v>
+      </c>
+      <c r="M448" s="5">
+        <v>0</v>
+      </c>
+      <c r="N448" s="5">
+        <v>0</v>
+      </c>
+      <c r="O448" s="5">
+        <v>0</v>
+      </c>
+      <c r="P448" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="449" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A449" s="5">
+        <v>73</v>
+      </c>
+      <c r="B449" s="5" t="s">
+        <v>1176</v>
+      </c>
+      <c r="C449" s="5">
+        <v>306</v>
+      </c>
+      <c r="D449" s="5" t="s">
+        <v>1180</v>
+      </c>
+      <c r="E449" s="5">
+        <v>1</v>
+      </c>
+      <c r="F449" s="5">
+        <v>1</v>
+      </c>
+      <c r="G449" s="5">
+        <v>1</v>
+      </c>
+      <c r="H449" s="5">
+        <v>1</v>
+      </c>
+      <c r="I449" s="5">
+        <v>1</v>
+      </c>
+      <c r="J449" s="5">
+        <v>1</v>
+      </c>
+      <c r="K449" s="5">
+        <v>0</v>
+      </c>
+      <c r="L449" s="5">
+        <v>0</v>
+      </c>
+      <c r="M449" s="5">
+        <v>0</v>
+      </c>
+      <c r="N449" s="5">
+        <v>0</v>
+      </c>
+      <c r="O449" s="5">
+        <v>0</v>
+      </c>
+      <c r="P449" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="450" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A450" s="5">
+        <v>73</v>
+      </c>
+      <c r="B450" s="5" t="s">
+        <v>1176</v>
+      </c>
+      <c r="C450" s="5">
+        <v>307</v>
+      </c>
+      <c r="D450" s="5" t="s">
+        <v>1181</v>
+      </c>
+      <c r="E450" s="5">
+        <v>1</v>
+      </c>
+      <c r="F450" s="5">
+        <v>1</v>
+      </c>
+      <c r="G450" s="5">
+        <v>1</v>
+      </c>
+      <c r="H450" s="5">
+        <v>1</v>
+      </c>
+      <c r="I450" s="5">
+        <v>1</v>
+      </c>
+      <c r="J450" s="5">
+        <v>1</v>
+      </c>
+      <c r="K450" s="5">
+        <v>0</v>
+      </c>
+      <c r="L450" s="5">
+        <v>0</v>
+      </c>
+      <c r="M450" s="5">
+        <v>0</v>
+      </c>
+      <c r="N450" s="5">
+        <v>0</v>
+      </c>
+      <c r="O450" s="5">
+        <v>0</v>
+      </c>
+      <c r="P450" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="451" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A451" s="5">
+        <v>73</v>
+      </c>
+      <c r="B451" s="5" t="s">
+        <v>1176</v>
+      </c>
+      <c r="C451" s="5">
+        <v>308</v>
+      </c>
+      <c r="D451" s="5" t="s">
+        <v>1182</v>
+      </c>
+      <c r="E451" s="5">
+        <v>1</v>
+      </c>
+      <c r="F451" s="5">
+        <v>1</v>
+      </c>
+      <c r="G451" s="5">
+        <v>1</v>
+      </c>
+      <c r="H451" s="5">
+        <v>1</v>
+      </c>
+      <c r="I451" s="5">
+        <v>1</v>
+      </c>
+      <c r="J451" s="5">
+        <v>1</v>
+      </c>
+      <c r="K451" s="5">
+        <v>0</v>
+      </c>
+      <c r="L451" s="5">
+        <v>0</v>
+      </c>
+      <c r="M451" s="5">
+        <v>0</v>
+      </c>
+      <c r="N451" s="5">
+        <v>0</v>
+      </c>
+      <c r="O451" s="5">
+        <v>0</v>
+      </c>
+      <c r="P451" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="452" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A452" s="5">
+        <v>73</v>
+      </c>
+      <c r="B452" s="5" t="s">
+        <v>1176</v>
+      </c>
+      <c r="C452" s="5">
+        <v>309</v>
+      </c>
+      <c r="D452" s="5" t="s">
+        <v>1183</v>
+      </c>
+      <c r="E452" s="5">
+        <v>1</v>
+      </c>
+      <c r="F452" s="5">
+        <v>1</v>
+      </c>
+      <c r="G452" s="5">
+        <v>1</v>
+      </c>
+      <c r="H452" s="5">
+        <v>1</v>
+      </c>
+      <c r="I452" s="5">
+        <v>1</v>
+      </c>
+      <c r="J452" s="5">
+        <v>1</v>
+      </c>
+      <c r="K452" s="5">
+        <v>0</v>
+      </c>
+      <c r="L452" s="5">
+        <v>0</v>
+      </c>
+      <c r="M452" s="5">
+        <v>0</v>
+      </c>
+      <c r="N452" s="5">
+        <v>0</v>
+      </c>
+      <c r="O452" s="5">
+        <v>0</v>
+      </c>
+      <c r="P452" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="453" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A453" s="5">
+        <v>73</v>
+      </c>
+      <c r="B453" s="5" t="s">
+        <v>1176</v>
+      </c>
+      <c r="C453" s="5">
+        <v>310</v>
+      </c>
+      <c r="D453" s="5" t="s">
+        <v>1184</v>
+      </c>
+      <c r="E453" s="5">
+        <v>1</v>
+      </c>
+      <c r="F453" s="5">
+        <v>1</v>
+      </c>
+      <c r="G453" s="5">
+        <v>1</v>
+      </c>
+      <c r="H453" s="5">
+        <v>1</v>
+      </c>
+      <c r="I453" s="5">
+        <v>1</v>
+      </c>
+      <c r="J453" s="5">
+        <v>1</v>
+      </c>
+      <c r="K453" s="5">
+        <v>0</v>
+      </c>
+      <c r="L453" s="5">
+        <v>0</v>
+      </c>
+      <c r="M453" s="5">
+        <v>0</v>
+      </c>
+      <c r="N453" s="5">
+        <v>0</v>
+      </c>
+      <c r="O453" s="5">
+        <v>0</v>
+      </c>
+      <c r="P453" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="454" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A454" s="5">
+        <v>73</v>
+      </c>
+      <c r="B454" s="5" t="s">
+        <v>1176</v>
+      </c>
+      <c r="C454" s="5">
+        <v>311</v>
+      </c>
+      <c r="D454" s="5" t="s">
+        <v>1185</v>
+      </c>
+      <c r="E454" s="5">
+        <v>1</v>
+      </c>
+      <c r="F454" s="5">
+        <v>1</v>
+      </c>
+      <c r="G454" s="5">
+        <v>1</v>
+      </c>
+      <c r="H454" s="5">
+        <v>1</v>
+      </c>
+      <c r="I454" s="5">
+        <v>1</v>
+      </c>
+      <c r="J454" s="5">
+        <v>1</v>
+      </c>
+      <c r="K454" s="5">
+        <v>0</v>
+      </c>
+      <c r="L454" s="5">
+        <v>0</v>
+      </c>
+      <c r="M454" s="5">
+        <v>0</v>
+      </c>
+      <c r="N454" s="5">
+        <v>0</v>
+      </c>
+      <c r="O454" s="5">
+        <v>0</v>
+      </c>
+      <c r="P454" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="455" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A455" s="5">
+        <v>73</v>
+      </c>
+      <c r="B455" s="5" t="s">
+        <v>1176</v>
+      </c>
+      <c r="C455" s="5">
+        <v>312</v>
+      </c>
+      <c r="D455" s="5" t="s">
+        <v>1186</v>
+      </c>
+      <c r="E455" s="5">
+        <v>1</v>
+      </c>
+      <c r="F455" s="5">
+        <v>1</v>
+      </c>
+      <c r="G455" s="5">
+        <v>1</v>
+      </c>
+      <c r="H455" s="5">
+        <v>1</v>
+      </c>
+      <c r="I455" s="5">
+        <v>1</v>
+      </c>
+      <c r="J455" s="5">
+        <v>1</v>
+      </c>
+      <c r="K455" s="5">
+        <v>0</v>
+      </c>
+      <c r="L455" s="5">
+        <v>0</v>
+      </c>
+      <c r="M455" s="5">
+        <v>0</v>
+      </c>
+      <c r="N455" s="5">
+        <v>0</v>
+      </c>
+      <c r="O455" s="5">
+        <v>0</v>
+      </c>
+      <c r="P455" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="456" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A456" s="5">
+        <v>73</v>
+      </c>
+      <c r="B456" s="5" t="s">
+        <v>1176</v>
+      </c>
+      <c r="C456" s="5">
+        <v>313</v>
+      </c>
+      <c r="D456" s="5" t="s">
+        <v>1187</v>
+      </c>
+      <c r="E456" s="5">
+        <v>1</v>
+      </c>
+      <c r="F456" s="5">
+        <v>1</v>
+      </c>
+      <c r="G456" s="5">
+        <v>1</v>
+      </c>
+      <c r="H456" s="5">
+        <v>1</v>
+      </c>
+      <c r="I456" s="5">
+        <v>1</v>
+      </c>
+      <c r="J456" s="5">
+        <v>1</v>
+      </c>
+      <c r="K456" s="5">
+        <v>0</v>
+      </c>
+      <c r="L456" s="5">
+        <v>0</v>
+      </c>
+      <c r="M456" s="5">
+        <v>0</v>
+      </c>
+      <c r="N456" s="5">
+        <v>0</v>
+      </c>
+      <c r="O456" s="5">
+        <v>0</v>
+      </c>
+      <c r="P456" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="457" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A457" s="5">
+        <v>73</v>
+      </c>
+      <c r="B457" s="5" t="s">
+        <v>1176</v>
+      </c>
+      <c r="C457" s="5">
+        <v>42</v>
+      </c>
+      <c r="D457" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="E457" s="5">
+        <v>1</v>
+      </c>
+      <c r="F457" s="5">
+        <v>1</v>
+      </c>
+      <c r="G457" s="5">
+        <v>1</v>
+      </c>
+      <c r="H457" s="5">
+        <v>1</v>
+      </c>
+      <c r="I457" s="5">
+        <v>1</v>
+      </c>
+      <c r="J457" s="5">
+        <v>1</v>
+      </c>
+      <c r="K457" s="5">
+        <v>0</v>
+      </c>
+      <c r="L457" s="5">
+        <v>0</v>
+      </c>
+      <c r="M457" s="5">
+        <v>0</v>
+      </c>
+      <c r="N457" s="5">
+        <v>0</v>
+      </c>
+      <c r="O457" s="5">
+        <v>0</v>
+      </c>
+      <c r="P457" s="5">
         <v>0</v>
       </c>
     </row>
@@ -41621,19 +42277,19 @@
       </c>
     </row>
     <row r="20" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="5">
+      <c r="A20" s="8">
         <v>18</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="C20" s="5">
-        <v>0</v>
-      </c>
-      <c r="D20" s="5">
-        <v>0</v>
-      </c>
-      <c r="E20" s="5">
+      <c r="C20" s="8">
+        <v>0</v>
+      </c>
+      <c r="D20" s="8">
+        <v>0</v>
+      </c>
+      <c r="E20" s="8">
         <v>0</v>
       </c>
     </row>
@@ -44398,7 +45054,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A20" sqref="A20:E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -44733,19 +45389,19 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="5">
+      <c r="A20" s="8">
         <v>18</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20" s="8">
         <v>0</v>
       </c>
     </row>
@@ -44790,10 +45446,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:B74"/>
+  <dimension ref="A1:B75"/>
   <sheetViews>
     <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A75" sqref="A75"/>
+      <selection activeCell="A75" sqref="A75:B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -45394,6 +46050,14 @@
         <v>1136</v>
       </c>
     </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A75" s="5">
+        <v>73</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>1176</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -45401,10 +46065,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:B304"/>
+  <dimension ref="A1:B315"/>
   <sheetViews>
-    <sheetView topLeftCell="A280" workbookViewId="0">
-      <selection activeCell="A305" sqref="A305"/>
+    <sheetView topLeftCell="A292" workbookViewId="0">
+      <selection activeCell="A305" sqref="A305:B315"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -47843,6 +48507,94 @@
       </c>
       <c r="B304" s="14" t="s">
         <v>1166</v>
+      </c>
+    </row>
+    <row r="305" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A305" s="5">
+        <v>303</v>
+      </c>
+      <c r="B305" s="5" t="s">
+        <v>1177</v>
+      </c>
+    </row>
+    <row r="306" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A306" s="5">
+        <v>304</v>
+      </c>
+      <c r="B306" s="5" t="s">
+        <v>1178</v>
+      </c>
+    </row>
+    <row r="307" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A307" s="5">
+        <v>305</v>
+      </c>
+      <c r="B307" s="5" t="s">
+        <v>1179</v>
+      </c>
+    </row>
+    <row r="308" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A308" s="5">
+        <v>306</v>
+      </c>
+      <c r="B308" s="5" t="s">
+        <v>1180</v>
+      </c>
+    </row>
+    <row r="309" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A309" s="5">
+        <v>307</v>
+      </c>
+      <c r="B309" s="5" t="s">
+        <v>1181</v>
+      </c>
+    </row>
+    <row r="310" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A310" s="5">
+        <v>308</v>
+      </c>
+      <c r="B310" s="5" t="s">
+        <v>1182</v>
+      </c>
+    </row>
+    <row r="311" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A311" s="5">
+        <v>309</v>
+      </c>
+      <c r="B311" s="5" t="s">
+        <v>1183</v>
+      </c>
+    </row>
+    <row r="312" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A312" s="5">
+        <v>310</v>
+      </c>
+      <c r="B312" s="5" t="s">
+        <v>1184</v>
+      </c>
+    </row>
+    <row r="313" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A313" s="5">
+        <v>311</v>
+      </c>
+      <c r="B313" s="5" t="s">
+        <v>1185</v>
+      </c>
+    </row>
+    <row r="314" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A314" s="5">
+        <v>312</v>
+      </c>
+      <c r="B314" s="5" t="s">
+        <v>1186</v>
+      </c>
+    </row>
+    <row r="315" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A315" s="5">
+        <v>313</v>
+      </c>
+      <c r="B315" s="5" t="s">
+        <v>1187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TFS 26432 - Audio issues in the eCoaching Log
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C52682
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TFS\eCoaching_V2\Design\DD\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D693DFFF-EE05-4ED6-8F11-24AF8FE64E46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E71A68D-9631-492F-B97F-9AA0CE9BEC4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57504" yWindow="1932" windowWidth="28992" windowHeight="15792" firstSheet="3" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57504" yWindow="1932" windowWidth="28992" windowHeight="15792" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_History" sheetId="14" r:id="rId1"/>
@@ -46,6 +46,8 @@
     <sheet name="Bingo_Images" sheetId="32" r:id="rId31"/>
     <sheet name="Warning_Log_StaticText" sheetId="33" r:id="rId32"/>
     <sheet name="Coaching_Support_Urls" sheetId="34" r:id="rId33"/>
+    <sheet name="Coaching_Log_Static_Text" sheetId="36" r:id="rId34"/>
+    <sheet name="Sheet1" sheetId="35" r:id="rId35"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">Coaching_Reason_Selection!$A$1:$P$416</definedName>
@@ -57,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4273" uniqueCount="1188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4289" uniqueCount="1191">
   <si>
     <t>SourceID</t>
   </si>
@@ -3671,6 +3673,15 @@
   </si>
   <si>
     <t>Claim Status</t>
+  </si>
+  <si>
+    <t>OMR: Speech Analytics Audio Issues</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Please work with your employee to determine if there are any issues that need to be resolved.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Audio issues in the eCoaching Log. Added new record in DIM_Sub_Coaching_Reason tab and add new tab for Coaching_Log_Static_Text</t>
   </si>
 </sst>
 </file>
@@ -4105,10 +4116,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L118"/>
+  <dimension ref="A1:L119"/>
   <sheetViews>
-    <sheetView topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="A118" sqref="A118:XFD118"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="A119" sqref="A119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -6095,21 +6106,38 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="118" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A118" s="5">
+    <row r="118" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A118" s="8">
         <v>107</v>
       </c>
-      <c r="B118" s="13">
+      <c r="B118" s="9">
         <v>45019</v>
       </c>
-      <c r="C118" s="5" t="s">
+      <c r="C118" s="8" t="s">
         <v>427</v>
       </c>
-      <c r="D118" s="5">
+      <c r="D118" s="8">
         <v>26411</v>
       </c>
-      <c r="E118" s="5" t="s">
+      <c r="E118" s="8" t="s">
         <v>1175</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A119" s="5">
+        <v>108</v>
+      </c>
+      <c r="B119" s="13">
+        <v>45029</v>
+      </c>
+      <c r="C119" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="D119" s="5">
+        <v>26432</v>
+      </c>
+      <c r="E119" s="5" t="s">
+        <v>1190</v>
       </c>
     </row>
   </sheetData>
@@ -7619,8 +7647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:P457"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A429" workbookViewId="0">
-      <selection activeCell="A446" sqref="A446:P457"/>
+    <sheetView topLeftCell="A429" workbookViewId="0">
+      <selection activeCell="A446" sqref="A446:XFD457"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -29879,603 +29907,603 @@
         <v>0</v>
       </c>
     </row>
-    <row r="446" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A446" s="5">
+    <row r="446" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A446" s="8">
         <v>73</v>
       </c>
-      <c r="B446" s="5" t="s">
+      <c r="B446" s="8" t="s">
         <v>1176</v>
       </c>
-      <c r="C446" s="5">
+      <c r="C446" s="8">
         <v>303</v>
       </c>
-      <c r="D446" s="5" t="s">
+      <c r="D446" s="8" t="s">
         <v>1177</v>
       </c>
-      <c r="E446" s="5">
-        <v>1</v>
-      </c>
-      <c r="F446" s="5">
-        <v>1</v>
-      </c>
-      <c r="G446" s="5">
-        <v>1</v>
-      </c>
-      <c r="H446" s="5">
-        <v>1</v>
-      </c>
-      <c r="I446" s="5">
-        <v>1</v>
-      </c>
-      <c r="J446" s="5">
-        <v>1</v>
-      </c>
-      <c r="K446" s="5">
-        <v>0</v>
-      </c>
-      <c r="L446" s="5">
-        <v>0</v>
-      </c>
-      <c r="M446" s="5">
-        <v>0</v>
-      </c>
-      <c r="N446" s="5">
-        <v>0</v>
-      </c>
-      <c r="O446" s="5">
-        <v>0</v>
-      </c>
-      <c r="P446" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="447" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A447" s="5">
+      <c r="E446" s="8">
+        <v>1</v>
+      </c>
+      <c r="F446" s="8">
+        <v>1</v>
+      </c>
+      <c r="G446" s="8">
+        <v>1</v>
+      </c>
+      <c r="H446" s="8">
+        <v>1</v>
+      </c>
+      <c r="I446" s="8">
+        <v>1</v>
+      </c>
+      <c r="J446" s="8">
+        <v>1</v>
+      </c>
+      <c r="K446" s="8">
+        <v>0</v>
+      </c>
+      <c r="L446" s="8">
+        <v>0</v>
+      </c>
+      <c r="M446" s="8">
+        <v>0</v>
+      </c>
+      <c r="N446" s="8">
+        <v>0</v>
+      </c>
+      <c r="O446" s="8">
+        <v>0</v>
+      </c>
+      <c r="P446" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="447" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A447" s="8">
         <v>73</v>
       </c>
-      <c r="B447" s="5" t="s">
+      <c r="B447" s="8" t="s">
         <v>1176</v>
       </c>
-      <c r="C447" s="5">
+      <c r="C447" s="8">
         <v>304</v>
       </c>
-      <c r="D447" s="5" t="s">
+      <c r="D447" s="8" t="s">
         <v>1178</v>
       </c>
-      <c r="E447" s="5">
-        <v>1</v>
-      </c>
-      <c r="F447" s="5">
-        <v>1</v>
-      </c>
-      <c r="G447" s="5">
-        <v>1</v>
-      </c>
-      <c r="H447" s="5">
-        <v>1</v>
-      </c>
-      <c r="I447" s="5">
-        <v>1</v>
-      </c>
-      <c r="J447" s="5">
-        <v>1</v>
-      </c>
-      <c r="K447" s="5">
-        <v>0</v>
-      </c>
-      <c r="L447" s="5">
-        <v>0</v>
-      </c>
-      <c r="M447" s="5">
-        <v>0</v>
-      </c>
-      <c r="N447" s="5">
-        <v>0</v>
-      </c>
-      <c r="O447" s="5">
-        <v>0</v>
-      </c>
-      <c r="P447" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="448" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A448" s="5">
+      <c r="E447" s="8">
+        <v>1</v>
+      </c>
+      <c r="F447" s="8">
+        <v>1</v>
+      </c>
+      <c r="G447" s="8">
+        <v>1</v>
+      </c>
+      <c r="H447" s="8">
+        <v>1</v>
+      </c>
+      <c r="I447" s="8">
+        <v>1</v>
+      </c>
+      <c r="J447" s="8">
+        <v>1</v>
+      </c>
+      <c r="K447" s="8">
+        <v>0</v>
+      </c>
+      <c r="L447" s="8">
+        <v>0</v>
+      </c>
+      <c r="M447" s="8">
+        <v>0</v>
+      </c>
+      <c r="N447" s="8">
+        <v>0</v>
+      </c>
+      <c r="O447" s="8">
+        <v>0</v>
+      </c>
+      <c r="P447" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="448" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A448" s="8">
         <v>73</v>
       </c>
-      <c r="B448" s="5" t="s">
+      <c r="B448" s="8" t="s">
         <v>1176</v>
       </c>
-      <c r="C448" s="5">
+      <c r="C448" s="8">
         <v>305</v>
       </c>
-      <c r="D448" s="5" t="s">
+      <c r="D448" s="8" t="s">
         <v>1179</v>
       </c>
-      <c r="E448" s="5">
-        <v>1</v>
-      </c>
-      <c r="F448" s="5">
-        <v>1</v>
-      </c>
-      <c r="G448" s="5">
-        <v>1</v>
-      </c>
-      <c r="H448" s="5">
-        <v>1</v>
-      </c>
-      <c r="I448" s="5">
-        <v>1</v>
-      </c>
-      <c r="J448" s="5">
-        <v>1</v>
-      </c>
-      <c r="K448" s="5">
-        <v>0</v>
-      </c>
-      <c r="L448" s="5">
-        <v>0</v>
-      </c>
-      <c r="M448" s="5">
-        <v>0</v>
-      </c>
-      <c r="N448" s="5">
-        <v>0</v>
-      </c>
-      <c r="O448" s="5">
-        <v>0</v>
-      </c>
-      <c r="P448" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="449" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A449" s="5">
+      <c r="E448" s="8">
+        <v>1</v>
+      </c>
+      <c r="F448" s="8">
+        <v>1</v>
+      </c>
+      <c r="G448" s="8">
+        <v>1</v>
+      </c>
+      <c r="H448" s="8">
+        <v>1</v>
+      </c>
+      <c r="I448" s="8">
+        <v>1</v>
+      </c>
+      <c r="J448" s="8">
+        <v>1</v>
+      </c>
+      <c r="K448" s="8">
+        <v>0</v>
+      </c>
+      <c r="L448" s="8">
+        <v>0</v>
+      </c>
+      <c r="M448" s="8">
+        <v>0</v>
+      </c>
+      <c r="N448" s="8">
+        <v>0</v>
+      </c>
+      <c r="O448" s="8">
+        <v>0</v>
+      </c>
+      <c r="P448" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="449" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A449" s="8">
         <v>73</v>
       </c>
-      <c r="B449" s="5" t="s">
+      <c r="B449" s="8" t="s">
         <v>1176</v>
       </c>
-      <c r="C449" s="5">
+      <c r="C449" s="8">
         <v>306</v>
       </c>
-      <c r="D449" s="5" t="s">
+      <c r="D449" s="8" t="s">
         <v>1180</v>
       </c>
-      <c r="E449" s="5">
-        <v>1</v>
-      </c>
-      <c r="F449" s="5">
-        <v>1</v>
-      </c>
-      <c r="G449" s="5">
-        <v>1</v>
-      </c>
-      <c r="H449" s="5">
-        <v>1</v>
-      </c>
-      <c r="I449" s="5">
-        <v>1</v>
-      </c>
-      <c r="J449" s="5">
-        <v>1</v>
-      </c>
-      <c r="K449" s="5">
-        <v>0</v>
-      </c>
-      <c r="L449" s="5">
-        <v>0</v>
-      </c>
-      <c r="M449" s="5">
-        <v>0</v>
-      </c>
-      <c r="N449" s="5">
-        <v>0</v>
-      </c>
-      <c r="O449" s="5">
-        <v>0</v>
-      </c>
-      <c r="P449" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="450" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A450" s="5">
+      <c r="E449" s="8">
+        <v>1</v>
+      </c>
+      <c r="F449" s="8">
+        <v>1</v>
+      </c>
+      <c r="G449" s="8">
+        <v>1</v>
+      </c>
+      <c r="H449" s="8">
+        <v>1</v>
+      </c>
+      <c r="I449" s="8">
+        <v>1</v>
+      </c>
+      <c r="J449" s="8">
+        <v>1</v>
+      </c>
+      <c r="K449" s="8">
+        <v>0</v>
+      </c>
+      <c r="L449" s="8">
+        <v>0</v>
+      </c>
+      <c r="M449" s="8">
+        <v>0</v>
+      </c>
+      <c r="N449" s="8">
+        <v>0</v>
+      </c>
+      <c r="O449" s="8">
+        <v>0</v>
+      </c>
+      <c r="P449" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="450" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A450" s="8">
         <v>73</v>
       </c>
-      <c r="B450" s="5" t="s">
+      <c r="B450" s="8" t="s">
         <v>1176</v>
       </c>
-      <c r="C450" s="5">
+      <c r="C450" s="8">
         <v>307</v>
       </c>
-      <c r="D450" s="5" t="s">
+      <c r="D450" s="8" t="s">
         <v>1181</v>
       </c>
-      <c r="E450" s="5">
-        <v>1</v>
-      </c>
-      <c r="F450" s="5">
-        <v>1</v>
-      </c>
-      <c r="G450" s="5">
-        <v>1</v>
-      </c>
-      <c r="H450" s="5">
-        <v>1</v>
-      </c>
-      <c r="I450" s="5">
-        <v>1</v>
-      </c>
-      <c r="J450" s="5">
-        <v>1</v>
-      </c>
-      <c r="K450" s="5">
-        <v>0</v>
-      </c>
-      <c r="L450" s="5">
-        <v>0</v>
-      </c>
-      <c r="M450" s="5">
-        <v>0</v>
-      </c>
-      <c r="N450" s="5">
-        <v>0</v>
-      </c>
-      <c r="O450" s="5">
-        <v>0</v>
-      </c>
-      <c r="P450" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="451" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A451" s="5">
+      <c r="E450" s="8">
+        <v>1</v>
+      </c>
+      <c r="F450" s="8">
+        <v>1</v>
+      </c>
+      <c r="G450" s="8">
+        <v>1</v>
+      </c>
+      <c r="H450" s="8">
+        <v>1</v>
+      </c>
+      <c r="I450" s="8">
+        <v>1</v>
+      </c>
+      <c r="J450" s="8">
+        <v>1</v>
+      </c>
+      <c r="K450" s="8">
+        <v>0</v>
+      </c>
+      <c r="L450" s="8">
+        <v>0</v>
+      </c>
+      <c r="M450" s="8">
+        <v>0</v>
+      </c>
+      <c r="N450" s="8">
+        <v>0</v>
+      </c>
+      <c r="O450" s="8">
+        <v>0</v>
+      </c>
+      <c r="P450" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="451" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A451" s="8">
         <v>73</v>
       </c>
-      <c r="B451" s="5" t="s">
+      <c r="B451" s="8" t="s">
         <v>1176</v>
       </c>
-      <c r="C451" s="5">
+      <c r="C451" s="8">
         <v>308</v>
       </c>
-      <c r="D451" s="5" t="s">
+      <c r="D451" s="8" t="s">
         <v>1182</v>
       </c>
-      <c r="E451" s="5">
-        <v>1</v>
-      </c>
-      <c r="F451" s="5">
-        <v>1</v>
-      </c>
-      <c r="G451" s="5">
-        <v>1</v>
-      </c>
-      <c r="H451" s="5">
-        <v>1</v>
-      </c>
-      <c r="I451" s="5">
-        <v>1</v>
-      </c>
-      <c r="J451" s="5">
-        <v>1</v>
-      </c>
-      <c r="K451" s="5">
-        <v>0</v>
-      </c>
-      <c r="L451" s="5">
-        <v>0</v>
-      </c>
-      <c r="M451" s="5">
-        <v>0</v>
-      </c>
-      <c r="N451" s="5">
-        <v>0</v>
-      </c>
-      <c r="O451" s="5">
-        <v>0</v>
-      </c>
-      <c r="P451" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="452" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A452" s="5">
+      <c r="E451" s="8">
+        <v>1</v>
+      </c>
+      <c r="F451" s="8">
+        <v>1</v>
+      </c>
+      <c r="G451" s="8">
+        <v>1</v>
+      </c>
+      <c r="H451" s="8">
+        <v>1</v>
+      </c>
+      <c r="I451" s="8">
+        <v>1</v>
+      </c>
+      <c r="J451" s="8">
+        <v>1</v>
+      </c>
+      <c r="K451" s="8">
+        <v>0</v>
+      </c>
+      <c r="L451" s="8">
+        <v>0</v>
+      </c>
+      <c r="M451" s="8">
+        <v>0</v>
+      </c>
+      <c r="N451" s="8">
+        <v>0</v>
+      </c>
+      <c r="O451" s="8">
+        <v>0</v>
+      </c>
+      <c r="P451" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="452" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A452" s="8">
         <v>73</v>
       </c>
-      <c r="B452" s="5" t="s">
+      <c r="B452" s="8" t="s">
         <v>1176</v>
       </c>
-      <c r="C452" s="5">
+      <c r="C452" s="8">
         <v>309</v>
       </c>
-      <c r="D452" s="5" t="s">
+      <c r="D452" s="8" t="s">
         <v>1183</v>
       </c>
-      <c r="E452" s="5">
-        <v>1</v>
-      </c>
-      <c r="F452" s="5">
-        <v>1</v>
-      </c>
-      <c r="G452" s="5">
-        <v>1</v>
-      </c>
-      <c r="H452" s="5">
-        <v>1</v>
-      </c>
-      <c r="I452" s="5">
-        <v>1</v>
-      </c>
-      <c r="J452" s="5">
-        <v>1</v>
-      </c>
-      <c r="K452" s="5">
-        <v>0</v>
-      </c>
-      <c r="L452" s="5">
-        <v>0</v>
-      </c>
-      <c r="M452" s="5">
-        <v>0</v>
-      </c>
-      <c r="N452" s="5">
-        <v>0</v>
-      </c>
-      <c r="O452" s="5">
-        <v>0</v>
-      </c>
-      <c r="P452" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="453" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A453" s="5">
+      <c r="E452" s="8">
+        <v>1</v>
+      </c>
+      <c r="F452" s="8">
+        <v>1</v>
+      </c>
+      <c r="G452" s="8">
+        <v>1</v>
+      </c>
+      <c r="H452" s="8">
+        <v>1</v>
+      </c>
+      <c r="I452" s="8">
+        <v>1</v>
+      </c>
+      <c r="J452" s="8">
+        <v>1</v>
+      </c>
+      <c r="K452" s="8">
+        <v>0</v>
+      </c>
+      <c r="L452" s="8">
+        <v>0</v>
+      </c>
+      <c r="M452" s="8">
+        <v>0</v>
+      </c>
+      <c r="N452" s="8">
+        <v>0</v>
+      </c>
+      <c r="O452" s="8">
+        <v>0</v>
+      </c>
+      <c r="P452" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="453" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A453" s="8">
         <v>73</v>
       </c>
-      <c r="B453" s="5" t="s">
+      <c r="B453" s="8" t="s">
         <v>1176</v>
       </c>
-      <c r="C453" s="5">
+      <c r="C453" s="8">
         <v>310</v>
       </c>
-      <c r="D453" s="5" t="s">
+      <c r="D453" s="8" t="s">
         <v>1184</v>
       </c>
-      <c r="E453" s="5">
-        <v>1</v>
-      </c>
-      <c r="F453" s="5">
-        <v>1</v>
-      </c>
-      <c r="G453" s="5">
-        <v>1</v>
-      </c>
-      <c r="H453" s="5">
-        <v>1</v>
-      </c>
-      <c r="I453" s="5">
-        <v>1</v>
-      </c>
-      <c r="J453" s="5">
-        <v>1</v>
-      </c>
-      <c r="K453" s="5">
-        <v>0</v>
-      </c>
-      <c r="L453" s="5">
-        <v>0</v>
-      </c>
-      <c r="M453" s="5">
-        <v>0</v>
-      </c>
-      <c r="N453" s="5">
-        <v>0</v>
-      </c>
-      <c r="O453" s="5">
-        <v>0</v>
-      </c>
-      <c r="P453" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="454" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A454" s="5">
+      <c r="E453" s="8">
+        <v>1</v>
+      </c>
+      <c r="F453" s="8">
+        <v>1</v>
+      </c>
+      <c r="G453" s="8">
+        <v>1</v>
+      </c>
+      <c r="H453" s="8">
+        <v>1</v>
+      </c>
+      <c r="I453" s="8">
+        <v>1</v>
+      </c>
+      <c r="J453" s="8">
+        <v>1</v>
+      </c>
+      <c r="K453" s="8">
+        <v>0</v>
+      </c>
+      <c r="L453" s="8">
+        <v>0</v>
+      </c>
+      <c r="M453" s="8">
+        <v>0</v>
+      </c>
+      <c r="N453" s="8">
+        <v>0</v>
+      </c>
+      <c r="O453" s="8">
+        <v>0</v>
+      </c>
+      <c r="P453" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="454" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A454" s="8">
         <v>73</v>
       </c>
-      <c r="B454" s="5" t="s">
+      <c r="B454" s="8" t="s">
         <v>1176</v>
       </c>
-      <c r="C454" s="5">
+      <c r="C454" s="8">
         <v>311</v>
       </c>
-      <c r="D454" s="5" t="s">
+      <c r="D454" s="8" t="s">
         <v>1185</v>
       </c>
-      <c r="E454" s="5">
-        <v>1</v>
-      </c>
-      <c r="F454" s="5">
-        <v>1</v>
-      </c>
-      <c r="G454" s="5">
-        <v>1</v>
-      </c>
-      <c r="H454" s="5">
-        <v>1</v>
-      </c>
-      <c r="I454" s="5">
-        <v>1</v>
-      </c>
-      <c r="J454" s="5">
-        <v>1</v>
-      </c>
-      <c r="K454" s="5">
-        <v>0</v>
-      </c>
-      <c r="L454" s="5">
-        <v>0</v>
-      </c>
-      <c r="M454" s="5">
-        <v>0</v>
-      </c>
-      <c r="N454" s="5">
-        <v>0</v>
-      </c>
-      <c r="O454" s="5">
-        <v>0</v>
-      </c>
-      <c r="P454" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="455" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A455" s="5">
+      <c r="E454" s="8">
+        <v>1</v>
+      </c>
+      <c r="F454" s="8">
+        <v>1</v>
+      </c>
+      <c r="G454" s="8">
+        <v>1</v>
+      </c>
+      <c r="H454" s="8">
+        <v>1</v>
+      </c>
+      <c r="I454" s="8">
+        <v>1</v>
+      </c>
+      <c r="J454" s="8">
+        <v>1</v>
+      </c>
+      <c r="K454" s="8">
+        <v>0</v>
+      </c>
+      <c r="L454" s="8">
+        <v>0</v>
+      </c>
+      <c r="M454" s="8">
+        <v>0</v>
+      </c>
+      <c r="N454" s="8">
+        <v>0</v>
+      </c>
+      <c r="O454" s="8">
+        <v>0</v>
+      </c>
+      <c r="P454" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="455" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A455" s="8">
         <v>73</v>
       </c>
-      <c r="B455" s="5" t="s">
+      <c r="B455" s="8" t="s">
         <v>1176</v>
       </c>
-      <c r="C455" s="5">
+      <c r="C455" s="8">
         <v>312</v>
       </c>
-      <c r="D455" s="5" t="s">
+      <c r="D455" s="8" t="s">
         <v>1186</v>
       </c>
-      <c r="E455" s="5">
-        <v>1</v>
-      </c>
-      <c r="F455" s="5">
-        <v>1</v>
-      </c>
-      <c r="G455" s="5">
-        <v>1</v>
-      </c>
-      <c r="H455" s="5">
-        <v>1</v>
-      </c>
-      <c r="I455" s="5">
-        <v>1</v>
-      </c>
-      <c r="J455" s="5">
-        <v>1</v>
-      </c>
-      <c r="K455" s="5">
-        <v>0</v>
-      </c>
-      <c r="L455" s="5">
-        <v>0</v>
-      </c>
-      <c r="M455" s="5">
-        <v>0</v>
-      </c>
-      <c r="N455" s="5">
-        <v>0</v>
-      </c>
-      <c r="O455" s="5">
-        <v>0</v>
-      </c>
-      <c r="P455" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="456" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A456" s="5">
+      <c r="E455" s="8">
+        <v>1</v>
+      </c>
+      <c r="F455" s="8">
+        <v>1</v>
+      </c>
+      <c r="G455" s="8">
+        <v>1</v>
+      </c>
+      <c r="H455" s="8">
+        <v>1</v>
+      </c>
+      <c r="I455" s="8">
+        <v>1</v>
+      </c>
+      <c r="J455" s="8">
+        <v>1</v>
+      </c>
+      <c r="K455" s="8">
+        <v>0</v>
+      </c>
+      <c r="L455" s="8">
+        <v>0</v>
+      </c>
+      <c r="M455" s="8">
+        <v>0</v>
+      </c>
+      <c r="N455" s="8">
+        <v>0</v>
+      </c>
+      <c r="O455" s="8">
+        <v>0</v>
+      </c>
+      <c r="P455" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="456" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A456" s="8">
         <v>73</v>
       </c>
-      <c r="B456" s="5" t="s">
+      <c r="B456" s="8" t="s">
         <v>1176</v>
       </c>
-      <c r="C456" s="5">
+      <c r="C456" s="8">
         <v>313</v>
       </c>
-      <c r="D456" s="5" t="s">
+      <c r="D456" s="8" t="s">
         <v>1187</v>
       </c>
-      <c r="E456" s="5">
-        <v>1</v>
-      </c>
-      <c r="F456" s="5">
-        <v>1</v>
-      </c>
-      <c r="G456" s="5">
-        <v>1</v>
-      </c>
-      <c r="H456" s="5">
-        <v>1</v>
-      </c>
-      <c r="I456" s="5">
-        <v>1</v>
-      </c>
-      <c r="J456" s="5">
-        <v>1</v>
-      </c>
-      <c r="K456" s="5">
-        <v>0</v>
-      </c>
-      <c r="L456" s="5">
-        <v>0</v>
-      </c>
-      <c r="M456" s="5">
-        <v>0</v>
-      </c>
-      <c r="N456" s="5">
-        <v>0</v>
-      </c>
-      <c r="O456" s="5">
-        <v>0</v>
-      </c>
-      <c r="P456" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="457" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A457" s="5">
+      <c r="E456" s="8">
+        <v>1</v>
+      </c>
+      <c r="F456" s="8">
+        <v>1</v>
+      </c>
+      <c r="G456" s="8">
+        <v>1</v>
+      </c>
+      <c r="H456" s="8">
+        <v>1</v>
+      </c>
+      <c r="I456" s="8">
+        <v>1</v>
+      </c>
+      <c r="J456" s="8">
+        <v>1</v>
+      </c>
+      <c r="K456" s="8">
+        <v>0</v>
+      </c>
+      <c r="L456" s="8">
+        <v>0</v>
+      </c>
+      <c r="M456" s="8">
+        <v>0</v>
+      </c>
+      <c r="N456" s="8">
+        <v>0</v>
+      </c>
+      <c r="O456" s="8">
+        <v>0</v>
+      </c>
+      <c r="P456" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="457" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A457" s="8">
         <v>73</v>
       </c>
-      <c r="B457" s="5" t="s">
+      <c r="B457" s="8" t="s">
         <v>1176</v>
       </c>
-      <c r="C457" s="5">
+      <c r="C457" s="8">
         <v>42</v>
       </c>
-      <c r="D457" s="5" t="s">
+      <c r="D457" s="8" t="s">
         <v>204</v>
       </c>
-      <c r="E457" s="5">
-        <v>1</v>
-      </c>
-      <c r="F457" s="5">
-        <v>1</v>
-      </c>
-      <c r="G457" s="5">
-        <v>1</v>
-      </c>
-      <c r="H457" s="5">
-        <v>1</v>
-      </c>
-      <c r="I457" s="5">
-        <v>1</v>
-      </c>
-      <c r="J457" s="5">
-        <v>1</v>
-      </c>
-      <c r="K457" s="5">
-        <v>0</v>
-      </c>
-      <c r="L457" s="5">
-        <v>0</v>
-      </c>
-      <c r="M457" s="5">
-        <v>0</v>
-      </c>
-      <c r="N457" s="5">
-        <v>0</v>
-      </c>
-      <c r="O457" s="5">
-        <v>0</v>
-      </c>
-      <c r="P457" s="5">
+      <c r="E457" s="8">
+        <v>1</v>
+      </c>
+      <c r="F457" s="8">
+        <v>1</v>
+      </c>
+      <c r="G457" s="8">
+        <v>1</v>
+      </c>
+      <c r="H457" s="8">
+        <v>1</v>
+      </c>
+      <c r="I457" s="8">
+        <v>1</v>
+      </c>
+      <c r="J457" s="8">
+        <v>1</v>
+      </c>
+      <c r="K457" s="8">
+        <v>0</v>
+      </c>
+      <c r="L457" s="8">
+        <v>0</v>
+      </c>
+      <c r="M457" s="8">
+        <v>0</v>
+      </c>
+      <c r="N457" s="8">
+        <v>0</v>
+      </c>
+      <c r="O457" s="8">
+        <v>0</v>
+      </c>
+      <c r="P457" s="8">
         <v>0</v>
       </c>
     </row>
@@ -45049,6 +45077,109 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE8E5AAB-2CB2-47A7-AC59-8DE4502992B4}">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:L2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1073</v>
+      </c>
+      <c r="C1" t="s">
+        <v>988</v>
+      </c>
+      <c r="D1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F1" t="s">
+        <v>172</v>
+      </c>
+      <c r="G1" t="s">
+        <v>173</v>
+      </c>
+      <c r="H1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I1" t="s">
+        <v>474</v>
+      </c>
+      <c r="J1" t="s">
+        <v>543</v>
+      </c>
+      <c r="K1" t="s">
+        <v>702</v>
+      </c>
+      <c r="L1" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="5">
+        <v>101</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>1189</v>
+      </c>
+      <c r="C2" s="5">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5">
+        <v>9</v>
+      </c>
+      <c r="E2" s="5">
+        <v>314</v>
+      </c>
+      <c r="F2" s="5">
+        <v>1</v>
+      </c>
+      <c r="G2" s="5">
+        <v>0</v>
+      </c>
+      <c r="H2" s="5">
+        <v>0</v>
+      </c>
+      <c r="I2" s="5">
+        <v>0</v>
+      </c>
+      <c r="J2" s="5">
+        <v>0</v>
+      </c>
+      <c r="K2" s="5">
+        <v>20230401</v>
+      </c>
+      <c r="L2" s="5">
+        <v>99991231</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABDF132E-5F02-4682-A8C9-083C5F415CDD}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E22"/>
@@ -46065,10 +46196,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:B315"/>
+  <dimension ref="A1:B316"/>
   <sheetViews>
     <sheetView topLeftCell="A292" workbookViewId="0">
-      <selection activeCell="A305" sqref="A305:B315"/>
+      <selection activeCell="A316" sqref="A316:B316"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -48510,91 +48641,99 @@
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A305" s="5">
+      <c r="A305" s="8">
         <v>303</v>
       </c>
-      <c r="B305" s="5" t="s">
+      <c r="B305" s="8" t="s">
         <v>1177</v>
       </c>
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A306" s="5">
+      <c r="A306" s="8">
         <v>304</v>
       </c>
-      <c r="B306" s="5" t="s">
+      <c r="B306" s="8" t="s">
         <v>1178</v>
       </c>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A307" s="5">
+      <c r="A307" s="8">
         <v>305</v>
       </c>
-      <c r="B307" s="5" t="s">
+      <c r="B307" s="8" t="s">
         <v>1179</v>
       </c>
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A308" s="5">
+      <c r="A308" s="8">
         <v>306</v>
       </c>
-      <c r="B308" s="5" t="s">
+      <c r="B308" s="8" t="s">
         <v>1180</v>
       </c>
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A309" s="5">
+      <c r="A309" s="8">
         <v>307</v>
       </c>
-      <c r="B309" s="5" t="s">
+      <c r="B309" s="8" t="s">
         <v>1181</v>
       </c>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A310" s="5">
+      <c r="A310" s="8">
         <v>308</v>
       </c>
-      <c r="B310" s="5" t="s">
+      <c r="B310" s="8" t="s">
         <v>1182</v>
       </c>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A311" s="5">
+      <c r="A311" s="8">
         <v>309</v>
       </c>
-      <c r="B311" s="5" t="s">
+      <c r="B311" s="8" t="s">
         <v>1183</v>
       </c>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A312" s="5">
+      <c r="A312" s="8">
         <v>310</v>
       </c>
-      <c r="B312" s="5" t="s">
+      <c r="B312" s="8" t="s">
         <v>1184</v>
       </c>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A313" s="5">
+      <c r="A313" s="8">
         <v>311</v>
       </c>
-      <c r="B313" s="5" t="s">
+      <c r="B313" s="8" t="s">
         <v>1185</v>
       </c>
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A314" s="5">
+      <c r="A314" s="8">
         <v>312</v>
       </c>
-      <c r="B314" s="5" t="s">
+      <c r="B314" s="8" t="s">
         <v>1186</v>
       </c>
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A315" s="5">
+      <c r="A315" s="8">
         <v>313</v>
       </c>
-      <c r="B315" s="5" t="s">
+      <c r="B315" s="8" t="s">
         <v>1187</v>
+      </c>
+    </row>
+    <row r="316" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A316" s="5">
+        <v>314</v>
+      </c>
+      <c r="B316" s="5" t="s">
+        <v>1188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TFS 25693  and TFS 25354 – Add El Paso and Remote East to eCoaching log
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C52692
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TFS\eCoaching_V2\Design\DD\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E71A68D-9631-492F-B97F-9AA0CE9BEC4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1E20B73-0467-4619-AB7D-612E5630E140}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57504" yWindow="1932" windowWidth="28992" windowHeight="15792" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4289" uniqueCount="1191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4300" uniqueCount="1198">
   <si>
     <t>SourceID</t>
   </si>
@@ -3682,6 +3682,28 @@
   </si>
   <si>
     <t>Audio issues in the eCoaching Log. Added new record in DIM_Sub_Coaching_Reason tab and add new tab for Coaching_Log_Static_Text</t>
+  </si>
+  <si>
+    <t>25693
+25354</t>
+  </si>
+  <si>
+    <t>Add El Paso and Remote East to eCoaching log. Added rows to DIM_Site and Survey_Sites tabs</t>
+  </si>
+  <si>
+    <t>Remote East</t>
+  </si>
+  <si>
+    <t>El Paso</t>
+  </si>
+  <si>
+    <t>RE</t>
+  </si>
+  <si>
+    <t>RE - Remote East</t>
+  </si>
+  <si>
+    <t>TX - El Paso</t>
   </si>
 </sst>
 </file>
@@ -3758,7 +3780,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -3778,6 +3800,9 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4116,10 +4141,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L119"/>
+  <dimension ref="A1:L120"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="A119" sqref="A119"/>
+      <selection activeCell="A120" sqref="A120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -6123,21 +6148,38 @@
         <v>1175</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A119" s="5">
+    <row r="119" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A119" s="8">
         <v>108</v>
       </c>
-      <c r="B119" s="13">
+      <c r="B119" s="9">
         <v>45029</v>
       </c>
-      <c r="C119" s="5" t="s">
+      <c r="C119" s="8" t="s">
         <v>427</v>
       </c>
-      <c r="D119" s="5">
+      <c r="D119" s="8">
         <v>26432</v>
       </c>
-      <c r="E119" s="5" t="s">
+      <c r="E119" s="8" t="s">
         <v>1190</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A120" s="5">
+        <v>109</v>
+      </c>
+      <c r="B120" s="13">
+        <v>45033</v>
+      </c>
+      <c r="C120" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="D120" s="15" t="s">
+        <v>1191</v>
+      </c>
+      <c r="E120" s="5" t="s">
+        <v>1192</v>
       </c>
     </row>
   </sheetData>
@@ -41970,10 +42012,10 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:E20"/>
+      <selection activeCell="A23" sqref="A23:E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -42352,6 +42394,40 @@
         <v>1</v>
       </c>
       <c r="E22" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="5">
+        <v>21</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>1193</v>
+      </c>
+      <c r="C23" s="5">
+        <v>1</v>
+      </c>
+      <c r="D23" s="5">
+        <v>1</v>
+      </c>
+      <c r="E23" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="5">
+        <v>22</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>1194</v>
+      </c>
+      <c r="C24" s="5">
+        <v>1</v>
+      </c>
+      <c r="D24" s="5">
+        <v>1</v>
+      </c>
+      <c r="E24" s="5">
         <v>0</v>
       </c>
     </row>
@@ -45126,40 +45202,40 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="5">
+      <c r="A2" s="8">
         <v>101</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="8" t="s">
         <v>1189</v>
       </c>
-      <c r="C2" s="5">
-        <v>1</v>
-      </c>
-      <c r="D2" s="5">
+      <c r="C2" s="8">
+        <v>1</v>
+      </c>
+      <c r="D2" s="8">
         <v>9</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="8">
         <v>314</v>
       </c>
-      <c r="F2" s="5">
-        <v>1</v>
-      </c>
-      <c r="G2" s="5">
-        <v>0</v>
-      </c>
-      <c r="H2" s="5">
-        <v>0</v>
-      </c>
-      <c r="I2" s="5">
-        <v>0</v>
-      </c>
-      <c r="J2" s="5">
-        <v>0</v>
-      </c>
-      <c r="K2" s="5">
+      <c r="F2" s="8">
+        <v>1</v>
+      </c>
+      <c r="G2" s="8">
+        <v>0</v>
+      </c>
+      <c r="H2" s="8">
+        <v>0</v>
+      </c>
+      <c r="I2" s="8">
+        <v>0</v>
+      </c>
+      <c r="J2" s="8">
+        <v>0</v>
+      </c>
+      <c r="K2" s="8">
         <v>20230401</v>
       </c>
-      <c r="L2" s="5">
+      <c r="L2" s="8">
         <v>99991231</v>
       </c>
     </row>
@@ -45182,10 +45258,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:E20"/>
+      <selection activeCell="A23" sqref="A23:E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -45567,6 +45643,40 @@
         <v>1162</v>
       </c>
       <c r="E22" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="5">
+        <v>21</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>1193</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>1195</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>1196</v>
+      </c>
+      <c r="E23" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="5">
+        <v>22</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>1194</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>1197</v>
+      </c>
+      <c r="E24" s="5">
         <v>1</v>
       </c>
     </row>
@@ -48729,10 +48839,10 @@
       </c>
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A316" s="5">
+      <c r="A316" s="8">
         <v>314</v>
       </c>
-      <c r="B316" s="5" t="s">
+      <c r="B316" s="8" t="s">
         <v>1188</v>
       </c>
     </row>

</xml_diff>

<commit_message>
TFS 26536 - Adding a link on the Quality Now eCLs to the Quality Now Feedback Form
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C52741
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TFS\eCoaching_V2\Design\DD\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1E20B73-0467-4619-AB7D-612E5630E140}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C272A7B-52BE-4C8C-B975-1FA660E2646C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57504" yWindow="1932" windowWidth="28992" windowHeight="15792" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57504" yWindow="1932" windowWidth="28992" windowHeight="15792" firstSheet="27" activeTab="33" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_History" sheetId="14" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4300" uniqueCount="1198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4303" uniqueCount="1200">
   <si>
     <t>SourceID</t>
   </si>
@@ -3704,6 +3704,12 @@
   </si>
   <si>
     <t>TX - El Paso</t>
+  </si>
+  <si>
+    <t>Adding a link on the Quality Now eCLs to the Quality Now Feedback Form</t>
+  </si>
+  <si>
+    <t>There is no appeal process for Quality Now, but &lt;a href='https://maximus365.sharepoint.com/sites/CCO/Support/QA-OPS/Leads/Lists/Quality_NOW_Feedback/NewForm.aspx?Source=https%3a%2f%2fmaximus365.sharepoint.com%2fsites%2fCCO%2fSupport%2fQA-OPS%2fLeads%2fLists%2fQuality_NOW_Feedback%2fMy_Items.aspx%3fviewid%3d9bec3890%252D53e3%252D40f9%252D8dc6%252Df8400e9a4f4d%26OR%3dTeams%252DHL%26CT%3d1681396370842%26clickparams%3deyJBcHBOYW1lIjoiVGVhbXMtRGVza3RvcCIsIkFwcFZlcnNpb24iOiIyNy8yMzAzMDUwMTExMCIsIkhhc0ZlZGVyYXRlZFVzZXIiOmZhbHNlfQ%253D%253D&amp;ContentTypeId=0x0100E3688E643B7C874CAD85E7C0C4441EFE&amp;RootFolder=%2fsites%2fCCO%2fSupport%2fQA-OPS%2fLeads%2fLists%2fQuality_NOW_Feedback'target='_blank'&gt;feedback&lt;/a&gt; for the Quality Team concerning this batch is welcomed. Please see SOP QA 33.0 for additional guidance.</t>
   </si>
 </sst>
 </file>
@@ -3800,8 +3806,8 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4141,10 +4147,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L120"/>
+  <dimension ref="A1:L121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="A120" sqref="A120"/>
+    <sheetView topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="A121" sqref="A121:E121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -6165,21 +6171,38 @@
         <v>1190</v>
       </c>
     </row>
-    <row r="120" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A120" s="5">
+    <row r="120" spans="1:5" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A120" s="8">
         <v>109</v>
       </c>
-      <c r="B120" s="13">
+      <c r="B120" s="9">
         <v>45033</v>
       </c>
-      <c r="C120" s="5" t="s">
+      <c r="C120" s="8" t="s">
         <v>427</v>
       </c>
       <c r="D120" s="15" t="s">
         <v>1191</v>
       </c>
-      <c r="E120" s="5" t="s">
+      <c r="E120" s="8" t="s">
         <v>1192</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A121" s="5">
+        <v>110</v>
+      </c>
+      <c r="B121" s="13">
+        <v>45050</v>
+      </c>
+      <c r="C121" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="D121" s="5">
+        <v>26536</v>
+      </c>
+      <c r="E121" s="5" t="s">
+        <v>1198</v>
       </c>
     </row>
   </sheetData>
@@ -42398,36 +42421,36 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="5">
+      <c r="A23" s="8">
         <v>21</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="8" t="s">
         <v>1193</v>
       </c>
-      <c r="C23" s="5">
-        <v>1</v>
-      </c>
-      <c r="D23" s="5">
-        <v>1</v>
-      </c>
-      <c r="E23" s="5">
+      <c r="C23" s="8">
+        <v>1</v>
+      </c>
+      <c r="D23" s="8">
+        <v>1</v>
+      </c>
+      <c r="E23" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="5">
+      <c r="A24" s="8">
         <v>22</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="8" t="s">
         <v>1194</v>
       </c>
-      <c r="C24" s="5">
-        <v>1</v>
-      </c>
-      <c r="D24" s="5">
-        <v>1</v>
-      </c>
-      <c r="E24" s="5">
+      <c r="C24" s="8">
+        <v>1</v>
+      </c>
+      <c r="D24" s="8">
+        <v>1</v>
+      </c>
+      <c r="E24" s="8">
         <v>0</v>
       </c>
     </row>
@@ -45155,10 +45178,10 @@
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE8E5AAB-2CB2-47A7-AC59-8DE4502992B4}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:L2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -45236,6 +45259,44 @@
         <v>20230401</v>
       </c>
       <c r="L2" s="8">
+        <v>99991231</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="5">
+        <v>102</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>1199</v>
+      </c>
+      <c r="C3" s="5">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5">
+        <v>57</v>
+      </c>
+      <c r="E3" s="5">
+        <v>42</v>
+      </c>
+      <c r="F3" s="5">
+        <v>1</v>
+      </c>
+      <c r="G3" s="5">
+        <v>0</v>
+      </c>
+      <c r="H3" s="5">
+        <v>0</v>
+      </c>
+      <c r="I3" s="5">
+        <v>0</v>
+      </c>
+      <c r="J3" s="5">
+        <v>0</v>
+      </c>
+      <c r="K3" s="5">
+        <v>20230101</v>
+      </c>
+      <c r="L3" s="5">
         <v>99991231</v>
       </c>
     </row>
@@ -45647,36 +45708,36 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="5">
+      <c r="A23" s="8">
         <v>21</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="8" t="s">
         <v>1193</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="8" t="s">
         <v>1195</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="8" t="s">
         <v>1196</v>
       </c>
-      <c r="E23" s="5">
+      <c r="E23" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="5">
+      <c r="A24" s="8">
         <v>22</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="8" t="s">
         <v>1194</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="8" t="s">
         <v>1197</v>
       </c>
-      <c r="E24" s="5">
+      <c r="E24" s="8">
         <v>1</v>
       </c>
     </row>
@@ -46292,10 +46353,10 @@
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A75" s="5">
+      <c r="A75" s="8">
         <v>73</v>
       </c>
-      <c r="B75" s="5" t="s">
+      <c r="B75" s="8" t="s">
         <v>1176</v>
       </c>
     </row>

</xml_diff>

<commit_message>
TFS 26691 - Removal of Bogalusa from eCoaching log
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C52808
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TFS\eCoaching_V2\Design\DD\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C272A7B-52BE-4C8C-B975-1FA660E2646C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{640D31E1-4F96-4E97-831C-342516FAE053}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57504" yWindow="1932" windowWidth="28992" windowHeight="15792" firstSheet="27" activeTab="33" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57504" yWindow="1932" windowWidth="28992" windowHeight="15792" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_History" sheetId="14" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4303" uniqueCount="1200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4305" uniqueCount="1201">
   <si>
     <t>SourceID</t>
   </si>
@@ -3710,6 +3710,9 @@
   </si>
   <si>
     <t>There is no appeal process for Quality Now, but &lt;a href='https://maximus365.sharepoint.com/sites/CCO/Support/QA-OPS/Leads/Lists/Quality_NOW_Feedback/NewForm.aspx?Source=https%3a%2f%2fmaximus365.sharepoint.com%2fsites%2fCCO%2fSupport%2fQA-OPS%2fLeads%2fLists%2fQuality_NOW_Feedback%2fMy_Items.aspx%3fviewid%3d9bec3890%252D53e3%252D40f9%252D8dc6%252Df8400e9a4f4d%26OR%3dTeams%252DHL%26CT%3d1681396370842%26clickparams%3deyJBcHBOYW1lIjoiVGVhbXMtRGVza3RvcCIsIkFwcFZlcnNpb24iOiIyNy8yMzAzMDUwMTExMCIsIkhhc0ZlZGVyYXRlZFVzZXIiOmZhbHNlfQ%253D%253D&amp;ContentTypeId=0x0100E3688E643B7C874CAD85E7C0C4441EFE&amp;RootFolder=%2fsites%2fCCO%2fSupport%2fQA-OPS%2fLeads%2fLists%2fQuality_NOW_Feedback'target='_blank'&gt;feedback&lt;/a&gt; for the Quality Team concerning this batch is welcomed. Please see SOP QA 33.0 for additional guidance.</t>
+  </si>
+  <si>
+    <t>Set Bogalusa to Inactive in DIM_Site and Survey_Sites tabs</t>
   </si>
 </sst>
 </file>
@@ -4147,10 +4150,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L121"/>
+  <dimension ref="A1:L122"/>
   <sheetViews>
-    <sheetView topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="A121" sqref="A121:E121"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="A122" sqref="A122:E122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -6189,20 +6192,37 @@
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A121" s="5">
+      <c r="A121" s="8">
         <v>110</v>
       </c>
-      <c r="B121" s="13">
+      <c r="B121" s="9">
         <v>45050</v>
       </c>
-      <c r="C121" s="5" t="s">
+      <c r="C121" s="8" t="s">
         <v>427</v>
       </c>
-      <c r="D121" s="5">
+      <c r="D121" s="8">
         <v>26536</v>
       </c>
-      <c r="E121" s="5" t="s">
+      <c r="E121" s="8" t="s">
         <v>1198</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A122" s="5">
+        <v>111</v>
+      </c>
+      <c r="B122" s="13">
+        <v>45083</v>
+      </c>
+      <c r="C122" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="D122" s="5">
+        <v>26691</v>
+      </c>
+      <c r="E122" s="5" t="s">
+        <v>1200</v>
       </c>
     </row>
   </sheetData>
@@ -42038,7 +42058,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:E24"/>
+      <selection activeCell="A3" sqref="A3:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -42081,19 +42101,19 @@
       </c>
     </row>
     <row r="3" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="A3" s="5">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
+      <c r="C3" s="5">
+        <v>0</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0</v>
+      </c>
+      <c r="E3" s="5">
         <v>0</v>
       </c>
     </row>
@@ -45180,7 +45200,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE8E5AAB-2CB2-47A7-AC59-8DE4502992B4}">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:L3"/>
     </sheetView>
   </sheetViews>
@@ -45263,40 +45283,40 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="5">
+      <c r="A3" s="8">
         <v>102</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="8" t="s">
         <v>1199</v>
       </c>
-      <c r="C3" s="5">
-        <v>1</v>
-      </c>
-      <c r="D3" s="5">
+      <c r="C3" s="8">
+        <v>1</v>
+      </c>
+      <c r="D3" s="8">
         <v>57</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="8">
         <v>42</v>
       </c>
-      <c r="F3" s="5">
-        <v>1</v>
-      </c>
-      <c r="G3" s="5">
-        <v>0</v>
-      </c>
-      <c r="H3" s="5">
-        <v>0</v>
-      </c>
-      <c r="I3" s="5">
-        <v>0</v>
-      </c>
-      <c r="J3" s="5">
-        <v>0</v>
-      </c>
-      <c r="K3" s="5">
+      <c r="F3" s="8">
+        <v>1</v>
+      </c>
+      <c r="G3" s="8">
+        <v>0</v>
+      </c>
+      <c r="H3" s="8">
+        <v>0</v>
+      </c>
+      <c r="I3" s="8">
+        <v>0</v>
+      </c>
+      <c r="J3" s="8">
+        <v>0</v>
+      </c>
+      <c r="K3" s="8">
         <v>20230101</v>
       </c>
-      <c r="L3" s="5">
+      <c r="L3" s="8">
         <v>99991231</v>
       </c>
     </row>
@@ -45322,7 +45342,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:E24"/>
+      <selection activeCell="A3" sqref="A3:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -45368,20 +45388,20 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="A3" s="5">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E3">
-        <v>1</v>
+      <c r="E3" s="5">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">

</xml_diff>

<commit_message>
TFS 27396 - NGD login issues in the eCoaching Log
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C53333
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TFS\eCoaching_V2\Design\DD\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{640D31E1-4F96-4E97-831C-342516FAE053}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2F80448-1852-48D9-8B25-54BD26451A93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57504" yWindow="1932" windowWidth="28992" windowHeight="15792" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57504" yWindow="1914" windowWidth="28992" windowHeight="15792" firstSheet="27" activeTab="33" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_History" sheetId="14" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4305" uniqueCount="1201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4309" uniqueCount="1204">
   <si>
     <t>SourceID</t>
   </si>
@@ -3713,6 +3713,15 @@
   </si>
   <si>
     <t>Set Bogalusa to Inactive in DIM_Site and Survey_Sites tabs</t>
+  </si>
+  <si>
+    <t>NGD login issues in the eCoaching Log. Added new record in DIM_Sub_Coaching_Reason tab and add new tab for Coaching_Log_Static_Text.</t>
+  </si>
+  <si>
+    <t>OMR:NGD System Log In</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Your CSR was logged in to NGD for more than 30 minutes outside their scheduled shift.  Please validate and ensure your CSR is fully aware of when they should and should not be logged in to the system, laptop, AWS, and NGD.&lt;/p&gt;</t>
   </si>
 </sst>
 </file>
@@ -3789,7 +3798,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -3807,7 +3816,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -4150,10 +4158,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L122"/>
+  <dimension ref="A1:L123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="A122" sqref="A122:E122"/>
+    <sheetView topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="E123" sqref="E123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -6184,7 +6192,7 @@
       <c r="C120" s="8" t="s">
         <v>427</v>
       </c>
-      <c r="D120" s="15" t="s">
+      <c r="D120" s="14" t="s">
         <v>1191</v>
       </c>
       <c r="E120" s="8" t="s">
@@ -6209,20 +6217,37 @@
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A122" s="5">
+      <c r="A122" s="8">
         <v>111</v>
       </c>
-      <c r="B122" s="13">
+      <c r="B122" s="9">
         <v>45083</v>
       </c>
-      <c r="C122" s="5" t="s">
+      <c r="C122" s="8" t="s">
         <v>427</v>
       </c>
-      <c r="D122" s="5">
+      <c r="D122" s="8">
         <v>26691</v>
       </c>
-      <c r="E122" s="5" t="s">
+      <c r="E122" s="8" t="s">
         <v>1200</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A123" s="8">
+        <v>112</v>
+      </c>
+      <c r="B123" s="1">
+        <v>45254</v>
+      </c>
+      <c r="C123" s="8" t="s">
+        <v>427</v>
+      </c>
+      <c r="D123">
+        <v>27396</v>
+      </c>
+      <c r="E123" t="s">
+        <v>1201</v>
       </c>
     </row>
   </sheetData>
@@ -7733,7 +7758,7 @@
   <dimension ref="A1:P457"/>
   <sheetViews>
     <sheetView topLeftCell="A429" workbookViewId="0">
-      <selection activeCell="A446" sqref="A446:XFD457"/>
+      <selection activeCell="B445" sqref="B445"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -30603,7 +30628,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="O41" sqref="O41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -45198,11 +45223,9 @@
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE8E5AAB-2CB2-47A7-AC59-8DE4502992B4}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:L3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
@@ -45317,6 +45340,44 @@
         <v>20230101</v>
       </c>
       <c r="L3" s="8">
+        <v>99991231</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="5">
+        <v>103</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>1203</v>
+      </c>
+      <c r="C4" s="5">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5">
+        <v>9</v>
+      </c>
+      <c r="E4" s="5">
+        <v>315</v>
+      </c>
+      <c r="F4" s="5">
+        <v>1</v>
+      </c>
+      <c r="G4" s="5">
+        <v>0</v>
+      </c>
+      <c r="H4" s="5">
+        <v>0</v>
+      </c>
+      <c r="I4" s="5">
+        <v>0</v>
+      </c>
+      <c r="J4" s="5">
+        <v>0</v>
+      </c>
+      <c r="K4" s="5">
+        <v>20231101</v>
+      </c>
+      <c r="L4" s="5">
         <v>99991231</v>
       </c>
     </row>
@@ -46387,10 +46448,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:B316"/>
+  <dimension ref="A1:B317"/>
   <sheetViews>
     <sheetView topLeftCell="A292" workbookViewId="0">
-      <selection activeCell="A316" sqref="A316:B316"/>
+      <selection activeCell="A317" sqref="A317:B317"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -48827,7 +48888,7 @@
       <c r="A304" s="6">
         <v>302</v>
       </c>
-      <c r="B304" s="14" t="s">
+      <c r="B304" s="13" t="s">
         <v>1166</v>
       </c>
     </row>
@@ -48925,6 +48986,14 @@
       </c>
       <c r="B316" s="8" t="s">
         <v>1188</v>
+      </c>
+    </row>
+    <row r="317" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A317" s="5">
+        <v>315</v>
+      </c>
+      <c r="B317" s="5" t="s">
+        <v>1202</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TFS 27523 - Dashboard to view the feed load history in the Admin Tool
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C53460
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TFS\eCoaching_V2\Design\DD\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B5AAD5A-88C6-4FCB-8C42-64662CBB9C65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{670A1062-1455-4705-9EA4-4368B124D78C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57504" yWindow="1914" windowWidth="28992" windowHeight="15792" firstSheet="3" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" firstSheet="30" activeTab="35" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_History" sheetId="14" r:id="rId1"/>
@@ -47,7 +47,8 @@
     <sheet name="Warning_Log_StaticText" sheetId="33" r:id="rId32"/>
     <sheet name="Coaching_Support_Urls" sheetId="34" r:id="rId33"/>
     <sheet name="Coaching_Log_Static_Text" sheetId="36" r:id="rId34"/>
-    <sheet name="Sheet1" sheetId="35" r:id="rId35"/>
+    <sheet name="Feed_Contacts" sheetId="35" r:id="rId35"/>
+    <sheet name="DIM_Feed_List" sheetId="37" r:id="rId36"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">Coaching_Reason_Selection!$A$1:$P$457</definedName>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4340" uniqueCount="1214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4517" uniqueCount="1273">
   <si>
     <t>SourceID</t>
   </si>
@@ -3752,6 +3753,183 @@
   </si>
   <si>
     <t>Workspace Audit/Violation</t>
+  </si>
+  <si>
+    <t>Added Tab for DIM_Feed_List Table</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>PrimaryPOC</t>
+  </si>
+  <si>
+    <t>SecondaryPOC</t>
+  </si>
+  <si>
+    <t>SEAA</t>
+  </si>
+  <si>
+    <t>Seasonal Employee Attendance Opportunity</t>
+  </si>
+  <si>
+    <t>Shelly J Encke</t>
+  </si>
+  <si>
+    <t>CCO BSA Team</t>
+  </si>
+  <si>
+    <t>SEAR</t>
+  </si>
+  <si>
+    <t>Seasonal Employee Attendance Re-Inforcement</t>
+  </si>
+  <si>
+    <t>APS</t>
+  </si>
+  <si>
+    <t>Attendance Perfect Shift</t>
+  </si>
+  <si>
+    <t>Lex Mishra</t>
+  </si>
+  <si>
+    <t>DL-CCOENGEASE</t>
+  </si>
+  <si>
+    <t>APW</t>
+  </si>
+  <si>
+    <t>Attendance perfect Weeks</t>
+  </si>
+  <si>
+    <t>AED</t>
+  </si>
+  <si>
+    <t>Outliers</t>
+  </si>
+  <si>
+    <t>BRL</t>
+  </si>
+  <si>
+    <t>James P Allen Johns</t>
+  </si>
+  <si>
+    <t>Analytics Team</t>
+  </si>
+  <si>
+    <t>BRN</t>
+  </si>
+  <si>
+    <t>IAE</t>
+  </si>
+  <si>
+    <t>IAEF</t>
+  </si>
+  <si>
+    <t>Inappropriate ARC Escalation FFM</t>
+  </si>
+  <si>
+    <t>ISQ</t>
+  </si>
+  <si>
+    <t>Inappropriate Short Calls</t>
+  </si>
+  <si>
+    <t>Eric Losby</t>
+  </si>
+  <si>
+    <t>LCS</t>
+  </si>
+  <si>
+    <t>Jennifer G Foster</t>
+  </si>
+  <si>
+    <t>Sue Rager</t>
+  </si>
+  <si>
+    <t>WCP</t>
+  </si>
+  <si>
+    <t>Written Correspondence Process</t>
+  </si>
+  <si>
+    <t>Barbara Kitchen-Powell, Kevin Burchette</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quality </t>
+  </si>
+  <si>
+    <t>IQS_QN</t>
+  </si>
+  <si>
+    <t>Dave Hinman</t>
+  </si>
+  <si>
+    <t>Leslie Keune</t>
+  </si>
+  <si>
+    <t>Quality Other</t>
+  </si>
+  <si>
+    <t>KUD</t>
+  </si>
+  <si>
+    <t>HFC</t>
+  </si>
+  <si>
+    <t>High Five CSAT</t>
+  </si>
+  <si>
+    <t>BQN</t>
+  </si>
+  <si>
+    <t>QN Bingo CSR</t>
+  </si>
+  <si>
+    <t>BQNS</t>
+  </si>
+  <si>
+    <t>QM Bingo Supervisor</t>
+  </si>
+  <si>
+    <t>Employee Info</t>
+  </si>
+  <si>
+    <t>Employee File From IQS</t>
+  </si>
+  <si>
+    <t>Employee File From Aspect</t>
+  </si>
+  <si>
+    <t>Aspect WFM Support</t>
+  </si>
+  <si>
+    <t>NGDS</t>
+  </si>
+  <si>
+    <t>NGDS System Log In Outside Shift</t>
+  </si>
+  <si>
+    <t>AUD</t>
+  </si>
+  <si>
+    <t>Audio Issues Feed</t>
+  </si>
+  <si>
+    <t>Sara M Stonecipher</t>
+  </si>
+  <si>
+    <t>SUR</t>
+  </si>
+  <si>
+    <t>CSR Survey Coaching Initiative</t>
+  </si>
+  <si>
+    <t>CategoryID</t>
+  </si>
+  <si>
+    <t>ReportID</t>
   </si>
 </sst>
 </file>
@@ -3828,7 +4006,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -3850,7 +4028,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4189,10 +4366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L124"/>
+  <dimension ref="A1:L125"/>
   <sheetViews>
-    <sheetView topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="E124" sqref="E124"/>
+    <sheetView topLeftCell="C100" workbookViewId="0">
+      <selection activeCell="E125" sqref="E125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -6282,20 +6459,37 @@
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A124" s="5">
+      <c r="A124" s="6">
         <v>113</v>
       </c>
-      <c r="B124" s="15">
+      <c r="B124" s="10">
         <v>45260</v>
       </c>
-      <c r="C124" s="5" t="s">
+      <c r="C124" s="6" t="s">
         <v>427</v>
       </c>
-      <c r="D124" s="5">
+      <c r="D124" s="6">
         <v>27375</v>
       </c>
-      <c r="E124" s="5" t="s">
+      <c r="E124" s="6" t="s">
         <v>1202</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A125" s="8">
+        <v>114</v>
+      </c>
+      <c r="B125" s="1">
+        <v>45301</v>
+      </c>
+      <c r="C125" s="8" t="s">
+        <v>427</v>
+      </c>
+      <c r="D125">
+        <v>27523</v>
+      </c>
+      <c r="E125" s="8" t="s">
+        <v>1214</v>
       </c>
     </row>
   </sheetData>
@@ -7806,7 +8000,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:P467"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A458" sqref="A458:P467"/>
     </sheetView>
   </sheetViews>
@@ -45944,12 +46138,811 @@
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABDF132E-5F02-4682-A8C9-083C5F415CDD}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1015625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.41796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.47265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>1215</v>
+      </c>
+      <c r="B1" t="s">
+        <v>498</v>
+      </c>
+      <c r="C1" t="s">
+        <v>499</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1216</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1217</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>827</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1218</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1219</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1220</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1221</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>827</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1222</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1223</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1220</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1221</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>827</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1224</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1225</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1226</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1227</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>827</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1228</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1229</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1226</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1227</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>827</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1230</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1105</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1226</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1227</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>1231</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1232</v>
+      </c>
+      <c r="C7" t="s">
+        <v>814</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1233</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>1231</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1235</v>
+      </c>
+      <c r="C8" t="s">
+        <v>813</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1233</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>1231</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1236</v>
+      </c>
+      <c r="C9" t="s">
+        <v>160</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1234</v>
+      </c>
+      <c r="E9" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>1231</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1237</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1238</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1234</v>
+      </c>
+      <c r="E10" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>1231</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1239</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1240</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1241</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>1231</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1242</v>
+      </c>
+      <c r="C12" t="s">
+        <v>164</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1243</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1244</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>1231</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1245</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1246</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1247</v>
+      </c>
+      <c r="E13" t="s">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
+        <v>1248</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1249</v>
+      </c>
+      <c r="C14" t="s">
+        <v>974</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1250</v>
+      </c>
+      <c r="E14" t="s">
+        <v>1251</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
+        <v>1252</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1253</v>
+      </c>
+      <c r="C15" t="s">
+        <v>188</v>
+      </c>
+      <c r="D15" t="s">
+        <v>1243</v>
+      </c>
+      <c r="E15" t="s">
+        <v>1244</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" t="s">
+        <v>1252</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1254</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1255</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1220</v>
+      </c>
+      <c r="E16" t="s">
+        <v>1221</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" t="s">
+        <v>1252</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1256</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1257</v>
+      </c>
+      <c r="D17" t="s">
+        <v>1241</v>
+      </c>
+      <c r="E17" t="s">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" t="s">
+        <v>1252</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1258</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1259</v>
+      </c>
+      <c r="D18" t="s">
+        <v>1241</v>
+      </c>
+      <c r="E18" t="s">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" t="s">
+        <v>1260</v>
+      </c>
+      <c r="B19" t="s">
+        <v>375</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1261</v>
+      </c>
+      <c r="D19" t="s">
+        <v>1250</v>
+      </c>
+      <c r="E19" t="s">
+        <v>1251</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" t="s">
+        <v>1260</v>
+      </c>
+      <c r="B20" t="s">
+        <v>375</v>
+      </c>
+      <c r="C20" t="s">
+        <v>1262</v>
+      </c>
+      <c r="D20" t="s">
+        <v>427</v>
+      </c>
+      <c r="E20" t="s">
+        <v>1263</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" t="s">
+        <v>1231</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1264</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1265</v>
+      </c>
+      <c r="D21" t="s">
+        <v>1220</v>
+      </c>
+      <c r="E21" t="s">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" t="s">
+        <v>1231</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1266</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1267</v>
+      </c>
+      <c r="D22" t="s">
+        <v>1268</v>
+      </c>
+      <c r="E22" t="s">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" t="s">
+        <v>827</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1269</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1270</v>
+      </c>
+      <c r="D23" t="s">
+        <v>1268</v>
+      </c>
+      <c r="E23" t="s">
+        <v>1234</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C104889-FE10-4E5D-AE85-AECF37E1F14D}">
+  <dimension ref="A1:F19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:F19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="5" max="5" width="38.41796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="5" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1215</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>1272</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>498</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>500</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>827</v>
+      </c>
+      <c r="C2" s="5">
+        <v>101</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>1230</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>1105</v>
+      </c>
+      <c r="F2" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="5">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>827</v>
+      </c>
+      <c r="C3" s="5">
+        <v>102</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>1224</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>1225</v>
+      </c>
+      <c r="F3" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="5">
+        <v>1</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>827</v>
+      </c>
+      <c r="C4" s="5">
+        <v>103</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>1228</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>1229</v>
+      </c>
+      <c r="F4" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="5">
+        <v>1</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>827</v>
+      </c>
+      <c r="C5" s="5">
+        <v>104</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>1218</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>1219</v>
+      </c>
+      <c r="F5" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="5">
+        <v>1</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>827</v>
+      </c>
+      <c r="C6" s="5">
+        <v>105</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>1222</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>1223</v>
+      </c>
+      <c r="F6" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="5">
+        <v>1</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>827</v>
+      </c>
+      <c r="C7" s="5">
+        <v>106</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>1269</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>1270</v>
+      </c>
+      <c r="F7" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="5">
+        <v>2</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>1231</v>
+      </c>
+      <c r="C8" s="5">
+        <v>201</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>1266</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>1267</v>
+      </c>
+      <c r="F8" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="5">
+        <v>2</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>1231</v>
+      </c>
+      <c r="C9" s="5">
+        <v>202</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>1232</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>814</v>
+      </c>
+      <c r="F9" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="5">
+        <v>2</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>1231</v>
+      </c>
+      <c r="C10" s="5">
+        <v>203</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>1235</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>813</v>
+      </c>
+      <c r="F10" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="5">
+        <v>2</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>1231</v>
+      </c>
+      <c r="C11" s="5">
+        <v>204</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>1236</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="F11" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="5">
+        <v>2</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>1231</v>
+      </c>
+      <c r="C12" s="5">
+        <v>205</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>1237</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>1238</v>
+      </c>
+      <c r="F12" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="5">
+        <v>2</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>1231</v>
+      </c>
+      <c r="C13" s="5">
+        <v>206</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>1239</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>1240</v>
+      </c>
+      <c r="F13" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="5">
+        <v>2</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>1231</v>
+      </c>
+      <c r="C14" s="5">
+        <v>207</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>1242</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="F14" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="5">
+        <v>2</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>1231</v>
+      </c>
+      <c r="C15" s="5">
+        <v>208</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>1264</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>1265</v>
+      </c>
+      <c r="F15" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="5">
+        <v>2</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>1231</v>
+      </c>
+      <c r="C16" s="5">
+        <v>209</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>1245</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>1246</v>
+      </c>
+      <c r="F16" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="5">
+        <v>3</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C17" s="5">
+        <v>301</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>1249</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>974</v>
+      </c>
+      <c r="F17" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="5">
+        <v>4</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>1252</v>
+      </c>
+      <c r="C18" s="5">
+        <v>401</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>1254</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>1255</v>
+      </c>
+      <c r="F18" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="5">
+        <v>4</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>1252</v>
+      </c>
+      <c r="C19" s="5">
+        <v>402</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>1253</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="F19" s="5">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
TFS 27638 - Wellbeing Break eCL data Feed
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C53513
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TFS\eCoaching_V2\Design\DD\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{670A1062-1455-4705-9EA4-4368B124D78C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12BFE63F-04AB-4ECF-AEE4-507D1C309819}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" firstSheet="30" activeTab="35" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" firstSheet="30" activeTab="34" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_History" sheetId="14" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4517" uniqueCount="1273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4528" uniqueCount="1276">
   <si>
     <t>SourceID</t>
   </si>
@@ -3930,6 +3930,15 @@
   </si>
   <si>
     <t>ReportID</t>
+  </si>
+  <si>
+    <t>Added new subcoaching reason and records to feed contacts and feed list tables to support wellbeing breaks</t>
+  </si>
+  <si>
+    <t>Wellbeing Breaks</t>
+  </si>
+  <si>
+    <t>BRW</t>
   </si>
 </sst>
 </file>
@@ -4046,9 +4055,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -4086,9 +4095,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4121,26 +4130,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4173,26 +4165,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4366,10 +4341,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L125"/>
+  <dimension ref="A1:L126"/>
   <sheetViews>
     <sheetView topLeftCell="C100" workbookViewId="0">
-      <selection activeCell="E125" sqref="E125"/>
+      <selection activeCell="E126" sqref="E126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -6490,6 +6465,23 @@
       </c>
       <c r="E125" s="8" t="s">
         <v>1214</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A126" s="8">
+        <v>115</v>
+      </c>
+      <c r="B126" s="1">
+        <v>45317</v>
+      </c>
+      <c r="C126" s="8" t="s">
+        <v>427</v>
+      </c>
+      <c r="D126">
+        <v>27638</v>
+      </c>
+      <c r="E126" s="8" t="s">
+        <v>1273</v>
       </c>
     </row>
   </sheetData>
@@ -8001,7 +7993,7 @@
   <dimension ref="A1:P467"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A458" sqref="A458:P467"/>
+      <selection activeCell="A392" sqref="A392:XFD467"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -27560,253 +27552,253 @@
         <v>1</v>
       </c>
     </row>
-    <row r="392" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A392">
+    <row r="392" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A392" s="6">
         <v>62</v>
       </c>
-      <c r="B392" s="5" t="s">
+      <c r="B392" s="6" t="s">
         <v>1203</v>
       </c>
-      <c r="C392">
+      <c r="C392" s="6">
         <v>42</v>
       </c>
-      <c r="D392" t="s">
+      <c r="D392" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="E392">
-        <v>1</v>
-      </c>
-      <c r="F392">
-        <v>1</v>
-      </c>
-      <c r="G392">
-        <v>1</v>
-      </c>
-      <c r="H392">
-        <v>1</v>
-      </c>
-      <c r="I392">
-        <v>1</v>
-      </c>
-      <c r="J392">
-        <v>1</v>
-      </c>
-      <c r="K392">
-        <v>1</v>
-      </c>
-      <c r="L392">
-        <v>1</v>
-      </c>
-      <c r="M392">
-        <v>0</v>
-      </c>
-      <c r="N392">
-        <v>0</v>
-      </c>
-      <c r="O392">
-        <v>0</v>
-      </c>
-      <c r="P392">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="393" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A393">
+      <c r="E392" s="6">
+        <v>1</v>
+      </c>
+      <c r="F392" s="6">
+        <v>1</v>
+      </c>
+      <c r="G392" s="6">
+        <v>1</v>
+      </c>
+      <c r="H392" s="6">
+        <v>1</v>
+      </c>
+      <c r="I392" s="6">
+        <v>1</v>
+      </c>
+      <c r="J392" s="6">
+        <v>1</v>
+      </c>
+      <c r="K392" s="6">
+        <v>1</v>
+      </c>
+      <c r="L392" s="6">
+        <v>1</v>
+      </c>
+      <c r="M392" s="6">
+        <v>0</v>
+      </c>
+      <c r="N392" s="6">
+        <v>0</v>
+      </c>
+      <c r="O392" s="6">
+        <v>0</v>
+      </c>
+      <c r="P392" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="393" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A393" s="6">
         <v>63</v>
       </c>
-      <c r="B393" s="5" t="s">
+      <c r="B393" s="6" t="s">
         <v>1204</v>
       </c>
-      <c r="C393">
+      <c r="C393" s="6">
         <v>277</v>
       </c>
-      <c r="D393" t="s">
+      <c r="D393" s="6" t="s">
         <v>1095</v>
       </c>
-      <c r="E393" s="5">
-        <v>0</v>
-      </c>
-      <c r="F393">
-        <v>1</v>
-      </c>
-      <c r="G393">
-        <v>1</v>
-      </c>
-      <c r="H393">
-        <v>1</v>
-      </c>
-      <c r="I393">
-        <v>1</v>
-      </c>
-      <c r="J393">
-        <v>1</v>
-      </c>
-      <c r="K393">
-        <v>0</v>
-      </c>
-      <c r="L393">
-        <v>0</v>
-      </c>
-      <c r="M393">
-        <v>0</v>
-      </c>
-      <c r="N393">
-        <v>0</v>
-      </c>
-      <c r="O393">
-        <v>0</v>
-      </c>
-      <c r="P393">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="394" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A394">
+      <c r="E393" s="6">
+        <v>0</v>
+      </c>
+      <c r="F393" s="6">
+        <v>1</v>
+      </c>
+      <c r="G393" s="6">
+        <v>1</v>
+      </c>
+      <c r="H393" s="6">
+        <v>1</v>
+      </c>
+      <c r="I393" s="6">
+        <v>1</v>
+      </c>
+      <c r="J393" s="6">
+        <v>1</v>
+      </c>
+      <c r="K393" s="6">
+        <v>0</v>
+      </c>
+      <c r="L393" s="6">
+        <v>0</v>
+      </c>
+      <c r="M393" s="6">
+        <v>0</v>
+      </c>
+      <c r="N393" s="6">
+        <v>0</v>
+      </c>
+      <c r="O393" s="6">
+        <v>0</v>
+      </c>
+      <c r="P393" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="394" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A394" s="6">
         <v>63</v>
       </c>
-      <c r="B394" s="5" t="s">
+      <c r="B394" s="6" t="s">
         <v>1204</v>
       </c>
-      <c r="C394">
+      <c r="C394" s="6">
         <v>278</v>
       </c>
-      <c r="D394" t="s">
+      <c r="D394" s="6" t="s">
         <v>1096</v>
       </c>
-      <c r="E394" s="5">
-        <v>0</v>
-      </c>
-      <c r="F394">
-        <v>1</v>
-      </c>
-      <c r="G394">
-        <v>1</v>
-      </c>
-      <c r="H394">
-        <v>1</v>
-      </c>
-      <c r="I394">
-        <v>1</v>
-      </c>
-      <c r="J394">
-        <v>1</v>
-      </c>
-      <c r="K394">
-        <v>0</v>
-      </c>
-      <c r="L394">
-        <v>0</v>
-      </c>
-      <c r="M394">
-        <v>0</v>
-      </c>
-      <c r="N394">
-        <v>0</v>
-      </c>
-      <c r="O394">
-        <v>0</v>
-      </c>
-      <c r="P394">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="395" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A395">
+      <c r="E394" s="6">
+        <v>0</v>
+      </c>
+      <c r="F394" s="6">
+        <v>1</v>
+      </c>
+      <c r="G394" s="6">
+        <v>1</v>
+      </c>
+      <c r="H394" s="6">
+        <v>1</v>
+      </c>
+      <c r="I394" s="6">
+        <v>1</v>
+      </c>
+      <c r="J394" s="6">
+        <v>1</v>
+      </c>
+      <c r="K394" s="6">
+        <v>0</v>
+      </c>
+      <c r="L394" s="6">
+        <v>0</v>
+      </c>
+      <c r="M394" s="6">
+        <v>0</v>
+      </c>
+      <c r="N394" s="6">
+        <v>0</v>
+      </c>
+      <c r="O394" s="6">
+        <v>0</v>
+      </c>
+      <c r="P394" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="395" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A395" s="6">
         <v>63</v>
       </c>
-      <c r="B395" s="5" t="s">
+      <c r="B395" s="6" t="s">
         <v>1204</v>
       </c>
-      <c r="C395">
+      <c r="C395" s="6">
         <v>279</v>
       </c>
-      <c r="D395" t="s">
+      <c r="D395" s="6" t="s">
         <v>1097</v>
       </c>
-      <c r="E395" s="5">
-        <v>0</v>
-      </c>
-      <c r="F395">
-        <v>1</v>
-      </c>
-      <c r="G395">
-        <v>1</v>
-      </c>
-      <c r="H395">
-        <v>1</v>
-      </c>
-      <c r="I395">
-        <v>1</v>
-      </c>
-      <c r="J395">
-        <v>1</v>
-      </c>
-      <c r="K395">
-        <v>0</v>
-      </c>
-      <c r="L395">
-        <v>0</v>
-      </c>
-      <c r="M395">
-        <v>0</v>
-      </c>
-      <c r="N395">
-        <v>0</v>
-      </c>
-      <c r="O395">
-        <v>0</v>
-      </c>
-      <c r="P395">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="396" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A396">
+      <c r="E395" s="6">
+        <v>0</v>
+      </c>
+      <c r="F395" s="6">
+        <v>1</v>
+      </c>
+      <c r="G395" s="6">
+        <v>1</v>
+      </c>
+      <c r="H395" s="6">
+        <v>1</v>
+      </c>
+      <c r="I395" s="6">
+        <v>1</v>
+      </c>
+      <c r="J395" s="6">
+        <v>1</v>
+      </c>
+      <c r="K395" s="6">
+        <v>0</v>
+      </c>
+      <c r="L395" s="6">
+        <v>0</v>
+      </c>
+      <c r="M395" s="6">
+        <v>0</v>
+      </c>
+      <c r="N395" s="6">
+        <v>0</v>
+      </c>
+      <c r="O395" s="6">
+        <v>0</v>
+      </c>
+      <c r="P395" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="396" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A396" s="6">
         <v>63</v>
       </c>
-      <c r="B396" s="5" t="s">
+      <c r="B396" s="6" t="s">
         <v>1204</v>
       </c>
-      <c r="C396">
+      <c r="C396" s="6">
         <v>280</v>
       </c>
-      <c r="D396" t="s">
+      <c r="D396" s="6" t="s">
         <v>1098</v>
       </c>
-      <c r="E396">
-        <v>1</v>
-      </c>
-      <c r="F396">
-        <v>1</v>
-      </c>
-      <c r="G396">
-        <v>1</v>
-      </c>
-      <c r="H396">
-        <v>1</v>
-      </c>
-      <c r="I396">
-        <v>1</v>
-      </c>
-      <c r="J396">
-        <v>1</v>
-      </c>
-      <c r="K396" s="5">
-        <v>1</v>
-      </c>
-      <c r="L396">
-        <v>0</v>
-      </c>
-      <c r="M396">
-        <v>0</v>
-      </c>
-      <c r="N396">
-        <v>0</v>
-      </c>
-      <c r="O396">
-        <v>0</v>
-      </c>
-      <c r="P396">
+      <c r="E396" s="6">
+        <v>1</v>
+      </c>
+      <c r="F396" s="6">
+        <v>1</v>
+      </c>
+      <c r="G396" s="6">
+        <v>1</v>
+      </c>
+      <c r="H396" s="6">
+        <v>1</v>
+      </c>
+      <c r="I396" s="6">
+        <v>1</v>
+      </c>
+      <c r="J396" s="6">
+        <v>1</v>
+      </c>
+      <c r="K396" s="6">
+        <v>1</v>
+      </c>
+      <c r="L396" s="6">
+        <v>0</v>
+      </c>
+      <c r="M396" s="6">
+        <v>0</v>
+      </c>
+      <c r="N396" s="6">
+        <v>0</v>
+      </c>
+      <c r="O396" s="6">
+        <v>0</v>
+      </c>
+      <c r="P396" s="6">
         <v>0</v>
       </c>
     </row>
@@ -30160,20 +30152,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="444" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="444" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A444" s="6">
         <v>62</v>
       </c>
-      <c r="B444" s="5" t="s">
+      <c r="B444" s="6" t="s">
         <v>1203</v>
       </c>
       <c r="C444" s="6">
         <v>302</v>
       </c>
-      <c r="D444" s="8" t="s">
+      <c r="D444" s="6" t="s">
         <v>1166</v>
       </c>
-      <c r="E444" s="5">
+      <c r="E444" s="6">
         <v>0</v>
       </c>
       <c r="F444" s="6">
@@ -30210,20 +30202,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="445" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="445" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A445" s="6">
         <v>63</v>
       </c>
-      <c r="B445" s="5" t="s">
+      <c r="B445" s="6" t="s">
         <v>1204</v>
       </c>
       <c r="C445" s="6">
         <v>302</v>
       </c>
-      <c r="D445" s="8" t="s">
+      <c r="D445" s="6" t="s">
         <v>1166</v>
       </c>
-      <c r="E445" s="5">
+      <c r="E445" s="6">
         <v>0</v>
       </c>
       <c r="F445" s="6">
@@ -30860,503 +30852,503 @@
         <v>0</v>
       </c>
     </row>
-    <row r="458" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A458" s="5">
+    <row r="458" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A458" s="6">
         <v>62</v>
       </c>
-      <c r="B458" s="5" t="s">
+      <c r="B458" s="6" t="s">
         <v>1203</v>
       </c>
-      <c r="C458" s="5">
+      <c r="C458" s="6">
         <v>321</v>
       </c>
-      <c r="D458" s="5" t="s">
+      <c r="D458" s="6" t="s">
         <v>1210</v>
       </c>
-      <c r="E458" s="5">
-        <v>1</v>
-      </c>
-      <c r="F458" s="5">
-        <v>1</v>
-      </c>
-      <c r="G458" s="5">
-        <v>1</v>
-      </c>
-      <c r="H458" s="5">
-        <v>1</v>
-      </c>
-      <c r="I458" s="5">
-        <v>1</v>
-      </c>
-      <c r="J458" s="5">
-        <v>1</v>
-      </c>
-      <c r="K458" s="5">
-        <v>1</v>
-      </c>
-      <c r="L458" s="5">
-        <v>0</v>
-      </c>
-      <c r="M458" s="5">
-        <v>0</v>
-      </c>
-      <c r="N458" s="5">
-        <v>0</v>
-      </c>
-      <c r="O458" s="5">
-        <v>0</v>
-      </c>
-      <c r="P458" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="459" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A459" s="5">
+      <c r="E458" s="6">
+        <v>1</v>
+      </c>
+      <c r="F458" s="6">
+        <v>1</v>
+      </c>
+      <c r="G458" s="6">
+        <v>1</v>
+      </c>
+      <c r="H458" s="6">
+        <v>1</v>
+      </c>
+      <c r="I458" s="6">
+        <v>1</v>
+      </c>
+      <c r="J458" s="6">
+        <v>1</v>
+      </c>
+      <c r="K458" s="6">
+        <v>1</v>
+      </c>
+      <c r="L458" s="6">
+        <v>0</v>
+      </c>
+      <c r="M458" s="6">
+        <v>0</v>
+      </c>
+      <c r="N458" s="6">
+        <v>0</v>
+      </c>
+      <c r="O458" s="6">
+        <v>0</v>
+      </c>
+      <c r="P458" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="459" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A459" s="6">
         <v>62</v>
       </c>
-      <c r="B459" s="5" t="s">
+      <c r="B459" s="6" t="s">
         <v>1203</v>
       </c>
-      <c r="C459" s="5">
+      <c r="C459" s="6">
         <v>317</v>
       </c>
-      <c r="D459" s="5" t="s">
+      <c r="D459" s="6" t="s">
         <v>1206</v>
       </c>
-      <c r="E459" s="5">
-        <v>1</v>
-      </c>
-      <c r="F459" s="5">
-        <v>1</v>
-      </c>
-      <c r="G459" s="5">
-        <v>1</v>
-      </c>
-      <c r="H459" s="5">
-        <v>1</v>
-      </c>
-      <c r="I459" s="5">
-        <v>1</v>
-      </c>
-      <c r="J459" s="5">
-        <v>1</v>
-      </c>
-      <c r="K459" s="5">
-        <v>1</v>
-      </c>
-      <c r="L459" s="5">
-        <v>0</v>
-      </c>
-      <c r="M459" s="5">
-        <v>0</v>
-      </c>
-      <c r="N459" s="5">
-        <v>0</v>
-      </c>
-      <c r="O459" s="5">
-        <v>0</v>
-      </c>
-      <c r="P459" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="460" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A460" s="5">
+      <c r="E459" s="6">
+        <v>1</v>
+      </c>
+      <c r="F459" s="6">
+        <v>1</v>
+      </c>
+      <c r="G459" s="6">
+        <v>1</v>
+      </c>
+      <c r="H459" s="6">
+        <v>1</v>
+      </c>
+      <c r="I459" s="6">
+        <v>1</v>
+      </c>
+      <c r="J459" s="6">
+        <v>1</v>
+      </c>
+      <c r="K459" s="6">
+        <v>1</v>
+      </c>
+      <c r="L459" s="6">
+        <v>0</v>
+      </c>
+      <c r="M459" s="6">
+        <v>0</v>
+      </c>
+      <c r="N459" s="6">
+        <v>0</v>
+      </c>
+      <c r="O459" s="6">
+        <v>0</v>
+      </c>
+      <c r="P459" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="460" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A460" s="6">
         <v>62</v>
       </c>
-      <c r="B460" s="5" t="s">
+      <c r="B460" s="6" t="s">
         <v>1203</v>
       </c>
-      <c r="C460" s="5">
+      <c r="C460" s="6">
         <v>324</v>
       </c>
-      <c r="D460" s="5" t="s">
+      <c r="D460" s="6" t="s">
         <v>1213</v>
       </c>
-      <c r="E460" s="5">
-        <v>1</v>
-      </c>
-      <c r="F460" s="5">
-        <v>1</v>
-      </c>
-      <c r="G460" s="5">
-        <v>1</v>
-      </c>
-      <c r="H460" s="5">
-        <v>1</v>
-      </c>
-      <c r="I460" s="5">
-        <v>1</v>
-      </c>
-      <c r="J460" s="5">
-        <v>1</v>
-      </c>
-      <c r="K460" s="5">
-        <v>1</v>
-      </c>
-      <c r="L460" s="5">
-        <v>0</v>
-      </c>
-      <c r="M460" s="5">
-        <v>0</v>
-      </c>
-      <c r="N460" s="5">
-        <v>0</v>
-      </c>
-      <c r="O460" s="5">
-        <v>0</v>
-      </c>
-      <c r="P460" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="461" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A461" s="5">
+      <c r="E460" s="6">
+        <v>1</v>
+      </c>
+      <c r="F460" s="6">
+        <v>1</v>
+      </c>
+      <c r="G460" s="6">
+        <v>1</v>
+      </c>
+      <c r="H460" s="6">
+        <v>1</v>
+      </c>
+      <c r="I460" s="6">
+        <v>1</v>
+      </c>
+      <c r="J460" s="6">
+        <v>1</v>
+      </c>
+      <c r="K460" s="6">
+        <v>1</v>
+      </c>
+      <c r="L460" s="6">
+        <v>0</v>
+      </c>
+      <c r="M460" s="6">
+        <v>0</v>
+      </c>
+      <c r="N460" s="6">
+        <v>0</v>
+      </c>
+      <c r="O460" s="6">
+        <v>0</v>
+      </c>
+      <c r="P460" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="461" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A461" s="6">
         <v>62</v>
       </c>
-      <c r="B461" s="5" t="s">
+      <c r="B461" s="6" t="s">
         <v>1203</v>
       </c>
-      <c r="C461" s="5">
+      <c r="C461" s="6">
         <v>319</v>
       </c>
-      <c r="D461" s="5" t="s">
+      <c r="D461" s="6" t="s">
         <v>1208</v>
       </c>
-      <c r="E461" s="5">
-        <v>1</v>
-      </c>
-      <c r="F461" s="5">
-        <v>1</v>
-      </c>
-      <c r="G461" s="5">
-        <v>1</v>
-      </c>
-      <c r="H461" s="5">
-        <v>1</v>
-      </c>
-      <c r="I461" s="5">
-        <v>1</v>
-      </c>
-      <c r="J461" s="5">
-        <v>1</v>
-      </c>
-      <c r="K461" s="5">
-        <v>1</v>
-      </c>
-      <c r="L461" s="5">
-        <v>0</v>
-      </c>
-      <c r="M461" s="5">
-        <v>0</v>
-      </c>
-      <c r="N461" s="5">
-        <v>0</v>
-      </c>
-      <c r="O461" s="5">
-        <v>0</v>
-      </c>
-      <c r="P461" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="462" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A462" s="5">
+      <c r="E461" s="6">
+        <v>1</v>
+      </c>
+      <c r="F461" s="6">
+        <v>1</v>
+      </c>
+      <c r="G461" s="6">
+        <v>1</v>
+      </c>
+      <c r="H461" s="6">
+        <v>1</v>
+      </c>
+      <c r="I461" s="6">
+        <v>1</v>
+      </c>
+      <c r="J461" s="6">
+        <v>1</v>
+      </c>
+      <c r="K461" s="6">
+        <v>1</v>
+      </c>
+      <c r="L461" s="6">
+        <v>0</v>
+      </c>
+      <c r="M461" s="6">
+        <v>0</v>
+      </c>
+      <c r="N461" s="6">
+        <v>0</v>
+      </c>
+      <c r="O461" s="6">
+        <v>0</v>
+      </c>
+      <c r="P461" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="462" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A462" s="6">
         <v>63</v>
       </c>
-      <c r="B462" s="5" t="s">
+      <c r="B462" s="6" t="s">
         <v>1204</v>
       </c>
-      <c r="C462" s="5">
+      <c r="C462" s="6">
         <v>321</v>
       </c>
-      <c r="D462" s="5" t="s">
+      <c r="D462" s="6" t="s">
         <v>1210</v>
       </c>
-      <c r="E462" s="5">
-        <v>1</v>
-      </c>
-      <c r="F462" s="5">
-        <v>1</v>
-      </c>
-      <c r="G462" s="5">
-        <v>1</v>
-      </c>
-      <c r="H462" s="5">
-        <v>1</v>
-      </c>
-      <c r="I462" s="5">
-        <v>1</v>
-      </c>
-      <c r="J462" s="5">
-        <v>1</v>
-      </c>
-      <c r="K462" s="5">
-        <v>1</v>
-      </c>
-      <c r="L462" s="5">
-        <v>0</v>
-      </c>
-      <c r="M462" s="5">
-        <v>0</v>
-      </c>
-      <c r="N462" s="5">
-        <v>0</v>
-      </c>
-      <c r="O462" s="5">
-        <v>0</v>
-      </c>
-      <c r="P462" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="463" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A463" s="5">
+      <c r="E462" s="6">
+        <v>1</v>
+      </c>
+      <c r="F462" s="6">
+        <v>1</v>
+      </c>
+      <c r="G462" s="6">
+        <v>1</v>
+      </c>
+      <c r="H462" s="6">
+        <v>1</v>
+      </c>
+      <c r="I462" s="6">
+        <v>1</v>
+      </c>
+      <c r="J462" s="6">
+        <v>1</v>
+      </c>
+      <c r="K462" s="6">
+        <v>1</v>
+      </c>
+      <c r="L462" s="6">
+        <v>0</v>
+      </c>
+      <c r="M462" s="6">
+        <v>0</v>
+      </c>
+      <c r="N462" s="6">
+        <v>0</v>
+      </c>
+      <c r="O462" s="6">
+        <v>0</v>
+      </c>
+      <c r="P462" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="463" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A463" s="6">
         <v>63</v>
       </c>
-      <c r="B463" s="5" t="s">
+      <c r="B463" s="6" t="s">
         <v>1204</v>
       </c>
-      <c r="C463" s="5">
+      <c r="C463" s="6">
         <v>316</v>
       </c>
-      <c r="D463" s="5" t="s">
+      <c r="D463" s="6" t="s">
         <v>1205</v>
       </c>
-      <c r="E463" s="5">
-        <v>1</v>
-      </c>
-      <c r="F463" s="5">
-        <v>1</v>
-      </c>
-      <c r="G463" s="5">
-        <v>1</v>
-      </c>
-      <c r="H463" s="5">
-        <v>1</v>
-      </c>
-      <c r="I463" s="5">
-        <v>1</v>
-      </c>
-      <c r="J463" s="5">
-        <v>1</v>
-      </c>
-      <c r="K463" s="5">
-        <v>1</v>
-      </c>
-      <c r="L463" s="5">
-        <v>0</v>
-      </c>
-      <c r="M463" s="5">
-        <v>0</v>
-      </c>
-      <c r="N463" s="5">
-        <v>0</v>
-      </c>
-      <c r="O463" s="5">
-        <v>0</v>
-      </c>
-      <c r="P463" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="464" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A464" s="5">
+      <c r="E463" s="6">
+        <v>1</v>
+      </c>
+      <c r="F463" s="6">
+        <v>1</v>
+      </c>
+      <c r="G463" s="6">
+        <v>1</v>
+      </c>
+      <c r="H463" s="6">
+        <v>1</v>
+      </c>
+      <c r="I463" s="6">
+        <v>1</v>
+      </c>
+      <c r="J463" s="6">
+        <v>1</v>
+      </c>
+      <c r="K463" s="6">
+        <v>1</v>
+      </c>
+      <c r="L463" s="6">
+        <v>0</v>
+      </c>
+      <c r="M463" s="6">
+        <v>0</v>
+      </c>
+      <c r="N463" s="6">
+        <v>0</v>
+      </c>
+      <c r="O463" s="6">
+        <v>0</v>
+      </c>
+      <c r="P463" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="464" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A464" s="6">
         <v>63</v>
       </c>
-      <c r="B464" s="5" t="s">
+      <c r="B464" s="6" t="s">
         <v>1204</v>
       </c>
-      <c r="C464" s="5">
+      <c r="C464" s="6">
         <v>322</v>
       </c>
-      <c r="D464" s="5" t="s">
+      <c r="D464" s="6" t="s">
         <v>1211</v>
       </c>
-      <c r="E464" s="5">
-        <v>1</v>
-      </c>
-      <c r="F464" s="5">
-        <v>1</v>
-      </c>
-      <c r="G464" s="5">
-        <v>1</v>
-      </c>
-      <c r="H464" s="5">
-        <v>1</v>
-      </c>
-      <c r="I464" s="5">
-        <v>1</v>
-      </c>
-      <c r="J464" s="5">
-        <v>1</v>
-      </c>
-      <c r="K464" s="5">
-        <v>1</v>
-      </c>
-      <c r="L464" s="5">
-        <v>0</v>
-      </c>
-      <c r="M464" s="5">
-        <v>0</v>
-      </c>
-      <c r="N464" s="5">
-        <v>0</v>
-      </c>
-      <c r="O464" s="5">
-        <v>0</v>
-      </c>
-      <c r="P464" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="465" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A465" s="5">
+      <c r="E464" s="6">
+        <v>1</v>
+      </c>
+      <c r="F464" s="6">
+        <v>1</v>
+      </c>
+      <c r="G464" s="6">
+        <v>1</v>
+      </c>
+      <c r="H464" s="6">
+        <v>1</v>
+      </c>
+      <c r="I464" s="6">
+        <v>1</v>
+      </c>
+      <c r="J464" s="6">
+        <v>1</v>
+      </c>
+      <c r="K464" s="6">
+        <v>1</v>
+      </c>
+      <c r="L464" s="6">
+        <v>0</v>
+      </c>
+      <c r="M464" s="6">
+        <v>0</v>
+      </c>
+      <c r="N464" s="6">
+        <v>0</v>
+      </c>
+      <c r="O464" s="6">
+        <v>0</v>
+      </c>
+      <c r="P464" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="465" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A465" s="6">
         <v>63</v>
       </c>
-      <c r="B465" s="5" t="s">
+      <c r="B465" s="6" t="s">
         <v>1204</v>
       </c>
-      <c r="C465" s="5">
+      <c r="C465" s="6">
         <v>323</v>
       </c>
-      <c r="D465" s="5" t="s">
+      <c r="D465" s="6" t="s">
         <v>1212</v>
       </c>
-      <c r="E465" s="5">
-        <v>1</v>
-      </c>
-      <c r="F465" s="5">
-        <v>1</v>
-      </c>
-      <c r="G465" s="5">
-        <v>1</v>
-      </c>
-      <c r="H465" s="5">
-        <v>1</v>
-      </c>
-      <c r="I465" s="5">
-        <v>1</v>
-      </c>
-      <c r="J465" s="5">
-        <v>1</v>
-      </c>
-      <c r="K465" s="5">
-        <v>1</v>
-      </c>
-      <c r="L465" s="5">
-        <v>0</v>
-      </c>
-      <c r="M465" s="5">
-        <v>0</v>
-      </c>
-      <c r="N465" s="5">
-        <v>0</v>
-      </c>
-      <c r="O465" s="5">
-        <v>0</v>
-      </c>
-      <c r="P465" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="466" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A466" s="5">
+      <c r="E465" s="6">
+        <v>1</v>
+      </c>
+      <c r="F465" s="6">
+        <v>1</v>
+      </c>
+      <c r="G465" s="6">
+        <v>1</v>
+      </c>
+      <c r="H465" s="6">
+        <v>1</v>
+      </c>
+      <c r="I465" s="6">
+        <v>1</v>
+      </c>
+      <c r="J465" s="6">
+        <v>1</v>
+      </c>
+      <c r="K465" s="6">
+        <v>1</v>
+      </c>
+      <c r="L465" s="6">
+        <v>0</v>
+      </c>
+      <c r="M465" s="6">
+        <v>0</v>
+      </c>
+      <c r="N465" s="6">
+        <v>0</v>
+      </c>
+      <c r="O465" s="6">
+        <v>0</v>
+      </c>
+      <c r="P465" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="466" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A466" s="6">
         <v>63</v>
       </c>
-      <c r="B466" s="5" t="s">
+      <c r="B466" s="6" t="s">
         <v>1204</v>
       </c>
-      <c r="C466" s="5">
+      <c r="C466" s="6">
         <v>320</v>
       </c>
-      <c r="D466" s="5" t="s">
+      <c r="D466" s="6" t="s">
         <v>1209</v>
       </c>
-      <c r="E466" s="5">
-        <v>1</v>
-      </c>
-      <c r="F466" s="5">
-        <v>1</v>
-      </c>
-      <c r="G466" s="5">
-        <v>1</v>
-      </c>
-      <c r="H466" s="5">
-        <v>1</v>
-      </c>
-      <c r="I466" s="5">
-        <v>1</v>
-      </c>
-      <c r="J466" s="5">
-        <v>1</v>
-      </c>
-      <c r="K466" s="5">
-        <v>1</v>
-      </c>
-      <c r="L466" s="5">
-        <v>0</v>
-      </c>
-      <c r="M466" s="5">
-        <v>0</v>
-      </c>
-      <c r="N466" s="5">
-        <v>0</v>
-      </c>
-      <c r="O466" s="5">
-        <v>0</v>
-      </c>
-      <c r="P466" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="467" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A467" s="5">
+      <c r="E466" s="6">
+        <v>1</v>
+      </c>
+      <c r="F466" s="6">
+        <v>1</v>
+      </c>
+      <c r="G466" s="6">
+        <v>1</v>
+      </c>
+      <c r="H466" s="6">
+        <v>1</v>
+      </c>
+      <c r="I466" s="6">
+        <v>1</v>
+      </c>
+      <c r="J466" s="6">
+        <v>1</v>
+      </c>
+      <c r="K466" s="6">
+        <v>1</v>
+      </c>
+      <c r="L466" s="6">
+        <v>0</v>
+      </c>
+      <c r="M466" s="6">
+        <v>0</v>
+      </c>
+      <c r="N466" s="6">
+        <v>0</v>
+      </c>
+      <c r="O466" s="6">
+        <v>0</v>
+      </c>
+      <c r="P466" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="467" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A467" s="6">
         <v>63</v>
       </c>
-      <c r="B467" s="5" t="s">
+      <c r="B467" s="6" t="s">
         <v>1204</v>
       </c>
-      <c r="C467" s="5">
+      <c r="C467" s="6">
         <v>318</v>
       </c>
-      <c r="D467" s="5" t="s">
+      <c r="D467" s="6" t="s">
         <v>1207</v>
       </c>
-      <c r="E467" s="5">
-        <v>1</v>
-      </c>
-      <c r="F467" s="5">
-        <v>1</v>
-      </c>
-      <c r="G467" s="5">
-        <v>1</v>
-      </c>
-      <c r="H467" s="5">
-        <v>1</v>
-      </c>
-      <c r="I467" s="5">
-        <v>1</v>
-      </c>
-      <c r="J467" s="5">
-        <v>1</v>
-      </c>
-      <c r="K467" s="5">
-        <v>1</v>
-      </c>
-      <c r="L467" s="5">
-        <v>0</v>
-      </c>
-      <c r="M467" s="5">
-        <v>0</v>
-      </c>
-      <c r="N467" s="5">
-        <v>0</v>
-      </c>
-      <c r="O467" s="5">
-        <v>0</v>
-      </c>
-      <c r="P467" s="5">
+      <c r="E467" s="6">
+        <v>1</v>
+      </c>
+      <c r="F467" s="6">
+        <v>1</v>
+      </c>
+      <c r="G467" s="6">
+        <v>1</v>
+      </c>
+      <c r="H467" s="6">
+        <v>1</v>
+      </c>
+      <c r="I467" s="6">
+        <v>1</v>
+      </c>
+      <c r="J467" s="6">
+        <v>1</v>
+      </c>
+      <c r="K467" s="6">
+        <v>1</v>
+      </c>
+      <c r="L467" s="6">
+        <v>0</v>
+      </c>
+      <c r="M467" s="6">
+        <v>0</v>
+      </c>
+      <c r="N467" s="6">
+        <v>0</v>
+      </c>
+      <c r="O467" s="6">
+        <v>0</v>
+      </c>
+      <c r="P467" s="6">
         <v>0</v>
       </c>
     </row>
@@ -42876,19 +42868,19 @@
       </c>
     </row>
     <row r="3" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="5">
-        <v>1</v>
-      </c>
-      <c r="B3" s="5" t="s">
+      <c r="A3" s="6">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="5">
-        <v>0</v>
-      </c>
-      <c r="D3" s="5">
-        <v>0</v>
-      </c>
-      <c r="E3" s="5">
+      <c r="C3" s="6">
+        <v>0</v>
+      </c>
+      <c r="D3" s="6">
+        <v>0</v>
+      </c>
+      <c r="E3" s="6">
         <v>0</v>
       </c>
     </row>
@@ -45975,7 +45967,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE8E5AAB-2CB2-47A7-AC59-8DE4502992B4}">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:L4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
@@ -46094,40 +46088,40 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="5">
+      <c r="A4" s="6">
         <v>103</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="6" t="s">
         <v>1201</v>
       </c>
-      <c r="C4" s="5">
-        <v>1</v>
-      </c>
-      <c r="D4" s="5">
+      <c r="C4" s="6">
+        <v>1</v>
+      </c>
+      <c r="D4" s="6">
         <v>9</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="6">
         <v>315</v>
       </c>
-      <c r="F4" s="5">
-        <v>1</v>
-      </c>
-      <c r="G4" s="5">
-        <v>0</v>
-      </c>
-      <c r="H4" s="5">
-        <v>0</v>
-      </c>
-      <c r="I4" s="5">
-        <v>0</v>
-      </c>
-      <c r="J4" s="5">
-        <v>0</v>
-      </c>
-      <c r="K4" s="5">
+      <c r="F4" s="6">
+        <v>1</v>
+      </c>
+      <c r="G4" s="6">
+        <v>0</v>
+      </c>
+      <c r="H4" s="6">
+        <v>0</v>
+      </c>
+      <c r="I4" s="6">
+        <v>0</v>
+      </c>
+      <c r="J4" s="6">
+        <v>0</v>
+      </c>
+      <c r="K4" s="6">
         <v>20231101</v>
       </c>
-      <c r="L4" s="5">
+      <c r="L4" s="6">
         <v>99991231</v>
       </c>
     </row>
@@ -46138,10 +46132,10 @@
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABDF132E-5F02-4682-A8C9-083C5F415CDD}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -46544,6 +46538,23 @@
         <v>1234</v>
       </c>
     </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="5" t="s">
+        <v>1231</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>1275</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>1274</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>1268</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>1234</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -46551,10 +46562,10 @@
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C104889-FE10-4E5D-AE85-AECF37E1F14D}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -46563,382 +46574,402 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>1271</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>1215</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>1272</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="6" t="s">
         <v>498</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="6" t="s">
         <v>500</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="6" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="5">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5" t="s">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>827</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="6">
         <v>101</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="6" t="s">
         <v>1230</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="6" t="s">
         <v>1105</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="5">
-        <v>1</v>
-      </c>
-      <c r="B3" s="5" t="s">
+      <c r="A3" s="6">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>827</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="6">
         <v>102</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="6" t="s">
         <v>1224</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="6" t="s">
         <v>1225</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="5">
-        <v>1</v>
-      </c>
-      <c r="B4" s="5" t="s">
+      <c r="A4" s="6">
+        <v>1</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>827</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="6">
         <v>103</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="6" t="s">
         <v>1228</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="6" t="s">
         <v>1229</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="5">
-        <v>1</v>
-      </c>
-      <c r="B5" s="5" t="s">
+      <c r="A5" s="6">
+        <v>1</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>827</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="6">
         <v>104</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="6" t="s">
         <v>1218</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="6" t="s">
         <v>1219</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="5">
-        <v>1</v>
-      </c>
-      <c r="B6" s="5" t="s">
+      <c r="A6" s="6">
+        <v>1</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>827</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="6">
         <v>105</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="6" t="s">
         <v>1222</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="6" t="s">
         <v>1223</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="5">
-        <v>1</v>
-      </c>
-      <c r="B7" s="5" t="s">
+      <c r="A7" s="6">
+        <v>1</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>827</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="6">
         <v>106</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="6" t="s">
         <v>1269</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="6" t="s">
         <v>1270</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="5">
+      <c r="A8" s="6">
         <v>2</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="6" t="s">
         <v>1231</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="6">
         <v>201</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="6" t="s">
         <v>1266</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="6" t="s">
         <v>1267</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="5">
+      <c r="A9" s="6">
         <v>2</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="6" t="s">
         <v>1231</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="6">
         <v>202</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="6" t="s">
         <v>1232</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="6" t="s">
         <v>814</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="5">
+      <c r="A10" s="6">
         <v>2</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="6" t="s">
         <v>1231</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="6">
         <v>203</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="6" t="s">
         <v>1235</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="6" t="s">
         <v>813</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="5">
+      <c r="A11" s="6">
         <v>2</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="6" t="s">
         <v>1231</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="6">
         <v>204</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="6" t="s">
         <v>1236</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="5">
+      <c r="A12" s="6">
         <v>2</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="6" t="s">
         <v>1231</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="6">
         <v>205</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="6" t="s">
         <v>1237</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="6" t="s">
         <v>1238</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="5">
+      <c r="A13" s="6">
         <v>2</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="6" t="s">
         <v>1231</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="6">
         <v>206</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="6" t="s">
         <v>1239</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="6" t="s">
         <v>1240</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="5">
+      <c r="A14" s="6">
         <v>2</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="6" t="s">
         <v>1231</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="6">
         <v>207</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="6" t="s">
         <v>1242</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="5">
+      <c r="A15" s="6">
         <v>2</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="6" t="s">
         <v>1231</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="6">
         <v>208</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="6" t="s">
         <v>1264</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="6" t="s">
         <v>1265</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="5">
+      <c r="A16" s="6">
         <v>2</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="6" t="s">
         <v>1231</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="6">
         <v>209</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="6" t="s">
         <v>1245</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="6" t="s">
         <v>1246</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="5">
+      <c r="A17" s="6">
         <v>3</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="6">
         <v>301</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="6" t="s">
         <v>1249</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="6" t="s">
         <v>974</v>
       </c>
-      <c r="F17" s="5">
+      <c r="F17" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="5">
+      <c r="A18" s="6">
         <v>4</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="6" t="s">
         <v>1252</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="6">
         <v>401</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="6" t="s">
         <v>1254</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" s="6" t="s">
         <v>1255</v>
       </c>
-      <c r="F18" s="5">
+      <c r="F18" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="5">
+      <c r="A19" s="6">
         <v>4</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="6" t="s">
         <v>1252</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="6">
         <v>402</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="6" t="s">
         <v>1253</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="E19" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="F19" s="5">
+      <c r="F19" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="5">
+        <v>2</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>1231</v>
+      </c>
+      <c r="C20" s="5">
+        <v>210</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>1275</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>1274</v>
+      </c>
+      <c r="F20" s="5">
         <v>1</v>
       </c>
     </row>
@@ -47997,10 +48028,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:B326"/>
+  <dimension ref="A1:B327"/>
   <sheetViews>
-    <sheetView topLeftCell="A292" workbookViewId="0">
-      <selection activeCell="A318" sqref="A318:B326"/>
+    <sheetView topLeftCell="A304" workbookViewId="0">
+      <selection activeCell="A327" sqref="A327:B327"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -50545,76 +50576,84 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="318" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A318" s="5">
+    <row r="318" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A318" s="6">
         <v>316</v>
       </c>
-      <c r="B318" s="5" t="s">
+      <c r="B318" s="6" t="s">
         <v>1205</v>
       </c>
     </row>
-    <row r="319" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A319" s="5">
+    <row r="319" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A319" s="6">
         <v>317</v>
       </c>
-      <c r="B319" s="5" t="s">
+      <c r="B319" s="6" t="s">
         <v>1206</v>
       </c>
     </row>
-    <row r="320" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A320" s="5">
+    <row r="320" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A320" s="6">
         <v>318</v>
       </c>
-      <c r="B320" s="5" t="s">
+      <c r="B320" s="6" t="s">
         <v>1207</v>
       </c>
     </row>
-    <row r="321" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A321" s="5">
+    <row r="321" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A321" s="6">
         <v>319</v>
       </c>
-      <c r="B321" s="5" t="s">
+      <c r="B321" s="6" t="s">
         <v>1208</v>
       </c>
     </row>
-    <row r="322" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A322" s="5">
+    <row r="322" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A322" s="6">
         <v>320</v>
       </c>
-      <c r="B322" s="5" t="s">
+      <c r="B322" s="6" t="s">
         <v>1209</v>
       </c>
     </row>
-    <row r="323" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A323" s="5">
+    <row r="323" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A323" s="6">
         <v>321</v>
       </c>
-      <c r="B323" s="5" t="s">
+      <c r="B323" s="6" t="s">
         <v>1210</v>
       </c>
     </row>
-    <row r="324" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A324" s="5">
+    <row r="324" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A324" s="6">
         <v>322</v>
       </c>
-      <c r="B324" s="5" t="s">
+      <c r="B324" s="6" t="s">
         <v>1211</v>
       </c>
     </row>
-    <row r="325" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A325" s="5">
+    <row r="325" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A325" s="6">
         <v>323</v>
       </c>
-      <c r="B325" s="5" t="s">
+      <c r="B325" s="6" t="s">
         <v>1212</v>
       </c>
     </row>
-    <row r="326" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A326" s="5">
+    <row r="326" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A326" s="6">
         <v>324</v>
       </c>
-      <c r="B326" s="5" t="s">
+      <c r="B326" s="6" t="s">
         <v>1213</v>
+      </c>
+    </row>
+    <row r="327" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A327" s="5">
+        <v>325</v>
+      </c>
+      <c r="B327" s="5" t="s">
+        <v>1274</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TFS 27851 - Quality Now Olympic Rewards Feed
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C53694
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TFS\eCoaching_V2\Design\DD\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0568BFAB-3E7C-4B62-86DD-E8CEEB140393}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95602435-5DC1-4FDC-A56E-60AE06BB2A4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57504" yWindow="1914" windowWidth="28992" windowHeight="15672" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_History" sheetId="14" r:id="rId1"/>
@@ -50,6 +50,7 @@
     <sheet name="Coaching_Log_Static_Text" sheetId="36" r:id="rId35"/>
     <sheet name="Feed_Contacts" sheetId="35" r:id="rId36"/>
     <sheet name="DIM_Feed_List" sheetId="37" r:id="rId37"/>
+    <sheet name="Sheet1" sheetId="39" r:id="rId38"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">Coaching_Reason_Selection!$A$1:$P$457</definedName>
@@ -61,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4574" uniqueCount="1306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4633" uniqueCount="1338">
   <si>
     <t>SourceID</t>
   </si>
@@ -4031,6 +4032,102 @@
   <si>
     <t>Quality Alignment Monitor</t>
   </si>
+  <si>
+    <t>QN Olympic Rewards</t>
+  </si>
+  <si>
+    <t>QRB</t>
+  </si>
+  <si>
+    <t>QRM</t>
+  </si>
+  <si>
+    <t>QualityNow Rewards Badges</t>
+  </si>
+  <si>
+    <t>QualityNow Rewards Medals</t>
+  </si>
+  <si>
+    <t>Robert O''Mahony</t>
+  </si>
+  <si>
+    <t>ImageName</t>
+  </si>
+  <si>
+    <t>RewardType</t>
+  </si>
+  <si>
+    <t>BusinessProcess</t>
+  </si>
+  <si>
+    <t>Smooth Sailor</t>
+  </si>
+  <si>
+    <t>Badge</t>
+  </si>
+  <si>
+    <t>InfoAccuracy</t>
+  </si>
+  <si>
+    <t>Accurate Archer</t>
+  </si>
+  <si>
+    <t>PrivacyDisclaimers</t>
+  </si>
+  <si>
+    <t>Defense Defender</t>
+  </si>
+  <si>
+    <t>IssueResolution</t>
+  </si>
+  <si>
+    <t>Hurdle Leaper</t>
+  </si>
+  <si>
+    <t>PersonalityFlexing</t>
+  </si>
+  <si>
+    <t>Nimble Gymnast</t>
+  </si>
+  <si>
+    <t>CallEfficiency</t>
+  </si>
+  <si>
+    <t>Lightning Relayer</t>
+  </si>
+  <si>
+    <t>ActiveListening</t>
+  </si>
+  <si>
+    <t>Mindful Titlist</t>
+  </si>
+  <si>
+    <t>BusinessCorr</t>
+  </si>
+  <si>
+    <t>Correspondent Champion</t>
+  </si>
+  <si>
+    <t>Gold</t>
+  </si>
+  <si>
+    <t>Medal</t>
+  </si>
+  <si>
+    <t>Silver</t>
+  </si>
+  <si>
+    <t>Bronze</t>
+  </si>
+  <si>
+    <t>HonorableMention</t>
+  </si>
+  <si>
+    <t>Honorable Mention</t>
+  </si>
+  <si>
+    <t>Quality Now Olympic Rewards Feed. Added records to Tables DIM_Sub_Coaching_Reason, DIM_Feed_List and Feed_Contact. Added new tab for Table QualityNow_Rewards_Images</t>
+  </si>
 </sst>
 </file>
 
@@ -4039,7 +4136,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss:mss"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4066,6 +4163,14 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -4106,7 +4211,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -4128,6 +4233,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4432,10 +4538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L127"/>
+  <dimension ref="A1:L128"/>
   <sheetViews>
-    <sheetView topLeftCell="C103" workbookViewId="0">
-      <selection activeCell="E127" sqref="E127"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="E128" sqref="E128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -6590,6 +6696,23 @@
       </c>
       <c r="E127" t="s">
         <v>1271</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A128" s="8">
+        <v>117</v>
+      </c>
+      <c r="B128" s="1">
+        <v>45380</v>
+      </c>
+      <c r="C128" s="8" t="s">
+        <v>427</v>
+      </c>
+      <c r="D128">
+        <v>27851</v>
+      </c>
+      <c r="E128" t="s">
+        <v>1337</v>
       </c>
     </row>
   </sheetData>
@@ -46434,10 +46557,10 @@
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABDF132E-5F02-4682-A8C9-083C5F415CDD}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:E24"/>
+      <selection activeCell="B25" sqref="B25:C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -46841,19 +46964,53 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="8" t="s">
         <v>1226</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="8" t="s">
         <v>1270</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="8" t="s">
         <v>1269</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="8" t="s">
         <v>1263</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="E24" s="8" t="s">
+        <v>1229</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" t="s">
+        <v>1247</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1307</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1309</v>
+      </c>
+      <c r="D25" t="s">
+        <v>1311</v>
+      </c>
+      <c r="E25" t="s">
+        <v>1216</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" t="s">
+        <v>1247</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1308</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1310</v>
+      </c>
+      <c r="D26" t="s">
+        <v>1311</v>
+      </c>
+      <c r="E26" t="s">
         <v>1229</v>
       </c>
     </row>
@@ -46864,10 +47021,10 @@
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C104889-FE10-4E5D-AE85-AECF37E1F14D}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:F20"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -47256,27 +47413,271 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="5">
+      <c r="A20" s="8">
         <v>2</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="8" t="s">
         <v>1226</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="8">
         <v>210</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="8" t="s">
         <v>1270</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E20" s="8" t="s">
         <v>1269</v>
       </c>
-      <c r="F20" s="5">
+      <c r="F20" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="5">
+        <v>4</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>1247</v>
+      </c>
+      <c r="C21" s="5">
+        <v>403</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>1307</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>1309</v>
+      </c>
+      <c r="F21" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="5">
+        <v>4</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>1247</v>
+      </c>
+      <c r="C22" s="5">
+        <v>404</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>1308</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>1310</v>
+      </c>
+      <c r="F22" s="5">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F115BE4-5313-4244-BBB8-116AE1FEE87D}">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="7.41796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7890625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.1015625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.89453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="15" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>1011</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>1314</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>1315</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>1316</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>1317</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>1318</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>1316</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>1319</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>1320</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>1316</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>1321</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>1316</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>1323</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>1324</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>1316</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>1325</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>1326</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>1316</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="5">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>1327</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>1328</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>1316</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="5">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>1329</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>1330</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>1316</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="5">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>1331</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>1331</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>1332</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="5">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>1333</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>1332</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="5">
+        <v>11</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>1334</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>1334</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>1332</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="5">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>1335</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>1336</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>1332</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -48520,10 +48921,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:B327"/>
+  <dimension ref="A1:B328"/>
   <sheetViews>
     <sheetView topLeftCell="A304" workbookViewId="0">
-      <selection activeCell="A327" sqref="A327:B327"/>
+      <selection activeCell="A328" sqref="A328"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -51141,11 +51542,19 @@
       </c>
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A327" s="5">
+      <c r="A327" s="6">
         <v>325</v>
       </c>
-      <c r="B327" s="5" t="s">
+      <c r="B327" s="6" t="s">
         <v>1269</v>
+      </c>
+    </row>
+    <row r="328" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A328" s="5">
+        <v>326</v>
+      </c>
+      <c r="B328" s="5" t="s">
+        <v>1306</v>
       </c>
     </row>
   </sheetData>
@@ -51704,7 +52113,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1:G11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
TFS 27851 - Quality Now Olympic Rewards Feed. Additional Changes from V&V feedback.
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C53777
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TFS\eCoaching_V2\Design\DD\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95602435-5DC1-4FDC-A56E-60AE06BB2A4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54CF62D6-7070-4219-A54A-29ACE280D839}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57504" yWindow="1914" windowWidth="28992" windowHeight="15672" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
     <sheet name="Coaching_Log_Static_Text" sheetId="36" r:id="rId35"/>
     <sheet name="Feed_Contacts" sheetId="35" r:id="rId36"/>
     <sheet name="DIM_Feed_List" sheetId="37" r:id="rId37"/>
-    <sheet name="Sheet1" sheetId="39" r:id="rId38"/>
+    <sheet name="QualityNow_Rewards_Images" sheetId="39" r:id="rId38"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">Coaching_Reason_Selection!$A$1:$P$457</definedName>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4633" uniqueCount="1338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4635" uniqueCount="1339">
   <si>
     <t>SourceID</t>
   </si>
@@ -4127,6 +4127,9 @@
   </si>
   <si>
     <t>Quality Now Olympic Rewards Feed. Added records to Tables DIM_Sub_Coaching_Reason, DIM_Feed_List and Feed_Contact. Added new tab for Table QualityNow_Rewards_Images</t>
+  </si>
+  <si>
+    <t>Renamed tab for QualityNow_Rewards_Images (from Sheet1)</t>
   </si>
 </sst>
 </file>
@@ -4538,10 +4541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L128"/>
+  <dimension ref="A1:L129"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="E128" sqref="E128"/>
+      <selection activeCell="E129" sqref="E129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -6713,6 +6716,23 @@
       </c>
       <c r="E128" t="s">
         <v>1337</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A129" s="8">
+        <v>117.1</v>
+      </c>
+      <c r="B129" s="1">
+        <v>45408</v>
+      </c>
+      <c r="C129" s="8" t="s">
+        <v>427</v>
+      </c>
+      <c r="D129">
+        <v>27851</v>
+      </c>
+      <c r="E129" t="s">
+        <v>1338</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TFS 28262 - CCO Motivate and Increase CSR-Level Promotions. Additional changes from V&V and UAT.
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C53995
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Log_Dimension_Table_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TFS\eCoaching_V2\Design\DD\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F6DC812-376E-490F-85D1-3F4A8357A9AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{734A2C26-66B9-452B-861C-8B6A91A993C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57504" yWindow="1914" windowWidth="28992" windowHeight="15672" firstSheet="29" activeTab="34" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_History" sheetId="14" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5356" uniqueCount="1341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5358" uniqueCount="1342">
   <si>
     <t>SourceID</t>
   </si>
@@ -4134,10 +4134,13 @@
     <t>CSR Uptraining Eligibility Feed</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;p&gt;According to the current active roster and certification data, this CSR has exceeded 6 months’ tenure in their current role and may be eligible for promotional/uptraining opportunities when new positions become available. As a supervisor, the support, guidance, and encouragement you offer to our CSRs is critical to building our internal candidate pool. Meet with your CSR to discuss their interest in future promotional opportunities, goals, and next steps. Refer to the [Motivational Coaching eLM] for more information, including tips for addressing promotional concerns and setting goals for career advancement.&lt;/p&gt;    &lt;p&gt;Note: When discussing and planning promotional opportunities with a CSR, be sure to confirm the status of any recently issued written warnings. If the CSR has been issued a written warning within 91 days of apply for a new position, they may be ineligible for promotion until that period has lapsed.&lt;/p&gt; </t>
-  </si>
-  <si>
     <t>TFS 28262 - CCO Motivate and Increase CSR-Level Promotions. Added records to DIM_Sub_Coaching_Reason, DIM_Feed_List and Feed_Contact and Coaching_Log_StaticText tables.</t>
+  </si>
+  <si>
+    <t>TFS 28262 - CCO Motivate and Increase CSR-Level Promotions. Updated text for TextID 104 on  Coaching_Log_StaticText tab.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;According to the current active roster and certification data, this CSR has exceeded 6 months’ tenure in their current role and may be eligible for promotional/uptraining opportunities when new positions become available. As a supervisor, the support, guidance, and encouragement you offer to our CSRs is critical to building our internal candidate pool. Meet with your CSR to discuss their interest in future promotional opportunities, goals, and next steps. Refer to the 2024 Career Path eLearning Module for Supervisors: Encouraging and Motivating Employee Promotions for more information, including tips for addressing promotional concerns and setting goals for career advancement.&lt;/p&gt;&lt;p&gt;Note: When discussing and planning promotional opportunities with a CSR, be sure to confirm the status of any recently issued written warnings. If the CSR has been issued a written warning within 91 days of applying for a new position, they may be ineligible for promotion until that period has lapsed.&lt;/p&gt;</t>
   </si>
 </sst>
 </file>
@@ -4222,7 +4225,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -4245,6 +4248,7 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4549,10 +4553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L131"/>
+  <dimension ref="A1:L132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C115" workbookViewId="0">
-      <selection activeCell="C131" sqref="C131"/>
+    <sheetView topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="E132" sqref="E132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -6761,6 +6765,12 @@
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A131" s="5">
+        <v>119</v>
+      </c>
+      <c r="B131" s="16">
+        <v>45461</v>
+      </c>
       <c r="C131" s="5" t="s">
         <v>418</v>
       </c>
@@ -6768,6 +6778,23 @@
         <v>28262</v>
       </c>
       <c r="E131" s="5" t="s">
+        <v>1339</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A132" s="5">
+        <v>119.1</v>
+      </c>
+      <c r="B132" s="16">
+        <v>45482</v>
+      </c>
+      <c r="C132" s="5" t="s">
+        <v>418</v>
+      </c>
+      <c r="D132" s="5">
+        <v>28262</v>
+      </c>
+      <c r="E132" s="5" t="s">
         <v>1340</v>
       </c>
     </row>
@@ -50994,11 +51021,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE8E5AAB-2CB2-47A7-AC59-8DE4502992B4}">
   <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:O5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="2" max="2" width="22.83984375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
@@ -51181,7 +51211,7 @@
         <v>104</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>1339</v>
+        <v>1341</v>
       </c>
       <c r="C5" s="5">
         <v>1</v>

</xml_diff>